<commit_message>
show age question answer choices as a dropdown list
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -5388,13 +5388,11 @@
 您尚未进行选择。请重新开始，并为每个问题选择选项，以便我可以帮助您提供护理建议。</v>
       </c>
       <c r="F214" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Seleccione una opción para que pueda aconsejarlo sobre la atención médica..**_x000d_
-_x000d_
+        <v xml:space="preserve">**Seleccione una opción para que pueda aconsejarlo sobre la atención médica.**
 No ha seleccionado ninguna opción. Vuelva a comenzar y seleccione opciones para cada pregunta; así podré aconsejarlo sobre la atención médica.</v>
       </c>
       <c r="G214" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Seleccione una opción para que pueda aconsejarlo sobre la atención médica..**_x000d_
-_x000d_
+        <v xml:space="preserve">**Seleccione una opción para que pueda aconsejarlo sobre la atención médica.**
 No ha seleccionado ninguna opción. Vuelva a comenzar y seleccione opciones para cada pregunta; así podré aconsejarlo sobre la atención médica.</v>
       </c>
     </row>
@@ -5948,45 +5946,27 @@
         <v>) para que lo redirijamos a ella.</v>
       </c>
     </row>
-    <row r="229" xml:space="preserve">
+    <row r="229">
       <c r="A229" t="str">
         <v>CDC/messages/local_a</v>
       </c>
-      <c r="B229" t="str" xml:space="preserve">
-        <v xml:space="preserve">_x000d_
-    _x000d_
-Please also see your local area’s website:_x000d_
-[</v>
-      </c>
-      <c r="C229" t="str" xml:space="preserve">
-        <v xml:space="preserve">_x000d_
-_x000d_
-해당 지역의 웹사이트를 참조하십시오._x000d_
-[</v>
-      </c>
-      <c r="D229" t="str" xml:space="preserve">
-        <v xml:space="preserve">_x000d_
-_x000d_
-Vui lòng xem trang web của khu vực địa phương quý vị:_x000d_
-[</v>
-      </c>
-      <c r="E229" t="str" xml:space="preserve">
-        <v xml:space="preserve">_x000d_
-_x000d_
-还请查看您所在地区的网站：_x000d_
-[</v>
-      </c>
-      <c r="F229" t="str" xml:space="preserve">
-        <v xml:space="preserve">_x000d_
-_x000d_
-También consulte el sitio web de su área local:_x000d_
-[</v>
-      </c>
-      <c r="G229" t="str" xml:space="preserve">
-        <v xml:space="preserve">_x000d_
-_x000d_
-También consulte el sitio web de su área local:_x000d_
-[</v>
+      <c r="B229" t="str">
+        <v>\n\nPlease also see your local area’s website: \n[</v>
+      </c>
+      <c r="C229" t="str">
+        <v>\n\n해당 지역의 웹사이트를 참조하십시오: \n[</v>
+      </c>
+      <c r="D229" t="str">
+        <v>\n\nVui lòng xem trang web của khu vực địa phương quý vị: \n[</v>
+      </c>
+      <c r="E229" t="str">
+        <v>\n\n还请查看您所在地区的网站：\n[</v>
+      </c>
+      <c r="F229" t="str">
+        <v>\n\nTambién consulte el sitio web de su área local: \n[</v>
+      </c>
+      <c r="G229" t="str">
+        <v>\n\nTambién consulte el sitio web de su área local: \n[</v>
       </c>
     </row>
     <row r="230">
@@ -6375,19 +6355,19 @@
         <v>Please select an age</v>
       </c>
       <c r="C242" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="D242" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="E242" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="F242" t="str">
-        <v/>
+        <v>-</v>
       </c>
       <c r="G242" t="str">
-        <v/>
+        <v>-</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade to algorithm version 60 for English scenarios and localization file
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G242"/>
+  <dimension ref="A1:G252"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2777,7 +2777,7 @@
         <v>CDC/comorbidity/chronic_lung</v>
       </c>
       <c r="B105" t="str">
-        <v>Chronic lung disease, moderate to severe asthma, or smoking</v>
+        <v>Chronic lung disease, moderate to severe asthma</v>
       </c>
       <c r="C105" t="str">
         <v>만성 폐 질환, 중등도 내지 중증의 천식 또는 흡연</v>
@@ -2869,7 +2869,7 @@
         <v>CDC/comorbidity/weak_immune</v>
       </c>
       <c r="B109" t="str">
-        <v>Weakened immune system (cancer treatment, prolonged use of steroids, transplant or HIV/AIDS)</v>
+        <v>Weakened immune system or taking medications that may cause immune suppression</v>
       </c>
       <c r="C109" t="str">
         <v>면역 체계 약화(암 치료, 스테로이드 장기간 사용, 이식 또는 HIV/AIDS)</v>
@@ -2961,7 +2961,7 @@
         <v>CDC/comorbidity/severe_obesity</v>
       </c>
       <c r="B113" t="str">
-        <v>Severe obesity (Body Mass Index [BMI] greater than or equal to 40)</v>
+        <v>Severe obesity</v>
       </c>
       <c r="C113" t="str">
         <v>중증 비만(체질량 지수) [BMI] 40 이상)</v>
@@ -3007,7 +3007,7 @@
         <v>CDC/comorbidity/underlying_conditions</v>
       </c>
       <c r="B115" t="str">
-        <v>Underlying conditions (diabetes, renal failure, or liver disease)</v>
+        <v>Diabetes, renal (kidney) failure, or liver disease</v>
       </c>
       <c r="C115" t="str">
         <v>기저 질환(당뇨병, 신부전 또는 간 질환)</v>
@@ -4019,7 +4019,7 @@
         <v>CDC/location_question</v>
       </c>
       <c r="B159" t="str">
-        <v>Where are you located?</v>
+        <v>Are you in the United States right now?</v>
       </c>
       <c r="C159" t="str">
         <v>귀하는 어디에 계십니까?</v>
@@ -4065,7 +4065,7 @@
         <v>CDC/location_response</v>
       </c>
       <c r="B161" t="str">
-        <v>["United States","Outside the US"]</v>
+        <v>["Yes","No"]</v>
       </c>
       <c r="C161" t="str">
         <v>["미국","미국 이외의 지역"]</v>
@@ -4111,7 +4111,7 @@
         <v>CDC/location_error</v>
       </c>
       <c r="B163" t="str">
-        <v>You must select a location to proceed.</v>
+        <v>Please select a location to keep using the self-checker</v>
       </c>
       <c r="C163" t="str">
         <v>계속 진행하려면 지역을 선택해야 합니다.</v>
@@ -4341,7 +4341,7 @@
         <v>CDC/age_response</v>
       </c>
       <c r="B173" t="str">
-        <v>["Younger than 2 years old","2-4 years","5-9","10-18","19-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
+        <v>["Under 18 years old","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="C173" t="str">
         <v>["2세 미만","2-4세","5-9","10-18","19-29","30-39","40-49","50-59","60-64","65-69","70-79","80세 이상"]</v>
@@ -4479,7 +4479,7 @@
         <v>CDC/second_person_questions/ppe</v>
       </c>
       <c r="B179" t="str">
-        <v>Did you wear all recommended personal protective equipment while you were caring for or in close contact with someone diagnosed with COVID-19?</v>
+        <v>Did you wear all recommended personal protective equipment while you were in close contact with someone diagnosed with COVID-19?</v>
       </c>
       <c r="C179" t="str">
         <v>COVID-19 진단을 받은 사람을 보살피거나 가까이 접촉하는 동안 권장 개인 보호 장비를 모두 착용했습니까?</v>
@@ -4778,7 +4778,7 @@
         <v>CDC/second_person_questions/hcf_question</v>
       </c>
       <c r="B192" t="str">
-        <v>In the last two weeks have you worked or volunteered in a hospital, emergency room, clinic, medical office, long-term care facility or nursing home, ambulance service, first responder services, or any health care setting or taken care of patients as a student or part of your work?</v>
+        <v>In the last two weeks, have you worked or volunteered in a healthcare facility or as a first responder? Facilities include a hospital, other medical setting, or long-term care facility.</v>
       </c>
       <c r="C192" t="str">
         <v>지난 2주 동안 병원, 응급실, 클리닉, 진료소, 장기 요양 시설 또는 요양원, 구급차 서비스, 초동 대응 서비스 또는 기타 의료 환경에서 근무하거나 자원봉사하거나 학생 자격 또는 일의 일부로서 환자를 치료한 적이 있습니까?</v>
@@ -4847,7 +4847,7 @@
         <v>CDC/second_person_questions/risk_factor_question</v>
       </c>
       <c r="B195" t="str">
-        <v>Do you have any of the following conditions (check any)</v>
+        <v>Do any of these apply to you? (check any)</v>
       </c>
       <c r="C195" t="str">
         <v>다음 질환 중 해당 사항이 있습니까?(해당 사항에 모두 체크)</v>
@@ -4869,9 +4869,8 @@
       <c r="A196" t="str">
         <v>CDC/second_person_questions/exposure_question</v>
       </c>
-      <c r="B196" t="str" xml:space="preserve">
-        <v xml:space="preserve">In the two weeks before you felt sick, did you:
-- Have contact with someone diagnosed with COVID-19\n- Live in or visit a place where COVID-19 is spreading</v>
+      <c r="B196" t="str">
+        <v>In the two weeks before you felt sick, did you have contact with someone diagnosed with COVID-19?</v>
       </c>
       <c r="C196" t="str" xml:space="preserve">
         <v xml:space="preserve">아프기 2주 전에 다음과 같은 일이 발생했나요?_x000d_
@@ -4904,7 +4903,7 @@
         <v>CDC/third_person_questions/ppe</v>
       </c>
       <c r="B197" t="str">
-        <v>Did they wear all recommended personal protective equipment while they were caring for or in close contact with someone diagnosed with COVID-19?</v>
+        <v>Did they wear all recommended personal protective equipment while they were in close contact with someone diagnosed with COVID-19?</v>
       </c>
       <c r="C197" t="str">
         <v>그 사람이 COVID-19 진단을 받은 사람을 보살피거나 가까이 접촉하는 동안 권장 개인 보호 장비를 모두 착용했습니까?</v>
@@ -5065,7 +5064,7 @@
         <v>CDC/third_person_questions/hcf_question</v>
       </c>
       <c r="B204" t="str">
-        <v>In the last two weeks have they worked or volunteered in a hospital, emergency room, clinic, medical office, long-term care facility or nursing home, ambulance service, first responder services, or any health care setting or taken care of patients as a student or part of their work?</v>
+        <v>In the last two weeks, have they worked or volunteered in a healthcare facility or as a first responder? Facilities include a hospital, other medical setting, or long-term care facility.</v>
       </c>
       <c r="C204" t="str">
         <v>그 사람이 지난 2주 동안 병원, 응급실, 클리닉, 진료소, 장기 요양 시설 또는 요양원, 구급차 서비스, 초동 대응 서비스 또는 기타 의료 환경에서 근무하거나 자원봉사하거나 학생이나 일의 일부로서 환자를 치료한 적이 있습니까?</v>
@@ -5134,7 +5133,7 @@
         <v>CDC/third_person_questions/risk_factor_question</v>
       </c>
       <c r="B207" t="str">
-        <v>Do they have any of the following conditions (check any)</v>
+        <v>Do any of these apply to them? (check any)</v>
       </c>
       <c r="C207" t="str">
         <v>그 사람에게 다음 질환 중 해당 사항이 있습니까?(해당 사항에 모두 체크)</v>
@@ -5156,9 +5155,8 @@
       <c r="A208" t="str">
         <v>CDC/third_person_questions/exposure_question</v>
       </c>
-      <c r="B208" t="str" xml:space="preserve">
-        <v xml:space="preserve">In the two weeks before they felt sick, did they:
-- Have contact with someone diagnosed with COVID-19\n- Live in or visit a place where COVID-19 is spreading</v>
+      <c r="B208" t="str">
+        <v>In the two weeks before they felt sick, did they have contact with someone diagnosed with COVID-19?</v>
       </c>
       <c r="C208" t="str" xml:space="preserve">
         <v xml:space="preserve">그 사람이 아프기 2주 전에 다음과 같은 일이 발생했나요?_x000d_
@@ -5226,7 +5224,7 @@
         <v>CDC/messages/decline_msg</v>
       </c>
       <c r="B210" t="str">
-        <v>Your consent is required to use the Coronavirus Self-Checker.</v>
+        <v>Please consent to use the Coronavirus Self-Checker.</v>
       </c>
       <c r="C210" t="str">
         <v>Coronavirus Self-Checker를 사용하려면 동의해야 합니다.</v>
@@ -5249,13 +5247,9 @@
         <v>CDC/messages/intro_msg</v>
       </c>
       <c r="B211" t="str" xml:space="preserve">
-        <v xml:space="preserve">Hi, I’m Clara. I’m here to guide you through the Coronavirus Self-Checker._x000d_
-_x000d_
-If you are experiencing a life-threatening emergency, please call 911 immediately. _x000d_
-_x000d_
-This system does not replace the judgment of healthcare professionals or the performance of any clinical assessment.  _x000d_
-_x000d_
-To provide information on the right level of care, we are going to ask you a series of questions.</v>
+        <v xml:space="preserve">Hi, I’m Clara. I’m  going to ask you some questions. I will use your answers to give you advice about the right level of medical care you should seek. 
+But first, if you are experiencing a life-threatening emergency, please call 911 immediately. 
+If you are not experiencing a life-threatening emergency, let’s get started.</v>
       </c>
       <c r="C211" t="str" xml:space="preserve">
         <v xml:space="preserve">안녕하세요? 저는 Clara입니다. 제가 Coronavirus Self-Checker를 안내해 드리겠습니다._x000d_
@@ -5307,10 +5301,8 @@
       <c r="A212" t="str">
         <v>CDC/messages/instruct_msg</v>
       </c>
-      <c r="B212" t="str" xml:space="preserve">
-        <v xml:space="preserve">During the assessment, you can refresh the page if you need to start again_x000d_
-_x000d_
-Ready? Let’s get started.</v>
+      <c r="B212" t="str">
+        <v>During the assessment, you can refresh the page if you need to start again.</v>
       </c>
       <c r="C212" t="str" xml:space="preserve">
         <v xml:space="preserve">평가 중 다시 시작해야 하는 경우 페이지를 새로 고치면 됩니다._x000d_
@@ -5328,15 +5320,11 @@
 准备好了吗？ 我们开始吧。</v>
       </c>
       <c r="F212" t="str" xml:space="preserve">
-        <v xml:space="preserve">Durante la evaluación, puede actualizar la página si necesita empezar de nuevo._x000d_
-_x000d_
-_x000d_
+        <v xml:space="preserve">Durante la evaluación, puede actualizar la página si necesita empezar de nuevo.
 ¿Todo listo? Empecemos.</v>
       </c>
       <c r="G212" t="str" xml:space="preserve">
-        <v xml:space="preserve">Durante la evaluación, puede actualizar la página si necesita empezar de nuevo._x000d_
-_x000d_
-_x000d_
+        <v xml:space="preserve">Durante la evaluación, puede actualizar la página si necesita empezar de nuevo.
 ¿Todo listo? Empecemos.</v>
       </c>
     </row>
@@ -5368,9 +5356,8 @@
         <v>CDC/messages/msg0</v>
       </c>
       <c r="B214" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Please make a selection so I can help give you care advice.**_x000d_
-_x000d_
-You have not made a selection. Please start again and select options for each question so that I can help give you care advice.</v>
+        <v xml:space="preserve">**Please make a selection so I can help give you care advice.**
+You have not made a selection. Please start again and select options for each question so that I can help give you advice.</v>
       </c>
       <c r="C214" t="str" xml:space="preserve">
         <v xml:space="preserve">**제가 치료 조언을 제공할 수 있도록 옵션을 선택하십시오.**_x000d_
@@ -5383,8 +5370,7 @@
 Quý vị chưa đưa ra lựa chọn. Vui lòng bắt đầu lại và chọn câu trả lời cho mỗi câu hỏi để tôi có thể giúp quý vị đưa ra lời khuyên về chăm sóc y tế cần thiết.</v>
       </c>
       <c r="E214" t="str" xml:space="preserve">
-        <v xml:space="preserve">**请做出选择，以便我可以帮助您提供护理建议。**_x000d_
-_x000d_
+        <v xml:space="preserve">**请做出选择，以便我可以帮助您提供护理建议**
 您尚未进行选择。请重新开始，并为每个问题选择选项，以便我可以帮助您提供护理建议。</v>
       </c>
       <c r="F214" t="str" xml:space="preserve">
@@ -5416,8 +5402,7 @@
 Tìm hiểu thêm về COVID-19 và những điều quý vị có thể làm để đảm bảo an toàn trên [trang web của CDC](https://www.cdc.gov/coronavirus/2019-ncov/index.html).</v>
       </c>
       <c r="E215" t="str" xml:space="preserve">
-        <v xml:space="preserve">**听起来您感觉很好。**_x000d_
-_x000d_
+        <v xml:space="preserve">**听起来您感觉很好**
 请访问[ CDC 网站](https://www.cdc.gov/coronavirus/2019-ncov/index.html)，了解更多关于新冠肺炎的信息和您可以做什么来保持安全。</v>
       </c>
       <c r="F215" t="str" xml:space="preserve">
@@ -5457,10 +5442,8 @@
 Nói với tổng đài 911 nếu quý vị đã tiếp xúc với ai đó nhiễm COVID-19 hoặc nếu gần đây quý vị đã đến một khu vực mà COVID-19 đang lan rộng.</v>
       </c>
       <c r="E216" t="str" xml:space="preserve">
-        <v xml:space="preserve">**拨打 911 - 您可能出现医疗紧急情况。**_x000d_
-_x000d_
-现在拨打 911。需要立即就医。_x000d_
-_x000d_
+        <v xml:space="preserve">**拨打 911 - 您可能出现医疗紧急情况**
+现在拨打 911。需要立即就医。
 如果您与新冠肺炎患者接触或如果您最近去过新冠肺炎传播的地区，请告知 911 接线员。</v>
       </c>
       <c r="F216" t="str" xml:space="preserve">
@@ -5483,9 +5466,8 @@
         <v>CDC/messages/msg3</v>
       </c>
       <c r="B217" t="str" xml:space="preserve">
-        <v xml:space="preserve">**This Coronavirus Self-Checker is for people who are at least 2 years old.**_x000d_
-_x000d_
-Visit the [CDC website](https://www.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html) to get information on COVID-19 and children.</v>
+        <v xml:space="preserve">**This Coronavirus Self-Checker is for people who are at least 18 years old.**
+Visit the [CDC website](https://www.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html) to get information on COVID-19 and younger people.</v>
       </c>
       <c r="C217" t="str" xml:space="preserve">
         <v xml:space="preserve">**이 Coronavirus Self-Checker는 2세 이상인 사람들을 위한 것입니다.**_x000d_
@@ -5498,8 +5480,7 @@
 Truy cập [trang web của CDC](https://www.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html) để có được thông tin về COVID-19 và trẻ em.</v>
       </c>
       <c r="E217" t="str" xml:space="preserve">
-        <v xml:space="preserve">**这种冠状病毒自我检查问卷是针对至少 2 岁的人。**_x000d_
-_x000d_
+        <v xml:space="preserve">**这种冠状病毒自我检查问卷是针对至少 2 岁的人**
 访问 [ CDC 网站 ](https://www.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html)来获得关于新冠肺炎和儿童的信息。</v>
       </c>
       <c r="F217" t="str" xml:space="preserve">
@@ -5518,11 +5499,9 @@
         <v>CDC/messages/msg4</v>
       </c>
       <c r="B218" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Urgent medical attention may be needed. Please call 911 or go to the Emergency Department.**_x000d_
-_x000d_
-Based on your symptoms, urgent medical attention may be needed. Please call 911 or go to the nearest emergency department._x000d_
-_x000d_
-Tell the 911 operator or emergency staff if you have had contact with someone with COVID-19 or if you have recently been to an area where COVID-19 is spreading.</v>
+        <v xml:space="preserve">**Urgent medical attention may be needed. Please call 911 or go to the Emergency Department.**
+Based on your symptoms, you may need urgent medical care. Please call 911 or go to the nearest emergency department.
+Tell the 911 operator or emergency staff if you have had contact with someone with COVID-19.</v>
       </c>
       <c r="C218" t="str" xml:space="preserve">
         <v xml:space="preserve">**긴급한 치료가 필요할 수 있습니다. 911에 전화하거나 응급실로 가십시오.**_x000d_
@@ -5539,10 +5518,8 @@
 Nói với tổng đài 911 hoặc nhân viên cấp cứu nếu quý vị đã tiếp xúc với ai đó nhiễm COVID-19 hoặc nếu gần đây quý vị đã đến một khu vực mà COVID-19 đang lan rộng.</v>
       </c>
       <c r="E218" t="str" xml:space="preserve">
-        <v xml:space="preserve">**可能需要紧急医疗护理。请拨打 911 或到急诊科就诊。**_x000d_
-_x000d_
-根据您的症状，可能需要紧急医疗护理。请拨打 911 或到最近的急诊科就诊。_x000d_
-_x000d_
+        <v xml:space="preserve">**可能需要紧急医疗护理。请拨打 911 或到急诊科就诊**
+根据您的症状，可能需要紧急医疗护理。请拨打 911 或到最近的急诊科就诊。
 如果您与新冠肺炎患者有过接触，或者如果您最近去过新冠肺炎传播的地区，请告知 911 接线员或急救人员。</v>
       </c>
       <c r="F218" t="str" xml:space="preserve">
@@ -5565,11 +5542,16 @@
         <v>CDC/messages/msg5</v>
       </c>
       <c r="B219" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Call a medical provider within 24 hours.**_x000d_
-  _x000d_
-Sorry you’re feeling ill. You have one or more symptoms that may be related to COVID-19. You also have medical conditions that may put you at more risk of illness. Call your healthcare provider, clinician advice line, or telemedicine provider within 24 hours.  Start home isolation. This means stay home except to get medical care, and do not go to work, school, or public areas. Do not use public transportation or ride sharing. Be sure to get care if you feel worse._x000d_
-_x000d_
-Read important information about [caring for yourself](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) or [someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html) and follow these steps to help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
+        <v xml:space="preserve">**Call a medical provider within 24 hours.**
+Sorry you’re not feeling well. Your symptoms may be related to COVID-19. You also have medical conditions that may put you at risk of becoming more seriously ill.
+- Call your healthcare provider, clinician advice line, or telemedicine provider within 24 hours.
+- Stay home except to get medical care.
+  - Do not go to work, school, or public areas.
+  - Do not use public transportation or ride sharing.
+- If you feel worse or you think it is an emergency, seek medical care.
+- Find [telehealth](https://telehealth.hhs.gov/) services.
+- Learn how to [take care of yourself](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) or [someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html).
+- Take these steps to help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
       </c>
       <c r="C219" t="str" xml:space="preserve">
         <v xml:space="preserve">**24시간 내에 의료진에게 전화하십시오.**_x000d_
@@ -5586,10 +5568,8 @@
 Đọc thông tin quan trọng về [tự chăm sóc](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) hoặc [chăm sóc ai đó bị bệnh](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html) và thực hiện theo các bước để giúp [bảo vệ những người khác không bị nhiễm bệnh](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
       </c>
       <c r="E219" t="str" xml:space="preserve">
-        <v xml:space="preserve">**在 24 小时内致电医疗服务提供者。**_x000d_
-  _x000d_
-听到您说感觉不舒服，我们很遗憾。您有一个或多个可能与新冠肺炎相关的症状。您还患有可能使您面临更高患病风险的疾病。在 24 小时内致电您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。开始居家隔离。这意味着除了得到医疗护理外，都要待在在家里，不要去工作、上学或公共区域。不要乘公共交通工具或拼车。如果您感觉恶化，请务必接受诊疗护理。_x000d_
-_x000d_
+        <v xml:space="preserve">**在 24 小时内致电医疗服务提供者**
+听到您说感觉不舒服，我们很遗憾。您有一个或多个可能与新冠肺炎相关的症状。您还患有可能使您面临更高患病风险的疾病。在 24 小时内致电您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。开始居家隔离。这意味着除了得到医疗护理外，都要待在在家里，不要去工作、上学或公共区域。不要乘公共交通工具或拼车。如果您感觉恶化，请务必接受诊疗护理。
 阅读有[](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)[关照顾自己或生病的其他人的重要信息，并遵循这些措施，以帮助保护他人免于生病。](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)[](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)</v>
       </c>
       <c r="F219" t="str" xml:space="preserve">
@@ -5612,9 +5592,8 @@
         <v>CDC/messages/msg6</v>
       </c>
       <c r="B220" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Contact the occupational health provider at your workplace immediately.**_x000d_
-_x000d_
-Please contact the occupational health provider (or supervisor) in your healthcare facility as soon as possible and let them know you’re feeling ill.</v>
+        <v xml:space="preserve">**Contact the occupational health provider at your workplace immediately.**
+Tell the occupational health provider (or supervisor) in your workplace that you’re feeling ill as soon as possible.</v>
       </c>
       <c r="C220" t="str" xml:space="preserve">
         <v xml:space="preserve">**직장의 직장 위생 전문가에게 즉시 연락하십시오.**_x000d_
@@ -5627,8 +5606,7 @@
 Vui lòng liên hệ với nhà cung cấp dịch vụ sức khỏe nghề nghiệp (hoặc cán bộ giám sát) tại cơ sở chăm sóc sức khỏe của quý vị càng sớm càng tốt và cho họ biết quý vị bị bệnh.</v>
       </c>
       <c r="E220" t="str" xml:space="preserve">
-        <v xml:space="preserve">**立即联系工作场所的职业保健提供者。**_x000d_
-_x000d_
+        <v xml:space="preserve">**立即联系工作场所的职业保健提供者**
 请尽快联系您医疗保健机构的职业保健提供者（或监督员），并告知他们您感觉不适。</v>
       </c>
       <c r="F220" t="str" xml:space="preserve">
@@ -5647,12 +5625,12 @@
         <v>CDC/messages/msg7</v>
       </c>
       <c r="B221" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Contact a healthcare provider in the long-term care facility where you live.**_x000d_
-_x000d_
-Living in a long-term care facility or nursing home may put you at a higher risk for severe illness. Tell a caregiver at the facility that you are sick and need to see a medical provider as soon as possible._x000d_
-_x000d_
-Help protect others from getting sick:_x000d_
-- Stay in your room except to get medical care\n- Cover your coughs and sneezes\n- Clean your hands often</v>
+        <v xml:space="preserve">**Contact a healthcare provider in the long-term care facility where you live.**
+Tell a caregiver in your facility that you are sick and need to see a medical provider as soon as possible. Living in a long-term care facility or nursing home may put you at a higher risk for severe illness.
+Help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):
+- Stay in your room except to get medical care
+- Cover your coughs and sneezes
+- Clean your hands often</v>
       </c>
       <c r="C221" t="str" xml:space="preserve">
         <v xml:space="preserve">**거주하는 장기 요양 시설에서 의료진에게 문의하십시오.**_x000d_
@@ -5671,11 +5649,9 @@
 - Ở trong phòng của quý vị trừ khi cần nhận chăm sóc y tế\n- Che mũi miệng khi ho và hắt hơi\n- Rửa tay thường xuyên</v>
       </c>
       <c r="E221" t="str" xml:space="preserve">
-        <v xml:space="preserve">**联系您居住的长期护理机构的医疗保健提供者。**_x000d_
-_x000d_
-生活在长期护理机构或疗养院可能会使您患严重疾病的风险更高。告知机构的看护者您生病，需要尽快就医。_x000d_
-_x000d_
-帮助保护他人免于生病：_x000d_
+        <v xml:space="preserve">**联系您居住的长期护理机构的医疗保健提供者**
+生活在长期护理机构或疗养院可能会使您患严重疾病的风险更高。告知机构的看护者您生病，需要尽快就医。
+帮助保护他人免于生病：
 - 除进行医疗保健之外，请待在家里\n- 遮挡咳嗽和喷嚏\n- 经常洗手</v>
       </c>
       <c r="F221" t="str" xml:space="preserve">
@@ -5700,11 +5676,14 @@
         <v>CDC/messages/msg8</v>
       </c>
       <c r="B222" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Stay home and take care of yourself. Call your provider if you get worse**_x000d_
-_x000d_
-Sorry you’re feeling ill. You have one or more symptom(s) that may be related to COVID-19. Stay home and take care of yourself. This means stay home except to get medical care, and do not go to work, school, or public areas. Do not use public transportation or ride sharing. Be sure to get care if you feel worse or you think it is an emergency._x000d_
-_x000d_
-Read important information about [caring for yourself](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) or [someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html) and follow these steps to help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
+        <v xml:space="preserve">**Stay home and take care of yourself. Call your provider if you get worse**
+Sorry you’re not feeling well. Your symptoms may be related to COVID-19.
+- Stay home except to get medical care.
+    - Do not go to work, school, or public areas. 
+    - Do not use public transportation or ride sharing. 
+- If you feel worse or you think it is an emergency, seek medical care.
+- Learn how to [take care of yourself](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) or [someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html).
+- Take steps to help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
       </c>
       <c r="C222" t="str" xml:space="preserve">
         <v xml:space="preserve">**집에 머물면서 자신을 돌보십시오. 상태가 나빠질 경우 의료진에게 연락하십시오**_x000d_
@@ -5721,10 +5700,8 @@
 Đọc thông tin quan trọng về [tự chăm sóc](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) hoặc [chăm sóc ai đó bị bệnh](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html) và thực hiện theo các bước để giúp [bảo vệ những người khác không bị nhiễm bệnh](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
       </c>
       <c r="E222" t="str" xml:space="preserve">
-        <v xml:space="preserve">**待在家里照顾自己。如果您恶化，请致电您的医疗服务提供者 **_x000d_
-_x000d_
-听到您说感觉不舒服，我们很遗憾。您有一个或多个可能与新冠肺炎相关的症状。待在家里照顾自己。这意味着除了得到医疗护理外，都要待在家里，不要去工作、上学或公共区域。不要乘公共交通工具或拼车。如果您感觉恶化或您认为是紧急情况，请务必进行护理。_x000d_
-_x000d_
+        <v xml:space="preserve">**待在家里照顾自己。如果您恶化，请致电您的医疗服务提供者**
+听到您说感觉不舒服，我们很遗憾。您有一个或多个可能与新冠肺炎相关的症状。待在家里照顾自己。这意味着除了得到医疗护理外，都要待在家里，不要去工作、上学或公共区域。不要乘公共交通工具或拼车。如果您感觉恶化或您认为是紧急情况，请务必进行护理。
 阅读有[](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)[关照顾自己或生病的其他人的重要信息，并遵循这些措施，以帮助保护他人免于生病。](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)[](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)</v>
       </c>
       <c r="F222" t="str" xml:space="preserve">
@@ -5747,11 +5724,16 @@
         <v>CDC/messages/msg9</v>
       </c>
       <c r="B223" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Stay home and take care of yourself. Call a medical provider within 24 hours.**_x000d_
-_x000d_
-Sorry you’re feeling ill. You have one or more symptoms that may be related to COVID-19. Stay home and take care of yourself. This means stay home except to get medical care, and do not go to work, school, or public areas. Do not use public transportation or ride sharing. Be sure to get care if you feel worse or you think it is an emergency._x000d_
-_x000d_
-Read important information about [caring for yourself](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) or [someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html) and follow these steps to help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
+        <v xml:space="preserve">**Stay home and take care of yourself. Call a medical provider within 24 hours.**
+Sorry you’re not feeling well.  Your symptom(s) may be related to COVID-19. 
+- Call your healthcare provider, clinician advice line, or telemedicine provider within 24 hours. 
+- Stay home except to get medical care. 
+    - Do not go to work, school, or public areas. 
+    - Do not use public transportation or ride sharing.
+- If you feel worse or think this is an emergency, seek medical care.
+- Find [telehealth](https://telehealth.hhs.gov/) services.
+- Learn how to [take care of yourself](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) or [someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html).
+- Take steps to help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
       </c>
       <c r="C223" t="str" xml:space="preserve">
         <v xml:space="preserve">**집에 머물면서 자신을 돌보십시오. 24시간 내에 의료진에게 전화하십시오.**_x000d_
@@ -5768,10 +5750,8 @@
 Đọc thông tin quan trọng về [tự chăm sóc](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) hoặc [chăm sóc ai đó bị bệnh](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html) và thực hiện theo các bước để giúp [bảo vệ những người khác không bị nhiễm bệnh](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
       </c>
       <c r="E223" t="str" xml:space="preserve">
-        <v xml:space="preserve">**待在家里照顾自己。在 24 小时内致电医疗服务提供者。**_x000d_
-_x000d_
-听到您说感觉不舒服，我们很遗憾。您有一个或多个可能与新冠肺炎相关的症状。待在家里照顾自己。在 24 小时内致电您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。开始居家隔离。这意味着除了得到医疗护理外，都要待在家里，不要去工作、上学或公共区域。不要乘公共交通工具或拼车。如果您感觉恶化或您认为是紧急情况，请务必进行护理。_x000d_
-_x000d_
+        <v xml:space="preserve">**待在家里照顾自己。在 24 小时内致电医疗服务提供者**
+听到您说感觉不舒服，我们很遗憾。您有一个或多个可能与新冠肺炎相关的症状。待在家里照顾自己。在 24 小时内致电您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。开始居家隔离。这意味着除了得到医疗护理外，都要待在家里，不要去工作、上学或公共区域。不要乘公共交通工具或拼车。如果您感觉恶化或您认为是紧急情况，请务必进行护理。
 阅读有[](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)[关照顾自己或生病的其他人的重要信息，并遵循这些措施，以帮助保护他人免于生病。](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)[](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)</v>
       </c>
       <c r="F223" t="str" xml:space="preserve">
@@ -5818,11 +5798,9 @@
 - Ở nhà và nghỉ ngơi. \n- Uống nhiều nước và các chất lỏng sạch khác để tránh bị mất nước (sự mất nước).\n- Che mũi miệng khi ho và hắt hơi. \n- Rửa tay thường xuyên.</v>
       </c>
       <c r="E224" t="str" xml:space="preserve">
-        <v xml:space="preserve">**听到您说感觉不舒服，我们很遗憾。待在家里监测症状。如果病情恶化，请致电医疗服务提供者。**_x000d_
-_x000d_
-观察留意[新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。如果您出现上述任何症状或开始感觉恶化，请致电您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。_x000d_
-_x000d_
-以下措施可以帮助您感觉好转：_x000d_
+        <v xml:space="preserve">**听到您说感觉不舒服，我们很遗憾。待在家里监测症状。如果病情恶化，请致电医疗服务提供者**
+观察留意[新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。如果您出现上述任何症状或开始感觉恶化，请致电您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。
+以下措施可以帮助您感觉好转：
 - 在家休息。\n- 饮用大量的水和其他清流质饮品，以免水分流失（脱水）。\n- 咳嗽和打喷嚏时请遮挡。\n- 经常洗手</v>
       </c>
       <c r="F224" t="str" xml:space="preserve">
@@ -5862,8 +5840,7 @@
 Vui lòng kiểm tra với bộ y tế để biết thêm thông tin về COVID-19 tại địa điểm của quý vị.</v>
       </c>
       <c r="E225" t="str" xml:space="preserve">
-        <v xml:space="preserve">**冠状病毒自我检查问卷适用于目前在美国境内居住的人群 **_x000d_
-_x000d_
+        <v xml:space="preserve">**冠状病毒自我检查问卷适用于目前在美国境内居住的人群**
 有关新冠肺炎的更多信息，请咨询您的卫生局门。</v>
       </c>
       <c r="F225" t="str" xml:space="preserve">
@@ -5882,7 +5859,7 @@
         <v>CDC/messages/msg12</v>
       </c>
       <c r="B226" t="str">
-        <v>Please provide your consent in order to use the Coronavirus Self-Checker. Refresh the page to start again.</v>
+        <v>Please consent to use the Coronavirus Self-Checker. Refresh the page to start again.</v>
       </c>
       <c r="C226" t="str">
         <v>Coronavirus Self-Checker를 사용하려면 동의하십시오. 페이지를 새로 고침하여 다시 시작하십시오.</v>
@@ -6020,7 +5997,7 @@
         <v>CDC/messages/msg14</v>
       </c>
       <c r="B232" t="str">
-        <v>If you start to feel ill, contact a healthcare provider in the long-term care facility where you live.</v>
+        <v>If you start to feel ill, tell a healthcare provider in the long-term care facility where you live.</v>
       </c>
       <c r="C232" t="str">
         <v>아프기 시작하면, 거주하는 장기 요양 시설에서 의료진에게 문의하십시오.</v>
@@ -6043,11 +6020,10 @@
         <v>CDC/messages/msg15</v>
       </c>
       <c r="B233" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Contact the occupational health provider at your workplace.**_x000d_
-  _x000d_
-Tell your occupational health provider (or supervisor) that you have been in contact with someone diagnosed with COVID-19. You may be asked to wear a mask to protect yourself and those around you. Check your temperature twice a day for 14 days. Watch for [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)._x000d_
-_x000d_
-Learn more about COVID-19 and steps you can take to protect yourself and others on the [CDC website](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
+        <v xml:space="preserve">**Contact the occupational health provider at your workplace.**
+Tell your occupational health provider (or supervisor) that you have been in contact with someone diagnosed with COVID-19. You may be asked to wear a mask to protect yourself and those around you.
+- Check your temperature twice a day for 14 days. 
+- Watch for [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Learn more about COVID-19 and how you can protect yourself and others on the [CDC website](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
       </c>
       <c r="C233" t="str" xml:space="preserve">
         <v xml:space="preserve">**직장의 직장 위생 전문가에게 연락하십시오.**_x000d_
@@ -6064,10 +6040,8 @@
 Tìm hiểu thêm về COVID-19 và các bước quý vị có thể thực hiện để bảo vệ bản thân và những người khác trên [trang web của CDC](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
       </c>
       <c r="E233" t="str" xml:space="preserve">
-        <v xml:space="preserve">**联系工作场所的职业保健提供者。**_x000d_
-  _x000d_
-告知您的职业保健提供者（或监督员）您接触过诊断为新冠肺炎的人。可能会要求您佩戴口罩以保护自己和周围人。每天检查两次体温，持续 14 天。观察留意[新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。_x000d_
-_x000d_
+        <v xml:space="preserve">**联系工作场所的职业保健提供者**
+告知您的职业保健提供者（或监督员）您接触过诊断为新冠肺炎的人。可能会要求您佩戴口罩以保护自己和周围人。每天检查两次体温，持续 14 天。观察留意[新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。
 访问[ CDC 网站 ](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html)，了解更多关于新冠肺炎和您可以采取的步骤的信息，以保护自己和其他人。</v>
       </c>
       <c r="F233" t="str" xml:space="preserve">
@@ -6108,9 +6082,8 @@
 Tìm hiểu thêm về COVID-19 và các bước quý vị có thể thực hiện để bảo vệ bản thân và những người khác trên [trang web của CDC](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
       </c>
       <c r="E234" t="str" xml:space="preserve">
-        <v xml:space="preserve">**监测症状。**_x000d_
-  _x000d_
-观察留意[新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。如果您出现症状，请致电您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。_x000d_
+        <v xml:space="preserve">**监测症状**
+观察留意[新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。如果您出现症状，请致电您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。
 访问[ CDC 网站 ](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html)，了解更多关于新冠肺炎和您可以采取的步骤的信息，以保护自己和其他人。</v>
       </c>
       <c r="F234" t="str" xml:space="preserve">
@@ -6146,8 +6119,7 @@
 Theo dõi [các triệu chứng COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Nếu quý vị phát triển các triệu chứng, hãy gọi cho nhà cung cấp dịch vụ sức khỏe nghề nghiệp cũng như nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị, đường dây tư vấn bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ sức khỏe từ xa. Vì quý vị làm việc hoặc tham gia hoạt động tình nguyện tại một cơ sở chăm sóc sức khỏe, quý vị có thể được yêu cầu đeo khẩu trang để bảo vệ bản thân và những người xung quanh.</v>
       </c>
       <c r="E235" t="str" xml:space="preserve">
-        <v xml:space="preserve">**监测症状，佩戴口罩。**_x000d_
-  _x000d_
+        <v xml:space="preserve">**监测症状，佩戴口罩**
 观察留意[新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。如果您出现症状，请致电您的职业保健提供者以及您的医疗保健提供者、临床医生建议热线或远程医疗服务提供者。由于您在医疗机构工作或做志愿者，可能会要求您佩戴口罩，以保护您自己和周围的人。</v>
       </c>
       <c r="F235" t="str" xml:space="preserve">
@@ -6166,9 +6138,13 @@
         <v>CDC/messages/msg18</v>
       </c>
       <c r="B236" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Monitor for symptoms, stay at home.**_x000d_
-  _x000d_
-Stay home for 14 days and self-monitor. This includes checking your temperature twice a day and watching for symptoms. Practice social distancing. Maintain 6 feet of distance from others and stay out of crowded places. If possible, stay away from people who are at [higher risk](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/index.html) for getting very sick from COVID-19. Follow [CDC guidance](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) if symptoms develop.</v>
+        <v xml:space="preserve">**Monitor for symptoms, stay at home.**
+- Stay home for 14 days
+- Take your temperature twice a day and watch for [symptoms of COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). 
+- Practice social distancing. 
+    - Stay at least 6 feet away from others and stay out of crowded places. 
+    - If possible, stay away from people who are at [higher risk](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/index.html) for getting very sick from COVID-19. 
+- If you develop symptoms, follow [CDC guidance](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
       </c>
       <c r="C236" t="str" xml:space="preserve">
         <v xml:space="preserve">**증상을 모니터링하고 집에 머무르십시오.**_x000d_
@@ -6181,8 +6157,7 @@
 Ở nhà trong 14 ngày và tự theo dõi. Điều này bao gồm kiểm tra nhiệt độ hai lần một ngày và theo dõi các triệu chứng của quý vị. Thực hiện giãn cách xã hội. Duy trì khoảng cách 6 feet với những người khác và tránh xa những nơi đông người. Nếu có thể, hãy tránh xa những người có [nguy cơ mắc bệnh cao hơn](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/index.html) từ COVID-19. Thực hiện [hướng dẫn của CDC](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) nếu phát triển các triệu chứng.</v>
       </c>
       <c r="E236" t="str" xml:space="preserve">
-        <v xml:space="preserve">**监测症状，待在家里。**_x000d_
-  _x000d_
+        <v xml:space="preserve">**监测症状，待在家里**
 待在家里 14 天，自我监测。这包括每天两次检查您的体温并观察症状。实行社交疏离。与他人保持 6 英尺的距离，并远离拥挤的地方。如果可能，远离因从新冠肺炎患病风险[较高](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/index.html)的人。如果出现症状，请遵循 CDC 指南[](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)。</v>
       </c>
       <c r="F236" t="str" xml:space="preserve">
@@ -6201,9 +6176,8 @@
         <v>CDC/messages/t0</v>
       </c>
       <c r="B237" t="str" xml:space="preserve">
-        <v xml:space="preserve">**No COVID-19 testing needed at this time**_x000d_
-_x000d_
-As of now, your answers suggest you do not need to get tested for COVID-19. If anything changes, take the self-checker again.</v>
+        <v xml:space="preserve">**No COVID-19 testing needed at this time**
+Based on the answers you’ve given, you do not need to get tested for COVID-19 at this time.</v>
       </c>
       <c r="C237" t="str" xml:space="preserve">
         <v xml:space="preserve">**현 시점에서 COVID-19 검사는 필요하지 않습니다**_x000d_
@@ -6216,8 +6190,7 @@
 Tính đến thời điểm này, câu trả lời của quý vị cho thấy quý vị chưa cần phải làm xét nghiệm COVID-19. Nếu có gì thay đổi, hãy tự kiểm tra lại.</v>
       </c>
       <c r="E237" t="str" xml:space="preserve">
-        <v xml:space="preserve">**此时无需进行新冠肺炎测试 **_x000d_
-_x000d_
+        <v xml:space="preserve">**此时无需进行新冠肺炎测试**
 到目前为止，您的回答表明您不需要接受新冠肺炎的测试。如果有任何变化，再次进行自检。</v>
       </c>
       <c r="F237" t="str" xml:space="preserve">
@@ -6251,8 +6224,7 @@
 Để biết thêm thông tin về xét nghiệm COVID-19, hãy gọi cho nhà cung cấp dịch vụ y tế của quý vị hoặc truy cập trang web của sở y tế.</v>
       </c>
       <c r="E238" t="str" xml:space="preserve">
-        <v xml:space="preserve">**关于新冠肺炎测试的信息 **_x000d_
-    _x000d_
+        <v xml:space="preserve">**关于新冠肺炎测试的信息**
 有关新冠肺炎检测的更多信息，请致电您的医疗服务提供者或访问您所在地的卫生局门网站。</v>
       </c>
       <c r="F238" t="str" xml:space="preserve">
@@ -6271,9 +6243,8 @@
         <v>CDC/messages/t2</v>
       </c>
       <c r="B239" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Talk to your provider about COVID-19 testing**_x000d_
-_x000d_
-Your answers suggest you may need to get tested for COVID-19. Talk to your medical provider or visit your health department’s website for more information. Testing access may vary by location and provider.</v>
+        <v xml:space="preserve">**You may be eligible for COVID-19 testing**
+Visit your health department’s website or talk to your healthcare provider for more information. Testing availability may vary by location and provider.</v>
       </c>
       <c r="C239" t="str" xml:space="preserve">
         <v xml:space="preserve">**COVID-19 검사에 대해서는 귀하의 담당 의료진에게 문의하십시오**_x000d_
@@ -6286,8 +6257,7 @@
 Câu trả lời của quý vị cho thấy quý vị có thể cần phải làm xét nghiệm COVID-19. Nói chuyện với nhà cung cấp dịch vụ y tế của quý vị hoặc truy cập trang web của sở y tế để biết thêm thông tin. Việc tiếp cận dịch vụ xét nghiệm có thể khác nhau tùy theo địa điểm và nhà cung cấp dịch vụ.</v>
       </c>
       <c r="E239" t="str" xml:space="preserve">
-        <v xml:space="preserve">**与您的医疗服务提供者讨论新冠肺炎检测 **_x000d_
-_x000d_
+        <v xml:space="preserve">**与您的医疗服务提供者讨论新冠肺炎检测**
 您的回答提示您可能需要接受新冠肺炎检测。如需了解更多信息，请咨询您的医疗服务提供者或访问您所在地的卫生局门网站。获得测试可能因所在地和医疗服务提供者而异。</v>
       </c>
       <c r="F239" t="str" xml:space="preserve">
@@ -6370,9 +6340,266 @@
         <v>-</v>
       </c>
     </row>
+    <row r="243">
+      <c r="A243" t="str">
+        <v>CDC/age_question</v>
+      </c>
+      <c r="B243" t="str">
+        <v>What is your age?</v>
+      </c>
+      <c r="C243" t="str">
+        <v>나이가 어떻게 되십니까?</v>
+      </c>
+      <c r="D243" t="str">
+        <v>Quý vị bao nhiêu tuổi?</v>
+      </c>
+      <c r="E243" t="str">
+        <v>您的年龄是多少?</v>
+      </c>
+      <c r="F243" t="str">
+        <v>¿Cuál es su edad?</v>
+      </c>
+      <c r="G243" t="str">
+        <v>¿Cuál es su edad?</v>
+      </c>
+    </row>
+    <row r="244" xml:space="preserve">
+      <c r="A244" t="str">
+        <v>CDC/life_threat_question</v>
+      </c>
+      <c r="B244" t="str" xml:space="preserve">
+        <v xml:space="preserve">Do you have any of these life-threatening symptoms?
+- Bluish lips or face
+- Severe and constant pain or pressure in the chest
+- Extreme difficulty breathing (gasping for air or cannot talk without catching your breath)
+- Severe and constant dizziness or lightheadedness
+- Serious disorientation (acting confused)
+- Unconscious or very difficult to wake up
+- Slurred speech (new or worsening)
+- Seizures 
+- Signs of low blood pressure (too weak to stand, light headed, feeling cold, pale, clammy skin)</v>
+      </c>
+      <c r="C244" t="str">
+        <v/>
+      </c>
+      <c r="D244" t="str">
+        <v/>
+      </c>
+      <c r="E244" t="str">
+        <v/>
+      </c>
+      <c r="F244" t="str">
+        <v/>
+      </c>
+      <c r="G244" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="str">
+        <v>CDC/yes_no_idk_response</v>
+      </c>
+      <c r="B245" t="str">
+        <v>["Yes", "No", "I don't know"]</v>
+      </c>
+      <c r="C245" t="str">
+        <v/>
+      </c>
+      <c r="D245" t="str">
+        <v/>
+      </c>
+      <c r="E245" t="str">
+        <v/>
+      </c>
+      <c r="F245" t="str">
+        <v/>
+      </c>
+      <c r="G245" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="str">
+        <v>CDC/covid_symptoms/mild_mod_breathing</v>
+      </c>
+      <c r="B246" t="str">
+        <v>Mild or moderate difficulty breathing</v>
+      </c>
+      <c r="C246" t="str">
+        <v/>
+      </c>
+      <c r="D246" t="str">
+        <v/>
+      </c>
+      <c r="E246" t="str">
+        <v/>
+      </c>
+      <c r="F246" t="str">
+        <v/>
+      </c>
+      <c r="G246" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="str">
+        <v>CDC/covid_symptoms/new_loss_taste_smell</v>
+      </c>
+      <c r="B247" t="str">
+        <v>New loss of taste or smell</v>
+      </c>
+      <c r="C247" t="str">
+        <v/>
+      </c>
+      <c r="D247" t="str">
+        <v/>
+      </c>
+      <c r="E247" t="str">
+        <v/>
+      </c>
+      <c r="F247" t="str">
+        <v/>
+      </c>
+      <c r="G247" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="str">
+        <v>CDC/third_person_questions/is_ill_question</v>
+      </c>
+      <c r="B248" t="str">
+        <v>Are they feeling ill?</v>
+      </c>
+      <c r="C248" t="str">
+        <v/>
+      </c>
+      <c r="D248" t="str">
+        <v/>
+      </c>
+      <c r="E248" t="str">
+        <v/>
+      </c>
+      <c r="F248" t="str">
+        <v/>
+      </c>
+      <c r="G248" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="str">
+        <v>CDC/second_person_questions/is_ill_question</v>
+      </c>
+      <c r="B249" t="str">
+        <v>Are you feeling ill?</v>
+      </c>
+      <c r="C249" t="str">
+        <v/>
+      </c>
+      <c r="D249" t="str">
+        <v/>
+      </c>
+      <c r="E249" t="str">
+        <v/>
+      </c>
+      <c r="F249" t="str">
+        <v/>
+      </c>
+      <c r="G249" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="250" xml:space="preserve">
+      <c r="A250" t="str">
+        <v>CDC/third_person_questions/life_threat_question</v>
+      </c>
+      <c r="B250" t="str" xml:space="preserve">
+        <v xml:space="preserve">Do they have any of these life-threatening symptoms?
+- Bluish lips or face
+- Severe and constant pain or pressure in the chest
+- Extreme difficulty breathing (gasping for air or cannot talk without catching your breath)
+- Severe and constant dizziness or lightheadedness
+- Serious disorientation (acting confused)
+- Unconscious or very difficult to wake up
+- Slurred speech (new or worsening)
+- Seizures 
+- Signs of low blood pressure (too weak to stand, light headed, feeling cold, pale, clammy skin)</v>
+      </c>
+      <c r="C250" t="str">
+        <v/>
+      </c>
+      <c r="D250" t="str">
+        <v/>
+      </c>
+      <c r="E250" t="str">
+        <v/>
+      </c>
+      <c r="F250" t="str">
+        <v/>
+      </c>
+      <c r="G250" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="251" xml:space="preserve">
+      <c r="A251" t="str">
+        <v>CDC/second_person_questions/life_threat_question</v>
+      </c>
+      <c r="B251" t="str" xml:space="preserve">
+        <v xml:space="preserve">Do you have any of these life-threatening symptoms?
+- Bluish lips or face
+- Severe and constant pain or pressure in the chest
+- Extreme difficulty breathing (gasping for air or cannot talk without catching your breath)
+- Severe and constant dizziness or lightheadedness
+- Serious disorientation (acting confused)
+- Unconscious or very difficult to wake up
+- Slurred speech (new or worsening)
+- Seizures 
+- Signs of low blood pressure (too weak to stand, light headed, feeling cold, pale, clammy skin)</v>
+      </c>
+      <c r="C251" t="str">
+        <v/>
+      </c>
+      <c r="D251" t="str">
+        <v/>
+      </c>
+      <c r="E251" t="str">
+        <v/>
+      </c>
+      <c r="F251" t="str">
+        <v/>
+      </c>
+      <c r="G251" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="str">
+        <v>CDC/yes_or_idk_no_response</v>
+      </c>
+      <c r="B252" t="str">
+        <v>["Yes or I don't know", "No"]</v>
+      </c>
+      <c r="C252" t="str">
+        <v/>
+      </c>
+      <c r="D252" t="str">
+        <v/>
+      </c>
+      <c r="E252" t="str">
+        <v/>
+      </c>
+      <c r="F252" t="str">
+        <v/>
+      </c>
+      <c r="G252" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G242"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G252"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating Foreign Languages to 66.2
Updating foreign language protocols and localization to match English version at 66.2
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -420,32 +420,24 @@
         <v>Dolor de cabeza</v>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
+    <row r="3">
       <c r="A3" t="str">
         <v>CDC/messages/t50</v>
       </c>
       <c r="B3" t="str">
         <v>**Because some of the symptoms of flu and COVID-19 are similar, you may want to consider asking your provider about testing or treatment for influenza.** See this [CDC webpage](https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm) for more information about COVID-19 and influenza.</v>
       </c>
-      <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)는 담당 의사에게 인플루엔자 검사와 치료에 대해 문의할 것을 고려할 수 있습니다.**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-독감과 COVID-19의 일부 증상이 비슷하기 때문에 증상만으로 둘을 구분하기는 힘드며 진단을 확인하는 데 검사가 필요할 수 있습니다. COVID-19와 인플루엔자에 대한 더 자세한 정보는 이 [CDC 웹페이지](https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm)를 확인하십시오.</v>
-      </c>
-      <c r="D3" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quý vị (họ) có thể hỏi  bác sỹ của mình về việc xét nghiệm và điều trị bệnh cúm.**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-Vì một số triệu chứng của bệnh cúm và COVID-19 giống nhau, có thể khó phân biệt nếu chỉ dựa vào các triệu chứng và có thể cần xét nghiệm để khẳng định. Xem [trang web của CDC] này (https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm) để biết thêm thông tin về COVID-19 và bệnh cúm.</v>
-      </c>
-      <c r="E3" t="str" xml:space="preserve">
-        <v xml:space="preserve">**您（他们）可能会考虑询问您（他们）的医疗服务提供者关于流感的检查和治疗的问题。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-由于流感的一些症状与新冠肺炎相似，仅根据症状可能很难区分两者的差异，可能需要进行检测以帮助确诊。 参见 [CDC 网页]（https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm）获取更多关于新冠肺炎和流感的信息。</v>
-      </c>
-      <c r="F3" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quizás considere preguntarle al proveedor sobre la prueba y el tratamiento de la influenza.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Debido a que algunos de los síntomas de la influenza y el COVID-19 son similares, podría ser difícil diferenciarlos solo con base en los síntomas y podría ser necesaria la prueba para confirmar el diagnóstico. Consulte esta [página web de los CDC](https://espanol.cdc.gov/flu/symptoms/flu-vs-covid19.htm) para obtener más información sobre el COVID-19 y la influenza.</v>
+      <c r="C3" t="str">
+        <v>**독감과 COVID-19의 일부 증상이 비슷하기 때문에 귀하는 제공자에게 인플루엔자 검사와 치료에 대해 문의할 것을 고려할 수 있습니다.** COVID-19와 인플루엔자에 대한 더 자세한 정보는 이 [CDC 웹페이지](https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm)를 확인하십시오.</v>
+      </c>
+      <c r="D3" t="str">
+        <v>**Vì một số triệu chứng của bệnh cúm và COVID-19 tương tự nhau, quý vị có thể cân nhắc việc hỏi nhà cung cấp dịch vụ về việc xét nghiệm hoặc điều trị bệnh cúm.** Xem [trang web CDC] này (https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm) để biết thêm thông tin về COVID-19 và bệnh cúm.</v>
+      </c>
+      <c r="E3" t="str">
+        <v>**由于流感和COVID-19的某些症状相似，您可能需要考虑向您的医疗服务提供者询问有关流感的检测或治疗。**有关COVID-19和流感的更多信息，请参见此[CDC网页](https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm)。</v>
+      </c>
+      <c r="F3" t="str">
+        <v>**Debido a que algunos de los síntomas de la influenza y del COVID-19 son similares, quizás considere preguntarle al proveedor sobre la prueba y el tratamiento de la influenza.** Consulte esta [página web de los CDC](https://espanol.cdc.gov/flu/symptoms/flu-vs-covid19.htm) para obtener más información sobre el COVID-19 y la influenza.</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
@@ -453,70 +445,49 @@
         <v>CDC/messages/t3</v>
       </c>
       <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">**CDC recommends that all close contacts of people with confirmed COVID-19 should:** 
-- get tested **and**
+        <v xml:space="preserve">**CDC recommends that all close contacts of people with confirmed COVID-19 should:** _x000d__x000d_
+- get tested **and**_x000d__x000d_
 - quarantine for 14 days from the day of their last exposure. Based on local testing availability, local authorities may have options to reduce the time people spend in quarantine. You may also receive a call from a contact tracing professional.</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)는 COVID-19 검사를 받아야 합니다.**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-답변에 따라 귀하(그 사람)는 COVID-19에 걸린 사람의 밀접 접촉자입니다._x000d__x000d__x000d__x000d__x000d_
-- 	COVID-19 확진자와 밀접 접촉한 모든 사람이 다음과 같이 할 것을 CDC는 권장합니다:_x000d__x000d__x000d__x000d__x000d_
- -	검사를 받으십시오 **그리고**_x000d__x000d__x000d__x000d__x000d_
- -	마지막으로 노출된 날부터 14일 동안 [격리하십시오](https://korean.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html). 또한 접촉자 추적 조사 전문가의 전화를 받을 수도 있습니다 – 더 자세한 정보를 확인하려면 이 [동영상](https://www.youtube.com/watch?v=u3dLoBj3YLo)을 시청하십시오._x000d__x000d__x000d__x000d__x000d_
- - 	지역 보건부의 권장사항을 준수하십시오._x000d__x000d__x000d__x000d__x000d_
-- 	지역에서 SARS-CoV-2 검사를 이용할 수 있는지의 여부에 따라, 격리를 위해 보내야 하는 시간을 줄일 방법이 있습니다. 더 자세한 정보는 이 [페이지](https://korean.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)를 확인하십시오.</v>
+        <v xml:space="preserve">**COVID-19 확진자와 밀접 접촉한 모든 사람이 다음과 같이 할 것을 CDC는 권장합니다.** _x000d__x000d_
+- 검사를 받으십시오 **그리고**_x000d__x000d_
+- 마지막으로 노출된 날부터 14일 동안 격리하십시오. 지역에서 검사를 이용할 수 있는지의 여부에 따라, 지역 당국이 격리를 위해 보내야 하는 시간을 줄일 방법을 가질 수 있습니다. 또한 추적 전문가의 전화를 받을 수도 있습니다.</v>
       </c>
       <c r="D4" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quý vị (họ) cần được xét nghiệm COVID-19.**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-Dựa trên các câu trả lời đã đưa ra, quý vị (họ) là người tiếp xúc gần với một người mắc COVID-19. _x000d__x000d__x000d__x000d__x000d_
-- 	CDC khuyến cáo rằng tất cả những ai tiếp xúc gần với những người đã được xác nhận mắc COVID-19 nên: _x000d__x000d__x000d__x000d__x000d_
- -	 xét nghiệm**và**_x000d__x000d__x000d__x000d__x000d_
- -	 [cách ly](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) trong thời gian 14 ngày kể từ ngày tiếp xúc gần nhất. Quý vị (họ) cũng có thể nhận được cuộc gọi từ một chuyên gia truy dấu người tiếp xúc - hãy xem [video] này (https://www.youtube.com/watch?v=u3dLoBj3YLo) để biết thêm thông tin._x000d__x000d__x000d__x000d__x000d_
- - 	làm theo các khuyến nghị của sở y tế công cộng tại nơi quý vị sinh sống._x000d__x000d__x000d__x000d__x000d_
-- 	Tuỳ theo khả năng xét nghiệm SARS-CoV-2 tại địa phương, thời gian cách ly có thể thay đổi. Xem [trang] này (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) để biết thêm thông tin.</v>
-      </c>
-      <c r="E4" t="str">
-        <v>**您（他们）需要接受新冠肺炎检测。**基于所提供的答案，您（他们）是新冠肺炎患者的密切接触者。 - 	-CDC 建议所有新冠肺炎确诊患者的密切接触者应：  -	 接受检测**和** -	 自其末次接触日起 [隔离](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html）14 天。 您（他们）还可能收到来自接触者追踪专业人员的电话-参见本[视频](https://www.youtube.com/watch?v=u3dLoBj3YLo) 以获取更多信息。 -	 遵循当地公共卫生部门的建议。- 	基于当地的 SARS-CoV-2 检测能力，有多种方案可减少人员隔离的时间。 参见本[页](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) 以获取更多信息。</v>
+        <v xml:space="preserve">**CDC khuyến cáo rằng tất cả những người tiếp xúc gần với những người đã được xác nhận mắc COVID-19 nên:** _x000d__x000d_
+- xét nghiệm **và**_x000d__x000d_
+- cách ly trong 14 ngày kể từ ngày tiếp xúc cuối cùng của họ. Dựa trên sự sẵn có về xét nghiệm tại địa phương, chính quyền địa phương có thể có các tùy chọn để giảm thời gian dành cho việc cách ly. Quý vị cũng có thể nhận được cuộc gọi từ một chuyên gia theo dõi người tiếp xúc.</v>
+      </c>
+      <c r="E4" t="str" xml:space="preserve">
+        <v xml:space="preserve">**CDC 建议所有COVID-19 确诊患者的密切接触者应：** _x000d__x000d_
+- 接受检测**和**_x000d__x000d_
+- 从最后一次接触之日算起，隔离14天。基于当地提供检测的能力，当地卫生当局可能有减少人们被隔离的时间的选项。您也可能会接到专业人员打来的电话。</v>
       </c>
       <c r="F4" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Necesita hacerse la prueba del COVID-19.**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-Según las respuestas dadas, usted (él/ella) es un contacto cercano de una persona con COVID-19. _x000d__x000d__x000d__x000d__x000d_
-- Los CDC recomiendan que todos los contactos cercanos de una persona con COVID-19 confirmado: _x000d__x000d__x000d__x000d__x000d_
-  -	se hagan la prueba **y**_x000d__x000d__x000d__x000d__x000d_
-  -	[se pongan en cuarentena](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) por 14 días desde la fecha de su última exposición. Es posible que reciban una llamada de un profesional de rastreo de contactos. Vean este [video](https://www.youtube.com/watch?v=u3dLoBj3YLo) para obtener más información._x000d__x000d__x000d__x000d__x000d_
-- Siga las recomendaciones del departamento de salud pública local._x000d__x000d__x000d__x000d__x000d_
-- Según la disponibilidad local de pruebas del SARS-CoV-2, hay opciones para reducir el tiempo que la gente pase en cuarentena. Consulte esta [página](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) para obtener más información.</v>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
+        <v xml:space="preserve">**Los CDC recomiendan que todos los contactos cercanos de una persona con COVID-19 confirmado:** _x000d__x000d_
+- se hagan la prueba **y**_x000d__x000d_
+- se pongan en cuarentena por 14 días desde la fecha de su última exposición. Según la disponibilidad local de pruebas, es posible que las autoridades locales tengan opciones para reducir el tiempo que la gente pase en cuarentena. Es posible que también reciba una llamada de un profesional de rastreo de contactos.</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="str">
         <v>CDC/messages/t4</v>
       </c>
       <c r="B5" t="str">
         <v>**CDC recommends that anyone with symptoms of COVID-19 should get tested and follow the advice of your healthcare provider.** [Contact](https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html) your local or state health department to find a testing location near you.</v>
       </c>
-      <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)에게 COVID-19의 증상이 있는 것 같습니다. 귀하(그 사람)는 COVID-19 검사를 받아야 합니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	CDC는 COVID-19 증상이 있는 모든 사람이 검사를 받고 의료 서비스 제공자의 조언에 따를 것을 권합니다. 검사를 언제 받아야 하는지에 대한 더 자세한 정보를 알아보려면 [CDC 웹사이트](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)에 방문하십시오. 주변의 검사 장소에 대해 문의하려면 귀하의 지역 또는 주 담당 부서에 [연락하십시오](https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	귀하(그 사람)가 COVID-19의 증상을 보이고 검사를 받지 않은 경우 집에 머무르는 것은 중요합니다. [귀하(그 사람)가 아픈] 경우 무엇을 해야 하는지 알아보십시오(https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="D5" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Có vẻ như quý vị (họ) có thể có các triệu chứng mắc COVID-19. Quý vị (họ) nên được xét nghiệm COVID-19.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	CDC khuyến cáo rằng bất kỳ ai có các triệu chứng mắc COVID-19 nên đi xét nghiệm và làm theo lời khuyên của nhà cung cấp dịch vụ y tế của mình. Để biết thêm thông tin về thời điểm xét nghiệm, hãy truy cập [trang web của CDC] (https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested). [Liên hệ] (https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html) sở y tế địa phương hoặc tiểu bang của quý vị để tìm địa điểm xét nghiệm gần quý vị. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Nếu quý vị (họ) có các triệu chứng mắc COVID-19 và chưa xét nghiệm, điều quan trọng là phải ở nhà. Tìm hiểu những việc cần làm nếu [quý vị (họ) mắc bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="E5" t="str" xml:space="preserve">
-        <v xml:space="preserve">**听起来像您（他们）可能出现了新冠肺炎的症状。 您（他们）应接受新冠肺炎检测。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 	CDC 建议，任何出现新冠肺炎症状的人都应该接受检测，并遵循您（他们）医疗服务提供者的建议。 关于何时检测的更多信息，请访问[CDC 网站]（https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested）。 [联系]（https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html）您的当地或州卫生部门在您附近找到一个检测地点。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 	如果您（他们）有新冠肺炎的症状，并且没有接受检测，那么请留在家中，这很重要。 如果[您（他们）生病该怎么办]（https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)。</v>
-      </c>
-      <c r="F5" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Parece que podría tener síntomas del COVID-19.  Debería hacerse la prueba del COVID-19.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Los CDC recomiendan que toda persona con síntomas del COVID-19 se haga la prueba y siga los consejos del proveedor de atención médica. Para obtener más información sobre cuándo hacerse la prueba, visite el [sitio web de los CDC](https://espanol.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html).  [Comuníquese con](https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html) su departamento de salud local o estatal para encontrar un sitio cercano donde hagan la prueba. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Si tiene síntomas del COVID-19 y no le han hecho la prueba, es importante que se quede en casa. Averigüe qué hacer si [está enfermo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
+      <c r="C5" t="str">
+        <v>**CDC는 COVID-19 증상이 있는 모든 사람이 검사를 받고 의료 서비스 제공자의 조언에 따를 것을 권합니다.** 주변의 검사 장소에 대해 문의하려면 귀하의 지역 또는 주 담당 부서에 [연락하십시오] (https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html).</v>
+      </c>
+      <c r="D5" t="str">
+        <v>**CDC khuyến cáo rằng bất kỳ ai có các triệu chứng của COVID-19 nên đi xét nghiệm và làm theo lời khuyên của nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị.** [Liên hệ] (https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html) sở y tế địa phương hoặc tiểu bang của quý vị để tìm một địa điểm xét nghiệm gần quý vị.</v>
+      </c>
+      <c r="E5" t="str">
+        <v>**CDC建议，任何有COVID-19症状的人都应该接受检测，并遵循医疗保健提供者的建议。** [联系](https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html)您当地或州的卫生部门，以找到您附近的检测地点。</v>
+      </c>
+      <c r="F5" t="str">
+        <v>**Los CDC recomiendan que toda persona con síntomas del COVID-19 se haga la prueba y siga los consejos del proveedor de atención médica.** [Comuníquese con](https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html) su departamento de salud local o estatal para encontrar un sitio cercano donde hagan la prueba.</v>
       </c>
     </row>
     <row r="6">
@@ -547,16 +518,16 @@
         <v>**Further testing is not needed unless a healthcare provider recommends it.**</v>
       </c>
       <c r="C7" t="str">
-        <v>**제공자에 의해 권장되지 않는 한 지금은 COVID-19 검사가 필요하지 않습니다.**</v>
+        <v>**의료 전문가가 권장하지 않는 한 추가 검사는 필요하지 않습니다.**</v>
       </c>
       <c r="D7" t="str">
-        <v>**Không cần xét nghiệm COVID-19 thêm vào lúc này, trừ khi được nhà cung cấp dịch vụ y tế khuyến nghị.**</v>
+        <v>**Không cần xét nghiệm thêm trừ khi nhà cung cấp dịch vụ chăm sóc sức khỏe đề nghị.**</v>
       </c>
       <c r="E7" t="str">
-        <v>**此时不需要进一步的新冠肺炎检测，除非医疗服务提供者推荐。**</v>
+        <v>**除非医疗保健提供者建议，否则不需要进一步检测。**</v>
       </c>
       <c r="F7" t="str">
-        <v>**No son necesarias más pruebas del COVID-19 por ahora, a menos que las recomiende un proveedor de atención médica.**</v>
+        <v>**No necesita pruebas adicionales, a menos que un proveedor de atención médica lo recomiende.**</v>
       </c>
     </row>
     <row r="8">
@@ -659,28 +630,24 @@
         <v>En los últimos 10 días, ¿ha dado positivo en la prueba del coronavirus?</v>
       </c>
     </row>
-    <row r="13" xml:space="preserve">
+    <row r="13">
       <c r="A13" t="str">
         <v>CDC/messages/msg29</v>
       </c>
       <c r="B13" t="str">
         <v>**While waiting for your test results, isolate at home and follow the advice of your health care provider or public health professional.**</v>
       </c>
-      <c r="C13" t="str" xml:space="preserve">
-        <v xml:space="preserve">**결과를 기다리는 동안 집에서 격리된 채로 지내십시오.**_x000d__x000d__x000d__x000d__x000d_
--	귀하(그 사람)는 검사 결과를 기다리는 동안 집에서 격리되어 있어야 하며 의료 서비스 제공자 또는 공중 보건 전문가의 조언에 따라야 합니다.</v>
-      </c>
-      <c r="D13" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Trong khi chờ đợi kết quả của quý vị (của họ), hãy tự cô lập ở nhà:**_x000d__x000d__x000d__x000d__x000d_
--	Quý vị (họ) nên cô lập tại nhà để chờ kết quả xét nghiệm và làm theo lời khuyên của nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị (của họ) hoặc chuyên gia y tế công cộng.</v>
-      </c>
-      <c r="E13" t="str" xml:space="preserve">
-        <v xml:space="preserve">**等待结果的过程时，请在家中自我隔离：**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	您（他们）应在等待检测结果期间在家隔离，并遵循您（他们）的医疗服务提供者或公共卫生专业人员的建议。</v>
-      </c>
-      <c r="F13" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Mientras espera los resultados, aíslese (aíslelo) en su casa:**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Debe aislarse en casa mientras espera los resultado de la prueba y seguir el consejo del proveedor de atención médica o profesional de la salud.</v>
+      <c r="C13" t="str">
+        <v>**귀하(그 사람)는 검사 결과를 기다리는 동안 집에서 분리되어 있어야 하며 의료 서비스 제공자 또는 전문가의 조언에 따라야 합니다.**</v>
+      </c>
+      <c r="D13" t="str">
+        <v>**Trong khi chờ đợi kết quả xét nghiệm, hãy cách ly tại nhà và làm theo lời khuyên của nhà cung cấp dịch vụ chăm sóc sức khỏe hoặc chuyên gia y tế công cộng của quý vị.**</v>
+      </c>
+      <c r="E13" t="str">
+        <v>**在等待您的检测结果期间，请在家隔离，并遵循您的医疗服务提供者或公共卫生专业人员的建议。**</v>
+      </c>
+      <c r="F13" t="str">
+        <v>**Mientras espera los resultados de la prueba, aíslese en casa y siga los consejos del proveedor de atención médica o profesional de la salud pública.**</v>
       </c>
     </row>
     <row r="14" xml:space="preserve">
@@ -688,23 +655,39 @@
         <v>CDC/third_person_questions/symptom_severity_question</v>
       </c>
       <c r="B14" t="str" xml:space="preserve">
-        <v xml:space="preserve">Would you say their symptoms are mild, moderate, or severe? _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mild: Can perform activities of daily living (such as cook, shower, eat and drink) without feeling short of breath._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Moderate: Has difficulty breathing (or shortness of breath) and can only perform limited activities of daily living such as eat and shower._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Would you say their symptoms are mild, moderate, or severe? _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Mild: Can perform activities of daily living (such as cook, shower, eat and drink) without feeling short of breath._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Moderate: Has difficulty breathing (or shortness of breath) and can only perform limited activities of daily living such as eat and shower._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - Severe: Has shortness of breath and/or rapid breathing with severely limited ability or inability to perform activities of daily living</v>
       </c>
-      <c r="C14" t="str">
-        <v/>
-      </c>
-      <c r="D14" t="str">
-        <v/>
-      </c>
-      <c r="E14" t="str">
-        <v/>
-      </c>
-      <c r="F14" t="str">
-        <v/>
+      <c r="C14" t="str" xml:space="preserve">
+        <v xml:space="preserve">그 사람의 증상이 경증, 중등증, 또는 중증이라고 하시겠습니까? _x000d__x000d__x000d__x000d__x000d__x000d__x000d_ _x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 경증: 호흡곤란을 느끼지 않고 일상 생활 활동을 이행할 수 있음(요리, 샤워하기, 먹고 마시기 등)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 중등증: 숨쉬기가 어려우며 (또는 호흡곤란) 먹고 마시기와 같은 일상 생활의 제한된 활동만 이행할 수 있음._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 중증: 호흡곤란 및/또는 일상 생활 활동을 이행하는 능력을 크게 제한받거나 이행할 수 없음</v>
+      </c>
+      <c r="D14" t="str" xml:space="preserve">
+        <v xml:space="preserve">Quý vị sẽ nói các triệu chứng của họ là nhẹ, trung bình hay nặng? _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Nhẹ:  Có thể thực hiện các hoạt động sinh hoạt hàng ngày (như nấu ăn, tắm rửa, ăn uống) mà không cảm thấy khó thở._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Vừa phải: Khó thở (hoặc thở gấp) và chỉ có thể thực hiện các hoạt động hạn chế trong sinh hoạt hàng ngày như ăn uống và tắm rửa._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Nặng: Khó thở và/hoặc thở nhanh với khả năng bị hạn chế nghiêm trọng hoặc không có khả năng thực hiện các hoạt động sinh hoạt hàng ngày</v>
+      </c>
+      <c r="E14" t="str" xml:space="preserve">
+        <v xml:space="preserve">您说他们的症状是轻度、中度还是重度？ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 轻度：能进行日常生活活动（如做饭、洗澡、吃饭、喝水）而不感到呼吸困难。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 中度：有呼吸困难（或呼吸急促），只能进行有限的日常生活活动，如吃饭和洗澡。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 重度：有呼吸短促和/或呼吸急促，日常生活能力严重受限或无法进行日常生活活动</v>
+      </c>
+      <c r="F14" t="str" xml:space="preserve">
+        <v xml:space="preserve">¿Diría usted que los síntomas son leves, moderados o graves? _x000d__x000d_
+_x000d__x000d_
+- Leves: Puede realizar actividades de la vida diaria (como cocinar, ducharse, comer y beber) sin dificultad para respirar._x000d__x000d_
+- Moderados: Tiene dificultad para respirar (o se queda sin aliento) y solo puede realizar ciertas actividades de la vida diaria (como comer y ducharse)._x000d__x000d_
+- Graves: Se queda sin aliento o tiene respiración acelerada con limitación grave en la capacidad (o incapacidad) de realizar actividades de la vida diaria</v>
       </c>
     </row>
     <row r="15" xml:space="preserve">
@@ -712,23 +695,39 @@
         <v>CDC/second_person_questions/symptom_severity_question</v>
       </c>
       <c r="B15" t="str" xml:space="preserve">
-        <v xml:space="preserve">Would you say your symptoms are mild, moderate, or severe? _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mild: Can perform activities of daily living (such as cook, shower, eat and drink) without feeling short of breath._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Moderate: Have difficulty breathing (or shortness of breath) and can only perform limited activities of daily living such as eat and shower._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Would you say your symptoms are mild, moderate, or severe? _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Mild: Can perform activities of daily living (such as cook, shower, eat and drink) without feeling short of breath._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Moderate: Have difficulty breathing (or shortness of breath) and can only perform limited activities of daily living such as eat and shower._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - Severe: Have shortness of breath and/or rapid breathing with severely limited ability or inability to perform activities of daily living</v>
       </c>
-      <c r="C15" t="str">
-        <v/>
-      </c>
-      <c r="D15" t="str">
-        <v/>
-      </c>
-      <c r="E15" t="str">
-        <v/>
-      </c>
-      <c r="F15" t="str">
-        <v/>
+      <c r="C15" t="str" xml:space="preserve">
+        <v xml:space="preserve">귀하의 증상이 경증, 중등증, 또는 중증이라고 하시겠습니까? _x000d__x000d__x000d__x000d__x000d__x000d__x000d_ _x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 경증: 호흡곤란을 느끼지 않고 일상 생활 활동을 이행할 수 있음(요리, 샤워하기, 먹고 마시기 등)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 중등증: 숨쉬기가 어려우며 (또는 호흡곤란) 먹고 마시기와 같은 일상 생활의 제한된 활동만 이행할 수 있음._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 중증: 호흡곤란 및/또는 일상 생활 활동을 이행하는 능력을 크게 제한받거나 이행할 수 없음</v>
+      </c>
+      <c r="D15" t="str" xml:space="preserve">
+        <v xml:space="preserve">Quý vị sẽ nói các triệu chứng của quý vị là nhẹ, trung bình hay nặng? _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Nhẹ:  Có thể thực hiện các hoạt động sinh hoạt hàng ngày (như nấu ăn, tắm rửa, ăn uống) mà không cảm thấy khó thở._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Vừa phải: Khó thở (hoặc thở gấp) và chỉ có thể thực hiện các hoạt động hạn chế trong sinh hoạt hàng ngày như ăn uống và tắm rửa._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Nặng: Khó thở và/hoặc thở nhanh với khả năng bị hạn chế nghiêm trọng hoặc không thể thực hiện các hoạt động sinh hoạt hàng ngày</v>
+      </c>
+      <c r="E15" t="str" xml:space="preserve">
+        <v xml:space="preserve">您说您的症状是轻度、中度还是重度？ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 轻度：能进行日常生活活动（如做饭、洗澡、吃饭、喝水）而不感到呼吸困难。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 中度：有呼吸困难（或呼吸急促），只能进行有限的日常生活活动，如吃饭和洗澡。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 重度：有呼吸短促和/或呼吸急促，日常生活能力严重受限或无法进行日常生活活动</v>
+      </c>
+      <c r="F15" t="str" xml:space="preserve">
+        <v xml:space="preserve">¿Diría usted que los síntomas son leves, moderados o graves? _x000d__x000d_
+_x000d__x000d_
+- Leves: Puede realizar actividades de la vida diaria (como cocinar, ducharse, comer y beber) sin dificultad para respirar._x000d__x000d_
+- Moderados: Tiene dificultad para respirar (o se queda sin aliento) y solo puede realizar ciertas actividades de la vida diaria como comer y ducharse._x000d__x000d_
+- Graves: Se queda sin aliento o tiene respiración acelerada con limitación grave en la capacidad (o incapacidad) de realizar actividades de la vida diaria</v>
       </c>
     </row>
     <row r="16">
@@ -739,16 +738,16 @@
         <v>["Mild", "Moderate", "Severe"]</v>
       </c>
       <c r="C16" t="str">
-        <v/>
+        <v>["경증", "중등증", "중증"]</v>
       </c>
       <c r="D16" t="str">
-        <v/>
+        <v>["Nhẹ", "Vừa phải", "Nặng"]</v>
       </c>
       <c r="E16" t="str">
-        <v/>
+        <v>【“轻度”、“中度”、“重度”】</v>
       </c>
       <c r="F16" t="str">
-        <v/>
+        <v>["Leves", "Moderados", "Graves"]</v>
       </c>
     </row>
     <row r="17" xml:space="preserve">
@@ -756,62 +755,34 @@
         <v>CDC/messages/msg27</v>
       </c>
       <c r="B17" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Stay home and away from others until:**
-- it has been 10 days from when your symptoms first appeared **and**
-- you have had no fever for 24 hours without the use medications **and**
+        <v xml:space="preserve">**Stay home and away from others until:**_x000d__x000d_
+- it has been 10 days from when your symptoms first appeared **and**_x000d__x000d_
+- you have had no fever for 24 hours without the use medications **and**_x000d__x000d_
 - your other symptoms of COVID-19 are improving* (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)</v>
       </c>
       <c r="C17" t="str" xml:space="preserve">
-        <v xml:space="preserve">**SARS-CoV-2 감염에 대해 양성인 경우:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-다음과 같을 때까지 집에 머물고 다른 사람들과 떨어져 있으십시오._x000d__x000d__x000d__x000d__x000d_
-- 첫 증상 발현 후 10일 이후 **그리고** _x000d__x000d__x000d__x000d__x000d_
-- 해열제 없이도 열이 나지 않은 지 24시간, **그리고** _x000d__x000d__x000d__x000d__x000d_
-- COVID-19의 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦추지 않음)_x000d__x000d__x000d__x000d__x000d_
-- SARS-CoV-2에 노출되었을 수 있는 밀접 접촉자가 있다면 알려주시기 바랍니다. 확진자 또는 COVID 가능성이 있는 사람들과 밀접 접촉한 모든 사람이 다음과 같이 할 것을 CDC는 권장합니다:_x000d__x000d__x000d__x000d__x000d_
- - 검사를 받으십시오 **그리고** _x000d__x000d__x000d__x000d__x000d_
- - 마지막으로 노출된 날부터 14일 동안 [격리하십시오](https://korean.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html). 또한 추적 전문가의 전화를 받을 수도 있습니다 – 더 자세한 정보를 확인하려면 이 [동영상](https://www.youtube.com/watch?v=u3dLoBj3YLo)을 시청하십시오._x000d__x000d__x000d__x000d__x000d_
-- 휴식을 취하고 수분을 충분히 보충하십시오. 회복에 도움이 되도록 필요한 경우 아세트아미노펜과 같은 일반의약품을 복용하십시오._x000d__x000d__x000d__x000d__x000d_
-다른 사람으로부터 분리되어 있으십시오. 가능한 한, 가정 내 특정 공간에 다른 구성원과 반려동물로부터 격리하여 머무르십시오.</v>
+        <v xml:space="preserve">**다음과 같을 때까지 집에 머물고 다른 사람들과 떨어져 있으십시오.**_x000d__x000d_
+- 첫 증상 발현 후 10일 이후 **그리고**_x000d__x000d_
+- 약 사용 없이 24시간 동안 발열이 없었음 **그리고**_x000d__x000d_
+- COVID-19의 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦추지 않음)</v>
       </c>
       <c r="D17" t="str" xml:space="preserve">
-        <v xml:space="preserve">** Nếu quý vị (họ) có kết quả xét nghiệm dương tính với virus SARS-CoV-2:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-Hãy ở nhà và tránh xa những người khác cho đến khi_x000d__x000d__x000d__x000d__x000d_
-- đã quáa 10 ngày kể từ khi xuất hiện các triệu chứng đầu tiên **và** _x000d__x000d__x000d__x000d__x000d_
-- đã quáa 24 giờ không sốt mà không cần sử dụng thuộc giảm sốt **và** _x000d__x000d__x000d__x000d__x000d_
-- các triệu chứng COVID-19 khác đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)_x000d__x000d__x000d__x000d__x000d_
-- Vui lòng thông báo cho những tiếp xúc gần với quý vị (họ) rằng họ có khả năng bị nhiễm SARS-CoV-2. CDC khuyến cáo rằng tất cả những người tiếp xúc gần với những người đã được xác nhận mắc hoặc có khả năng mắc COVID nên: _x000d__x000d__x000d__x000d__x000d_
- - xét nghiệm **và** _x000d__x000d__x000d__x000d__x000d_
- - [cách ly](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) trong thời gian 14 ngày kể từ ngày tiếp xúc gần nhất. Quý vị (họ) cũng có thể nhận được cuộc gọi từ một chuyên gia truy dấu người tiếp xúc - hãy xem [video] này (https://www.youtube.com/watch?v=u3dLoBj3YLo) để biết thêm thông tin. _x000d__x000d__x000d__x000d__x000d_
-- Nghỉ ngơi và uống đủ nước. Dùng các loại thuốc không cần kê toa, ví dụ như acetaminophen, nếu cần để giúp quý (họ) cảm thấy tốt hơn. _x000d__x000d__x000d__x000d__x000d_
-Cách ly khỏi những người khác. Nên ở một phòng riêng càng nhiều càng tốt trong phòng riêng và tránh xa những người và vật nuôi khác trong nhà quý vị (họ).</v>
+        <v xml:space="preserve">**Ở nhà và tránh xa những người khác cho đến khi:**_x000d__x000d_
+- đã qua 10 ngày từ khi quý vị xuất hiện các triệu chứng đầu tiên **và**_x000d__x000d_
+- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc **và**_x000d__x000d_
+- các triệu chứng COVID-19 khác của quý vị đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)</v>
       </c>
       <c r="E17" t="str" xml:space="preserve">
-        <v xml:space="preserve">**如果您（他们）的 SARS-CoV-2 感染检测结果呈阳性：**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-待在家里，远离他人，直到_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 距离症状首次出现已经 10 天**和** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 在未使用退热药物的情况下，24 小时无发热**和** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 新冠肺炎的其他症状正在改善*（*恢复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 请告知您（他们）的密切接触者他们可能接触 SARS-CoV-2。 CDC 建议确诊或疑似新冠肺炎的人的密切接触者应： _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 接受检测**和** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 自其末次接触日起 [隔离] （https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html）14 天。 您（他们）还可能收到来自接触者追踪专业人员的电话-参见本[视频]（https://www.youtube.com/watch?v=u3dLoBj3YLo）以获取更多信息。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 注意休息并保持不要脱水。 如果需要帮助您（他们）感觉好转，可使用非处方药，如对乙酰氨基酚。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-将自己与他人隔离。 尽可能地呆在特定的房间中，并远离（他们的）家中其他人和宠物。</v>
+        <v xml:space="preserve">**待在家里，远离他人，直到：**_x000d__x000d_
+- 距离您的症状首次出现已经 10 天**并且**_x000d__x000d_
+- 在没有使用药物的情况下，24小时内没有发烧 **并且**_x000d__x000d_
+- 您的COVID-19的其他症状正在改善*（*康复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）</v>
       </c>
       <c r="F17" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Si dio positivo en la prueba de infección por el SARS-CoV-2:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-Quédese (manténgalo) en casa alejado de los demás hasta que..._x000d__x000d__x000d__x000d__x000d_
-- hayan pasado 10 días desde el inicio de los síntomas **y** _x000d__x000d__x000d__x000d__x000d_
-- 24 horas sin fiebre sin usar medicamentos para reducirla **y** _x000d__x000d__x000d__x000d__x000d_
-- otros síntomas del COVID-19 estén mejorando* Pasar a (*la pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)_x000d__x000d__x000d__x000d__x000d_
-- Infórmeles a los contactos cercanos que posiblemente estuvieron expuestos al SARS-CoV-2. Los CDC recomiendan que todos los contactos cercanos de una persona con COVID-19 confirmado o probable: _x000d__x000d__x000d__x000d__x000d_
-   - se hagan la prueba **y** _x000d__x000d__x000d__x000d__x000d_
-   - [Se pongan en cuarentena](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) por 14 días desde la fecha de su última exposición. Es posible que reciban una llamada de un profesional de rastreo de contactos – vean este [video](https://www.youtube.com/watch?v=u3dLoBj3YLo) para obtener más información. _x000d__x000d__x000d__x000d__x000d_
-- Descanse y manténgase hidratado. Tome medicamentos de venta sin receta, como acetaminofeno, para ayudar a sentirse mejor. _x000d__x000d__x000d__x000d__x000d_
-- Aléjese (aléjelo) de las otras personas. En la medida de lo posible, permanezca (manténgalo) en una habitación específica y lejos de las otras personas y mascotas en su casa.</v>
+        <v xml:space="preserve">**Quédese en casa y lejos de los demás hasta que:**_x000d__x000d_
+- hayan pasado 10 días desde el inicio de los síntomas **y**_x000d__x000d_
+- 24 horas sin fiebre sin usar medicamentos para reducirla **y**_x000d__x000d_
+- otros síntomas del COVID-19 estén mejorando* (*La pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)</v>
       </c>
     </row>
     <row r="18" xml:space="preserve">
@@ -819,35 +790,44 @@
         <v>CDC/messages/msg28</v>
       </c>
       <c r="B18" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Stay home and away from others until:** 
-- it has been 10 days from when your symptoms first appeared **and**
-- you have had no fever for 24 hours without the use of medications **and**
-- your other symptoms are improving* (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)
+        <v xml:space="preserve">**Stay home and away from others until:** _x000d__x000d_
+- it has been 10 days from when your symptoms first appeared **and**_x000d__x000d_
+- you have had no fever for 24 hours without the use of medications **and**_x000d__x000d_
+- your other symptoms are improving* (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)_x000d__x000d_
+_x000d__x000d_
 **\*Please note**: It is possible that you were very early in your infection when your sample was collected and that you could test positive later. If your symptoms worsen after testing negative, please contact your healthcare provider.</v>
       </c>
       <c r="C18" t="str" xml:space="preserve">
-        <v xml:space="preserve">**SARS-CoV-2 감염에 대해 음성인 경우:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-- 검체를 채취할 당시 감염 초기에 있었으며 나중에 검사 결과 양성으로 나타날 수 있습니다._x000d__x000d__x000d__x000d__x000d_
-- 검사 결과 음성으로 나타난 이후 증상이 악화된 경우 의료 전문가에게 연락하십시오.</v>
+        <v xml:space="preserve">**다음과 같을 때까지 집에 머물고 다른 사람들과 떨어져 있으십시오.** _x000d__x000d_
+- 첫 증상 발현 후 10일 이후 **그리고**_x000d__x000d_
+- 약 사용 없이 24시간 동안 발열이 없었음 **그리고**_x000d__x000d_
+- 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦추지 않음)_x000d__x000d_
+_x000d__x000d_
+**\*참고하십시오**: 검체를 채취할 당시 감염 초기에 있었으며 나중에 검사 결과 양성으로 나타날 수 있습니다. 검사 결과 음성으로 나타난 이후 증상이 악화된 경우 의료 전문가에게 연락하십시오.</v>
       </c>
       <c r="D18" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Nếu quý vị (họ) có kết quả xét nghiệm âm tính với virú SARS-CoV-2:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-- Có thể quý vị (họ) đã bị nhiễm rất sớm khi mẫu xét nghiệm của quý vị (họ) được thu thập và quý vị (họ) có thể có kết quả dương tính sau đó. _x000d__x000d__x000d__x000d__x000d_
-- Nếu các triệu chứng của quý vị (họ) trở nên xấu đi sau khi xét nghiệm âm tính, vui lòng liên hệ với nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị (họ).</v>
+        <v xml:space="preserve">**Ở nhà và tránh xa những người khác cho đến khi:** _x000d__x000d_
+- đã qua 10 ngày từ khi quý vị xuất hiện các triệu chứng đầu tiên **và**_x000d__x000d_
+- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc **và**_x000d__x000d_
+- các triệu chứng khác của quý vị đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)_x000d__x000d_
+_x000d__x000d_
+**\*Xin lưu ý**: Có thể quý vị đã bị nhiễm rất sớm khi mẫu xét nghiệm của quý vị được thu thập và quý vị có thể có kết quả dương tính sau đó. Nếu các triệu chứng của quý vị trở nên xấu đi sau khi xét nghiệm âm tính, vui lòng liên hệ với nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị.</v>
       </c>
       <c r="E18" t="str" xml:space="preserve">
-        <v xml:space="preserve">**如果您（他们）的 SARS-CoV-2 感染检测结果为阴性：**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 当您（他们）采集您（他们）的样本时，您（他们）可能处在感染的极早期，过一段时间，您（他们）可能检测为阳性。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 如果您的（他们的）症状在检测阴性后恶化，请联系您的（他们的）医疗服务提供者。</v>
+        <v xml:space="preserve">**待在家里，远离他人，直到：** _x000d__x000d_
+- 距离您的症状首次出现已经 10 天**并且**_x000d__x000d_
+- 在没有使用药物的情况下，24小时内没有发烧 **并且**_x000d__x000d_
+- 您的其他症状正在改善*（*康复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）_x000d__x000d_
+_x000d__x000d_
+**、*请注意**：有可能您在采集样本的时候是在感染的早期，您以后可能会检测出阳性。如果您的症状在检测阴性后恶化，请联系您的医疗保健提供者。</v>
       </c>
       <c r="F18" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Si dio negativo en la prueba de infección por el SARS-CoV-2:**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--  Es posible que apenas estuviera comenzando la infección cuando le tomaron la muestra y que pudiera dar positivo más adelante. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--  Si los síntomas empeoran después de dar negativo, contacte al proveedor de atención médica.</v>
+        <v xml:space="preserve">**Quédese en casa y lejos de los demás hasta que:** _x000d__x000d_
+- hayan pasado 10 días desde el inicio de los síntomas **y**_x000d__x000d_
+- 24 horas sin fiebre sin usar medicamentos para reducirla **y**_x000d__x000d_
+- otros síntomas del COVID-19 estén mejorando* (*La pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)_x000d__x000d_
+_x000d__x000d_
+**\*Tenga en cuenta**: Es posible que apenas estuviera comenzando la infección cuando le tomaron la muestra y que pudiera dar positivo más adelante. Si los síntomas empeoran después de dar negativo, contacte al proveedor de atención médica.</v>
       </c>
     </row>
     <row r="19" xml:space="preserve">
@@ -855,122 +835,74 @@
         <v>CDC/messages/msg30</v>
       </c>
       <c r="B19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Stay home and away from others until:**
-- it has been 10 days from when your symptoms first appeared **and** 
-- you have had no fever for 24 hours without the use of medications **and** 
+        <v xml:space="preserve">**Stay home and away from others until:**_x000d__x000d_
+- it has been 10 days from when your symptoms first appeared **and** _x000d__x000d_
+- you have had no fever for 24 hours without the use of medications **and** _x000d__x000d_
 - your other symptoms of COVID-19 are improving* (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)</v>
       </c>
       <c r="C19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**검사를 아직 받지 않았다면 다음과 같이 해야 합니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다음과 같을 때까지 집에 머물고 다른 사람들과 떨어져 있으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 첫 증상 발현 후 10일 이후 **그리고** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 해열제 없이도 열이 나지 않은 지 24시간, **그리고** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - COVID-19의 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦추지 않음)</v>
+        <v xml:space="preserve">**다음과 같을 때까지 집에 머물고 다른 사람들과 떨어져 있으십시오.**_x000d__x000d_
+- 첫 증상 발현 후 10일 이후 **그리고** _x000d__x000d_
+- 약 사용 없이 24시간 동안 발열이 없었음 **그리고** _x000d__x000d_
+- COVID-19의 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦추지 않음)</v>
       </c>
       <c r="D19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Nếu chưa làm xét nghiệm, quý vị (họ) nên:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-- Ở nhà và tránh xa những người khác cho đến khi _x000d__x000d__x000d__x000d__x000d_
- - đã quá 10 ngày kể từ khi xuất hiện các triệu chứng đầu tiên **và** _x000d__x000d__x000d__x000d__x000d_
- - đã quá 24 giờ không sốt mà không cần sử dụng thuộc giảm sốt **và** _x000d__x000d__x000d__x000d__x000d_
- - các triệu chứng COVID-19 khác đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)</v>
+        <v xml:space="preserve">**Ở nhà và tránh xa những người khác cho đến khi:**_x000d__x000d_
+- đã qua 10 ngày từ khi quý vị xuất hiện các triệu chứng đầu tiên **và** _x000d__x000d_
+- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc **và** _x000d__x000d_
+- các triệu chứng COVID-19 khác của quý vị đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)</v>
       </c>
       <c r="E19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**如果您未接受检测，您（他们）应该：**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 待在家里，远离他人，直到 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 距离症状首次出现已经 10 天**和** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 在未使用退热药物的情况下，24 小时无发热**和** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 新冠肺炎的其他症状正在改善*（*恢复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）</v>
+        <v xml:space="preserve">**待在家里，远离他人，直到：**_x000d__x000d_
+- 距离您的症状首次出现已经 10 天**并且** _x000d__x000d_
+- 在没有使用药物的情况下，24小时内没有发烧 **并且** _x000d__x000d_
+- 您的COVID-19的其他症状正在改善*（*康复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）</v>
       </c>
       <c r="F19" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Si no se ha hecho la prueba, debe:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-Quedarse (mantenerlo) en casa alejado de los demás hasta que..._x000d__x000d__x000d__x000d__x000d_
-- hayan pasado 10 días desde el inicio de los síntomas **y** _x000d__x000d__x000d__x000d__x000d_
-- 24 horas sin fiebre sin usar medicamentos para reducirla **y** _x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Quédese en casa y lejos de los demás hasta que:**_x000d__x000d_
+- hayan pasado 10 días desde el inicio de los síntomas **y**_x000d__x000d_
+- 24 horas sin fiebre sin usar medicamentos para reducirla **y**_x000d__x000d_
 - otros síntomas del COVID-19 estén mejorando* (*La pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)</v>
       </c>
     </row>
-    <row r="20" xml:space="preserve">
+    <row r="20">
       <c r="A20" t="str">
         <v>CDC/messages/msg31</v>
       </c>
       <c r="B20" t="str">
         <v>**CDC recommends that all close contacts of people with confirmed COVID-19 should quarantine for 14 days from the day of their last exposure.** Based on local testing availability, local health authorities may have options to reduce the time people spend in quarantine. You may also receive a call from a contact tracing professional.</v>
       </c>
-      <c r="C20" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)가 COVID-19 확진자와 밀접 접촉한 경우:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
- - COVID-19 확진자와 밀접 접촉한 모든 사람이 다음과 같이 할 것을 CDC는 권장합니다:_x000d__x000d__x000d__x000d__x000d_
- - 마지막으로 노출된 날부터 14일 동안 [격리하십시오](https://korean.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html). 또한 접촉자 추적 조사 전문가의 전화를 받을 수도 있습니다 – 더 자세한 정보를 확인하려면 이 [동영상](https://www.youtube.com/watch?v=u3dLoBj3YLo)을 시청하십시오._x000d__x000d__x000d__x000d__x000d_
- - 지역 보건부의 권장사항을 준수하십시오._x000d__x000d__x000d__x000d__x000d_
- - 지역에서 SARS-CoV-2 검사를 이용할 수 있는지의 여부에 따라, 격리를 위해 보내야 하는 시간을 줄일 방법이 있습니다. 더 자세한 정보는 이 [페이지](https://korean.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)를 확인하십시오.</v>
-      </c>
-      <c r="D20" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Nếu quý vị (họ) đã tiếp xúc gần với người đã được xác định là mắc COVID-19:**_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
- - CDC khuyến cáo rằng tất cả những người tiếp xúc gần với những người đã được xác nhận mắc COVID-19 nên: _x000d__x000d__x000d__x000d__x000d_
- - [cách ly](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) trong thời gian 14 ngày kể từ ngày tiếp xúc gần nhất. Quý vị (họ) cũng có thể nhận được cuộc gọi từ một chuyên gia truy dấu người tiếp xúc - hãy xem [video] này (https://www.youtube.com/watch?v=u3dLoBj3YLo) để biết thêm thông tin._x000d__x000d__x000d__x000d__x000d_
- - làm theo các khuyến nghị của sở y tế công cộng địa phương của quý vị._x000d__x000d__x000d__x000d__x000d_
- - Dựa trên sự sẵn có về xét nghiệm SARS-CoV-2 tại địa phương, có các tùy chọn để giảm thời gian dành cho việc cách ly. Xem [trang] này (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) để biết thêm thông tin.</v>
-      </c>
-      <c r="E20" t="str" xml:space="preserve">
-        <v xml:space="preserve">**如果您（他们）与新冠肺炎的确诊人员有密切接触：**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- -CDC 建议所有新冠肺炎确诊患者的密切接触者应： _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 自其末次接触日起 [隔离] （https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html）14 天。 您（他们）还可能收到来自接触者追踪专业人员的电话-参见本[视频]（https://www.youtube.com/watch?v=u3dLoBj3YLo）以获取更多信息。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 遵循当地公共卫生部门的建议。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- 基于当地的 SARS-CoV-2 检测能力，有多种方案可减少人员隔离的时间。 参见本[页]（https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html）以获取更多信息。</v>
-      </c>
-      <c r="F20" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Si ha estado en contacto cercano con alguien con COVID-19 confirmado:**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-  - Los CDC recomiendan que todos los contactos cercanos de una persona con COVID-19 confirmado: _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    - [Se pongan en cuarentena](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) por 14 días desde la fecha de su última exposición. Es posible que reciban una llamada de un profesional de rastreo de contactos – vean este [video](https://www.youtube.com/watch?v=u3dLoBj3YLo) para obtener más información._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    - Siga las pautas de las autoridades de salud pública locales._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-  - Según la disponibilidad local de pruebas del SARS-CoV-2, hay opciones para reducir el tiempo que la gente pase en cuarentena. Consulte esta [página](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html) para obtener más información.</v>
-      </c>
-    </row>
-    <row r="21" xml:space="preserve">
+      <c r="C20" t="str">
+        <v>**COVID-19 확진자와 밀접 접촉한 모든 사람이 마지막으로 노출된 날부터 14일 동안 격리할 것을 CDC는 권장합니다.** 지역에서 검사를 이용할 수 있는지의 여부에 따라, 지역 당국이 격리를 위해 보내야 하는 시간을 줄일 방법을 가질 수 있습니다. 또한 추적 전문가의 전화를 받을 수도 있습니다.</v>
+      </c>
+      <c r="D20" t="str">
+        <v>**CDC khuyến cáo rằng tất cả những người tiếp xúc gần gũi với những người đã được xác nhận COVID-19 nên cách ly trong 14 ngày kể từ ngày tiếp xúc cuối cùng của họ.** Dựa trên khả năng xét nghiệm tại địa phương, cơ quan y tế địa phương có thể có các lựa chọn để giảm thời gian cách ly. Quý vị cũng có thể nhận được cuộc gọi từ một chuyên gia theo dõi người tiếp xúc.</v>
+      </c>
+      <c r="E20" t="str">
+        <v>**疾控中心建议，所有确诊COVID-19患者的密切接触者应自最后一次接触之日起免疫隔离14天**。根据当地提供检测的能力，当地卫生当局可能有减少人们被隔离的时间的选项。您也可能会接到专业人员打来的电话。</v>
+      </c>
+      <c r="F20" t="str">
+        <v>**Los CDC recomiendan que todos los contactos cercanos de personas con COVID-19 confirmado deben ponerse en cuarentena por 14 días desde el día de su última exposición.** Según la disponibilidad local de pruebas, es posible que las autoridades de salud locales tengan opciones para reducir el tiempo que la gente pase en cuarentena. Es posible que también reciba una llamada de un profesional de rastreo de contactos.</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="str">
         <v>CDC/messages/msg26</v>
       </c>
       <c r="B21" t="str">
         <v>**Tell an administrator or nurse at your school or child care that you may have been in contact with someone with suspected COVID-19.**</v>
       </c>
-      <c r="C21" t="str" xml:space="preserve">
-        <v xml:space="preserve">**학교 또는 데이케어의 관리자나 간호사에게 문의하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그 사람)의 학교 또는 데이케어의 관리자나 간호사에게 귀하(그 사람)가 COVID-19가 의심되는 사람과 접촉했을 수 있음을 알리십시오. _x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	귀하(그 사람)와 귀하(그 사람) 주변 사람들을 보호하기 위해 귀하(그 사람)의 코와 입에 마스크를 착용하십시오. _x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	14일 동안 하루에 두 번 귀하(그 사람)의 체온을 확인하십시오. _x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	[COVID-19 증상]이 있는지 관찰하십시오(https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). [CDC 웹사이트]에서 COVID-19 및 자신(그 사람)과 타인을 보호하는 방법에 대해 자세히 알아보십시오(https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
-      </c>
-      <c r="D21" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ với quản lý hoặc y tá tại trường học hoặc nhà trẻ của quý vị (của họ).**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Nói với quản lý hoặc y tá tại trường học hoặc nhà trẻ của quý vị (họ) rằng quý vị (họ) có thể đã tiếp xúc với người bị nghi ngờ mắc COVID-19. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Đeo khẩu trang che mũi và miệng của quý vị (họ) để bảo vệ bản thân và những người xung quanh. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 	Kiểm tra nhiệt độ cơ thể của quý vị (họ) hai lần một ngày trong 14 ngày. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Theo dõi [các triệu chứng COVID-19] (https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Tìm hiểu thêm về COVID-19 và cách mà quý vị (họ) có thể thực hiện để bảo vệ bản thân và những người khác trên [trang web của CDC] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
-      </c>
-      <c r="E21" t="str" xml:space="preserve">
-        <v xml:space="preserve">**联系您（他们）学校或日托的管理员或护士。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-告知您（他们）学校或日托的管理员或护士，您（他们）可能与疑似新冠肺炎患者接触。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	在您（他们）的鼻子和嘴上佩戴口罩，以保护您（他们）和您周围的人（他们）。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	每天检查两次体温，持续 14 天。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	观察 [新冠肺炎症状]（https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。 访问[CDC 网站]了解更多关于新冠肺炎以及如何保护自己（他们）和他人的信息（https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html)。</v>
-      </c>
-      <c r="F21" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Comuníquese con un administrador o el personal de enfermería de la escuela o guardería.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dígale a un administrador o al personal de enfermería de la escuela o guardería que pudo haber tenido contacto con alguien con COVID-19 presunto. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Póngase (póngale) una mascarilla sobre la nariz y boca para protegerse (protegerlo) y proteger a los demás que estén cerca. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Tómese (tómele) la temperatura dos veces al día por 14 días. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Esté atento a los [síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Aprenda más acerca del COVID-19 y cómo puede protegerse (protegerlo) y proteger a los demás en el [sitio web de los CDC](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
+      <c r="C21" t="str">
+        <v>**귀하의 학교 또는 보육 관리자나 간호사에게 귀하가 COVID-19가 의심되는 사람과 접촉했을 수 있음을 알리십시오.**</v>
+      </c>
+      <c r="D21" t="str">
+        <v>**Nói với quản lý hoặc y tá tại trường học hoặc nhà trẻ của quý vị rằng quý vị có thể đã tiếp xúc với người bị nghi ngờ mắc COVID-19.**</v>
+      </c>
+      <c r="E21" t="str">
+        <v>**告知您学校或日托的管理员或护士，您可能与疑似COVID-19患者接触。**</v>
+      </c>
+      <c r="F21" t="str">
+        <v>** Dígale a un administrador o al personal de enfermería de la escuela o guardería que pudo haber tenido contacto con alguien con COVID-19 presunto.**</v>
       </c>
     </row>
     <row r="22">
@@ -1033,91 +965,24 @@
         <v>Afección neurológica, como parálisis cerebral</v>
       </c>
     </row>
-    <row r="25" xml:space="preserve">
+    <row r="25">
       <c r="A25" t="str">
         <v>CDC/messages/msg25</v>
       </c>
       <c r="B25" t="str">
         <v>**Tell a caregiver in your facility that you may have been in close contact with someone who may have COVID-19.**</v>
       </c>
-      <c r="C25" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)가 거주하고 계신 보호 센터, 요양원 또는 노숙자 보호소의 의료진에게 문의하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그 사람)의 시설에 있는 간병인에게 귀하(그 사람)가 COVID-19에 걸렸을 가능성이 있는 사람과 밀접하게 접촉했을 수 있다고 말하십시오. 그들은 귀하(그 사람)의 시설 또는 보호소에서 감염을 예방하는 것을 도울 수 있습니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-[다른 사람을 질병으로부터 보호]하도록 도움을 주십시오(https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	의학적 치료를 받는 경우를 제외하고 가급적 방에 머무르십시오(그 사람이 방에 머무르도록 하십시오)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	손을 자주 씻으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	다른 사람과 가까이 하지 마십시오. 다른 사람과 최소 6피트의 간격을 유지하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	다른 사람들과 함께 있을 때는 가능한 한 마스크를 착용하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	자신의 건강 상태를 모니터링하여 아프기 시작하면 의료진에게 알리십시오.</v>
-      </c>
-      <c r="D25" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ với nhà cung cấp dịch vụ y tế tại trung tâm chăm sóc, viện dưỡng lão hoặc nơi tạm trú cho người vô gia cư nơi quý vị (họ) sống.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Nói với người chăm sóc trong cơ sở của quý vị (họ) rằng quý vị (họ) có thể đã tiếp xúc gần với người có thể mắc COVID-19. Họ có thể giúp ngăn ngừa mắc virus tại cơ sở hoặc nơi ở của quý vị (của họ). _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Giúp [bảo vệ người khác không mắc bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Ở trong phòng của quý vị (giữ họ trong phòng của mình) càng nhiều càng tốt, ngoại trừ khi cần chăm sóc y tế._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Dùng khăn giấy để che khi ho và hắt hơi._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Rửa tay thường xuyên._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Tránh tiếp xúc gần với người khác. - Giữ khoảng cách với người khác ít nhất 6 feet (2 mét)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Đeo khẩu trang khi ở gần người khác, nếu có thể._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Theo dõi sức khỏe của mình và thông báo cho nhà cung cấp dịch vụ y tế nếu quý vị bắt đầu cảm thấy mắc bệnh.</v>
-      </c>
-      <c r="E25" t="str" xml:space="preserve">
-        <v xml:space="preserve">**联系您（他们）居住的护理中心、疗养院或无家可归者收容所的医疗服务提供者。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-告知您（他们）机构的护理人员，您（他们）可能与可能患有新冠肺炎的人密切接触。 它们可以帮助预防您（他们）机构或庇护所的感染。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-帮助 [保护他人免于生病] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	除就医外，尽可能多地待在（将他们留在）您的房间里。尽可能多地留在房间。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	咳嗽以及打喷嚏时，用纸巾捂住口鼻。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	经常洗手。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	 避免与他人密切接触。 尝试与他人保持至少 6 英尺的距离。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	在可能的情况下，在他人周围佩戴口罩。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	监测您的健康状况，如果您开始感觉不适，请通知医疗服务人员。</v>
-      </c>
-      <c r="F25" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Comuníquese con un proveedor de atención médica en el centro de cuidados, hogar de ancianos o refugio para personas “sin hogar" donde viva.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dígale a un cuidador en su establecimiento que pudo haber tenido contacto cercano con alguien que podría tener COVID-19. Pueden ayudarlo a prevenir infecciones en su establecimiento o refugio. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Ayude a [proteger a otras personas para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quédese (manténgalo) en su habitación lo más posible, excepto para conseguir atención médica._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cúbrase la nariz y la boca al toser o estornudar con un pañuelo desechable o con la parte interna del codo._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Límpiese las manos con frecuencia._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Evite el contacto cercano con otras personas. Manténgase a por lo menos 6 pies o 2 metros de las otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Póngase una mascarilla cuando esté cerca de otras personas, si es posible._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Monitoree su salud y notifique a un proveedor de atención médica si empieza a sentirse enfermo.</v>
+      <c r="C25" t="str">
+        <v>**귀하의 시설에 있는 간병인에게 귀하가 COVID-19에 걸렸을 가능성이 있는 사람과 밀접하게 접촉했을 수 있다고 말하십시오.**</v>
+      </c>
+      <c r="D25" t="str">
+        <v>**Nói với người chăm sóc trong cơ sở của quý vị rằng quý vị có thể đã tiếp xúc gần với người có thể mắc COVID-19.**</v>
+      </c>
+      <c r="E25" t="str">
+        <v>**告知您机构的护理人员，您可能与可能患有COVID-19的人有过密切接触。**</v>
+      </c>
+      <c r="F25" t="str">
+        <v>**Dígale a un cuidador en su establecimiento que usted pudo haber tenido contacto cercano con alguien que podría tener COVID-19.**</v>
       </c>
     </row>
     <row r="26">
@@ -1168,16 +1033,16 @@
         <v>**Please ask your parent or guardian to answer these questions with you.**</v>
       </c>
       <c r="C28" t="str">
-        <v>부모님이나 보호자에게 이 질문에 귀하와 함께 답해달라고 요청하십시오.</v>
+        <v>**부모님이나 보호자에게 이 질문에 답해달라고 요청하십시오.**</v>
       </c>
       <c r="D28" t="str">
-        <v>Vui lòng nhờ cha mẹ hoặc người giám hộ của bạn trả lời những câu hỏi này cùng với bạn.</v>
+        <v>**Vui lòng yêu cầu cha mẹ hoặc người giám hộ của quý vị trả lời những câu hỏi này với quý vị.**</v>
       </c>
       <c r="E28" t="str">
-        <v>请让您的父母或监护人与您一起回答这些问题。</v>
+        <v>**请让您的父母或监护人与您一起回答这些问题。**</v>
       </c>
       <c r="F28" t="str">
-        <v>Pídele a tu papá, mamá o tutor legal que responda estas preguntas contigo.</v>
+        <v>**Pídele a tu papá, mamá o tutor legal que responda estas preguntas contigo.**</v>
       </c>
     </row>
     <row r="29">
@@ -1188,72 +1053,56 @@
         <v>**Please ask your parent or guardian to help you complete these questions.**</v>
       </c>
       <c r="C29" t="str">
-        <v>부모님이나 보호자에게 이 질문에 답하는 것을 도와달라고 요청하십시오.</v>
+        <v>**부모님이나 보호자에게 이 질문을 완료하는 데 도와달라고 요청하십시오.**</v>
       </c>
       <c r="D29" t="str">
-        <v>Vui lòng nhờ cha mẹ hoặc người giám hộ của bạn giúp bạn hoàn tất những câu hỏi này.</v>
+        <v>**Vui lòng yêu cầu cha mẹ hoặc người giám hộ của quý vị giúp quý vị hoàn thành các câu hỏi này.**</v>
       </c>
       <c r="E29" t="str">
-        <v>请询问您的父母或监护人，以帮助您完成这些问题。</v>
+        <v>**请询问您的父母或监护人，以帮助您完成这些问题。**</v>
       </c>
       <c r="F29" t="str">
-        <v>Pídele a tu papá, mamá o tutor legal que te ayude a completar estas preguntas.</v>
-      </c>
-    </row>
-    <row r="30" xml:space="preserve">
+        <v>**Pídele a tu papá, mamá o tutor legal que te ayude a completar estas preguntas.**</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" t="str">
         <v>CDC/messages/msg19</v>
       </c>
       <c r="B30" t="str">
         <v>**This tool is intended for people 2 years or older.** Please call the child’s medical provider, clinician advice line, or telemedicine provider if your child is less than 2 years old and sick</v>
       </c>
-      <c r="C30" t="str" xml:space="preserve">
-        <v xml:space="preserve">**의료진에게 문의하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-이 도구는 만 2세 이상을 대상으로 합니다. 귀하의 자녀가 만 2세 미만이며 아픈 경우 아동의 의료 제공자, 임상의 상담 전화 또는 의료진에게 전화하십시오.</v>
-      </c>
-      <c r="D30" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ với một nhà cung cấp dịch vụ y tế.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Công cụ này dành cho những người từ 2 tuổi trở lên. Vui lòng gọi cho nhà cung cấp dịch vụ y tế, đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa của trẻ nếu con quý vị dưới 2 tuổi và bị bệnh.</v>
-      </c>
-      <c r="E30" t="str" xml:space="preserve">
-        <v xml:space="preserve">**联系医疗服务提供者。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-该工具适用于 2 岁或以上的人群。 如果您的孩子不到 2 岁且生病，请致电儿童的医疗服务提供者、临床医生咨询热线或远程医疗服务提供者。</v>
-      </c>
-      <c r="F30" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Comuníquese con un proveedor de atención médica.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Esta herramienta es para personas de 2 años o más. Llame al proveedor de atención médica del niño, a una línea de asesoría clínica o a un proveedor de telemedicina.</v>
-      </c>
-    </row>
-    <row r="31" xml:space="preserve">
+      <c r="C30" t="str">
+        <v>**이 도구는 만 2세 이상을 대상으로 합니다.** 귀하의 자녀가 만 2세 미만이며 아픈 경우 아동의 의료 제공자, 임상의 상담 전화 또는 의료진에게 전화하십시오</v>
+      </c>
+      <c r="D30" t="str">
+        <v>**Công cụ này dành cho những người từ 2 tuổi trở lên.** Vui lòng gọi cho nhà cung cấp dịch vụ y tế, đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa của trẻ nếu con quý vị dưới 2 tuổi và bị bệnh</v>
+      </c>
+      <c r="E30" t="str">
+        <v>**本工具适用于2岁以上的人**。如果您的孩子不到 2 岁且生病，请致电儿童的医疗服务提供者、临床医生咨询热线或远程医疗服务提供者</v>
+      </c>
+      <c r="F30" t="str">
+        <v>** Esta herramienta es para personas de 2 años o más.** Llame al proveedor de atención médica del niño, a una línea de asesoría clínica o a un proveedor de telemedicina si su niño tiene menos de 2 años y está enfermo</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" t="str">
         <v>CDC/messages/msg24</v>
       </c>
       <c r="B31" t="str">
         <v>**Contact an administrator or nurse at your  school or child care as soon as possible.**</v>
       </c>
-      <c r="C31" t="str" xml:space="preserve">
-        <v xml:space="preserve">**가능한 한 빨리 학교 또는 보육 관리자나 간호사에게 문의하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그 사람)의 학교 또는 보육 관리자나 간호사에게 귀하(그 사람)가 아프다고 말하십시오.</v>
-      </c>
-      <c r="D31" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ với quản lý hoặc y tá tại trường học hoặc nơi giữ trẻ của quý vị (của họ) càng sớm càng tốt.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Nói với quản lý hoặc y tá tại trường học hoặc nơi giữ trẻ của quý vị (họ) rằng quý vị (họ) đang cảm thấy bị bệnh.</v>
-      </c>
-      <c r="E31" t="str" xml:space="preserve">
-        <v xml:space="preserve">**尽快联系您（他们）所在学校或儿童保育的管理员或护士。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-告知您（他们）学校或儿童保育的管理员或护士您（他们）感觉恶心。</v>
-      </c>
-      <c r="F31" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Comuníquese con un administrador o el personal de enfermería de la escuela, centro educativo o guardería infantil lo más pronto posible.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dígale al administrador o al personal de enfermería de la escuela, centro educativo o guardería infantil que no se siente bien.</v>
+      <c r="C31" t="str">
+        <v>**가능한 한 빨리 학교 또는 보육 관리자나 간호사에게 문의하십시오.**</v>
+      </c>
+      <c r="D31" t="str">
+        <v>**Liên hệ với quản lý hoặc y tá tại trường học hoặc nơi giữ trẻ của quý vị càng sớm càng tốt.**</v>
+      </c>
+      <c r="E31" t="str">
+        <v>**尽快联系您所在学校或儿童保育的管理员或护士。**</v>
+      </c>
+      <c r="F31" t="str">
+        <v>**Comuníquese con un administrador o el personal de enfermería de su escuela o guardería lo más pronto posible.**</v>
       </c>
     </row>
     <row r="32" xml:space="preserve">
@@ -1261,98 +1110,98 @@
         <v>CDC/messages/msg23</v>
       </c>
       <c r="B32" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Contact a medical provider if you (they) get sick.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Stay in your room as much as possible except to get medical care._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cover your coughs and sneezes with a tissue._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Clean your hands often._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Avoid close contact with other people. Stay at least 6 feet away from other people._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Wear a mask when around others._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Clean and disinfect commonly touched surfaces in your room._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Contact a medical provider if you (they) get sick.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Stay in your room as much as possible except to get medical care._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Cover your coughs and sneezes with a tissue._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Clean your hands often._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Avoid close contact with other people. Stay at least 6 feet away from other people._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Wear a mask when around others._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Clean and disinfect commonly touched surfaces in your room._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - Monitor your health and notify a medical provider if you think you are getting sicker.</v>
       </c>
       <c r="C32" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)가 아플 경우 의료진에게 연락하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-[다른 사람을 질병으로부터 보호]하도록 도움을 주십시오(https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의학적 치료를 받는 경우를 제외하고 가급적 방에 머무르십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 손을 자주 씻으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다른 사람과 가까이 하지 마십시오. 다른 사람과 최소 6피트의 간격을 유지하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다른 사람들과 함께 있을 때는 마스크를 착용하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 방안에서 자주 접촉하는 표면을 청소하고 소독하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**귀하(그 사람)가 아플 경우 의료진에게 연락하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+[다른 사람을 질병으로부터 보호]하도록 도움을 주십시오(https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 의학적 치료를 받는 경우를 제외하고 가급적 방에 머무르십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 손을 자주 씻으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 다른 사람과 가까이 하지 마십시오. 다른 사람과 최소 6피트의 간격을 유지하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 다른 사람들과 함께 있을 때는 마스크를 착용하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 방안에서 자주 접촉하는 표면을 청소하고 소독하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - 자신의 건강 상태를 모니터링하여, 악화된다고 생각되면 의료진에게 알리십시오.</v>
       </c>
       <c r="D32" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ với một nhà cung cấp dịch vụ y tế nếu quý vị (họ) mắc bệnh.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Giúp [bảo vệ người khác không mắc bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Ở trong phòng của mình càng nhiều càng tốt, ngoại trừ khi cần chăm sóc y tế._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dùng khăn giấy để che khi ho và hắt hơi._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Rửa tay thường xuyên._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tránh tiếp xúc gần với người khác. - Giữ khoảng cách với người khác ít nhất 6 feet (2 mét)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đeo khẩu trang khi ở gần người khác._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Làm sạch và khử trùng các bề mặt thường chạm vào trong phòng của quý vị._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Liên hệ với một nhà cung cấp dịch vụ y tế nếu quý vị (họ) mắc bệnh.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Giúp [bảo vệ người khác không mắc bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Ở trong phòng của mình càng nhiều càng tốt, ngoại trừ khi cần chăm sóc y tế._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Dùng khăn giấy để che khi ho và hắt hơi._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Rửa tay thường xuyên._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Tránh tiếp xúc gần với người khác. - Giữ khoảng cách với người khác ít nhất 6 feet (2 mét)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Đeo khẩu trang khi ở gần người khác._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Làm sạch và khử trùng các bề mặt thường chạm vào trong phòng của quý vị._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - Theo dõi sức khỏe của quý vị và thông báo cho nhà cung cấp dịch vụ y tế nếu quý vị nghĩ rằng mình đang bị bệnh nặng hơn.</v>
       </c>
       <c r="E32" t="str" xml:space="preserve">
-        <v xml:space="preserve">**如果您生病，请联系医务人员。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-帮助 [保护他人免于生病] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 除就医外，尽可能多地待在您的房间里。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 咳嗽以及打喷嚏时，用纸巾捂住口鼻。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 经常洗手。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 避免与他人密切接触。 尝试与他人保持至少 6 英尺的距离。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--在他人周围时戴口罩。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 清洁和消毒您房间中的经常接触的表面。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**如果您生病，请联系医务人员。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+帮助 [保护他人免于生病] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 除就医外，尽可能多地待在您的房间里。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 咳嗽以及打喷嚏时，用纸巾捂住口鼻。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 经常洗手。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 避免与他人密切接触。 尝试与他人保持至少 6 英尺的距离。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-在他人周围时戴口罩。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 清洁和消毒您房间中的经常接触的表面。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - 监测您的健康状况，如果您认为您病情加重，请通知医疗服务人员。</v>
       </c>
       <c r="F32" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Comuníquese con un proveedor de atención médica si se enferma.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Ayude a [proteger a otras personas para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quédese en su habitación lo más posible, excepto para conseguir atención médica._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cúbrase la nariz y la boca al toser y estornudar con un pañuelo desechable o con la parte interna del codo._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Límpiese las manos con frecuencia._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Evite el contacto cercano con otras personas. Manténgase a por lo menos 6 pies o 2 metros de las otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Póngase una mascarilla cuando esté cerca de otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Limpie y desinfecte las superficies en su habitación que se tocan con frecuencia._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Comuníquese con un proveedor de atención médica si se enferma.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Ayude a [proteger a otras personas para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Quédese en su habitación lo más posible, excepto para conseguir atención médica._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Cúbrase la nariz y la boca al toser y estornudar con un pañuelo desechable o con la parte interna del codo._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Límpiese las manos con frecuencia._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Evite el contacto cercano con otras personas. Manténgase a por lo menos 6 pies o 2 metros de las otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Póngase una mascarilla cuando esté cerca de otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Limpie y desinfecte las superficies en su habitación que se tocan con frecuencia._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - Monitoree su salud y notifique a un proveedor de atención médica si piensa que está empeorando.</v>
       </c>
     </row>
@@ -1364,16 +1213,16 @@
         <v>**Ask a parent or guardian to assist you, or if taking by yourself, share these results with your parent/guardian.**</v>
       </c>
       <c r="C33" t="str">
-        <v>부모님 또는 보호자에게 도움을 요청하거나 본인이 하는 경우 결과를 부모님/보호자와 공유하십시오.</v>
+        <v>**부모님 또는 보호자에게 도움을 요청하거나 본인이 하는 경우 이러한 결과를 부모님/보호자와 공유하십시오.**</v>
       </c>
       <c r="D33" t="str">
-        <v>Nhờ cha mẹ hoặc người giám hộ hỗ trợ cho bạn, hoặc nếu tự làm, hãy chia sẻ những kết quả này với cha mẹ/người giám hộ của bạn.</v>
+        <v>**Nhờ cha mẹ hoặc người giám hộ hỗ trợ quý vị hoặc nếu quý vị tự làm, hãy chia sẻ những kết quả này với cha mẹ/người giám hộ của quý vị.**</v>
       </c>
       <c r="E33" t="str">
-        <v>请父母或监护人协助您，或者如果您自己在回答，与您的父母/监护人分享这些结果。</v>
+        <v>**请父母或监护人协助您，或者如果您自己服用，与您的父母/监护人分享这些结果。**</v>
       </c>
       <c r="F33" t="str">
-        <v>Pídele a uno de tus padres o tutor legal que te ayude, o si lo completas por tu cuenta, comparte estos resultados con alguno de ellos.</v>
+        <v>**Pídele a uno de tus padres o tutor legal que te ayude, o si lo haces por tu cuenta, comparte estos resultados con alguno de ellos.**</v>
       </c>
     </row>
     <row r="34" xml:space="preserve">
@@ -1381,72 +1230,68 @@
         <v>CDC/pediatric_third_person_questions/life_threat_question</v>
       </c>
       <c r="B34" t="str" xml:space="preserve">
-        <v xml:space="preserve">Do they have any of these life-threatening symptoms?
-- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone
-- Severe and constant pain or pressure in the chest
-- Extreme difficulty breathing (such as gasping for air, being unable to walk or talk without catching their breath, severe wheezing, nostrils flaring, grunting, or using extra muscles around the chest to help breathe)
-- Disoriented (acting confused or very irritable)
-- Unconscious or very difficult to wake up
-- New or worsening seizures 
-- Signs of low blood pressure (too weak to stand, dizziness, light headed, feeling cold, pale, clammy skin)
-- Dehydration (dry lips and mouth, not urinating much, sunken eyes)
-- Refusing to drink liquids 
+        <v xml:space="preserve">Do they have any of these life-threatening symptoms?_x000d__x000d_
+- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone_x000d__x000d_
+- Severe and constant pain or pressure in the chest_x000d__x000d_
+- Extreme difficulty breathing (such as gasping for air, being unable to walk or talk without catching their breath, severe wheezing, nostrils flaring, grunting, or using extra muscles around the chest to help breathe)_x000d__x000d_
+- Disoriented (acting confused or very irritable)_x000d__x000d_
+- Unconscious or very difficult to wake up_x000d__x000d_
+- New or worsening seizures _x000d__x000d_
+- Signs of low blood pressure (too weak to stand, dizziness, light headed, feeling cold, pale, clammy skin)_x000d__x000d_
+- Dehydration (dry lips and mouth, not urinating much, sunken eyes)_x000d__x000d_
+- Refusing to drink liquids _x000d__x000d_
 - Frequent vomiting</v>
       </c>
       <c r="C34" t="str" xml:space="preserve">
-        <v xml:space="preserve">그 사람에게 이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 창백한 입술 또는 얼굴_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 가슴에 심하고 지속적인 통증이나 압박감_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 극심한 호흡 곤란(예: 숨이 막힘, 숨을 참고 걷거나 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐, 앓는 소리를 냄 또는 숨을 쉬기 위해 가슴 주위에 다른 근육 사용)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 방향 감각이 상실됨(혼란스럽거나 매우 짜증나는 행동)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의식이 없거나 깨우기가 매우 어려움_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 신규 또는 악화되는 발작 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 차갑고, 창백하며, 칙칙한 피부)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 탈수(입술과 입 건조, 소변량이 많지 않음, 움푹 들어간 눈)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 액체를 마시기를 거부함 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">그 사람에게 이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d_
+- 피부, 입술 또는 손발톱 바닥이 창백해지거나 회색 또는 파란색이 됨(피부 색조에 따라 상이)_x000d__x000d_
+- 가슴에 심하고 지속적인 통증이나 압박감_x000d__x000d_
+- 극심한 호흡 곤란(예: 숨이 막힘, 숨을 참고 걷거나 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐, 앓는 소리를 냄 또는 숨을 쉬기 위해 가슴 주위에 다른 근육 사용)_x000d__x000d_
+- 방향 감각이 상실됨(혼란스럽거나 매우 짜증나는 행동)_x000d__x000d_
+- 의식이 없거나 깨우기가 매우 어려움_x000d__x000d_
+- 신규 또는 악화되는 발작 _x000d__x000d_
+- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 차갑고, 창백하며, 칙칙한 피부)_x000d__x000d_
+- 탈수(입술과 입 건조, 소변량이 많지 않음, 움푹 들어간 눈)_x000d__x000d_
+- 액체를 마시기를 거부함 _x000d__x000d_
 - 잦은 구토</v>
       </c>
       <c r="D34" t="str" xml:space="preserve">
-        <v xml:space="preserve">Họ có bất kỳ triệu chứng đe dọa đến tính mạng nào dưới đây không?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Môi hoặc mặt hơi tím tái_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đau hoặc tức ngực dữ dội và liên tục_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Khó thở cực độ (ví dụ như thở hổn hển, không thể đi lại hoặc nói chuyện liền câu mà không thở, thở khò khè dữ dội, lỗ mũi phập phồng, khụt khịt hoặc phải sử dụng thêm các cơ xung quanh ngực để giúp thở được)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất phương hướng (hành động khó hiểu hoặc dễ bị kích thích)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Bất tỉnh hoặc rất khó đánh thức dậy_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cơn co giật mới hoặc nặng hơn _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dấu hiệu của huyết áp thấp (không thể đứng vững, chóng mặt, choáng váng, ớn lạnh, xanh xao, da lạnh và mướt mồ hôi)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất nước (môi và miệng khô, không đi tiểu nhiều, mắt trũng sâu)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Từ chối uống các chất lỏng _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Họ có bất kỳ triệu chứng đe dọa đến tính mạng nào dưới đây không?_x000d__x000d_
+- Da, môi hoặc móng tay màu nhợt nhạt, xám hoặc xanh, tùy thuộc vào tông màu da_x000d__x000d_
+- Đau hoặc tức ngực dữ dội và liên tục_x000d__x000d_
+- Khó thở cực độ (ví dụ như thở hổn hển, không thể đi lại hoặc nói chuyện liền câu mà không thở, thở khò khè dữ dội, lỗ mũi phập phồng, khụt khịt hoặc phải sử dụng thêm các cơ xung quanh ngực để giúp thở được)_x000d__x000d_
+- Mất phương hướng (hành động khó hiểu hoặc dễ bị kích thích)_x000d__x000d_
+- Bất tỉnh hoặc rất khó đánh thức dậy_x000d__x000d_
+- Cơn co giật mới hoặc nặng hơn  _x000d__x000d_
+- Dấu hiệu của huyết áp thấp (không thể đứng vững, chóng mặt, choáng váng, ớn lạnh, xanh xao, da lạnh và mướt mồ hôi)_x000d__x000d_
+- Mất nước (môi và miệng khô, không đi tiểu nhiều, mắt trũng sâu)_x000d__x000d_
+- Từ chối uống các chất lỏng _x000d__x000d_
 - Thường xuyên nôn ói</v>
       </c>
       <c r="E34" t="str" xml:space="preserve">
-        <v xml:space="preserve">他们是否出现这些危及生命的症状？_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 嘴唇或面部青紫_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 重度和持续性胸痛或胸部压迫感_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--极度呼吸困难（如喘气、无法行走或说话而未屏住呼吸、严重喘息、鼻孔张开、呼噜声或使用胸部周围的额外肌肉帮助呼吸）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--定向障碍（行为混乱或非常易怒）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 意识丧失或很难唤醒_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--新发癫痫发作或癫痫发作恶化 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--拒绝饮用液体 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--频繁呕吐</v>
+        <v xml:space="preserve">他们是否出现这些危及生命的症状？_x000d__x000d_
+- 根据肤色的不同，皮肤、嘴唇或指甲呈浅色、灰色或蓝色_x000d__x000d_
+- 重度和持续性胸痛或胸部压迫感_x000d__x000d_
+-极度呼吸困难（如喘气、无法行走或说话而未屏住呼吸、严重喘息、鼻孔张开、呼噜声或使用胸部周围的额外肌肉帮助呼吸）_x000d__x000d_
+- 定向障碍（行为混乱或非常易怒）_x000d__x000d_
+- 意识丧失或很难唤醒_x000d__x000d_
+- 新发癫痫发作或癫痫发作恶化 _x000d__x000d_
+- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d_
+- 脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）_x000d__x000d_
+- 低血压体征（太虚弱无法站立、头晕目眩、感觉寒冷、苍白、皮肤湿冷） _x000d__x000d_
+- 频繁呕吐</v>
       </c>
       <c r="F34" t="str" xml:space="preserve">
-        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Labios o cara azulados_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Presión o dolor intensos y constantes en el pecho _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dificultad extrema para respirar (falta el aire o no poder caminar o hablar sin quedarse sin aliento, sibilancias intensas al respirar, se ensanchan los agujeros de la nariz, gruñido, o usa músculos adicionales en el pecho como ayuda para respirar)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Desorientación (actuar confuso o muy irritable)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Estado inconsciente o mucha dificultad para despertarse _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Convulsiones de aparición reciente o que han empeorado _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Signos de presión arterial baja (demasiado débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Deshidratación (boca y labios secos, no orinar mucho, ojos hundidos)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Negarse a consumir líquidos _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d__x000d_
+- Color pálido, gris o azulado de la piel, los labios, o el lecho de las uñas, dependiendo del tono de piel_x000d__x000d_
+- Presión o dolor intensos y constantes en el pecho _x000d__x000d_
+- Dificultad extrema para respirar (le falta el aire o no puede caminar o hablar sin quedarse sin aliento, sibilancias intensas, se ensanchan los agujeros de la nariz, gruñidos, o usa músculos adicionales en el pecho para ayudarse a respirar)_x000d__x000d_
+- Desorientación (actuar confuso o muy irritable)_x000d__x000d_
+- Estado inconsciente o mucha dificultad para despertarse _x000d__x000d_
+- Convulsiones de aparición reciente o que han empeorado _x000d__x000d_
+- Signos de presión arterial baja (muy débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa)_x000d__x000d_
+- Deshidratación (boca y labios secos, no orinar mucho, ojos hundidos)_x000d__x000d_
+- Negarse a consumir líquidos _x000d__x000d_
 - Vómitos frecuentes</v>
       </c>
     </row>
@@ -1455,70 +1300,169 @@
         <v>CDC/pediatric_second_person_questions/life_threat_question</v>
       </c>
       <c r="B35" t="str" xml:space="preserve">
-        <v xml:space="preserve">Do you have any of these life-threatening symptoms?
-- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone
-- Severe and constant pain or pressure in the chest
-- Extreme difficulty breathing (such as gasping for air, being unable to walk or talk without catching your breath, severe wheezing, nostrils flaring, grunting, or using extra muscles around the chest to help breathe)
-- Disorientation (acting confused or very irritable)
-- Unconscious or very difficult to wake up
-- New or worsening seizures 
-- Signs of low blood pressure (too weak to stand, dizziness, light headed, feeling cold, pale, clammy skin)
+        <v xml:space="preserve">Do you have any of these life-threatening symptoms?_x000d__x000d_
+- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone_x000d__x000d_
+- Severe and constant pain or pressure in the chest_x000d__x000d_
+- Extreme difficulty breathing (such as gasping for air, being unable to walk or talk without catching your breath, severe wheezing, nostrils flaring, grunting, or using extra muscles around the chest to help breathe)_x000d__x000d_
+- Disorientation (acting confused or very irritable)_x000d__x000d_
+- Unconscious or very difficult to wake up_x000d__x000d_
+- New or worsening seizures _x000d__x000d_
+- Signs of low blood pressure (too weak to stand, dizziness, light headed, feeling cold, pale, clammy skin)_x000d__x000d_
 - Dehydration (dry lips and mouth, not urinating much, sunken eyes)- Refusing to drink liquids - Frequent vomiting</v>
       </c>
       <c r="C35" t="str" xml:space="preserve">
-        <v xml:space="preserve">이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 창백한 입술 또는 얼굴_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 가슴에 심하고 지속적인 통증이나 압박감_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 극심한 호흡 곤란(예: 숨이 막힘, 숨을 참고 걷거나 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐, 앓는 소리를 냄 또는 숨을 쉬기 위해 가슴 주위에 다른 근육 사용)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 방향 감각 상실(혼란스럽거나 매우 짜증나는 행동)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의식이 없거나 깨우기가 매우 어려움_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 신규 또는 악화되는 발작 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 차갑고, 창백하며, 칙칙한 피부)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 탈수(입술과 입 건조, 소변량이 많지 않음, 움푹 들어간 눈)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 액체를 마시기를 거부함 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 창백한 입술 또는 얼굴_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 가슴에 심하고 지속적인 통증이나 압박감_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 극심한 호흡 곤란(예: 숨이 막힘, 숨을 참고 걷거나 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐, 앓는 소리를 냄 또는 숨을 쉬기 위해 가슴 주위에 다른 근육 사용)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 방향 감각 상실(혼란스럽거나 매우 짜증나는 행동)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 의식이 없거나 깨우기가 매우 어려움_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 신규 또는 악화되는 발작 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 차갑고, 창백하며, 칙칙한 피부)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 탈수(입술과 입 건조, 소변량이 많지 않음, 움푹 들어간 눈)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 액체를 마시기를 거부함 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - 잦은 구토</v>
       </c>
       <c r="D35" t="str" xml:space="preserve">
-        <v xml:space="preserve">Quý vị có bất kỳ triệu chứng đe dọa đến tính mạng nào dưới đây không?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Môi hoặc mặt hơi tím tái_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đau hoặc tức ngực dữ dội và liên tục_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Khó thở cực độ (ví dụ như thở hổn hển, không thể đi lại hoặc nói chuyện liền câu mà không thở, thở khò khè dữ dội, lỗ mũi phập phồng, khụt khịt hoặc phải sử dụng thêm các cơ xung quanh ngực để giúp thở được)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất phương hướng (hành động khó hiểu hoặc dễ bị kích thích)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Bất tỉnh hoặc rất khó đánh thức dậy_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cơn co giật mới hoặc nặng hơn _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dấu hiệu của huyết áp thấp (không thể đứng vững, chóng mặt, choáng váng, ớn lạnh, xanh xao, da lạnh và mướt mồ hôi)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất nước (môi và miệng khô, không đi tiểu nhiều, mắt trũng sâu)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Từ chối uống các chất lỏng _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Quý vị có bất kỳ triệu chứng đe dọa đến tính mạng nào dưới đây không?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Môi hoặc mặt hơi tím tái_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Đau hoặc tức ngực dữ dội và liên tục_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Khó thở cực độ (ví dụ như thở hổn hển, không thể đi lại hoặc nói chuyện liền câu mà không thở, thở khò khè dữ dội, lỗ mũi phập phồng, khụt khịt hoặc phải sử dụng thêm các cơ xung quanh ngực để giúp thở được)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Mất phương hướng (hành động khó hiểu hoặc dễ bị kích thích)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Bất tỉnh hoặc rất khó đánh thức dậy_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Cơn co giật mới hoặc nặng hơn _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Dấu hiệu của huyết áp thấp (không thể đứng vững, chóng mặt, choáng váng, ớn lạnh, xanh xao, da lạnh và mướt mồ hôi)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Mất nước (môi và miệng khô, không đi tiểu nhiều, mắt trũng sâu)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Từ chối uống các chất lỏng _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - Thường xuyên nôn ói</v>
       </c>
       <c r="E35" t="str" xml:space="preserve">
-        <v xml:space="preserve">您是否出现这些危及生命的症状？_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 嘴唇或面部青紫_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 重度和持续性胸痛或胸部压迫感_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--极度呼吸困难（如喘气、无法行走或说话而未屏住呼吸、重度喘息、鼻孔张开、呼噜声或使用胸部周围的额外肌肉帮助呼吸）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--定向障碍（行为混乱或非常易怒）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 意识丧失或很难唤醒_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--新发癫痫发作或癫痫发作恶化 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--拒绝饮用液体 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">您是否出现这些危及生命的症状？_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 嘴唇或面部青紫_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 重度和持续性胸痛或胸部压迫感_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-极度呼吸困难（如喘气、无法行走或说话而未屏住呼吸、重度喘息、鼻孔张开、呼噜声或使用胸部周围的额外肌肉帮助呼吸）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-定向障碍（行为混乱或非常易怒）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 意识丧失或很难唤醒_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-新发癫痫发作或癫痫发作恶化 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-拒绝饮用液体 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 -频繁呕吐</v>
       </c>
       <c r="F35" t="str" xml:space="preserve">
-        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Labios o cara azulados_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Presión o dolor intensos y constantes en el pecho _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dificultad extrema para respirar (falta el aire o no poder caminar o hablar sin quedarse sin aliento, sibilancias intensas al respirar, se ensanchan los agujeros de la nariz, gruñido, o usa músculos adicionales en el pecho como ayuda para respirar)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Desorientación (actuar confuso o muy irritable)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Estado inconsciente o mucha dificultad para despertarte _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Convulsiones de aparición reciente o que han empeorado _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Signos de presión arterial baja (demasiado débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Deshidratación (boca y labios secos, no orinar mucho, ojos hundidos)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Negarse a consumir líquidos _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Color pálido, gris o azulado de la piel, los labios, o el lecho de las uñas, dependiendo del tono de piel_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Presión o dolor intensos y constantes en el pecho _x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Dificultad extrema para respirar (falta el aire o no poder caminar o hablar sin quedarse sin aliento, sibilancias intensas al respirar, se ensanchan los agujeros de la nariz, gruñido, o usa músculos adicionales en el pecho como ayuda para respirar)_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Desorientación (actuar confuso o muy irritable)_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Estado inconsciente o mucha dificultad para despertarte _x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Convulsiones de aparición reciente o que han empeorado _x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Signos de presión arterial baja (demasiado débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa)_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Deshidratación (boca y labios secos, no orinar mucho, ojos hundidos)_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Negarse a consumir líquidos _x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
 - Vómitos frecuentes</v>
       </c>
     </row>
@@ -1650,16 +1594,16 @@
         <v>New rash</v>
       </c>
       <c r="C42" t="str">
-        <v>발진</v>
+        <v>새로운 발진</v>
       </c>
       <c r="D42" t="str">
-        <v>Phát ban</v>
+        <v>Phát ban mới</v>
       </c>
       <c r="E42" t="str">
-        <v>皮疹</v>
+        <v>新的皮疹</v>
       </c>
       <c r="F42" t="str">
-        <v>Sarpullido</v>
+        <v>Sarpullido nuevo</v>
       </c>
     </row>
     <row r="43">
@@ -1782,32 +1726,24 @@
         <v>Nacimiento prematuro</v>
       </c>
     </row>
-    <row r="49" xml:space="preserve">
+    <row r="49">
       <c r="A49" t="str">
         <v>CDC/messages/t2_nonUS</v>
       </c>
       <c r="B49" t="str">
         <v>**You may be eligible for COVID-19 testing. Contact your local emergency services for more information.**</v>
       </c>
-      <c r="C49" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)는 COVID-19 검사를 받을 자격이 될 수 있습니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-자세한 정보는 지역 보건부나 의료진에게 문의하십시오.</v>
-      </c>
-      <c r="D49" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quý vị (họ) có thể hội đủ điều kiện để xét nghiệm COVID-19.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Liên hệ với sở y tế địa phương hoặc nhà cung cấp dịch vụ y tế của quý vị để biết thêm thông tin.</v>
-      </c>
-      <c r="E49" t="str" xml:space="preserve">
-        <v xml:space="preserve">**您（他们）可能有资格接受新冠肺炎检测。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-如需了解更多信息，请联系当地卫生部门或医务人员。</v>
-      </c>
-      <c r="F49" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Puede que sea elegible para hacerse una prueba de COVID-19.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Comuníquese con el departamento de salud local o su proveedor de atención médica para obtener más información.</v>
+      <c r="C49" t="str">
+        <v>**귀하는 COVID-19 검사를 받을 자격이 될 수 있습니다. 더 자세한 정보를 확인하려면 지역 응급 서비스에 연락하십시오.**</v>
+      </c>
+      <c r="D49" t="str">
+        <v>**Quý vị có thể hội đủ điều kiện để xét nghiệm COVID-19. Liên hệ với các dịch vụ khẩn cấp tại địa phương của quý vị để biết thêm thông tin.**</v>
+      </c>
+      <c r="E49" t="str">
+        <v>**您可能有资格接受新冠肺炎（COVID-19）检测。如需了解更多信息，请联系当地的紧急服务机构。**</v>
+      </c>
+      <c r="F49" t="str">
+        <v>**Puede que sea elegible para hacerse una prueba del COVID-19. Comuníquese con los servicios de emergencia locales para obtener más información.**</v>
       </c>
     </row>
     <row r="50">
@@ -1975,28 +1911,28 @@
         <v>CDC/messages/t2</v>
       </c>
       <c r="B58" t="str" xml:space="preserve">
-        <v xml:space="preserve">**You (they) may be eligible for COVID-19 testing.**_x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">**You (they) may be eligible for COVID-19 testing.**_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
 Visit your health department’s website or talk to your healthcare provider for more information. To find a testing location near you, visit the [HHS website](https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html).</v>
       </c>
       <c r="C58" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)는 COVID-19 검사를 받을 자격이 될 수 있습니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**귀하(그 사람)는 COVID-19 검사를 받을 자격이 될 수 있습니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 자세한 내용은 보건부 웹사이트를 방문하거나 귀하의 담당 의료진에게 문의하십시오. 가까운 검사 장소를 찾으려면 [HHS 웹 사이트](https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html)를 방문하세요.</v>
       </c>
       <c r="D58" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quý vị (họ) có thể hội đủ điều kiện để xét nghiệm COVID-19.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Quý vị (họ) có thể hội đủ điều kiện để xét nghiệm COVID-19.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Truy cập trang web của sở y tế địa phương của quý vị hoặc nói chuyện với nhà cung cấp dịch vụ y tế của quý vị để biết thêm thông tin. Để tìm một địa điểm xét nghiệm gần quý vị, hãy truy cập [trang web HHS] (https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html).</v>
       </c>
       <c r="E58" t="str" xml:space="preserve">
-        <v xml:space="preserve">**您（他们）可能有资格接受新冠肺炎检测。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**您（他们）可能有资格接受新冠肺炎检测。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 访问您的卫生部门的网站或与您的医疗服务提供者讨论以获得更多信息。 要在您附近找到检测地点，请访问 [HHS网站]（https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html).</v>
       </c>
       <c r="F58" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Puede que sea elegible para hacerse una prueba de COVID-19.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Puede que sea elegible para hacerse una prueba de COVID-19.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Visite el sitio web de su departamento de salud o hable con su proveedor de atención médica para obtener más información. Para encontrar un lugar cercano donde realizarse la prueba, visite [el sitio web del HHS](https://www.hhs.gov/coronavirus/community-based-testing-sites/index.html).</v>
       </c>
     </row>
@@ -2005,231 +1941,129 @@
         <v>CDC/messages/t1</v>
       </c>
       <c r="B59" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Information about COVID-19 testing**_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Information about COVID-19 testing**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 For more information about testing for COVID-19, call your medical provider or visit your health department’s website.</v>
       </c>
       <c r="C59" t="str" xml:space="preserve">
-        <v xml:space="preserve">**COVID-19 검사에 대한 정보**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**COVID-19 검사에 대한 정보**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 COVID-19 검사에 대한 자세한 내용은 귀하의 담당 의료진에게 문의하거나 보건부 웹사이트를 방문하십시오.</v>
       </c>
       <c r="D59" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Thông tin về xét nghiệm COVID-19**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Thông tin về xét nghiệm COVID-19**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Để biết thêm thông tin về xét nghiệm COVID-19, hãy gọi cho nhà cung cấp dịch vụ y tế của quý vị hoặc truy cập trang web của sở y tế địa phương.</v>
       </c>
       <c r="E59" t="str" xml:space="preserve">
-        <v xml:space="preserve">**关于新冠肺炎检测的信息 **_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**关于新冠肺炎检测的信息 **_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 有关新冠肺炎检测的更多信息，请致电您的医疗服务提供者或访问您所在地的卫生局门网站。</v>
       </c>
       <c r="F59" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Información sobre la prueba de COVID-19**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Información sobre la prueba de COVID-19**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Para obtener más información sobre la prueba de COVID-19, llame a su proveedor médico o visite el sitio web de su departamento de salud.</v>
       </c>
     </row>
-    <row r="60" xml:space="preserve">
+    <row r="60">
       <c r="A60" t="str">
         <v>CDC/messages/t0</v>
       </c>
       <c r="B60" t="str">
         <v>**Based on the answers given, you do not need to get tested unless recommended or required by your healthcare provider, employer, or public health official**</v>
       </c>
-      <c r="C60" t="str" xml:space="preserve">
-        <v xml:space="preserve">**현 시점에서 COVID-19 검사는 필요하지 않습니다**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-제공한 답변에 따라 의료 전문가, 고용주, 공중 보건 당국이 권고하거나 요구하지 않는 경우 검사를 받을 필요가 없습니다.</v>
-      </c>
-      <c r="D60" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Không cần xét nghiệm COVID-19 tại thời điểm này**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dựa trên các câu trả lời được đưa ra, quý vị (họ) không cần phải làm xét nghiệm, trừ khi được nhà cung cấp dịch vụ y tế, chủ lao động hoặc quan chức y tế công cộng của quý vị (họ) đề nghị hoặc yêu cầu.</v>
-      </c>
-      <c r="E60" t="str" xml:space="preserve">
-        <v xml:space="preserve">**此时无需进行新冠肺炎检测 **_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-根据提供的答案，您（他们）不需要接受检测，除非您（他们）的医疗服务提供者、雇主或公共卫生官员推荐或要求这样做。</v>
-      </c>
-      <c r="F60" t="str" xml:space="preserve">
-        <v xml:space="preserve">**No necesita una prueba de COVID-19 en este momento**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Hasta ahora, sus respuestas parecen indicar que no necesita hacerse la prueba de COVID-19. Si algo cambia, responda el autoverificador de nuevo.</v>
-      </c>
-    </row>
-    <row r="61" xml:space="preserve">
+      <c r="C60" t="str">
+        <v>**제공한 답변에 따라 의료 전문가, 고용주, 공중 보건 당국이 권고하거나 요구하지 않는 경우 검사를 받을 필요가 없습니다.**</v>
+      </c>
+      <c r="D60" t="str">
+        <v>**Dựa trên các câu trả lời được đưa ra, quý vị không cần phải làm xét nghiệm, trừ khi được nhà cung cấp dịch vụ y tế, chủ lao động hoặc quan chức y tế công cộng của quý vị đề nghị hoặc yêu cầu**</v>
+      </c>
+      <c r="E60" t="str">
+        <v>**根据提供的答案，您不需要接受检测，除非您的医疗保健提供者、雇主或公共卫生官员推荐或要求这样做**</v>
+      </c>
+      <c r="F60" t="str">
+        <v>**Según las respuestas que nos ha dado, no necesita hacerse la prueba a menos que se lo recomiende o exija su proveedor de atención médica, empleador o funcionario de salud pública**</v>
+      </c>
+    </row>
+    <row r="61">
       <c r="A61" t="str">
         <v>CDC/messages/msg18</v>
       </c>
       <c r="B61" t="str">
         <v>**Stay home for 14 days from the day you last had contact.** Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing. If you develop any of these symptoms, call your medical provider, clinician advice line, or telemedicine provider</v>
       </c>
-      <c r="C61" t="str" xml:space="preserve">
-        <v xml:space="preserve">**증상을 모니터링하고 집에 머무르십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 마지막으로 접촉한 날부터 14일 동안 집에 머무르십시오. 격리를 시작하고 종료할 시기를 결정하려면 CDC 지침을 따르십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 하루 2번 귀하(그 사람)의 체온을 재고, [COVID-19 증상이 있는지](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html) 관찰하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- [사회적 거리두기](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/social-distancing.html)를 실천하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 다른 사람과 6피트 이상 간격을 유지하고 밀집된 장소를 피하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 가능하다면, COVID-19로 인해 중증 질환을 겪을 수 있는 [고위험](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/index.html) 환자로부터 거리를 두십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 귀하(그 사람)에게 증상이 발현되면 [CDC 지침](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)을 따르십시오.</v>
-      </c>
-      <c r="D61" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Theo dõi các triệu chứng, ở nhà.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Ở nhà trong 14 ngày kể từ ngày quý vị (họ) tiếp xúc lần cuối. Để xác định thời điểm bắt đầu và kết thúc cô lập, hãy làm theo hướng dẫn của CDC._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đo nhiệt độ cơ thể của quý vị (của họ) hai lần một ngày và theo dõi [các triệu chứng mắc COVID-19] (https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Thực hành [giãn cách xã hội] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/social-distancing.html). _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - Tránh xa những người khác ít nhất 6 feet (2 mét) và tránh xa những nơi đông người. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - Nếu có thể, hãy tránh xa những người có [nguy cơ cao hơn] (https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/index.html) mắc bệnh nặng do COVID-19 . _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Nếu bạn (họ) phát triển các triệu chứng, hãy làm theo [hướng dẫn của CDC] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="E61" t="str" xml:space="preserve">
-        <v xml:space="preserve">**监测症状，待在家里。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 自您（他们）最后一次接触之日起，请呆在家里 14 天。 至于何时开始和结束分离，请遵循 CDC 指南。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 每天测量两次体温，并观察 [新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 执行 [社交疏离](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/social-distancing.html)。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 远离他人，至少保持 6 英尺距离，远离拥挤的地方。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 如可能，远离非常严重的新冠肺炎病情的[风险较高](https://www.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/index.html）者。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 如果您（他们）出现症状，请遵循 [CDC 指南](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)。</v>
-      </c>
-      <c r="F61" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Monitoréese en busca de síntomas, quédese en casa.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quédese en casa por 14 días._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tómese (tómele) la temperatura dos veces por día y esté atento a los [síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Practique [el distanciamiento social](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/social-distancing.html). _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    - Manténgase a por lo menos 6 pies o 2 metros de distancia de los demás y fuera de los lugares con mucha gente. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    - Si es posible, manténgase alejado de las personas con [mayor riesgo](https://espanol.cdc.gov/coronavirus/2019-ncov/need-extra-precautions/index.html) de enfermarse gravemente con el COVID-19. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Si presenta síntomas, siga las [directrices de los CDC](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-    </row>
-    <row r="62" xml:space="preserve">
+      <c r="C61" t="str">
+        <v>**마지막으로 접촉한 날부터 14일 동안 집에 머무르십시오.** 발열, 기침, 또는 호흡곤란과 같은 COVID-19 증상이 있는지 관찰하십시오. 귀하에게 이러한 증상들 중 어느 것이라도 발생하면, 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오</v>
+      </c>
+      <c r="D61" t="str">
+        <v>**Ở nhà trong 14 ngày kể từ ngày quý vị tiếp xúc lần cuối.** Theo dõi các triệu chứng COVID-19 như sốt, ho hoặc khó thở. Nếu quý vị phát triển bất kỳ trong số các triệu chứng này, hãy gọi cho nhà cung cấp dịch vụ y tế của quý vị, đường dây tư vấn bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa.</v>
+      </c>
+      <c r="E61" t="str">
+        <v>**从最后一次接触之日起，请留在家中14天**。注意观察是否有COVID-19症状，如发烧、咳嗽或呼吸困难。如果您出现任何症状，请致电您（他们）的医疗服务提供者、临床医生建议热线或远程医疗服务提供者</v>
+      </c>
+      <c r="F61" t="str">
+        <v>**Quédese en casa por 14 días desde el día en que tuvo el último contacto.** Esté atento a síntomas del COVID-19 como fiebre, tos o dificultad para respirar. Si presenta alguno de estos síntomas, llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina</v>
+      </c>
+    </row>
+    <row r="62">
       <c r="A62" t="str">
         <v>CDC/messages/msg17</v>
       </c>
       <c r="B62" t="str">
         <v>**Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing.** If you develop any of these symptoms, call your medical provider, clinician advice line, or telemedicine provider.</v>
       </c>
-      <c r="C62" t="str" xml:space="preserve">
-        <v xml:space="preserve">**증상을 모니터링하고 마스크를 착용하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-[COVID-19 증상]이 있는지 관찰하십시오(https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). 귀하(그 사람)에게 이러한 증상이 발생하면, 귀하(그 사람)의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오. 다른 사람들과 함께 있을 때, 귀하(그 사람) 본인과 귀하(그 사람)의 주변 사람들을 보호하기 위해 귀하(그 사람)의 코와 입에 마스크를 쓰도록 요청 받게 됩니다. 호흡곤란이 있거나, 의식이 없거나, 무능력하거나, 스스로 마스크를 벗을 수 없는 사람에게는 마스크를 사용해서는 안 됩니다.</v>
-      </c>
-      <c r="D62" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Theo dõi các triệu chứng, đeo khẩu trang.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Theo dõi [các triệu chứng COVID-19] (https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Nếu quý vị (họ) phát triển các triệu chứng, hãy gọi cho nhà cung cấp dịch vụ y tế của quý vị (của họ), đường dây tư vấn bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa. Khi ở gần người khác, quý vị (họ) sẽ được yêu cầu đeo khẩu trang che mũi và miệng để bảo vệ bản thân và những người xung quanh. Không nên sử dụng khẩu trang cho người bị khó thở, bất tỉnh, mất khả năng vận động hoặc không thể tự tháo khẩu trang ra.</v>
-      </c>
-      <c r="E62" t="str" xml:space="preserve">
-        <v xml:space="preserve">**监测症状，佩戴口罩。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-观察 [新冠肺炎症状]（https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。 如果您（他们）出现症状，请致电您（他们）的医疗服务提供者、临床医生建议热线或远程医疗服务提供者。 当与他人在一起时，您（他们）将被要求在您（他们）的鼻子和嘴上佩戴口罩，以保护您（自己）和您（他们）周围的人。 任何出现呼吸困难、无意识、无行为能力或无法自行摘下口罩的人吧应该佩戴口罩。</v>
-      </c>
-      <c r="F62" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Monitoréese en busca de síntomas, póngase una mascarilla.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Esté atento a los [síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Si presenta síntomas, llame a su proveedor de atención médica, a una línea de asesoría clínica o a un proveedor de telemedicina. Cuando esté cerca de otras personas, le pedirán que se ponga una mascarilla sobre su nariz y boca para protegerse y proteger a quienes estén cerca. No se deben poner mascarillas a personas con problemas para respirar, o que estén inconscientes o incapacitadas, o que de otra forma no puedan quitársela sin ayuda.</v>
-      </c>
-    </row>
-    <row r="63" xml:space="preserve">
+      <c r="C62" t="str">
+        <v>**발열, 기침, 또는 호흡곤란과 같은 COVID-19 증상이 있는지 관찰하십시오.** 귀하에게 이러한 증상들 중 어느 것이라도 발생하면, 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오.</v>
+      </c>
+      <c r="D62" t="str">
+        <v>**Theo dõi các triệu chứng COVID-19 như sốt, ho hoặc khó thở.** Nếu quý vị phát triển bất kỳ triệu chứng nào trong số này, hãy gọi cho nhà cung cấp dịch vụ y tế, đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa.</v>
+      </c>
+      <c r="E62" t="str">
+        <v>**注意COVID-19的症状，如发烧、咳嗽或呼吸困难。**如果您出现任何症状，请致电您的医疗服务提供者、临床医生咨询热线或远程医疗服务提供者。</v>
+      </c>
+      <c r="F62" t="str">
+        <v>**Esté atento a síntomas del COVID-19 como fiebre, tos o dificultad para respirar.** Si presenta alguno de estos síntomas, llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina.</v>
+      </c>
+    </row>
+    <row r="63">
       <c r="A63" t="str">
         <v>CDC/messages/msg16</v>
       </c>
       <c r="B63" t="str">
         <v>**Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing.** If you develop any of these symptoms, call your medical provider, clinician advice line, or telemedicine provider.</v>
       </c>
-      <c r="C63" t="str" xml:space="preserve">
-        <v xml:space="preserve">**증상을 모니터링하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-[COVID-19 증상]이 있는지 관찰하십시오(https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). 귀하(그 사람)에게 이러한 증상이 발생하면, 귀하(그 사람)의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오. _x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-[CDC 웹사이트]에서 COVID-19 및 자신(그 사람)과 타인을 보호하는 방법에 대해 자세히 알아보십시오(https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
-      </c>
-      <c r="D63" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Theo dõi các triệu chứng.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Theo dõi [các triệu chứng COVID-19] (https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Nếu quý vị (họ) phát triển các triệu chứng, hãy gọi cho nhà cung cấp dịch vụ y tế của quý vị (của họ), đường dây tư vấn bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Tìm hiểu thêm về COVID-19 và các bước mà quý vị (họ) có thể thực hiện để bảo vệ bản thân và những người khác trên [trang web của CDC] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
-      </c>
-      <c r="E63" t="str" xml:space="preserve">
-        <v xml:space="preserve">**监测症状。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-观察 [新冠肺炎症状]（https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。 如果您（他们）出现症状，请致电您（他们）的医疗服务提供者、临床医生建议热线或远程医疗服务提供者。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-访问[CDC 网站]了解更多关于新冠肺炎以及如何保护自己（他们）和他人的信息（https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html)。</v>
-      </c>
-      <c r="F63" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Monitoréese (monitoréelo) en busca de síntomas.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Esté atento a los [síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Si presenta síntomas, llame a su proveedor de atención médica, a una línea de asesoría clínica o a un proveedor de telemedicina. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Obtenga más información sobre el COVID-19 y las medidas que puede tomar para protegerse (protegerlo) y proteger a los demás en el [sitio web de los CDC](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
-      </c>
-    </row>
-    <row r="64" xml:space="preserve">
+      <c r="C63" t="str">
+        <v>**발열, 기침, 또는 호흡곤란과 같은 COVID-19 증상이 있는지 관찰하십시오.** 귀하에게 이러한 증상들 중 어느 것이라도 발생하면, 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오.</v>
+      </c>
+      <c r="D63" t="str">
+        <v>**Theo dõi các triệu chứng COVID-19 như sốt, ho hoặc khó thở.** Nếu quý vị phát triển bất kỳ triệu chứng nào trong số này, hãy gọi cho nhà cung cấp dịch vụ y tế, đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa.</v>
+      </c>
+      <c r="E63" t="str">
+        <v>**注意COVID-19的症状，如发烧、咳嗽或呼吸困难。**如果您出现任何症状，请致电您的医疗服务提供者、临床医生咨询热线或远程医疗服务提供者。</v>
+      </c>
+      <c r="F63" t="str">
+        <v>**Esté atento a síntomas del COVID-19 como fiebre, tos o dificultad para respirar.** Si presenta alguno de estos síntomas, llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina.</v>
+      </c>
+    </row>
+    <row r="64">
       <c r="A64" t="str">
         <v>CDC/messages/msg15</v>
       </c>
       <c r="B64" t="str">
         <v>**As soon as possible, tell your occupational health provider (or supervisor) that you may have been in contact with someone with suspected COVID-19.**</v>
       </c>
-      <c r="C64" t="str" xml:space="preserve">
-        <v xml:space="preserve">**직장의 직장 위생 전문가에게 연락하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-COVID-19로 진단된 사람과 접촉했음을 직장 위생 전문가(또는 감독자)에게 알리십시오. 자신과 주변 사람들을 보호하기 위해 코와 입에 마스크를 착용해야 할 수도 있습니다. _x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 14일 동안 하루에 두 번 체온을 확인하십시오. _x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- [COVID-19 증상]이 있는지 관찰하십시오(https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). [CDC 웹사이트]에서 COVID-19 및 자신과 타인을 보호하는 방법에 대해 자세히 알아보십시오(https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
-      </c>
-      <c r="D64" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ với nhà cung cấp dịch vụ sức khỏe nghề nghiệp tại nơi làm việc của quý vị.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Nói với nhà cung cấp dịch vụ sức khỏe nghề nghiệp của quý vị (hoặc quản lý trực tiếp của quý vị) rằng quý vị đã tiếp xúc với người được chẩn đoán mắc COVID-19. Quý vị có thể được yêu cầu đeo khẩu trang che mũi và miệng để bảo vệ bản thân và những người xung quanh. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Kiểm tra nhiệt đô cơ thể của quý vị hai lần một ngày trong 14 ngày. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Theo dõi [các triệu chứng COVID-19] (https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Tìm hiểu thêm về COVID-19 và cách quý vị có thể tự bảo vệ mình và những người khác trên [trang web của CDC] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
-      </c>
-      <c r="E64" t="str" xml:space="preserve">
-        <v xml:space="preserve">**联系工作场所的职业保健提供者。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-告知您的职业保健提供者（或监督员）您接触过诊断为新冠肺炎的人。 可能会要求您在口鼻上方佩戴口罩，以保护自己和周围的人。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--每天检查两次体温，持续 14 天。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--观察 [新冠肺炎症状]（https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。 访问[CDC 网站]了解更多关于新冠肺炎以及如何保护自己和他人的信息（https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html)。</v>
-      </c>
-      <c r="F64" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Póngase en contacto con el proveedor de salud ocupacional de su lugar de trabajo.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dígale a su proveedor de salud ocupacional (o supervisor) que usted ha estado en contacto con alguien a quien le diagnosticaron COVID-19. Es posible que le pidan que use una mascarilla para protegerse y proteger a quienes lo rodean._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tómese la temperatura dos veces al día por 14 días. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Esté atento a los [síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Obtenga más información sobre el COVID-19 y cómo puede protegerse y proteger a los demás en el [sitio web de los CDC](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/index.html).</v>
+      <c r="C64" t="str">
+        <v>**가능한 한 빨리 귀하가 COVID-19가 의심되는 사람과 접촉했을 수 있음을 직장 위생 전문가(또는 감독자)에게 알리십시오.**</v>
+      </c>
+      <c r="D64" t="str">
+        <v>**Càng sớm càng tốt, hãy thông báo cho nhà cung cấp dịch vụ sức khỏe nghề nghiệp (hoặc người giám sát) của quý vị rằng quý vị có thể đã tiếp xúc với người bị nghi ngờ nhiễm COVID-19.**</v>
+      </c>
+      <c r="E64" t="str">
+        <v>**请尽快告知您的职业保健提供者（或监督员）您可能接触过COVID-19疑似患者。**</v>
+      </c>
+      <c r="F64" t="str">
+        <v>**Tan pronto como sea posible, dígale a su proveedor de salud ocupacional (o supervisor) que usted puede haber estado en contacto con alguien con COVID-19 presunto.**</v>
       </c>
     </row>
     <row r="65">
@@ -2240,16 +2074,16 @@
         <v>**If you start to feel sick, tell a medical provider in the care center, nursing home, or shelter where you live.**</v>
       </c>
       <c r="C65" t="str">
-        <v>귀하가 아프기 시작하면 거주하고 계신 보호 센터, 요양원 또는 보호소의 의료진에게 알리십시오.</v>
+        <v>**귀하가 아프기 시작하면 거주하고 계신 보호 센터, 요양원 또는 보호소의 의료진에게 알리십시오.**</v>
       </c>
       <c r="D65" t="str">
-        <v>Nếu bạn bắt đầu cảm thấy bệnh, hãy thông báo với nhân viên y tế tại trung tâm chăm sóc, nhà điều dưỡng hoặc nhà ở xã hội nơi bạn sinh sống.</v>
+        <v>**Nếu quý vị bắt đầu cảm thấy không khỏe, hãy nói với nhà cung cấp dịch vụ y tế tại trung tâm chăm sóc, viện dưỡng lão hoặc nơi tạm trú nơi quý vị sống.**</v>
       </c>
       <c r="E65" t="str">
-        <v>如果您开始感觉不适，请告知您居住的护理中心、疗养院或收容所的医疗服务提供者。</v>
+        <v>**如果您开始感觉不适，请告知您居住的护理中心、疗养院或收容所的医疗服务提供者。**</v>
       </c>
       <c r="F65" t="str">
-        <v>Si empieza a sentirse enfermo, dígale a un proveedor de atención médica del centro de salud, hogar de ancianos o refugio donde viva.</v>
+        <v>** Si empieza a sentirse enfermo, dígale a un proveedor médico del centro de salud, hogar de ancianos o refugio donde viva.**</v>
       </c>
     </row>
     <row r="66">
@@ -2360,16 +2194,16 @@
         <v>**Please consent to use the Coronavirus Self-Checker.** Refresh the page to start again.</v>
       </c>
       <c r="C71" t="str">
-        <v>코로나 바이러스 자가 점검 시스템을 사용하려면 동의하십시오. 페이지를 새로 고침하여 다시 시작하십시오.</v>
+        <v>**코로나 바이러스 자가 점검 시스템을 사용하려면 동의하십시오.** 페이지를 새로 고치고 다시 시작하십시오.</v>
       </c>
       <c r="D71" t="str">
-        <v>Vui lòng chấp thuận sử dụng Công cụ Tự Kiểm tra Coronavirus. Làm mới trang để bắt đầu lại.</v>
+        <v>** Vui lòng đồng ý sử dụng Công cụ tự kiểm tra Vi rút Corona.** Hãy làm mới trang để bắt đầu lại.</v>
       </c>
       <c r="E71" t="str">
-        <v>使用冠状病毒自我检查问卷时，请给予同意。刷新页面以重新开始。</v>
+        <v>**请同意使用Coronavirus Self-Checker（冠状病毒自检器）。** 刷新页面重新开始。</v>
       </c>
       <c r="F71" t="str">
-        <v>Dé su consentimiento para poder usar el Autoverificador del Coronavirus. Actualice la página para empezar de nuevo.</v>
+        <v>**Dé su consentimiento para usar el Autoverificador del Coronavirus.** Actualice la página para empezar de nuevo.</v>
       </c>
     </row>
     <row r="72" xml:space="preserve">
@@ -2383,7 +2217,7 @@
         <v>\n\n**해당 지역의 COVID-19에 대한 추가 정보 및 지침은 보건부 또는 지역 보건 부서에 확인하십시오.**</v>
       </c>
       <c r="D72" t="str" xml:space="preserve">
-        <v xml:space="preserve">_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 _x000d__x000d__x000d__x000d_\n\n**Vui lòng kiểm tra với Bộ Y tế hoặc phòng y tế địa phương để có thêm thông tin và hướng dẫn về COVID-19 ở địa điểm của bạn.**</v>
       </c>
       <c r="E72" t="str">
@@ -2393,531 +2227,144 @@
         <v>\n\n**Consulte al Ministerio de Salud o el departamento de salud local para obtener información adicional y directrices sobre el COVID-19 en su área.**</v>
       </c>
     </row>
-    <row r="73" xml:space="preserve">
+    <row r="73">
       <c r="A73" t="str">
         <v>CDC/messages/msg10</v>
       </c>
       <c r="B73" t="str">
         <v>**Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing.** If you develop any of these symptoms or if you start feeing worse, call your medical provider, clinician advice line, or telemedicine provider.</v>
       </c>
-      <c r="C73" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)가 아프다고 하시니 염려됩니다. 집에 머무르고(그 사람이 집에 머무르도록 하고) 귀하(그 사람)의 증상을 모니터링하십시오. 상태가 나빠질 경우 귀하(그 사람)의 의료진에게 연락하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-[COVID-19 증상](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html) 이 있는지 관찰하십시오. 귀하(그 사람)에게 이러한 증상들 중 어느 것이라도 발생하거나 귀하(그 사람)의 상태가 나빠지기 시작하면, 귀하(그 사람)의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그 사람)의 상태가 좋아질 수 있는 몇 가지 방법은 다음과 같습니다:_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 집에서 머무르면서 휴식을 취하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 물과 기타 음료수를 많이 마셔 체액 손실(탈수)이 일어나지 않도록 하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 비누와 물로 자주 손을 씻으십시오.</v>
-      </c>
-      <c r="D73" t="str" xml:space="preserve">
-        <v xml:space="preserve">** Xin lỗi quý vị (họ) đang cảm thấy không khỏe. Hãy ở nhà (giữ họ ở nhà) và theo dõi các triệu chứng của quý vị (của họ). Gọi cho nhà cung cấp dịch vụ y tế của quý vị (của họ) nếu tình trạng trở nên xấu hơn.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Theo dõi [các triệu chứng COVID-19] (https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Nếu quý vị (họ) phát triển bất kỳ triệu chứng nào trong số này hoặc nếu quý vị (họ) bắt đầu cảm thấy tình trạng xấu hơn, hãy gọi cho nhà cung cấp dịch vụ y tế của quý vị (của họ), đường dây tư vấn bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dưới đây là một số bước có thể giúp quý vị (họ) cảm thấy tốt hơn:_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Ở nhà và nghỉ ngơi. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Uống nhiều nước và các chất lỏng trong khác để tránh bị mất nước._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dùng khăn giấy để che khi ho và hắt hơi. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Thường xuyên rửa tay bằng xà phòng và nước.</v>
-      </c>
-      <c r="E73" t="str" xml:space="preserve">
-        <v xml:space="preserve">**很遗憾得知您（他们）感觉不舒服。 呆在家里（让他们呆在家里）并监测您（他们）的症状。 如果您（他们）病情恶化，请致电您的医疗服务提供者 **_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-观察 [新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)。 如果您（他们）出现任何这些症状，或者您（他们）开始感觉恶化，请致电您（他们）的医疗服务提供者、临床医生建议热线或远程医疗服务提供者。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-以下措施可以帮助您（他们）感觉好转：_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 在家休息。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 饮用大量的水和其他清流质饮品，以免水分流失（脱水）。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 咳嗽以及打喷嚏时，用纸巾捂住口鼻。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 经常用肥皂和清水洗手。</v>
-      </c>
-      <c r="F73" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Lamento que no se sienta bien. Quédese (manténgalo) en casa y monitoree sus síntomas. Llame a su proveedor de atención médica si empeora.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Esté atento a los [síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html). Si presenta cualquiera de estos síntomas o si comienza a sentirse peor, llame a su proveedor de atención médica, a una línea de asesoría clínica o a un proveedor de telemedicina. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Aquí hay algunas medidas que podrían ayudarlo a sentirse mejor:_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quedarse en casa y descansar. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Beber mucha agua y otros líquidos claros para evitar la pérdida de líquidos (deshidratación)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cubrirse la boca y la nariz al toser o estornudar. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Lavarse las manos frecuentemente con agua y jabón.</v>
-      </c>
-    </row>
-    <row r="74" xml:space="preserve">
+      <c r="C73" t="str">
+        <v>**발열, 기침, 또는 호흡곤란과 같은 COVID-19 증상이 있는지 관찰하십시오.** 귀하에게 이러한 증상들 중 어느 것이라도 발생하거나 귀하의 상태가 나빠지기 시작하면, 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오.</v>
+      </c>
+      <c r="D73" t="str">
+        <v>**Theo dõi các triệu chứng COVID-19 như sốt, ho, hoặc khó thở.** Nếu quý vị phát triển bất kỳ triệu chứng nào trong số này hoặc nếu quý vị bắt đầu nặng hơn, hãy gọi cho nhà cung cấp dịch vụ y tế, đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa.</v>
+      </c>
+      <c r="E73" t="str">
+        <v>**注意COVID-19的症状，如发烧、咳嗽或呼吸困难。**如果您出现任何症状，或如果您的病情开始恶化，请致电您的医疗服务提供者、临床医生咨询热线或远程医疗服务提供者。</v>
+      </c>
+      <c r="F73" t="str">
+        <v>**Esté atento a síntomas del COVID-19 como fiebre, tos o dificultad para respirar.** Si presenta cualquiera de estos síntomas o si comienza a sentirse peor, llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina.</v>
+      </c>
+    </row>
+    <row r="74">
       <c r="A74" t="str">
         <v>CDC/messages/msg9</v>
       </c>
       <c r="B74" t="str">
         <v>**Stay home except to get medical care and take care of yourself.** Call your medical provider, clinician advice line, or telemedicine provider.</v>
       </c>
-      <c r="C74" t="str" xml:space="preserve">
-        <v xml:space="preserve">**집에 머무르고(그 사람이 집에 머무르도록 하고) 자신(그 사람)을 돌보십시오. 귀하(그 사람)의 의료진에게 전화하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그 사람)가 몸 상태가 좋지 않다고 하시니 염려됩니다. 귀하(그 사람)의 증상이 COVID-19와 관련 있을 수 있습니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 귀하(그 사람)의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의학적 치료를 받는 경우를 제외하고 집에 머무르십시오(그 사람이 집에 머무르도록 하십시오)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 직장, 학교 또는 식료품점, 약국 또는 식당을 포함한 공공 장소에 가지 마십시오. 음식과 약에 대해 배달 옵션을 고려하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 대중 교통수단을 이용하거나 승차 공유를 하지 마십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 비누와 물로 자주 손을 씻으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다른 사람과 가까이 하지 마십시오. 다른 사람과 최소 6피트의 간격을 유지하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다른 사람들과 함께 있을 때는 마스크를 착용하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 귀하(그 사람)의 상태가 나빠지고 귀하가 응급 상황이라고 생각하면, 911에 전화하거나 즉시 의료 서비스를 받으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 가능한 경우 [원격 의료 서비스](https://telehealth.hhs.gov/)를 사용해보십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- [자신을 돌보는 방법](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) 또는 [아픈 누군가를 돌보는 방법](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)에 대해 알아보십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- [다른 사람을 질병으로부터 보호]하는 데 도움이 될 수 있도록 절차를 따르십시오(https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="D74" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Ở nhà (giữ họ ở nhà) và chăm sóc bản thân (cho họ). Gọi cho nhà cung cấp dịch vụ y tế của quý vị (của họ).**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Rất tiếc quý vị (họ) không được khỏe. (Các) triệu chứng của quý vị (của họ) có thể liên quan đến COVID-19. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Gọi cho nhà cung cấp dịch vụ y tế của quý vị (của họ), đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Hãy ở nhà (giữ họ ở nhà) trừ khi cần chăm sóc y tế. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - Không đến cơ quan, trường học hoặc các khu vực công cộng bao gồm cả cửa hàng tạp hóa, hiệu thuốc hoặc nhà hàng. Cân nhắc các lựa chọn giao hàng thực phẩm và thuốc. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - Không sử dụng phương tiện giao thông công cộng hoặc đi xe chung._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dùng khăn giấy để che khi ho và hắt hơi._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Thường xuyên rửa tay bằng xà phòng và nước._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tránh tiếp xúc gần với người khác. - Giữ khoảng cách với người khác ít nhất 6 feet (2 mét)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đeo khẩu trang khi ở gần người khác._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Nếu quý vị (họ) cảm thấy tình trạng trở nên xấu hơn và cho rằng đó là trường hợp khẩn cấp, hãy gọi 911 hoặc tìm kiếm sự chăm sóc y tế ngay lập tức. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cân nhắc sử dụng [dịch vụ chăm sóc sức khỏe từ xa] (https://telehealth.hhs.gov/) nếu có._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Học cách [chăm sóc bản thân] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) hoặc [người khác bị bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Thực hiện các bước để giúp [bảo vệ người khác không mắc bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="E74" t="str" xml:space="preserve">
-        <v xml:space="preserve">**呆在家里（让他们呆在家里）照顾自己（他们）。 请致电您的（他们的）医疗服务提供者。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-很遗憾得知您（他们）感觉不舒服。 您（他们）的症状可能与新冠肺炎有关。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 在 24 小时内致电您的医疗服务提供者、临床医生建议热线或远程医疗服务提供者。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 除非要接受诊疗护理，否则请留在家中（让他们呆在家里）。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- -请勿去工作、学校或公共区域，包括杂货店、药店或餐馆。 考虑通过快递获得食物和药物。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 不要乘公共交通工具或拼车。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 咳嗽以及打喷嚏时，用纸巾捂住口鼻。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 经常用肥皂和清水洗手。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 避免与他人密切接触。 尝试与他人保持至少 6 英尺的距离。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--在他人周围时戴口罩。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--如果您（他们）感觉恶化，并且您认为这是紧急情况，请拨打 911 或立即就医。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--考虑使用 [远程医疗服务]（https://telehealth.hhs.gov/）如可用。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 学习如何 [照顾自己] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) 或 [其他生病的人] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 采取措施帮助 [保护他人免于生病] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)。</v>
-      </c>
-      <c r="F74" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quédese (manténgalo) en casa y cuídese (cuídelo). Llame a su proveedor de atención médica.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Lamento que no se sienta bien. Sus síntomas podrían estar relacionados con el COVID-19.  _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Llame a su proveedor de atención médica, a una línea de asesoría clínica o a un proveedor de telemedicina. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quédese (manténgalo) en casa, excepto para conseguir atención médica. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    - No vaya al trabajo, centro educativo o lugares públicos, como tiendas de alimentos, farmacias o restaurantes. Considere opciones como entrega de comidas y medicamentos a domicilio. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    - No use el transporte público ni vehículos compartidos._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Si se siente peor y piensa que es una emergencia, llame al 911 o busque atención médica de inmediato. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Considere usar [servicios de telesalud](https://telehealth.hhs.gov/) si están disponibles._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Sepa cómo [cuidarse](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) o [cuidar a alguien que esté enfermo] (https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tome medidas para ayudar a [proteger a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-    </row>
-    <row r="75" xml:space="preserve">
+      <c r="C74" t="str">
+        <v>**의학적 치료를 받는 경우를 제외하고 집에 머무르고 자신을 돌보십시오.** 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오.</v>
+      </c>
+      <c r="D74" t="str">
+        <v>**Ở nhà ngoại trừ để nhận chăm sóc y tế và chăm sóc bản thân.** Gọi cho nhà cung cấp dịch vụ y tế, đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa.</v>
+      </c>
+      <c r="E74" t="str">
+        <v>**除了接受医疗护理和照顾自己外，请留在家中。**致电您的医疗服务提供者、临床医生咨询热线或远程医疗服务提供者。</v>
+      </c>
+      <c r="F74" t="str">
+        <v>**Quédese en casa, excepto para conseguir atención médica, y cuídese.** Llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina.</v>
+      </c>
+    </row>
+    <row r="75">
       <c r="A75" t="str">
         <v>CDC/messages/msg8</v>
       </c>
       <c r="B75" t="str">
         <v>**Stay home except to get medical care and take care of yourself.** Call your medical provider if you start feeling worse.</v>
       </c>
-      <c r="C75" t="str" xml:space="preserve">
-        <v xml:space="preserve">**집에 머무르고(그 사람이 집에 머무르도록 하고) 자신(그 사람)을 돌보십시오. 귀하(그 사람)의 상태가 악화되면 귀하(그 사람)의 의료진에게 전화하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그 사람)가 몸 상태가 좋지 않다고 하시니 염려됩니다. 귀하(그 사람)의 증상이 COVID-19와 관련 있을 수 있습니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의학적 치료를 받는 경우를 제외하고 집에 머무르십시오(그 사람이 집에 머무르도록 하십시오)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 직장, 학교 또는 식료품점, 약국 또는 식당을 포함한 공공 장소에 가지 마십시오. 음식과 약에 대해 배달 옵션을 고려하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 대중 교통수단을 이용하거나 승차 공유를 하지 마십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 비누와 물로 자주 손을 씻으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다른 사람과 가까이 하지 마십시오. 다른 사람과 최소 6피트의 간격을 유지하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다른 사람들과 함께 있을 때는 마스크를 착용하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 귀하(그 사람)의 상태가 나빠지고 귀하가 응급 상황이라고 생각하면, 911에 전화하거나 즉시 의료 서비스를 받으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- [자신을 돌보는 방법](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) 또는 [아픈 누군가를 돌보는 방법](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)에 대해 알아보십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- [다른 사람을 질병으로부터 보호]하는 데 도움이 될 수 있도록 절차를 따르십시오(https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="D75" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Ở nhà (giữ họ ở nhà) và chăm sóc bản thân (cho họ). Gọi cho nhà cung cấp dịch vụ y tế của quý vị (của họ) nếu tình trạng trở nên xấu hơn.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Rất tiếc quý vị (họ) không được khỏe. Các triệu chứng của quý vị (của họ) có thể liên quan đến COVID-19._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Hãy ở nhà (giữ họ ở nhà) trừ khi cần chăm sóc y tế._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - Không đến cơ quan, trường học hoặc các khu vực công cộng bao gồm cả cửa hàng tạp hóa, hiệu thuốc hoặc nhà hàng. Cân nhắc các lựa chọn giao hàng thực phẩm và thuốc._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - Không sử dụng phương tiện giao thông công cộng hoặc đi xe chung. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dùng khăn giấy để che khi ho và hắt hơi._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Thường xuyên rửa tay bằng xà phòng và nước._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tránh tiếp xúc gần với người khác. - Giữ khoảng cách với người khác ít nhất 6 feet (2 mét)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đeo khẩu trang khi ở gần người khác._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Nếu quý vị (họ) cảm thấy tình trạng trở nên xấu hơn và cho rằng đó là trường hợp khẩn cấp, hãy gọi 911 hoặc tìm kiếm sự chăm sóc y tế ngay lập tức. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Học cách [chăm sóc bản thân] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) hoặc [người khác bị bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Thực hiện các bước để giúp [bảo vệ người khác không mắc bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="E75" t="str" xml:space="preserve">
-        <v xml:space="preserve">**呆在家里（让他们呆在家里）照顾自己（他们）。 如果您（他们）病情恶化，请联系您（他们）的医疗服务提供者。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-很遗憾得知您（他们）感觉不舒服。 您（他们）的症状可能与新冠肺炎相关。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 除非要接受诊疗护理，否则请留在家中（让他们呆在家里）。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- -请勿去工作、学校或公共区域，包括杂货店、药店或餐馆。 考虑通过快递获得食物和药物。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 不要乘公共交通工具或拼车。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 咳嗽以及打喷嚏时，用纸巾捂住口鼻。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 经常用肥皂和清水洗手。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 避免与他人密切接触。 尝试与他人保持至少 6 英尺的距离。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--在他人周围时戴口罩。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--如果您（他们）感觉恶化，并且您认为这是紧急情况，请拨打 911 或立即就医。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 学习如何 [照顾自己](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) 或 [其他生病的人](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)。_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 采取措施帮助 [保护他人免于生病](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)。</v>
-      </c>
-      <c r="F75" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quédese (manténgalo) en casa y cuídese (cuídelo). Llame a su proveedor de atención médica si empeora.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Lamento que no se sienta bien. Sus síntomas podrían estar relacionados con el COVID-19._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quédese (manténgalo) en casa, excepto para conseguir atención médica._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    - No vaya al trabajo, centro educativo o lugares públicos, como tiendas de alimentos, farmacias o restaurantes. Considere opciones como entrega de comidas y medicamentos a domicilio._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    - No use el transporte público ni vehículos compartidos. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Si se siente peor y piensa que es una emergencia, llame al 911 o busque atención médica de inmediato.  _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Sepa cómo [cuidarse](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) o [cuidar a alguien que esté enfermo] (https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tome medidas para ayudar a [proteger a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-    </row>
-    <row r="76" xml:space="preserve">
+      <c r="C75" t="str">
+        <v>**의학적 치료를 받는 경우를 제외하고 집에 머무르고 자신을 돌보십시오.** 귀하의 상태가 나빠지기 시작하면 귀하의 의료진에게 전화하십시오.</v>
+      </c>
+      <c r="D75" t="str">
+        <v>**Ở nhà ngoại trừ để nhận chăm sóc y tế và chăm sóc bản thân.** Gọi cho nhà cung cấp dịch vụ y tế của quý vị nếu quý vị bắt đầu cảm thấy tồi tệ hơn.</v>
+      </c>
+      <c r="E75" t="str">
+        <v>**除了就医和照顾自己外，请留在家中。**如果您开始感觉更糟，请致电您的医疗提供者。</v>
+      </c>
+      <c r="F75" t="str">
+        <v>**Quédese en casa, excepto para conseguir atención médica, y cuídese.** Llame a su proveedor de atención médica si empeora.</v>
+      </c>
+    </row>
+    <row r="76">
       <c r="A76" t="str">
         <v>CDC/messages/msg7</v>
       </c>
       <c r="B76" t="str">
         <v>**Tell a caregiver in your facility that you are sick and need to see a medical provider as soon as possible.** Stay in your room as much as possible except to get medical care.</v>
       </c>
-      <c r="C76" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)가 거주하고 계신 보호 센터, 요양원 또는 노숙자 보호소의 의료진에게 문의하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그 사람)가 계시는 시설의 간병인에게 귀하(그 사람)가 아프고 가능한 빨리 의료진을 만나야 한다고 말하십시오. 장기 요양 시설이나 요양원에서 생활하면 중증 질병에 걸릴 위험이 높아질 수 있습니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-[다른 사람을 질병으로부터 보호](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html) 하도록 도움을 주십시오:_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	의학적 치료를 받는 경우를 제외하고 가급적 방에 머무르십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	비누와 물로 자주 손을 씻으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	다른 사람과 가까이 하지 마십시오. 다른 사람과 최소 6피트의 간격을 유지하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	다른 사람들과 함께 있을 때는 마스크를 착용하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	방 안의 자주 접촉하는 표면을 세척하고 소독하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	자신의 건강 상태를 모니터링하여, 악화된다고 생각되면 의료진에게 알리십시오.</v>
-      </c>
-      <c r="D76" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ với nhà cung cấp dịch vụ y tế tại trung tâm chăm sóc, viện dưỡng lão hoặc nơi tạm trú cho người vô gia cư nơi quý vị (họ) sống.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Nói với người chăm sóc trong cơ sở của quý vị (họ) rằng quý vị (họ) bị bệnh và cần đến gặp bác sĩ càng sớm càng tốt. Sống trong cơ sở chăm sóc dài hạn hoặc viện dưỡng lão có thể khiến quý vị (họ) có nguy cơ bị bệnh nặng cao hơn._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Giúp [bảo vệ người khác không mắc bệnh](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Ở trong phòng của mình càng nhiều càng tốt, ngoại trừ khi cần chăm sóc y tế._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Dùng khăn giấy để che khi ho và hắt hơi._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Thường xuyên rửa tay bằng xà phòng và nước._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Tránh tiếp xúc gần với người khác. - Giữ khoảng cách với người khác ít nhất 6 feet (2 mét)._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Đeo khẩu trang khi ở gần người khác._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Vệ sinh và khử trùng các bề mặt thường xuyên chạm vào trong phòng của quý vị._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	Theo dõi sức khỏe của quý vị và thông báo cho nhà cung cấp dịch vụ y tế nếu quý vị nghĩ rằng mình đang bị bệnh nặng hơn.</v>
-      </c>
-      <c r="E76" t="str" xml:space="preserve">
-        <v xml:space="preserve">**联系您（他们）居住的护理中心、疗养院或无家可归者收容所的医疗服务提供者。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-告知您（他们）机构的看护者您（他们）生病了，需要尽快就医。 生活在长期护理机构或疗养院可能会使您（他们）患严重疾病的风险更高。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-帮助 [保护他人免于生病] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	除就医外，尽可能多地待在您的房间里。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	咳嗽以及打喷嚏时，用纸巾捂住口鼻。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	经常用肥皂和清水洗手。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	 避免与他人密切接触。 尝试与他人保持至少 6 英尺的距离。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	在他人周围时戴口罩。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	 清洁和消毒您房间中频繁接触的表面。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--	监测您的健康状况，如果您认为您病情加重，请通知医疗服务人员。</v>
-      </c>
-      <c r="F76" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Póngase en contacto con el proveedor de atención médica en el establecimiento de cuidados a largo plazo donde vive.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dígale a algún cuidador del establecimiento que usted está enfermo y que necesita ver a un proveedor de atención médica lo antes posible. Vivir en un establecimiento de cuidados a largo plazo o en un hogar de ancianos puede poner a las personas en un mayor riesgo de enfermedades graves._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Ayude a [proteger a otras personas de enfermarse](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quédese en su habitación, excepto para obtener atención médica._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cúbrase la nariz y la boca con un pañuelo desechable o con la parte interna del codo cuando tosa o estornude._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Límpiese las manos con frecuencia._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Evite el contacto cercano con otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Manténgase a por lo menos 6 pies o 2 metros de las otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Use una cubierta de tela para la cara cuando esté cerca de otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Limpie y desinfecte las superficies que se tocan comúnmente en su habitación._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Monitoree su salud y notifique a un proveedor médico si piensa que está empeorando._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-</v>
-      </c>
-    </row>
-    <row r="77" xml:space="preserve">
+      <c r="C76" t="str">
+        <v>**귀하가 계시는 시설의 간병인에게 귀하가 아프고 가능한 빨리 의료진을 만나야 한다고 말하십시오.** 의학적 치료를 받는 경우를 제외하고 가급적 방에 머무르십시오.</v>
+      </c>
+      <c r="D76" t="str">
+        <v>**Cho người chăm sóc tại cơ sở của quý vị biết rằng quý vị bị bệnh và cần đến gặp nhà cung cấp dịch vụ y tế sớm nhất có thể.** Ở trong phòng càng nhiều càng tốt ngoại trừ để nhận chăm sóc y tế.</v>
+      </c>
+      <c r="E76" t="str">
+        <v>**告知您机构的看护者您生病了，需要尽快就医。**除了就医外，请尽量呆在房间里。</v>
+      </c>
+      <c r="F76" t="str">
+        <v>**Dígale a un cuidador de su establecimiento que usted está enfermo y que necesita ver a un proveedor de atención médica lo antes posible.** Quédese en su habitación lo más posible, excepto para conseguir atención médica.</v>
+      </c>
+    </row>
+    <row r="77">
       <c r="A77" t="str">
         <v>CDC/messages/msg6</v>
       </c>
       <c r="B77" t="str">
         <v>**Tell the occupational health provider (or supervisor) in your workplace that you’re feeling sick as soon as possible.**</v>
       </c>
-      <c r="C77" t="str" xml:space="preserve">
-        <v xml:space="preserve">**직장의 직장 위생 전문가에게 즉시 연락하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-직장의 산업 보건 제공자(또는 감독자)에게 가능한 한 빨리 귀하가 아프다고 말하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - **[공공 보건 당국](https://www.cdc.gov/coronavirus/2019-nCoV/hcp/index.html)의 추가 지침이 있다면 따르십시오**</v>
-      </c>
-      <c r="D77" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ ngay với nhà cung cấp dịch vụ sức khỏe nghề nghiệp tại nơi làm việc của quý vị.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Nói với nhà cung cấp dịch vụ sức khỏe nghề nghiệp (hoặc quản lý trực tiếp) ở nơi làm việc của quý vị càng sớm càng tốt rằng quý vị cảm thấy bị bệnh._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - ** Thực hiện theo bất kỳ hướng dẫn bổ sung nào từ [các viên chức y tế công cộng] (https://www.cdc.gov/coronavirus/2019-nCoV/hcp/index.html)**</v>
-      </c>
-      <c r="E77" t="str" xml:space="preserve">
-        <v xml:space="preserve">**立即联系工作场所的职业保健提供者。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-尽快告知工作场所的职业保健提供者（或主管），您感觉不适。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- -**遵循 [公共卫生官员] 的其他指南（https://www.cdc.gov/coronavirus/2019-nCoV/hcp/index.html)**</v>
-      </c>
-      <c r="F77" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Póngase en contacto con el proveedor de salud ocupacional de su lugar de trabajo de inmediato.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dígale al proveedor de salud ocupacional (o supervisor) de su lugar de trabajo que se siente mal lo más pronto posible.</v>
-      </c>
-    </row>
-    <row r="78" xml:space="preserve">
+      <c r="C77" t="str">
+        <v>**직장의 산업 보건 제공자(또는 감독자)에게 가능한 한 빨리 귀하가 아프다고 말하십시오.**</v>
+      </c>
+      <c r="D77" t="str">
+        <v>**Nói với nhà cung cấp dịch vụ sức khỏe nghề nghiệp (hoặc quản lý trực tiếp) ở nơi làm việc của quý vị càng sớm càng tốt rằng quý vị cảm thấy bị bệnh.**</v>
+      </c>
+      <c r="E77" t="str">
+        <v>**尽快告知工作场所的职业保健提供者（或主管），您感觉不适。**</v>
+      </c>
+      <c r="F77" t="str">
+        <v>**Dígale al proveedor de salud ocupacional (o supervisor) de su lugar de trabajo que se siente mal lo más pronto posible.**</v>
+      </c>
+    </row>
+    <row r="78">
       <c r="A78" t="str">
         <v>CDC/messages/msg5</v>
       </c>
       <c r="B78" t="str">
         <v>**Call your medical provider, clinician advice line, or telemedicine provider as soon as possible.** You also have medical conditions that may put you at risk of becoming more seriously ill.</v>
       </c>
-      <c r="C78" t="str" xml:space="preserve">
-        <v xml:space="preserve">**의료진에게 전화하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그 사람)가 몸 상태가 좋지 않다고 하시니 염려됩니다. 귀하(그 사람)의 증상이 COVID-19와 관련 있을 수 있습니다. 또한 귀하(그 사람)에게는 중대한 질병으로 악화될 수 있는 질환도 있습니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 귀하(그 사람)의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 귀하(그 사람)의 상태가 나빠지고 귀하(그 사람)가 응급 상황이라고 생각하면, 911에 전화하거나 즉시 의료 서비스를 받으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의학적 치료를 받는 경우를 제외하고 집에 머무르십시오(그 사람이 집에 머무르도록 하십시오)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 직장, 학교 또는 식료품점, 약국 또는 식당을 포함한 공공 장소에 가지 마십시오. 음식과 약에 대해 배달 옵션을 고려하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 대중 교통수단을 이용하거나 승차 공유를 하지 마십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 가능한 경우 [원격 의료 서비스](https://telehealth.hhs.gov/)를 사용해보십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- [자신을 돌보는 방법](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) 또는 [아픈 누군가를 돌보는 방법](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)에 대해 알아보십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- [다른 사람을 질병으로부터 보호]하는 데 도움이 될 수 있도록 이 절차를 따르십시오(https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="D78" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Gọi cho một nhà cung cấp dịch vụ y tế.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Rất tiếc quý vị (họ) không được khỏe. Các triệu chứng của quý vị (của họ) có thể liên quan đến COVID-19. Quý vị (họ) cũng mắc các bệnh có thể khiến quý vị (họ) có nguy cơ bị bệnh nặng hơn._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Gọi cho nhà cung cấp dịch vụ y tế của quý vị (của họ), đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Nếu quý vị (họ) cảm thấy tình trạng trở nên xấu hơn và cho rằng đó là trường hợp khẩn cấp, hãy gọi 911 hoặc tìm kiếm sự chăm sóc y tế ngay lập tức._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Hãy ở nhà (giữ họ ở nhà) trừ khi cần chăm sóc y tế._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - Không đến cơ quan, trường học hoặc các khu vực công cộng bao gồm cả cửa hàng tạp hóa, hiệu thuốc hoặc nhà hàng. Cân nhắc các lựa chọn giao hàng thực phẩm và thuốc._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - Không sử dụng phương tiện giao thông công cộng hoặc đi xe chung._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cân nhắc sử dụng [dịch vụ chăm sóc sức khỏe từ xa nếu có] (https://telehealth.hhs.gov/)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Học cách [chăm sóc bản thân] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) hoặc [người khác bị bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Thực hiện các bước sau để giúp [bảo vệ người khác không mắc bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-      <c r="E78" t="str" xml:space="preserve">
-        <v xml:space="preserve">**致电医疗服务提供者。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-很遗憾得知您（他们）感觉不舒服。 您（他们）的症状可能与新冠肺炎相关。 您（他们）还患有可能使您（他们）面临病情严重风险的疾病。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 在 24 小时内致电您的医疗服务提供者、临床医生建议热线或远程医疗服务提供者。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--如果您（他们）感觉恶化，并且您（他们）认为这是紧急情况，请拨打 911 或立即就医。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 除非要接受诊疗护理，否则请留在家中（让他们呆在家里）。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- -请勿去工作、学校或公共区域，包括杂货店、药店或餐馆。 考虑通过快递获得食物和药物。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- - 不要乘公共交通工具或拼车。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--考虑使用 [远程医疗服务，如可用]（https://telehealth.hhs.gov/)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 学习如何 [照顾自己] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) 或 [其他生病的人] (https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 采取这些步骤来帮助 [保护他人免于生病](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)。</v>
-      </c>
-      <c r="F78" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Llame a un proveedor de atención médica.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Lamento que no se sienta bien. Sus síntomas podrían estar relacionados con el COVID-19. También tiene afecciones que podrían ponerlo en riesgo de enfermarse gravemente._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Llame a su proveedor de atención médica, a una línea de asesoría clínica o a un proveedor de telemedicina._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quédese (manténgalo) en casa, excepto para conseguir atención médica._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- No vaya al trabajo, centro educativo o lugares públicos, como tiendas de alimentos, farmacias o restaurantes. Considere opciones como entrega de comidas y medicamentos a domicilio._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- No use transporte público ni vehículos compartidos._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Si se siente peor y piensa que es una emergencia, llame al 911 o busque atención médica de inmediato._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Considere usar [servicios de telesalud, si están disponibles](https://telehealth.hhs.gov/)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Sepa cómo [cuidarse](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html) o [cuidar a alguien que esté enfermo] (https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tome estas medidas para ayudar a [proteger a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html).</v>
-      </c>
-    </row>
-    <row r="79" xml:space="preserve">
+      <c r="C78" t="str">
+        <v>**가능한 한 빨리 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오.** 또한 귀하에게는 중대한 질병으로 악화될 수 있는 질환도 있습니다.</v>
+      </c>
+      <c r="D78" t="str">
+        <v>**Gọi cho nhà cung cấp dịch vụ y tế, đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa càng sớm càng tốt.** Quý vị cũng mắc các bệnh lý có thể khiến quý vị có nguy cơ bị bệnh nặng hơn.</v>
+      </c>
+      <c r="E78" t="str">
+        <v>**尽快致电您的医疗服务提供者、临床医生咨询热线或远程医疗服务提供者**。您的身体状况也可能会让您面临更严重的疾病风险。</v>
+      </c>
+      <c r="F78" t="str">
+        <v>** Llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina lo más pronto posible.** También tiene afecciones que podrían ponerlo en un mayor riesgo de enfermarse gravemente.</v>
+      </c>
+    </row>
+    <row r="79">
       <c r="A79" t="str">
         <v>CDC/messages/msg4</v>
       </c>
       <c r="B79" t="str">
         <v>**Based on your symptoms, you may need urgent medical care.** Please call 911 or go to the nearest emergency department.</v>
       </c>
-      <c r="C79" t="str" xml:space="preserve">
-        <v xml:space="preserve">**긴급한 치료가 필요할 수 있습니다. 911에 전화하거나 응급실로 가십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-귀하(그들)의 증상에 따라 긴급한 치료가 필요할 수 있습니다. 911에 전화하거나 가까운 응급실로 가십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-COVID-19에 걸린 사람과 접촉한 적이 있는 경우 911 교환원 또는 응급 직원에게 알리십시오.</v>
-      </c>
-      <c r="D79" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Có thể cần chăm sóc y tế khẩn cấp. Vui lòng gọi 911 hoặc đến Khoa Cấp cứu.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dựa trên các triệu chứng của quý vị (của họ), quý vị có thể cần được chăm sóc y tế khẩn cấp. Vui lòng gọi 911 hoặc đến khoa cấp cứu gần nhất._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Hãy cho tổng đài 911 hoặc nhân viên cấp cứu biết nếu quý vị đã tiếp xúc với người mắc COVID-19.</v>
-      </c>
-      <c r="E79" t="str" xml:space="preserve">
-        <v xml:space="preserve">**可能需要紧急医疗护理。 请拨打 911 或到急诊科就诊。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-根据您（他们）的症状，您可能需要紧急医疗护理。 请拨打 911 或到最近的急诊科就诊。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-如果您曾与新冠肺炎患者接触，请告知 911 接线员或急救人员。</v>
-      </c>
-      <c r="F79" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Es posible que necesite atención médica de urgencia. Llame al 911 o diríjase a la sala de emergencias.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Según sus síntomas, es posible que necesite atención médica de urgencia. Llame al 911 o vaya a la sala de emergencias más cercana._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dígale al operador del 911 o personal de emergencia si estuvo en contacto con alguna persona con COVID-19.</v>
+      <c r="C79" t="str">
+        <v>**증상에 따라 긴급한 치료가 필요할 수 있습니다.** 911에 전화하거나 응급실로 가십시오.</v>
+      </c>
+      <c r="D79" t="str">
+        <v>**Dựa trên các triệu chứng của quý vị, quý vị có thể cần được chăm sóc y tế khẩn cấp. **Vui lòng gọi 911 hoặc đến phòng cấp cứu gần nhất.</v>
+      </c>
+      <c r="E79" t="str">
+        <v>**根据您的症状，您可能需要紧急医疗护理**，请拨打911或去最近的急诊科。</v>
+      </c>
+      <c r="F79" t="str">
+        <v>**Según sus síntomas, es posible que necesite atención médica de urgencia.** Llame al 911 o vaya a la sala de emergencias más cercana.</v>
       </c>
     </row>
     <row r="80" xml:space="preserve">
@@ -2925,28 +2372,28 @@
         <v>CDC/messages/msg3</v>
       </c>
       <c r="B80" t="str" xml:space="preserve">
-        <v xml:space="preserve">**This Coronavirus Self-Checker is for people who are at least 18 years old.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**This Coronavirus Self-Checker is for people who are at least 18 years old.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Visit the [CDC website](https://www.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html) to get information on COVID-19 and younger people.</v>
       </c>
       <c r="C80" t="str" xml:space="preserve">
-        <v xml:space="preserve">**이 Coronavirus Self-Checker는 18세 이상인 사람들을 위한 것입니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**이 Coronavirus Self-Checker는 18세 이상인 사람들을 위한 것입니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 [CDC 웹사이트](https://www.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html)에 방문하여 COVID-19와 청소년에 대한 더 자세한 정보를 확인하십시오.</v>
       </c>
       <c r="D80" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Công cụ tự kiểm tra virus corona này dành cho người từ 18 tuổi trở lên.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Công cụ tự kiểm tra virus corona này dành cho người từ 18 tuổi trở lên.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Truy cập [trang web của CDC] (https://www.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html) để nhận thông tin về COVID-19 và những người trẻ.</v>
       </c>
       <c r="E80" t="str" xml:space="preserve">
-        <v xml:space="preserve">**这种冠状病毒自我检查问卷是针对至少 18 岁的人。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**这种冠状病毒自我检查问卷是针对至少 18 岁的人。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 访问 [CDC 网站]（https://www.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html）以获取新冠肺炎和年轻人群情况的信息。</v>
       </c>
       <c r="F80" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Este Autoverificador del Coronavirus es para personas que tengan como mínimo 18 años de edad.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Este Autoverificador del Coronavirus es para personas que tengan como mínimo 18 años de edad.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Visite el [sitio web de los CDC](https://espanol.cdc.gov/coronavirus/2019-ncov/daily-life-coping/children.html) para obtener información sobre el COVID-19 y las personas más jóvenes.</v>
       </c>
     </row>
@@ -2955,95 +2402,79 @@
         <v>CDC/messages/msg2</v>
       </c>
       <c r="B81" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Call 911 - You may be having a medical emergency.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Call 911 now. Immediate medical attention is needed. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Call 911 - You may be having a medical emergency.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Call 911 now. Immediate medical attention is needed. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Tell the 911 operator if you have been in contact with someone with COVID-19 or if you have recently been to an area where COVID-19 is spreading.</v>
       </c>
       <c r="C81" t="str" xml:space="preserve">
-        <v xml:space="preserve">**911에 전화하십시오 - 의학적 응급 상황일 수 있습니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**911에 전화하십시오 - 의학적 응급 상황일 수 있습니다.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+지금 911로 전화하십시오. 즉각적인 치료가 필요합니다. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+COVID-19에 걸린 사람과 접촉했거나 최근에 COVID-19가 퍼져 있는 지역을 방문한 경우 911 오퍼레이터에게 알리십시오.</v>
+      </c>
+      <c r="D81" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Gọi 911 - Quý vị có thể đang gặp trường hợp khẩn cấp về y tế. **_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Gọi 911 ngay. Cần chăm sóc y tế ngay. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Hãy cho tổng đài 911 biết nếu quý vị đã tiếp xúc với người mắc COVID-19 hoặc nếu gần đây quý vị đã đến một khu vực mà dịch COVID-19 đang lan rộng.</v>
+      </c>
+      <c r="E81" t="str" xml:space="preserve">
+        <v xml:space="preserve">**拨打 911 - 您可能出现医疗紧急情况。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+现在拨打 911。 需要立即就医。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+如果您与新冠肺炎患者接触或如果您最近去过新冠肺炎传播的地区，请告知 911 接线员。</v>
+      </c>
+      <c r="F81" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Llame al 911. Podría tratarse de una emergencia médica.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-지금 911로 전화하십시오. 즉각적인 치료가 필요합니다. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Llame al 911 ahora mismo. Se recomienda atención médica inmediata. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-COVID-19에 걸린 사람과 접촉했거나 최근에 COVID-19가 퍼져 있는 지역을 방문한 경우 911 오퍼레이터에게 알리십시오.</v>
-      </c>
-      <c r="D81" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Gọi 911 - Quý vị có thể đang gặp trường hợp khẩn cấp về y tế. **_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Gọi 911 ngay. Cần chăm sóc y tế ngay. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Hãy cho tổng đài 911 biết nếu quý vị đã tiếp xúc với người mắc COVID-19 hoặc nếu gần đây quý vị đã đến một khu vực mà dịch COVID-19 đang lan rộng.</v>
-      </c>
-      <c r="E81" t="str" xml:space="preserve">
-        <v xml:space="preserve">**拨打 911 - 您可能出现医疗紧急情况。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-现在拨打 911。 需要立即就医。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-如果您与新冠肺炎患者接触或如果您最近去过新冠肺炎传播的地区，请告知 911 接线员。</v>
-      </c>
-      <c r="F81" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Llame al 911. Podría tratarse de una emergencia médica.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Llame al 911 ahora mismo. Se recomienda atención médica inmediata. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Dígale al operador del 911 si estuvo en contacto con alguna persona con COVID-19 o si recientemente estuvo en un área en la que se está propagando el COVID-19.</v>
       </c>
     </row>
-    <row r="82" xml:space="preserve">
+    <row r="82">
       <c r="A82" t="str">
         <v>CDC/messages/msg1</v>
       </c>
       <c r="B82" t="str">
         <v>**Sounds like you are feeling ok.**</v>
       </c>
-      <c r="C82" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)가 괜찮으신 것 같네요.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-COVID-19에 대해 자세히 알아보고 [CDC 웹사이트](https://www.cdc.gov/coronavirus/2019-ncov/index.html)에서 귀하(그 사람)의 안전을 위해 무엇을 할 수 있는지 알아보세요.</v>
-      </c>
-      <c r="D82" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Có vẻ như quý vị (họ) đang cảm thấy ổn.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Tìm hiểu thêm về COVID-19 và những gì quý vị (họ) có thể làm để giữ an toàn trên [trang web của CDC] (https://www.cdc.gov/coronavirus/2019-ncov/index.html).</v>
-      </c>
-      <c r="E82" t="str" xml:space="preserve">
-        <v xml:space="preserve">**听起来您（他们）感觉很好。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-了解更多关于新冠肺炎的信息，以及您（他们）可以在 [CDC网站] 上做些什么来确保安全（https://www.cdc.gov/coronavirus/2019-ncov/index.html).</v>
-      </c>
-      <c r="F82" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Parece que se siente bien.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Obtenga más información sobre el COVID-19 y lo que puede hacer para mantenerse (mantenerlo) seguro en el [sitio web de los CDC](https://espanol.cdc.gov/enes/coronavirus/2019-ncov/index.html).</v>
-      </c>
-    </row>
-    <row r="83" xml:space="preserve">
+      <c r="C82" t="str">
+        <v>**괜찮으신 것 같네요.**</v>
+      </c>
+      <c r="D82" t="str">
+        <v>**Có vẻ như quý vị đang cảm thấy ổn.**</v>
+      </c>
+      <c r="E82" t="str">
+        <v>**听起来您感觉还可以。**</v>
+      </c>
+      <c r="F82" t="str">
+        <v>**Parece que se siente bien.**</v>
+      </c>
+    </row>
+    <row r="83">
       <c r="A83" t="str">
         <v>CDC/messages/msg0</v>
       </c>
       <c r="B83" t="str">
         <v>**You have not made a selection. Please start again and select options for each question so that I can help give you advice.**</v>
       </c>
-      <c r="C83" t="str" xml:space="preserve">
-        <v xml:space="preserve">**제가 치료 조언을 제공할 수 있도록 옵션을 선택하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-선택하지 않으셨습니다. 다시 시작하고 제가 조언을 드릴 수 있도록 각 질문에 대한 옵션을 선택하십시오.</v>
-      </c>
-      <c r="D83" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Vui lòng lựa chọn để tôi có thể giúp đưa ra lời khuyên chăm sóc cho quý vị.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Quý vị chưa thực hiện lựa chọn. Vui lòng bắt đầu lại và chọn các tùy chọn cho từng câu hỏi để tôi có thể giúp đưa ra lời khuyên cho quý vị.</v>
-      </c>
-      <c r="E83" t="str" xml:space="preserve">
-        <v xml:space="preserve">**请做出选择，以便我可以帮助您提供护理建议。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-您尚未进行选择。 请重新开始，并为每个问题选择选项，以便我可以帮助您提供建议。</v>
-      </c>
-      <c r="F83" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Seleccione una opción para que pueda aconsejarlo sobre la atención médica.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-No ha seleccionado ninguna opción. Vuelva a comenzar y seleccione opciones para cada pregunta; así podré aconsejarlo sobre la atención médica.</v>
+      <c r="C83" t="str">
+        <v>**선택하지 않으셨습니다. 다시 시작하고 제가 조언을 드릴 수 있도록 각 질문에 대한 옵션을 선택하십시오.**</v>
+      </c>
+      <c r="D83" t="str">
+        <v>**Quý vị chưa thực hiện lựa chọn. Vui lòng bắt đầu lại và chọn các tùy chọn cho từng câu hỏi để tôi có thể giúp đưa ra lời khuyên cho quý vị.**</v>
+      </c>
+      <c r="E83" t="str">
+        <v>**您尚未进行选择。请重新开始，并为每个问题选择选项，以便我可以帮助您提供建议。**</v>
+      </c>
+      <c r="F83" t="str">
+        <v>**No ha seleccionado ninguna opción. Vuelva a comenzar y seleccione opciones para cada pregunta, para que pueda aconsejarlo.</v>
       </c>
     </row>
     <row r="84">
@@ -3077,7 +2508,7 @@
         <v>평가 중 다시 시작해야 하는 경우 페이지를 새로 고치면 됩니다.</v>
       </c>
       <c r="D85" t="str" xml:space="preserve">
-        <v xml:space="preserve">Trong quá trình đánh giá, quý vị có thể làm mới trang nếu quý vị cần bắt đầu lại_x000d_._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Trong quá trình đánh giá, quý vị có thể làm mới trang nếu quý vị cần bắt đầu lại_x000d_._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 </v>
       </c>
       <c r="E85" t="str">
@@ -3092,42 +2523,69 @@
         <v>CDC/messages/intro_msg</v>
       </c>
       <c r="B86" t="str" xml:space="preserve">
-        <v xml:space="preserve">Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the level of medical care you should seek. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again.
-If you are experiencing a life-threatening emergency, please call 911 immediately. 
-If you are not experiencing a life-threatening emergency, let’s get started.
-## **CDC recommends these steps to reduce your risk of getting and spreading COVID-19:**
-- **Wear** a mask over your nose and mouth.
-- **Stay** at least 6 feet away from people who don’t live with you.
-- **Avoid** crowded areas and poorly ventilated spaces.
+        <v xml:space="preserve">Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the level of medical care you should seek. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again._x000d__x000d_
+_x000d__x000d_
+If you are experiencing a life-threatening emergency, please call 911 immediately. _x000d__x000d_
+  _x000d__x000d_
+If you are not experiencing a life-threatening emergency, let’s get started._x000d__x000d_
+_x000d__x000d_
+## **CDC recommends these steps to reduce your risk of getting and spreading COVID-19:**_x000d__x000d_
+- **Wear** a mask over your nose and mouth._x000d__x000d_
+- **Stay** at least 6 feet away from people who don’t live with you._x000d__x000d_
+- **Avoid** crowded areas and poorly ventilated spaces._x000d__x000d_
 - **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol.</v>
       </c>
       <c r="C86" t="str" xml:space="preserve">
-        <v xml:space="preserve">안녕하세요? 저는 Clara입니다. 몇 가지 질문을 하겠습니다. 귀하의 답변을 통해 귀하에게 어느 정도 수준의 진료가 필요한지 조언할 것입니다. _x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-그러나 먼저 생명을 위협하는 응급 상황이 발생하면 즉시 911에 전화하십시오. _x000d__x000d__x000d__x000d__x000d_ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-생명을 위협하는 응급 상황을 겪고 있지 않다면, 이제 시작하겠습니다.</v>
+        <v xml:space="preserve">안녕하세요? 저는 Clara입니다. 몇 가지 질문을 하겠습니다. 귀하의 답변을 통해 귀하에게 어느 정도 수준의 진료가 필요한지 조언할 것입니다. 다른 사람을 위해 응답하고 계시다면 본인이 그 사람인 것처럼 모든 질문에 답하십시오. 처음부터 다시 시작해야 한다면 페이지를 새로 고치고 다시 시작하십시오._x000d__x000d_
+_x000d__x000d_
+생명을 위협하는 응급 상황이 발생하면 즉시 911에 전화하십시오._x000d__x000d_
+  _x000d__x000d_
+생명을 위협하는 응급 상황을 겪고 있지 않다면, 이제 시작하겠습니다._x000d__x000d_
+_x000d__x000d_
+## **귀하가 COVID-19에 걸리고 퍼뜨릴 위험을 줄이기 위해 CDC는 다음과 같은 방법을 권장합니다.**_x000d__x000d_
+- 코와 입을 가리는 마스크를 **착용하십시오**._x000d__x000d_
+- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**._x000d__x000d_
+- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**._x000d__x000d_
+- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오.</v>
       </c>
       <c r="D86" t="str" xml:space="preserve">
-        <v xml:space="preserve">Xin chào, tôi là Clara. Tôi sẽ hỏi quý vị một số câu hỏi. Tôi sẽ sử dụng câu trả lời của quý vị để cung cấp cho quý vị lời khuyên về mức độ chăm sóc y tế mà quý vị nên tìm kiếm. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Nhưng trước tiên, nếu quý vị đang gặp trường hợp khẩn cấp đe dọa tính mạng, vui lòng gọi 911 ngay lập tức. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Nếu quý vị không đang trong tình trạng khẩn cấp đe dọa tính mạng, hãy bắt đầu.</v>
+        <v xml:space="preserve">Xin chào, tôi là Clara. Tôi sẽ hỏi quý vị một số câu hỏi. Tôi sẽ sử dụng câu trả lời của quý vị để cung cấp cho quý vị lời khuyên về mức độ chăm sóc y tế mà quý vị nên tìm kiếm.   Nếu trả lời cho người khác, vui lòng trả lời tất cả các câu hỏi như thể quý vị là họ. Nếu quý vị cần bắt đầu lại, hãy làm mới trang và bắt đầu lại._x000d__x000d_
+_x000d__x000d_
+Nếu quý vị đang gặp trường hợp khẩn cấp đe dọa tính mạng, vui lòng gọi 911 ngay lập tức.   _x000d__x000d_
+  _x000d__x000d_
+Nếu quý vị không đang trong tình trạng khẩn cấp đe dọa tính mạng, hãy bắt đầu._x000d__x000d_
+_x000d__x000d_
+## **CDC đề xuất các bước sau để giảm nguy cơ nhiễm và lây lan COVID-19:**_x000d__x000d_
+- **Đeo** khẩu trang lên mũi và miệng của quý vị._x000d__x000d_
+- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet._x000d__x000d_
+- **Tránh** những khu vực đông đúc và không gian kém thông thoáng._x000d__x000d_
+- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước khử trùng tay có ít nhất 60% cồn.</v>
       </c>
       <c r="E86" t="str" xml:space="preserve">
-        <v xml:space="preserve">嗨，我是 Clara。 我要问您一些问题。 我将使用您的回答为您提供关于您应寻求的医疗护理水平的建议。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-但首先，如果您出现危及生命的紧急情况，请立即拨打 911。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-如果您没有出现危及生命的紧急情况，我们开始吧。</v>
+        <v xml:space="preserve">嗨，我是 Clara。我要问您一些问题。我将使用您的回答为您提供关于您应寻求的医疗护理水平的建议。如果替别人回答，请把所有的问题都当作自己的问题来回答。如果您需要重新开始，请刷新页面并重新开始。_x000d__x000d_
+_x000d__x000d_
+如果您出现危及生命的紧急情况，请立即拨打 911。_x000d__x000d_
+  _x000d__x000d_
+如果您没有出现危及生命的紧急情况，我们开始吧。_x000d__x000d_
+_x000d__x000d_
+## **疾控中心建议采取这些步骤，以减少感染和传播COVID-19的风险：**_x000d__x000d_
+- **佩戴**口罩遮住您的口鼻。_x000d__x000d_
+- 与不和您住在一起的人**保持**至少6英尺的距离。_x000d__x000d_
+- **避免**拥挤的地方和通风不良的空间。_x000d__x000d_
+- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。</v>
       </c>
       <c r="F86" t="str" xml:space="preserve">
-        <v xml:space="preserve">Hola, me llamo Clara. Le voy a hacer algunas preguntas. Usaré sus respuestas para aconsejarle sobre el nivel de atención médica que debe buscar. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Pero primero, si tiene una emergencia potencialmente mortal, llame al 911 de inmediato. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Si no tiene una emergencia potencialmente mortal, comencemos.</v>
+        <v xml:space="preserve">Hola, me llamo Clara. Le voy a hacer algunas preguntas. Usaré sus respuestas para aconsejarle sobre el nivel de atención médica que debe buscar. Si está respondiendo por alguien más, responda todas las preguntas como si fuera esa persona. Si necesita comenzar de nuevo, refresque la página y comience otra vez._x000d__x000d_
+_x000d__x000d_
+Si tiene una emergencia potencialmente mortal, llame al 911 inmediatamente. _x000d__x000d_
+  _x000d__x000d_
+Si no tiene una emergencia potencialmente mortal, comencemos._x000d__x000d_
+_x000d__x000d_
+## **Los CDC recomiendan que tome estas medidas para reducir el riesgo de contraer o propagar el COVID-19:**_x000d__x000d_
+- **Póngase** una mascarilla que le cubra la nariz y la boca._x000d__x000d_
+- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted._x000d__x000d_
+- **Evite** lugares con mucha gente y áreas con poca ventilación._x000d__x000d_
+- **Lávese** las manos a menudo con agua y jabón o use un desinfectante de manos que contenga al menos un 60 % de alcohol.</v>
       </c>
     </row>
     <row r="87">
@@ -3155,37 +2613,39 @@
         <v>CDC/messages/disclaimer_msg</v>
       </c>
       <c r="B88" t="str" xml:space="preserve">
-        <v xml:space="preserve">The purpose of the Coronavirus Self-Checker is to help you make decisions about seeking appropriate medical care. This system is not intended for the diagnosis or treatment of disease, including COVID-19. 
-This project was made possible through a partnership with the CDC Foundation and is enabled by Microsoft’s Azure platform. CDC’s collaboration with a non-federal organization does not imply an endorsement of any one particular service, product, or enterprise. 
+        <v xml:space="preserve">The purpose of the Coronavirus Self-Checker is to help you make decisions about seeking appropriate medical care. This system is not intended for the diagnosis or treatment of disease, including COVID-19. _x000d__x000d_
+_x000d__x000d_
+This project was made possible through a partnership with the CDC Foundation and is enabled by Microsoft’s Azure platform. CDC’s collaboration with a non-federal organization does not imply an endorsement of any one particular service, product, or enterprise. _x000d__x000d_
+_x000d__x000d_
 ###### ver66.2 (02.23.2021)</v>
       </c>
       <c r="C88" t="str" xml:space="preserve">
-        <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 것에 대한 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-이 프로젝트는 CDC Foundation과의 파트너십을 통해 가능했으며 Microsoft의 Azure 플랫폼에서 가능합니다. CDC가 비연방 조직과 협력한다고 해서 특정 서비스, 제품 또는 기업을 보증한다는 의미는 아닙니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-버전65.1(2020-12-23)</v>
+        <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 것에 대한 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다._x000d__x000d_
+_x000d__x000d_
+이 프로젝트는 CDC Foundation과의 파트너십을 통해 가능했으며 Microsoft의 Azure 플랫폼에서 가능합니다. CDC가 비연방 조직과 협력한다고 해서 특정 서비스, 제품 또는 기업을 보증한다는 의미는 아닙니다._x000d__x000d_
+_x000d__x000d_
+###### ver66.2 (2021년 02월 23일)</v>
       </c>
       <c r="D88" t="str" xml:space="preserve">
-        <v xml:space="preserve">Mục đích của việc Hệ thống Câu hỏi Tự Kiểm tra Mắc Virus Corona là để giúp quý vị đưa ra quyết định về việc tìm kiếm dịch vụ chăm sóc y tế thích hợp. Hệ thống này không dùng để chẩn đoán hoặc điều trị bệnh, kể cả COVID-19. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Dự án này được thực hiện thông qua sự hợp tác với CDC Foundation và được hỗ trợ bởi nền tảng Azure của Microsoft. Sự hợp tác của CDC với một tổ chức không thuộc liên bang không ngụ ý xác nhận bất kỳ dịch vụ, sản phẩm hoặc doanh nghiệp cụ thể nào. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-ᵥₑᵣ₆₅.₁ ₍₂₀₂₀₋₁₂₋₂₃₎</v>
+        <v xml:space="preserve">Mục đích của việc Hệ thống Câu hỏi Tự Kiểm tra Mắc Virus Corona là để giúp quý vị đưa ra quyết định về việc tìm kiếm dịch vụ chăm sóc y tế thích hợp. Hệ thống này không dùng để chẩn đoán hoặc điều trị bệnh, kể cả COVID-19. _x000d__x000d_
+_x000d__x000d_
+Dự án này được thực hiện thông qua sự hợp tác với CDC Foundation và được hỗ trợ bởi nền tảng Azure của Microsoft. Sự hợp tác của CDC với một tổ chức không thuộc liên bang không ngụ ý xác nhận bất kỳ dịch vụ, sản phẩm hoặc doanh nghiệp cụ thể nào. _x000d__x000d_
+_x000d__x000d_
+###### ver66.2 (02.23.2021)</v>
       </c>
       <c r="E88" t="str" xml:space="preserve">
-        <v xml:space="preserve">冠状病毒自我检查问卷的目的是帮助您做出寻求适当医疗护理的决策。 该系统不适用于疾病的诊断或治疗，包括新冠肺炎。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-这个项目是通过与 CDC 基金会的合作而实现，并由 Microsoft 的 Azure 平台启用。 CDC 与非联邦组织的合作并不意味着对任何特定服务、产品或企业的认可。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-版本 65.1（2020 年 12 月 23 日)</v>
+        <v xml:space="preserve">冠状病毒自我检查问卷的目的是帮助您做出寻求适当医疗护理的决策。该系统不适用于疾病的诊断或治疗，包括新冠肺炎。_x000d__x000d_
+_x000d__x000d_
+这个项目是通过与 CDC 基金会的合作而实现，并由 Microsoft 的 Azure 平台启用。CDC 与非联邦组织的合作并不意味着对任何特定服务、产品或企业的认可。_x000d__x000d_
+_x000d__x000d_
+###### ver66.2 (02.23.2021)</v>
       </c>
       <c r="F88" t="str" xml:space="preserve">
-        <v xml:space="preserve">La finalidad del Autoverificador del Coronavirus es ayudarlo a tomar decisiones sobre la obtención de atención médica adecuada. Este sistema no se ha diseñado para fines de diagnóstico o tratamiento de enfermedades u otras afecciones, incluido el COVID-19. Este proyecto ha sido posible mediante la colaboración con la Fundación de los CDC y se ha habilitado a través de la plataforma Azure de Microsoft. La colaboración de los CDC con una organización no federal no implica el respaldo a ningún servicio, producto o empresa específicos._x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-ᵥₑᵣ₆₅.₁ ₍₂₀₂₀₋₁₂₋₂₃₎</v>
+        <v xml:space="preserve">La finalidad del Autoverificador del Coronavirus es ayudarlo a tomar decisiones sobre la obtención de atención médica adecuada. Este sistema no se ha diseñado para fines de diagnóstico o tratamiento de enfermedades, incluido el COVID-19. _x000d_
+_x000d_
+Este proyecto ha sido posible mediante la colaboración con la Fundación de los CDC y se ha habilitado a través de la plataforma Azure de Microsoft. La colaboración de los CDC con una organización no federal no implica el respaldo a ningún servicio, producto o empresa específicos. _x000d_
+_x000d_
+###### ver66.2 (02.23.2021)</v>
       </c>
     </row>
     <row r="89" xml:space="preserve">
@@ -3193,52 +2653,53 @@
         <v>CDC/third_person_questions/exposure_question</v>
       </c>
       <c r="B89" t="str" xml:space="preserve">
-        <v xml:space="preserve">In the two weeks before they felt sick, have they been in close contact with someone who has COVID-19? —excluding people who have had COVID-19 within the past 3 months. 
-They have been in close contact if they have\n
-a.	been within 6 feet of someone who has COVID-19 for a combined total of 15 minutes or more over a 24 hour period **or** \n
-b.	provided care at home to someone who is sick with COVID-19 **or** \n
-c.	had direct physical contact (hugged or kissed) with someone who has COVID-19 **or** \n
-d.	shared eating or drinking utensils with someone who has COVID-19 **or** \n
+        <v xml:space="preserve">In the two weeks before they felt sick, have they been in close contact with someone who has COVID-19? —excluding people who have had COVID-19 within the past 3 months. _x000d__x000d_
+_x000d__x000d_
+They have been in close contact if they have\n_x000d__x000d_
+a.	been within 6 feet of someone who has COVID-19 for a combined total of 15 minutes or more over a 24 hour period **or** \n_x000d__x000d_
+b.	provided care at home to someone who is sick with COVID-19 **or** \n_x000d__x000d_
+c.	had direct physical contact (hugged or kissed) with someone who has COVID-19 **or** \n_x000d__x000d_
+d.	shared eating or drinking utensils with someone who has COVID-19 **or** \n_x000d__x000d_
 e.	been sneezed on or coughed on by someone who has COVID-19 \n</v>
       </c>
       <c r="C89" t="str" xml:space="preserve">
-        <v xml:space="preserve">아프기 전 2주 동안 COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까? —이전 3개월 이내에 COVID-19에 걸린 사람 제외._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-다음에 해당하는 경우 귀하는 밀접 접촉한 것입니다\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-a.	24시간 내에 총 15분 이상 COVID-19를 앓고 있는 사람과 6피트 이내에 있었습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-b.	COVID-19에 걸린 사람에게 집에서 치료를 제공했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-c.	COVID-19에 걸린 사람과 직접적인 신체적 접촉(포옹 또는 키스)을 했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-d.	COVID-19에 걸린 사람과 먹거나 마실 때 도구를 공유했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">아프기 전 2주 동안 COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까? —이전 3개월 이내에 COVID-19에 걸린 사람 제외._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+다음에 해당하는 경우 귀하는 밀접 접촉한 것입니다\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	24시간 내에 총 15분 이상 COVID-19를 앓고 있는 사람과 6피트 이내에 있었습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	COVID-19에 걸린 사람에게 집에서 치료를 제공했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	COVID-19에 걸린 사람과 직접적인 신체적 접촉(포옹 또는 키스)을 했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	COVID-19에 걸린 사람과 먹거나 마실 때 도구를 공유했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	COVID-19에 걸린 사람이 귀하에게 재채기나 기침을 했습니다 \n</v>
       </c>
       <c r="D89" t="str" xml:space="preserve">
-        <v xml:space="preserve">Trong hai tuần trước khi cảm thấy bị bệnh, quý vị có tiếp xúc gần với người bị nhiễm COVID-19 không? —Ngoại trừ những người đã mắc COVID-19 trong vòng 3 tháng qua. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Quý vị đã tiếp xúc gần nếu đã\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-a.	cách người mắc COVID-19 trong vòng 6 feet (2 mét) trong tổng cộng 15 phút trở lên trong khoảng thời gian 24 giờ **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-b.	cung cấp dịch vụ chăm sóc tại nhà cho người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-c.	tiếp xúc trực tiếp (ôm hoặc hôn) người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-d.	dùng chung dụng cụ ăn uống với người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Trong hai tuần trước khi cảm thấy bị bệnh, quý vị có tiếp xúc gần với người bị nhiễm COVID-19 không? —Ngoại trừ những người đã mắc COVID-19 trong vòng 3 tháng qua. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Quý vị đã tiếp xúc gần nếu đã\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	cách người mắc COVID-19 trong vòng 6 feet (2 mét) trong tổng cộng 15 phút trở lên trong khoảng thời gian 24 giờ **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	cung cấp dịch vụ chăm sóc tại nhà cho người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	tiếp xúc trực tiếp (ôm hoặc hôn) người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	dùng chung dụng cụ ăn uống với người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	bị một người mắc COVID-19 hắt hơi hoặc ho vào người\n</v>
       </c>
       <c r="E89" t="str" xml:space="preserve">
-        <v xml:space="preserve">在您 (他们) 感觉生病前的两周内，您 (他们) 是否与患有新冠肺炎的人密切接触？——不包括在过去 3 个月内确诊新冠肺炎的人。 _x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-如果您 (他们) 有以下情况，请与我们保持密切联系_x000d__x000d__x000d__x000d__x000d_
-a.	距离新冠肺炎患者 6 英尺以内，24 小时内总时长 15 分钟 或更长时间**或**\n_x000d__x000d__x000d__x000d__x000d_
-b.	为患有新冠肺炎疾病的患者提供居家护理**或**\n _x000d__x000d__x000d__x000d__x000d_
-c.	与患有新冠肺炎的人有直接身体接触（拥抱或接吻）**或**\n _x000d__x000d__x000d__x000d__x000d_
-d.	与患有新冠肺炎的人共用饮食器具**或**\n_x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">在您 (他们) 感觉生病前的两周内，您 (他们) 是否与患有新冠肺炎的人密切接触？——不包括在过去 3 个月内确诊新冠肺炎的人。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+如果您 (他们) 有以下情况，请与我们保持密切联系_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	距离新冠肺炎患者 6 英尺以内，24 小时内总时长 15 分钟 或更长时间**或**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	为患有新冠肺炎疾病的患者提供居家护理**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	与患有新冠肺炎的人有直接身体接触（拥抱或接吻）**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	与患有新冠肺炎的人共用饮食器具**或**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	有新冠肺炎患者朝着您打喷嚏或咳嗽\n</v>
       </c>
       <c r="F89" t="str" xml:space="preserve">
-        <v xml:space="preserve">En las dos semanas antes de sentirse enfermo, ¿tuvo contacto cercano con alguien que tuviera COVID-19? Excluya a las personas que habían tenido COVID-19 en los 3 meses anteriores. _x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-Usted ha tenido contacto cercano si_x000d__x000d__x000d__x000d__x000d_
-a.	ha estado\n a menos de 6 pies o 2 metros de alguien con COVID-19 por un total de 15 minutos o más en un periodo de 24 horas **O** \n_x000d__x000d__x000d__x000d__x000d_
-b.	le brindó atención en casa a alguien enfermo con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
-c.	tuvo contacto físico directo (abrazó o besó) a alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
-d.	compartió utensilios para comer o beber con alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">En las dos semanas antes de sentirse enfermo, ¿tuvo contacto cercano con alguien que tuviera COVID-19? Excluya a las personas que habían tenido COVID-19 en los 3 meses anteriores. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Usted ha tenido contacto cercano si_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	ha estado\n a menos de 6 pies o 2 metros de alguien con COVID-19 por un total de 15 minutos o más en un periodo de 24 horas **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	le brindó atención en casa a alguien enfermo con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	tuvo contacto físico directo (abrazó o besó) a alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	compartió utensilios para comer o beber con alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	alguien con COVID-19 \n tosió o estornudó cerca de usted</v>
       </c>
     </row>
@@ -3270,16 +2731,16 @@
         <v>What sex were they assigned at birth on their original birth certificate?</v>
       </c>
       <c r="C91" t="str">
-        <v>그 사람의 성별은 무엇입니까?</v>
+        <v>그 사람이 태어났을 때에 출생 증명서 원본에 어떤 성별이 주어졌습니까?</v>
       </c>
       <c r="D91" t="str">
-        <v>Giới tính của họ là gì?</v>
+        <v>Họ được chỉ định giới tính nào khi sinh trên giấy khai sinh ban đầu của họ?</v>
       </c>
       <c r="E91" t="str">
-        <v>他们的性别是什么？</v>
+        <v>他们在出生时在原出生证上被分配的性别是什么？</v>
       </c>
       <c r="F91" t="str">
-        <v>¿Cuál es su sexo?</v>
+        <v>¿Qué sexo se le asignó al nacer en su certificado de nacimiento original?</v>
       </c>
     </row>
     <row r="92">
@@ -3407,53 +2868,53 @@
         <v>CDC/third_person_questions/close_contact</v>
       </c>
       <c r="B98" t="str" xml:space="preserve">
-        <v xml:space="preserve">In the last two weeks, have they been in close contact with someone who has COVID-19? —excluding people who have had COVID-19 within the past 3 months. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">In the last two weeks, have they been in close contact with someone who has COVID-19? —excluding people who have had COVID-19 within the past 3 months. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+They have been in close contact if they have\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	been within 6 feet of someone who has COVID-19 for a combined total of 15 minutes or more over a 24 hour period **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	provided care at home to someone who is sick with COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	had direct physical contact (hugged or kissed) with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	shared eating or drinking utensils with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+e.	been sneezed on or coughed on by someone who has COVID-19 \n</v>
+      </c>
+      <c r="C98" t="str" xml:space="preserve">
+        <v xml:space="preserve">2주 동안 COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까? —이전 3개월 이내에 COVID-19에 걸린 사람 제외_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
  _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-They have been in close contact if they have\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-a.	been within 6 feet of someone who has COVID-19 for a combined total of 15 minutes or more over a 24 hour period **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-b.	provided care at home to someone who is sick with COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-c.	had direct physical contact (hugged or kissed) with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-d.	shared eating or drinking utensils with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-e.	been sneezed on or coughed on by someone who has COVID-19 \n</v>
-      </c>
-      <c r="C98" t="str" xml:space="preserve">
-        <v xml:space="preserve">2주 동안 COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까? —이전 3개월 이내에 COVID-19에 걸린 사람 제외_x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-다음에 해당하는 경우 귀하(그 사람)는 밀접 접촉한 것입니다\n_x000d__x000d__x000d__x000d__x000d_
-a.	24시간 내에 총 15분 이상 COVID-19를 앓고 있는 사람과 6피트 이내에 있었습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d_
-b.	COVID-19에 걸린 사람에게 집에서 치료를 제공했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d_
-c.	COVID-19에 걸린 사람과 직접적인 신체적 접촉(포옹 또는 키스)을 했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d_
-d.	COVID-19에 걸린 사람과 먹거나 마실 때 도구를 공유했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d_
+다음에 해당하는 경우 귀하(그 사람)는 밀접 접촉한 것입니다\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	24시간 내에 총 15분 이상 COVID-19를 앓고 있는 사람과 6피트 이내에 있었습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	COVID-19에 걸린 사람에게 집에서 치료를 제공했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	COVID-19에 걸린 사람과 직접적인 신체적 접촉(포옹 또는 키스)을 했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	COVID-19에 걸린 사람과 먹거나 마실 때 도구를 공유했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	COVID-19에 걸린 사람이 귀하에게 재채기나 기침을 했습니다 \n</v>
       </c>
       <c r="D98" t="str" xml:space="preserve">
-        <v xml:space="preserve">Trong hai tuần qua, quý vị có tiếp xúc gần với người bị nhiễm COVID-19 không? —ngoại trừ những người đã mắc COVID-19 trong vòng 3 tháng qua._x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-Quý vị đã tiếp xúc gần nếu đã\n_x000d__x000d__x000d__x000d__x000d_
-a.	cách người mắc COVID-19 trong vòng 6 feet (2 mét) trong tổng cộng 15 phút trở lên trong khoảng thời gian 24 giờ **hoặc**\n_x000d__x000d__x000d__x000d__x000d_
-b.	cung cấp dịch vụ chăm sóc tại nhà cho người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d_
-c.	tiếp xúc trực tiếp (ôm hoặc hôn) người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d_
-d.	dùng chung dụng cụ ăn uống với người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Trong hai tuần qua, quý vị có tiếp xúc gần với người bị nhiễm COVID-19 không? —ngoại trừ những người đã mắc COVID-19 trong vòng 3 tháng qua._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Quý vị đã tiếp xúc gần nếu đã\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	cách người mắc COVID-19 trong vòng 6 feet (2 mét) trong tổng cộng 15 phút trở lên trong khoảng thời gian 24 giờ **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	cung cấp dịch vụ chăm sóc tại nhà cho người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	tiếp xúc trực tiếp (ôm hoặc hôn) người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	dùng chung dụng cụ ăn uống với người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	bị một người mắc COVID-19 hắt hơi hoặc ho vào người\n</v>
       </c>
       <c r="E98" t="str" xml:space="preserve">
-        <v xml:space="preserve">在过去两周内，您 (他们) 是否与患有新冠肺炎的人密切接触？——不包括在过去 3 个月内确诊新冠肺炎的人。 _x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-如果您 ( 他们) 有以下情况，请与我们保持密切联系_x000d__x000d__x000d__x000d__x000d_
-a.	距离新冠肺炎患者 6 英尺以内，24 小时内总时长 15 分钟 或更长时间**或**\n_x000d__x000d__x000d__x000d__x000d_
-b.	为患有新冠肺炎疾病的患者提供居家护理**或**\n _x000d__x000d__x000d__x000d__x000d_
-c.	与患有新冠肺炎的人有直接身体接触（拥抱或接吻）**或**\n _x000d__x000d__x000d__x000d__x000d_
-d.	与患有新冠肺炎的人共用饮食器具**或**\n _x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">在过去两周内，您 (他们) 是否与患有新冠肺炎的人密切接触？——不包括在过去 3 个月内确诊新冠肺炎的人。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+如果您 ( 他们) 有以下情况，请与我们保持密切联系_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	距离新冠肺炎患者 6 英尺以内，24 小时内总时长 15 分钟 或更长时间**或**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	为患有新冠肺炎疾病的患者提供居家护理**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	与患有新冠肺炎的人有直接身体接触（拥抱或接吻）**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	与患有新冠肺炎的人共用饮食器具**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	有新冠肺炎患者朝着您打喷嚏或咳嗽\n</v>
       </c>
       <c r="F98" t="str" xml:space="preserve">
-        <v xml:space="preserve">En las últimas dos semanas, ¿tuvo contacto cercano con alguien que tuviera COVID-19? Excluya a las personas que habían tenido COVID-19 en los 3 meses anteriores. _x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-Usted ha tenido contacto cercano si:_x000d__x000d__x000d__x000d__x000d_
-a.	ha estado\n a menos de 6 pies o 2 metros de alguien con COVID-19 por un total de 15 minutos o más en un periodo de 24 horas **O** \n_x000d__x000d__x000d__x000d__x000d_
-b.	le brindó atención en casa a alguien enfermo con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
-c.	tuvo contacto físico directo (abrazó o besó) a alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
-d.	compartió utensilios para comer o beber con alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">En las últimas dos semanas, ¿tuvo contacto cercano con alguien que tuviera COVID-19? Excluya a las personas que habían tenido COVID-19 en los 3 meses anteriores. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Usted ha tenido contacto cercano si:_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	ha estado\n a menos de 6 pies o 2 metros de alguien con COVID-19 por un total de 15 minutos o más en un periodo de 24 horas **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	le brindó atención en casa a alguien enfermo con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	tuvo contacto físico directo (abrazó o besó) a alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	compartió utensilios para comer o beber con alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	alguien con COVID-19 \n tosió o estornudó cerca de usted</v>
       </c>
     </row>
@@ -3485,16 +2946,16 @@
         <v>Did they wear personal protective equipment (gown, mask or respirator, goggles or face shield, and gloves) while working or volunteering at the healthcare facility?</v>
       </c>
       <c r="C100" t="str">
-        <v>그 사람이 의료 시설에서 일하거나 자원 봉사하는 동안 개인 보호 장비(N95 또는 수술용 마스크, 가운, 눈 보호구)를 착용했습니까?</v>
+        <v>의료 시설에서 일하거나 자원 봉사하는 동안 개인 보호 장비(가운, 마스크 또는 산소호흡기, 고글 또는 얼굴 가리개 및 장갑)를 착용했습니까?</v>
       </c>
       <c r="D100" t="str">
-        <v>Họ có đeo thiết bị bảo hộ cá nhân (khẩu trang N95 hoặc khẩu trang phẫu thuật, áo choàng, kính bảo vệ mắt) khi làm việc hoặc làm tình nguyện tại cở sở y tế không?</v>
+        <v>Họ có mang thiết bị bảo vệ cá nhân (áo choàng, khẩu trang hoặc máy hô hấp, kính bảo hộ hoặc tấm che mặt và găng tay) khi làm việc hoặc tình nguyện tại cơ sở chăm sóc sức khỏe không?</v>
       </c>
       <c r="E100" t="str">
-        <v>他们在医疗机构工作或志愿工作时，是否穿戴个人防护设备（N95 或手术口罩、手术衣、眼睛保护）？</v>
+        <v>他们在医疗保健机构工作或做志愿者时是否穿戴了个人防护设备（工作服、口罩或呼吸器、护目镜或面罩和手套）？</v>
       </c>
       <c r="F100" t="str">
-        <v>¿Usó equipo de protección personal (respirador N95 o mascarilla quirúrgica, bata, protección para los ojos) mientras trabajaba o realizaba tareas de voluntariado en el establecimiento de atención médica?</v>
+        <v>¿Usó equipo de protección personal (bata, mascarilla o respirador, gafas protectoras o protector facial, y guantes) mientras trabajaba o servía de voluntario en el establecimiento de atención médica?</v>
       </c>
     </row>
     <row r="101" xml:space="preserve">
@@ -3502,53 +2963,53 @@
         <v>CDC/second_person_questions/exposure_question</v>
       </c>
       <c r="B101" t="str" xml:space="preserve">
-        <v xml:space="preserve">In the two weeks before you felt sick, have you been in close contact with someone who has COVID-19? —excluding people who have had COVID-19 within the past 3 months. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">In the two weeks before you felt sick, have you been in close contact with someone who has COVID-19? —excluding people who have had COVID-19 within the past 3 months. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+You have been in close contact if you have\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	been within 6 feet of someone who has COVID-19 for a combined total of 15 minutes or more over a 24 hour period **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	provided care at home to someone who is sick with COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	had direct physical contact (hugged or kissed) with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	shared eating or drinking utensils with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+e.	been sneezed on or coughed on by someone who has COVID-19 \n</v>
+      </c>
+      <c r="C101" t="str" xml:space="preserve">
+        <v xml:space="preserve">아프기 전 2주 동안 COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까? —이전 3개월 이내에 COVID-19에 걸린 사람 제외._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+다음에 해당하는 경우 귀하는 밀접 접촉한 것입니다\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	24시간 내에 총 15분 이상 COVID-19를 앓고 있는 사람과 6피트 이내에 있었습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	COVID-19에 걸린 사람에게 집에서 치료를 제공했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	COVID-19에 걸린 사람과 직접적인 신체적 접촉(포옹 또는 키스)을 했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	COVID-19에 걸린 사람과 먹거나 마실 때 도구를 공유했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+e.	COVID-19에 걸린 사람이 귀하에게 재채기나 기침을 했습니다 \n</v>
+      </c>
+      <c r="D101" t="str" xml:space="preserve">
+        <v xml:space="preserve">Trong hai tuần trước khi cảm thấy bị bệnh, quý vị có tiếp xúc gần với người bị nhiễm COVID-19 không? —Ngoại trừ những người đã mắc COVID-19 trong vòng 3 tháng qua. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Quý vị đã tiếp xúc gần nếu đã\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	cách người mắc COVID-19 trong vòng 6 feet (2 mét) trong tổng cộng 15 phút trở lên trong khoảng thời gian 24 giờ **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	cung cấp dịch vụ chăm sóc tại nhà cho người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	tiếp xúc trực tiếp (ôm hoặc hôn) người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	dùng chung dụng cụ ăn uống với người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+e.	bị một người mắc COVID-19 hắt hơi hoặc ho vào người\n</v>
+      </c>
+      <c r="E101" t="str" xml:space="preserve">
+        <v xml:space="preserve">在您 (他们) 感觉生病前的两周内，您 (他们) 是否与患有新冠肺炎的人密切接触？——不包括在过去 3 个月内确诊新冠肺炎的人。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
  _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-You have been in close contact if you have\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-a.	been within 6 feet of someone who has COVID-19 for a combined total of 15 minutes or more over a 24 hour period **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-b.	provided care at home to someone who is sick with COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-c.	had direct physical contact (hugged or kissed) with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-d.	shared eating or drinking utensils with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-e.	been sneezed on or coughed on by someone who has COVID-19 \n</v>
-      </c>
-      <c r="C101" t="str" xml:space="preserve">
-        <v xml:space="preserve">아프기 전 2주 동안 COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까? —이전 3개월 이내에 COVID-19에 걸린 사람 제외._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-다음에 해당하는 경우 귀하는 밀접 접촉한 것입니다\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-a.	24시간 내에 총 15분 이상 COVID-19를 앓고 있는 사람과 6피트 이내에 있었습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-b.	COVID-19에 걸린 사람에게 집에서 치료를 제공했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-c.	COVID-19에 걸린 사람과 직접적인 신체적 접촉(포옹 또는 키스)을 했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-d.	COVID-19에 걸린 사람과 먹거나 마실 때 도구를 공유했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-e.	COVID-19에 걸린 사람이 귀하에게 재채기나 기침을 했습니다 \n</v>
-      </c>
-      <c r="D101" t="str" xml:space="preserve">
-        <v xml:space="preserve">Trong hai tuần trước khi cảm thấy bị bệnh, quý vị có tiếp xúc gần với người bị nhiễm COVID-19 không? —Ngoại trừ những người đã mắc COVID-19 trong vòng 3 tháng qua. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Quý vị đã tiếp xúc gần nếu đã\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-a.	cách người mắc COVID-19 trong vòng 6 feet (2 mét) trong tổng cộng 15 phút trở lên trong khoảng thời gian 24 giờ **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-b.	cung cấp dịch vụ chăm sóc tại nhà cho người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-c.	tiếp xúc trực tiếp (ôm hoặc hôn) người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-d.	dùng chung dụng cụ ăn uống với người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-e.	bị một người mắc COVID-19 hắt hơi hoặc ho vào người\n</v>
-      </c>
-      <c r="E101" t="str" xml:space="preserve">
-        <v xml:space="preserve">在您 (他们) 感觉生病前的两周内，您 (他们) 是否与患有新冠肺炎的人密切接触？——不包括在过去 3 个月内确诊新冠肺炎的人。 _x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-如果您 (他们) 有以下情况，请与我们保持密切联系_x000d__x000d__x000d__x000d__x000d_
-a.	距离新冠肺炎患者 6 英尺以内，24 小时内总时长 15 分钟 或更长时间**或**\n_x000d__x000d__x000d__x000d__x000d_
-b.	为患有新冠肺炎疾病的患者提供居家护理**或**\n _x000d__x000d__x000d__x000d__x000d_
-c.	与患有新冠肺炎的人有直接身体接触（拥抱或接吻）**或**\n _x000d__x000d__x000d__x000d__x000d_
-d.	与患有新冠肺炎的人共用饮食器具**或**\n_x000d__x000d__x000d__x000d__x000d_
+如果您 (他们) 有以下情况，请与我们保持密切联系_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	距离新冠肺炎患者 6 英尺以内，24 小时内总时长 15 分钟 或更长时间**或**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	为患有新冠肺炎疾病的患者提供居家护理**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	与患有新冠肺炎的人有直接身体接触（拥抱或接吻）**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	与患有新冠肺炎的人共用饮食器具**或**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	有新冠肺炎患者朝着您打喷嚏或咳嗽\n</v>
       </c>
       <c r="F101" t="str" xml:space="preserve">
-        <v xml:space="preserve">En las dos semanas antes de sentirse enfermo, ¿tuvo contacto cercano con alguien que tuviera COVID-19? Excluya a las personas que habían tenido COVID-19 en los 3 meses anteriores. _x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-Usted ha tenido contacto cercano si_x000d__x000d__x000d__x000d__x000d_
-a.	ha estado\n a menos de 6 pies o 2 metros de alguien con COVID-19 por un total de 15 minutos o más en un periodo de 24 horas **O** \n_x000d__x000d__x000d__x000d__x000d_
-b.	le brindó atención en casa a alguien enfermo con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
-c.	tuvo contacto físico directo (abrazó o besó) a alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
-d.	compartió utensilios para comer o beber con alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">En las dos semanas antes de sentirse enfermo, ¿tuvo contacto cercano con alguien que tuviera COVID-19? Excluya a las personas que habían tenido COVID-19 en los 3 meses anteriores. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Usted ha tenido contacto cercano si_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	ha estado\n a menos de 6 pies o 2 metros de alguien con COVID-19 por un total de 15 minutos o más en un periodo de 24 horas **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	le brindó atención en casa a alguien enfermo con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	tuvo contacto físico directo (abrazó o besó) a alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	compartió utensilios para comer o beber con alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	alguien con COVID-19 \n tosió o estornudó cerca de usted</v>
       </c>
     </row>
@@ -3580,16 +3041,16 @@
         <v>What sex were you assigned at birth, or on your original birth certificate?</v>
       </c>
       <c r="C103" t="str">
-        <v>성별은 무엇입니까?</v>
+        <v>귀하가 태어났을 때에 출생 증명서 원본에 어떤 성별이 주어졌습니까?</v>
       </c>
       <c r="D103" t="str">
-        <v>Giới tính của quý vị là gì?</v>
+        <v>Quý vị được chỉ định giới tính nào khi sinh hoặc trong giấy khai sinh ban đầu của quý vị?</v>
       </c>
       <c r="E103" t="str">
-        <v>您的性别是什么？</v>
+        <v>您在出生时在原出生证上被分配的性别是什么？</v>
       </c>
       <c r="F103" t="str">
-        <v>¿Cuál es su sexo?</v>
+        <v>¿Qué sexo se te asignó al nacer en tu certificado de nacimiento original?</v>
       </c>
     </row>
     <row r="104">
@@ -3797,53 +3258,53 @@
         <v>CDC/second_person_questions/close_contact</v>
       </c>
       <c r="B114" t="str" xml:space="preserve">
-        <v xml:space="preserve">In the last two weeks, have you been in close contact with someone who has COVID-19? —excluding people who have had COVID-19 within the past 3 months. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">In the last two weeks, have you been in close contact with someone who has COVID-19? —excluding people who have had COVID-19 within the past 3 months. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+You have been in close contact if you have\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	been within 6 feet of someone who has COVID-19 for a combined total of 15 minutes or more over a 24 hour period **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	provided care at home to someone who is sick with COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	had direct physical contact (hugged or kissed) with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	shared eating or drinking utensils with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+e.	been sneezed on or coughed on by someone who has COVID-19 \n</v>
+      </c>
+      <c r="C114" t="str" xml:space="preserve">
+        <v xml:space="preserve">2주 동안 COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까? —이전 3개월 이내에 COVID-19에 걸린 사람 제외_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
  _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-You have been in close contact if you have\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-a.	been within 6 feet of someone who has COVID-19 for a combined total of 15 minutes or more over a 24 hour period **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-b.	provided care at home to someone who is sick with COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-c.	had direct physical contact (hugged or kissed) with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-d.	shared eating or drinking utensils with someone who has COVID-19 **or** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-e.	been sneezed on or coughed on by someone who has COVID-19 \n</v>
-      </c>
-      <c r="C114" t="str" xml:space="preserve">
-        <v xml:space="preserve">2주 동안 COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까? —이전 3개월 이내에 COVID-19에 걸린 사람 제외_x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-다음에 해당하는 경우 귀하(그 사람)는 밀접 접촉한 것입니다\n_x000d__x000d__x000d__x000d__x000d_
-a.	24시간 내에 총 15분 이상 COVID-19를 앓고 있는 사람과 6피트 이내에 있었습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d_
-b.	COVID-19에 걸린 사람에게 집에서 치료를 제공했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d_
-c.	COVID-19에 걸린 사람과 직접적인 신체적 접촉(포옹 또는 키스)을 했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d_
-d.	COVID-19에 걸린 사람과 먹거나 마실 때 도구를 공유했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d_
+다음에 해당하는 경우 귀하(그 사람)는 밀접 접촉한 것입니다\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	24시간 내에 총 15분 이상 COVID-19를 앓고 있는 사람과 6피트 이내에 있었습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	COVID-19에 걸린 사람에게 집에서 치료를 제공했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	COVID-19에 걸린 사람과 직접적인 신체적 접촉(포옹 또는 키스)을 했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	COVID-19에 걸린 사람과 먹거나 마실 때 도구를 공유했습니다 **또는** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	COVID-19에 걸린 사람이 귀하에게 재채기나 기침을 했습니다 \n</v>
       </c>
       <c r="D114" t="str" xml:space="preserve">
-        <v xml:space="preserve">Trong hai tuần qua, quý vị có tiếp xúc gần với người bị nhiễm COVID-19 không? —ngoại trừ những người đã mắc COVID-19 trong vòng 3 tháng qua._x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-Quý vị đã tiếp xúc gần nếu đã\n_x000d__x000d__x000d__x000d__x000d_
-a.	cách người mắc COVID-19 trong vòng 6 feet (2 mét) trong tổng cộng 15 phút trở lên trong khoảng thời gian 24 giờ **hoặc**\n_x000d__x000d__x000d__x000d__x000d_
-b.	cung cấp dịch vụ chăm sóc tại nhà cho người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d_
-c.	tiếp xúc trực tiếp (ôm hoặc hôn) người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d_
-d.	dùng chung dụng cụ ăn uống với người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Trong hai tuần qua, quý vị có tiếp xúc gần với người bị nhiễm COVID-19 không? —ngoại trừ những người đã mắc COVID-19 trong vòng 3 tháng qua._x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Quý vị đã tiếp xúc gần nếu đã\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	cách người mắc COVID-19 trong vòng 6 feet (2 mét) trong tổng cộng 15 phút trở lên trong khoảng thời gian 24 giờ **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	cung cấp dịch vụ chăm sóc tại nhà cho người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	tiếp xúc trực tiếp (ôm hoặc hôn) người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	dùng chung dụng cụ ăn uống với người mắc COVID-19 **hoặc**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	bị một người mắc COVID-19 hắt hơi hoặc ho vào người\n</v>
       </c>
       <c r="E114" t="str" xml:space="preserve">
-        <v xml:space="preserve">在过去两周内，您 (他们) 是否与患有新冠肺炎的人密切接触？——不包括在过去 3 个月内确诊新冠肺炎的人。 _x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-如果您 ( 他们) 有以下情况，请与我们保持密切联系_x000d__x000d__x000d__x000d__x000d_
-a.	距离新冠肺炎患者 6 英尺以内，24 小时内总时长 15 分钟 或更长时间**或**\n_x000d__x000d__x000d__x000d__x000d_
-b.	为患有新冠肺炎疾病的患者提供居家护理**或**\n _x000d__x000d__x000d__x000d__x000d_
-c.	与患有新冠肺炎的人有直接身体接触（拥抱或接吻）**或**\n _x000d__x000d__x000d__x000d__x000d_
-d.	与患有新冠肺炎的人共用饮食器具**或**\n _x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">在过去两周内，您 (他们) 是否与患有新冠肺炎的人密切接触？——不包括在过去 3 个月内确诊新冠肺炎的人。 _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+如果您 ( 他们) 有以下情况，请与我们保持密切联系_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	距离新冠肺炎患者 6 英尺以内，24 小时内总时长 15 分钟 或更长时间**或**\n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	为患有新冠肺炎疾病的患者提供居家护理**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	与患有新冠肺炎的人有直接身体接触（拥抱或接吻）**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	与患有新冠肺炎的人共用饮食器具**或**\n _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	有新冠肺炎患者朝着您打喷嚏或咳嗽\n</v>
       </c>
       <c r="F114" t="str" xml:space="preserve">
-        <v xml:space="preserve">En las últimas dos semanas, ¿tuvo contacto cercano con alguien que tuviera COVID-19? Excluya a las personas que habían tenido COVID-19 en los 3 meses anteriores. _x000d__x000d__x000d__x000d__x000d_
- _x000d__x000d__x000d__x000d__x000d_
-Usted ha tenido contacto cercano si:_x000d__x000d__x000d__x000d__x000d_
-a.	ha estado\n a menos de 6 pies o 2 metros de alguien con COVID-19 por un total de 15 minutos o más en un periodo de 24 horas **O** \n_x000d__x000d__x000d__x000d__x000d_
-b.	le brindó atención en casa a alguien enfermo con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
-c.	tuvo contacto físico directo (abrazó o besó) a alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
-d.	compartió utensilios para comer o beber con alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">En las últimas dos semanas, ¿tuvo contacto cercano con alguien que tuviera COVID-19? Excluya a las personas que habían tenido COVID-19 en los 3 meses anteriores. _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+ _x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+Usted ha tenido contacto cercano si:_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+a.	ha estado\n a menos de 6 pies o 2 metros de alguien con COVID-19 por un total de 15 minutos o más en un periodo de 24 horas **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+b.	le brindó atención en casa a alguien enfermo con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+c.	tuvo contacto físico directo (abrazó o besó) a alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+d.	compartió utensilios para comer o beber con alguien con COVID-19 **O** \n_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 e.	alguien con COVID-19 \n tosió o estornudó cerca de usted</v>
       </c>
     </row>
@@ -3915,16 +3376,16 @@
         <v>Did you wear personal protective equipment (gown, mask or respirator, goggles or face shield, and gloves) while working or volunteering at the healthcare facility?</v>
       </c>
       <c r="C118" t="str">
-        <v>의료 시설에서 일하거나 자원 봉사하는 동안 개인 보호 장비(N95 또는 수술용 마스크, 가운, 눈 보호구)를 착용했습니까?</v>
+        <v>의료 시설에서 일하거나 자원 봉사하는 동안 개인 보호 장비(가운, 마스크 또는 산소호흡기, 고글 또는 얼굴 가리개 및 장갑)를 착용했습니까?</v>
       </c>
       <c r="D118" t="str">
-        <v>Bạn có đeo thiết bị bảo hộ cá nhân (khẩu trang N95 hoặc khẩu trang phẫu thuật, áo choàng, kính bảo vệ mắt) khi làm việc hoặc làm tình nguyện tại cở sở y tế không?</v>
+        <v>Quý vị có mang thiết bị bảo vệ cá nhân (áo choàng, khẩu trang hoặc mặt nạ phòng độc, kính bảo hộ hoặc tấm che mặt và găng tay) khi làm việc hoặc tình nguyện tại cơ sở chăm sóc sức khỏe không?</v>
       </c>
       <c r="E118" t="str">
-        <v>您在医疗机构工作或志愿工作时，是否穿戴个人防护设备（N95 或手术口罩、手术衣、眼睛保护）？</v>
+        <v>您在医疗保健机构工作或做志愿者时是否穿戴了个人防护设备（工作服、口罩或呼吸器、护目镜或面罩和手套）？</v>
       </c>
       <c r="F118" t="str">
-        <v>¿Usó equipo de protección personal (respirador N95 o mascarilla quirúrgica, bata, protección para los ojos) mientras trabajaba o realizaba tareas de voluntariado en el establecimiento de atención médica?</v>
+        <v>¿Usó equipo de protección personal (bata, mascarilla o respirador, gafas protectoras o protector facial, y guantes) mientras trabajaba o servía de voluntario en el establecimiento de atención médica?</v>
       </c>
     </row>
     <row r="119">
@@ -3995,16 +3456,16 @@
         <v>["Male","Female","I prefer not to say.","I don't know."]</v>
       </c>
       <c r="C122" t="str">
-        <v>["남성","여성","기타"]</v>
+        <v>["남성","여성","말하고 싶지 않음.","모름."]</v>
       </c>
       <c r="D122" t="str">
-        <v>["Nam","Nữ","Khác"]</v>
+        <v>["Nam","Nữ","Tôi không muốn nói.","Tôi không biết."]</v>
       </c>
       <c r="E122" t="str">
-        <v>["男性","女性","其他"]</v>
+        <v>["男","女","我不想说","我不知道。"]</v>
       </c>
       <c r="F122" t="str">
-        <v>["Masculino","Femenino","Otro"]</v>
+        <v>["Masculino","Femenino","Prefiero no decirlo","No sé"]</v>
       </c>
     </row>
     <row r="123">
@@ -7492,63 +6953,153 @@
         <v>CDC/second_person_questions/life_threat_question</v>
       </c>
       <c r="B297" t="str" xml:space="preserve">
-        <v xml:space="preserve">Do you have any of these life-threatening symptoms?
-- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone
-- Severe and constant pain or pressure in the chest
-- Extreme difficulty breathing (such as gasping for air, being unable to talk without catching your breath, severe wheezing, nostrils flaring)
-- New disorientation (acting confused)
-- Unconscious or very difficult to wake up
-- Slurred speech or difficulty speaking (new or worsening)
-- New or worsening seizures
-- Signs of low blood pressure (too weak to stand, dizziness, lightheaded, feeling cold, pale, clammy skin)
+        <v xml:space="preserve">Do you have any of these life-threatening symptoms?_x000d__x000d_
+- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone_x000d__x000d_
+- Severe and constant pain or pressure in the chest_x000d__x000d_
+- Extreme difficulty breathing (such as gasping for air, being unable to talk without catching your breath, severe wheezing, nostrils flaring)_x000d__x000d_
+- New disorientation (acting confused)_x000d__x000d_
+- Unconscious or very difficult to wake up_x000d__x000d_
+- Slurred speech or difficulty speaking (new or worsening)_x000d__x000d_
+- New or worsening seizures_x000d__x000d_
+- Signs of low blood pressure (too weak to stand, dizziness, lightheaded, feeling cold, pale, clammy skin)_x000d__x000d_
 - Dehydration (dry lips and mouth, not urinating much, sunken eyes)</v>
       </c>
       <c r="C297" t="str" xml:space="preserve">
-        <v xml:space="preserve">이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 창백한 입술 또는 얼굴- 가슴에 심하고 지속적인 통증이나 압박감- 숨쉬기 매우 어려움(예: 숨이 막힘, 숨을 고르지 않고는 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 시간, 장소, 또는 관계를 제대로 인식하지 못하게 됨 (혼란스러워함)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의식이 없거나 깨우기가 매우 어려움- 불분명한 발음 또는 말하기 어려움(새로운 또는 악화된 증상)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 신규 또는 악화된 발작_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 추위를 느낌, 창백함, 차갑고 축축한 피부)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 창백한 입술 또는 얼굴- 가슴에 심하고 지속적인 통증이나 압박감- 숨쉬기 매우 어려움(예: 숨이 막힘, 숨을 고르지 않고는 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 시간, 장소, 또는 관계를 제대로 인식하지 못하게 됨 (혼란스러워함)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 의식이 없거나 깨우기가 매우 어려움- 불분명한 발음 또는 말하기 어려움(새로운 또는 악화된 증상)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 신규 또는 악화된 발작_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 추위를 느낌, 창백함, 차갑고 축축한 피부)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - 탈수(입술과 입 건조, 소변량이 많지 않음, 움푹 들어간 눈)</v>
       </c>
       <c r="D297" t="str" xml:space="preserve">
-        <v xml:space="preserve">Bạn có bất cứ triệu chứng đe dọa tính mạng nào trong số này không?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Môi hoặc mặt thâm_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đau hoặc có áp lực nặng và liên tục ở ngực_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Vô cùng khó thở (chẳng hạn như thở hổn hển, không thể nói chuyện mà không bị hụt hơn, thở khò khè nặng, mũi phập phồng)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất phương hướng mới xuất hiện (hành động lẫn lộn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất tri giác hoặc rất khó thức dậy_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Nói đớt hoặc khó nói (mới xuất hiện hoặc bị nặng hơn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cơn co giật mới xuất hiện hoặc nặng thêm_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dấu hiệu huyết áp thấp (quá yếu không thể đứng, chóng mặt, choáng vàng, cảm thấy lạnh, da nhợt nhạt, sần sùi)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Bạn có bất cứ triệu chứng đe dọa tính mạng nào trong số này không?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Môi hoặc mặt thâm_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Đau hoặc có áp lực nặng và liên tục ở ngực_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Vô cùng khó thở (chẳng hạn như thở hổn hển, không thể nói chuyện mà không bị hụt hơn, thở khò khè nặng, mũi phập phồng)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Mất phương hướng mới xuất hiện (hành động lẫn lộn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Mất tri giác hoặc rất khó thức dậy_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Nói đớt hoặc khó nói (mới xuất hiện hoặc bị nặng hơn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Cơn co giật mới xuất hiện hoặc nặng thêm_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- Dấu hiệu huyết áp thấp (quá yếu không thể đứng, chóng mặt, choáng vàng, cảm thấy lạnh, da nhợt nhạt, sần sùi)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 - Mất nước (môi và miệng khô, không đi tiểu nhiều, mắt trũng sâu)</v>
       </c>
       <c r="E297" t="str" xml:space="preserve">
-        <v xml:space="preserve">您是否出现这些危及生命的症状？_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 嘴唇或面部青紫_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 重度和持续性胸痛或胸部压迫感_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--极度呼吸困难（如喘不过气或因为喘不上气而无法说话、重度喘息、鼻孔张开）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--新发的定向障碍（行为混乱）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 意识丧失或很难唤醒_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 言语不清或说话困难（新发或恶化）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--新发癫痫发作或癫痫发作恶化_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">您是否出现这些危及生命的症状？_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 嘴唇或面部青紫_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 重度和持续性胸痛或胸部压迫感_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-极度呼吸困难（如喘不过气或因为喘不上气而无法说话、重度喘息、鼻孔张开）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-新发的定向障碍（行为混乱）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 意识丧失或很难唤醒_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 言语不清或说话困难（新发或恶化）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+-新发癫痫发作或癫痫发作恶化_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 -脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）</v>
       </c>
       <c r="F297" t="str" xml:space="preserve">
-        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Labios o cara azulados_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Presión o dolor intensos y constantes en el pecho _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dificultad extrema para respirar (le falta el aire o no puede hablar sin quedarse sin aliento, sibilancias intensas, se ensanchan los agujeros de la nariz)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Desorientación (actuar confuso) de aparición reciente_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Estado inconsciente o mucha dificultad para despertarte_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Habla arrastrada o enredada, o dificultad para hablar (de aparición reciente o que empeora) _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Convulsiones de aparición reciente o que empeoran_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Signos de presión arterial baja (muy débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa) _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Color pálido, gris o azulado de la piel, los labios, o el lecho de las uñas, dependiendo del tono de piel_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Presión o dolor intensos y constantes en el pecho _x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Dificultad extrema para respirar (le falta el aire o no puede hablar sin quedarse sin aliento, sibilancias intensas, se ensanchan los agujeros de la nariz)_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Desorientación (actuar confuso) de aparición reciente_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Estado inconsciente o mucha dificultad para despertarte_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Habla arrastrada o enredada, o dificultad para hablar (de aparición reciente o que empeora) _x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Convulsiones de aparición reciente o que empeoran_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+- Signos de presión arterial baja (muy débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa) _x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
 - Deshidratación (boca y labios secos, no orinar mucho, ojos hundidos)</v>
       </c>
     </row>
@@ -7557,64 +7108,59 @@
         <v>CDC/third_person_questions/life_threat_question</v>
       </c>
       <c r="B298" t="str" xml:space="preserve">
-        <v xml:space="preserve">Do they have any of these life-threatening symptoms?
-- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone
-- Severe and constant pain or pressure in the chest
-- Extreme difficulty breathing (such as gasping for air, being unable to talk without catching their breath, severe wheezing, nostrils flaring)
-- New disorientation (acting confused)- Unconscious or very difficult to wake up
-- Slurred speech or difficulty speaking (new or worsening)
-- New or worsening seizures
-- Signs of low blood pressure (too weak to stand, dizziness, lightheaded, feeling cold, pale, clammy skin)
+        <v xml:space="preserve">Do they have any of these life-threatening symptoms?_x000d__x000d_
+- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone_x000d__x000d_
+- Severe and constant pain or pressure in the chest_x000d__x000d_
+- Extreme difficulty breathing (such as gasping for air, being unable to talk without catching their breath, severe wheezing, nostrils flaring)_x000d__x000d_
+- New disorientation (acting confused)- Unconscious or very difficult to wake up_x000d__x000d_
+- Slurred speech or difficulty speaking (new or worsening)_x000d__x000d_
+- New or worsening seizures_x000d__x000d_
+- Signs of low blood pressure (too weak to stand, dizziness, lightheaded, feeling cold, pale, clammy skin)_x000d__x000d_
 - Dehydration (dry lips and mouth, not urinating much, sunken eyes)</v>
       </c>
       <c r="C298" t="str" xml:space="preserve">
-        <v xml:space="preserve">그 사람에게 이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 창백한 입술 또는 얼굴- 가슴에 심하고 지속적인 통증이나 압박감_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 숨쉬기 매우 어려움(예: 숨이 막힘, 숨을 고르지 않고는 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 시간, 장소, 또는 관계를 제대로 인식하지 못하게 됨 (혼란스러워함)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의식이 없거나 깨우기가 매우 어려움_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 불분명한 발음 또는 말하기 어려움(새로운 또는 악화된 증상)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 신규 또는 악화된 발작_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 추위를 느낌, 창백함, 차갑고 축축한 피부)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">그 사람에게 이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d_
+- 피부, 입술 또는 손발톱 바닥이 창백해지거나 회색 또는 파란색이 됨(피부 색조에 따라 상이)_x000d__x000d_
+- 가슴에 심하고 지속적인 통증이나 압박감_x000d__x000d_
+- 숨쉬기 매우 어려움(예: 숨이 막힘, 숨을 참고 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐)_x000d__x000d_
+- 새로운 방향 감각 상실(혼란스러워 하는 행동)- 의식이 없거나 깨우기가 매우 어려움_x000d__x000d_
+- 불분명한 발음 또는 말하기 어려움(새로운 증상 또는 악화되는 증상)_x000d__x000d_
+- 신규 또는 악화되는 발작_x000d__x000d_
+- 저혈압 징후(너무 힘이 없어 서 있을 수 없고, 어지러움, 머리가 핑핑 도는 느낌, 차갑고, 창백하며, 칙칙한 피부)_x000d__x000d_
 - 탈수(입술과 입 건조, 소변량이 많지 않음, 움푹 들어간 눈)</v>
       </c>
       <c r="D298" t="str" xml:space="preserve">
-        <v xml:space="preserve">Họ có bất cứ triệu chứng đe dọa tính mạng nào trong số này không?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Môi hoặc mặt thâm_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đau hoặc có áp lực nặng và liên tục ở ngực_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Vô cùng khó thở (chẳng hạn như thở hổn hển, không thể nói chuyện mà không bị hụt hơn, thở khò khè nặng, mũi phập phồng)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất phương hướng mới xuất hiện (hành động lẫn lộn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất tri giác hoặc rất khó thức dậy_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Nói đớt hoặc khó nói (mới xuất hiện hoặc bị nặng hơn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cơn co giật mới xuất hiện hoặc nặng thêm_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dấu hiệu huyết áp thấp (quá yếu không thể đứng, chóng mặt, choáng vàng, cảm thấy lạnh, da nhợt nhạt, sần sùi)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Họ có bất kỳ triệu chứng đe dọa đến tính mạng nào dưới đây không?_x000d__x000d_
+- Da, môi hoặc móng tay màu nhợt nhạt, xám hoặc xanh, tùy thuộc vào tông màu da_x000d__x000d_
+- Đau hoặc tức ngực dữ dội và liên tục_x000d__x000d_
+- Khó thở cực độ (ví dụ như thở hổn hển, không thể đi lại hoặc nói chuyện liền câu mà không thở, thở khò khè dữ dội, lỗ mũi phập phồng)_x000d__x000d_
+- Mất phương hướng mới (hành động bối rối) - Bất tỉnh hoặc rất khó đánh thức_x000d__x000d_
+- Nói ngọng hoặc khó nói (mới hoặc nặng hơn)_x000d__x000d_
+- Cơn co giật mới hoặc nặng hơn _x000d__x000d_
+-  Dấu hiệu của huyết áp thấp (không thể đứng vững, chóng mặt, choáng váng, ớn lạnh, xanh xao, da lạnh và mướt mồ hôi)_x000d__x000d_
 - Mất nước (môi và miệng khô, không đi tiểu nhiều, mắt trũng sâu)</v>
       </c>
       <c r="E298" t="str" xml:space="preserve">
-        <v xml:space="preserve">他们是否出现这些危及生命的症状？_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 嘴唇或面部青紫_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 重度和持续性胸痛或胸部压迫感_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--极度呼吸困难（如喘不过气或因为喘不上气而无法说话、重度喘息、鼻孔张开）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--新发的定向障碍（行为混乱）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 意识丧失或很难唤醒_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 言语不清或说话困难（新发或恶化）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--新发癫痫发作或癫痫发作恶化_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）</v>
+        <v xml:space="preserve">他们是否出现这些危及生命的症状？_x000d__x000d_
+- 根据肤色的不同，皮肤、嘴唇或指甲呈浅色、灰色或蓝色_x000d__x000d_
+- 重度和持续性胸痛或胸部压迫感_x000d__x000d_
+-极度呼吸困难（如喘不过气或因为喘不上气而无法说话、重度喘息、鼻孔张开）_x000d__x000d_
+- 新的迷失方向(行为混乱)-无意识或很难被唤醒_x000d__x000d_
+- 言语不清或说话困难（新发或恶化）_x000d__x000d_
+- 新发癫痫发作或癫痫发作恶化_x000d__x000d_
+- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d_
+- 脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）</v>
       </c>
       <c r="F298" t="str" xml:space="preserve">
-        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Labios o cara azulados_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Presión o dolor intensos y constantes en el pecho _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dificultad extrema para respirar (falta el aire o no poder hablar sin quedarse sin aliento, sibilancias intensas, se ensanchan los agujeros de la nariz)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Desorientación (actuar confuso) de aparición reciente_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Estado inconsciente o mucha dificultad para despertarse_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Habla arrastrada o enredada, o dificultad para hablar (de aparición reciente o que empeora) _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Convulsiones de aparición reciente o que empeoran_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Signos de presión arterial baja (muy débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa) _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d_
+- Color pálido, gris o azulado de la piel, los labios, o el lecho de las uñas, dependiendo del tono de piel_x000d_
+- Presión o dolor intensos y constantes en el pecho _x000d_
+- Dificultad extrema para respirar (le falta el aire o no puede hablar sin quedarse sin aliento, sibilancias intensas, se ensanchan los agujeros de la nariz)_x000d_
+- Desorientación (actuar confuso) de aparición reciente_x000d_
+- Estado inconsciente o mucha dificultad para despertarse_x000d_
+- Habla arrastrada o enredada, o dificultad para hablar (de aparición reciente o que empeora) _x000d_
+- Convulsiones de aparición reciente o que empeoran_x000d_
+- Signos de presión arterial baja (muy débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa) _x000d_
 - Deshidratación (boca y labios secos, no orinar mucho, ojos hundidos)</v>
       </c>
     </row>
@@ -7723,58 +7269,64 @@
         <v>CDC/life_threat_question</v>
       </c>
       <c r="B304" t="str" xml:space="preserve">
-        <v xml:space="preserve">Do you have any of these life-threatening symptoms?
-- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone
-- Severe and constant pain or pressure in the chest
-- Extreme difficulty breathing (gasping for air or cannot talk without catching your breath)
-- Severe and constant dizziness or lightheadedness
-- Serious disorientation (acting confused)
-- Unconscious or very difficult to wake up
-- Slurred speech (new or worsening)
-- Seizures 
+        <v xml:space="preserve">Do you have any of these life-threatening symptoms?_x000d__x000d_
+- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone_x000d__x000d_
+- Severe and constant pain or pressure in the chest_x000d__x000d_
+- Extreme difficulty breathing (gasping for air or cannot talk without catching your breath)_x000d__x000d_
+- Severe and constant dizziness or lightheadedness_x000d__x000d_
+- Serious disorientation (acting confused)_x000d__x000d_
+- Unconscious or very difficult to wake up_x000d__x000d_
+- Slurred speech (new or worsening)_x000d__x000d_
+- Seizures _x000d__x000d_
 - Signs of low blood pressure (too weak to stand, light headed, feeling cold, pale, clammy skin)</v>
       </c>
       <c r="C304" t="str" xml:space="preserve">
-        <v xml:space="preserve">이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 창백한 입술 또는 얼굴_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 가슴에 심하고 지속적인 통증이나 압박감_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 숨쉬기 매우 어려움(숨이 막히거나 숨을 참고 말을 할 수 없는 경우)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 심한 지속적인 어지러움이나 현기증_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 심각한 방향 감각 상실(혼란한 행동)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의식이 없거나 깨우기가 매우 어려움_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- (새로운 또는 악화된) 분명하지 않은 말투_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 발작 _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d_
+- 피부, 입술 또는 손발톱 바닥이 창백해지거나 회색 또는 파란색이 됨(피부 색조에 따라 상이)_x000d__x000d_
+- 가슴에 심하고 지속적인 통증이나 압박감_x000d__x000d_
+- 숨쉬기 매우 어려움(숨이 막히거나 숨을 참고 말을 할 수 없는 경우)_x000d__x000d_
+- 심한 지속적인 어지러움이나 현기증_x000d__x000d_
+- 중대한 방향 감각 상실(혼란한 행동)_x000d__x000d_
+- 의식이 없거나 깨우기가 매우 어려움_x000d__x000d_
+- (새로운 또는 악화된) 분명하지 않은 말투_x000d__x000d_
+- 발작 _x000d__x000d_
 - 저혈압 징후(너무 힘이 없어 서 있을 수 없고, 머리가 핑핑 도는 느낌, 차갑고, 창백하며, 칙칙한 피부)</v>
       </c>
       <c r="D304" t="str" xml:space="preserve">
-        <v xml:space="preserve">Quý vị có bất kỳ triệu chứng đe dọa đến tính mạng nào dưới đây không?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Môi hoặc mặt hơi tím tái_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đau hoặc tức ngực dữ dội và liên tục_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Rất khó thở (thở hổn hển hoặc không thể nói chuyện liền câu mà không thở)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Chóng mặt hoặc choáng váng nghiêm trọng và liên tục_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất phương hướng nghiêm trọng (hành động khó hiểu)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Bất tỉnh hoặc rất khó đánh thức dậy_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Nói ngọng (mới bị hoặc tình trạng tệ hơn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Co giật _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Quý vị có bất kỳ triệu chứng đe dọa đến tính mạng nào dưới đây không?_x000d__x000d_
+- Da, môi hoặc móng tay màu nhợt nhạt, xám hoặc xanh, tùy thuộc vào tông màu da_x000d__x000d_
+- Đau hoặc tức ngực dữ dội và liên tục_x000d__x000d_
+- Rất khó thở (thở hổn hển hoặc không thể nói chuyện liền câu mà không thở)_x000d__x000d_
+- Chóng mặt hoặc choáng váng nghiêm trọng và liên tục_x000d__x000d_
+- Mất phương hướng nghiêm trọng (hành động khó hiểu)_x000d__x000d_
+- Bất tỉnh hoặc rất khó đánh thức dậy_x000d__x000d_
+- Nói ngọng (mới bị hoặc tình trạng tệ hơn)_x000d__x000d_
+- Co giật _x000d__x000d_
 - Dấu hiệu của huyết áp thấp (không thể đứng vững, choáng váng, ớn lạnh, xanh xao, da lạnh và mướt mồ hôi)</v>
       </c>
       <c r="E304" t="str" xml:space="preserve">
-        <v xml:space="preserve">您是否出现这些危及生命的症状？_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 嘴唇或面部青紫_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 重度和持续性胸痛或胸部压迫感_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--极度呼吸困难（喘不过气或不喘息就无法讲话）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 重度和持续性头晕或头晕目眩_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--严重的定向障碍（表现神智错乱）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 意识丧失或很难唤醒_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--言语不清（新发或恶化）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 癫痫发作_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">您是否出现这些危及生命的症状？_x000d__x000d_
+- 根据肤色的不同，皮肤、嘴唇或指甲呈浅色、灰色或蓝色_x000d__x000d_
+- 重度和持续性胸痛或胸部压迫感_x000d__x000d_
+- 极度呼吸困难（喘不过气或不喘息就无法讲话）_x000d__x000d_
+- 重度和持续性头晕或头晕目眩_x000d__x000d_
+- 严重的定向障碍（表现神智错乱）_x000d__x000d_
+- 意识丧失或很难唤醒_x000d__x000d_
+- 言语不清（新发或恶化）_x000d__x000d_
+癫痫发作 _x000d__x000d_
 - 低血压体征（太虚弱无法站立、头晕目眩、感觉寒冷、苍白、皮肤湿冷）</v>
       </c>
-      <c r="F304" t="str">
-        <v>¿Tiene alguno de estos síntomas potencialmente mortales?- Labios o cara azulados- Presión o dolor intensos y constantes en el pecho- Dificultad extrema para respirar (falta de aire o no puede hablar sin quedarse sin aliento)- Mareos o aturdimiento intensos y constantes- Desorientación grave (actuar confuso)- Estado inconsciente o mucha dificultad para despertarse- Habla arrastrada o enredada (de aparición reciente o que empeora)- Convulsiones- Signos de presión arterial baja (muy débil para estar de pie, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa)</v>
+      <c r="F304" t="str" xml:space="preserve">
+        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d__x000d_
+- Color pálido, gris o azulado de la piel, los labios, o el lecho de las uñas, dependiendo del tono de piel_x000d__x000d_
+- Presión o dolor intensos y constantes en el pecho _x000d__x000d_
+- Dificultad extrema para respirar (le falta el aire o no puede hablar sin quedarse sin aliento)_x000d__x000d_
+- Mareos o aturdimiento intensos y constantes _x000d__x000d_
+- Desorientación grave (actuar confuso)_x000d__x000d_
+- Estado inconsciente o mucha dificultad para despertarse_x000d__x000d_
+- Habla arrastrada o enredada (de aparición reciente o que empeora) _x000d__x000d_
+- Convulsiones _x000d__x000d_
+- Signos de presión arterial baja (muy débil para estar de pie, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa)</v>
       </c>
     </row>
     <row r="305">
@@ -7805,16 +7357,16 @@
         <v>What is your ZIP code? (optional)</v>
       </c>
       <c r="C306" t="str">
-        <v/>
+        <v>우편번호가 무엇입니까? (선택 사항)</v>
       </c>
       <c r="D306" t="str">
-        <v/>
+        <v xml:space="preserve">Mã ZIP của quý vị là gì? (không bắt buộc) </v>
       </c>
       <c r="E306" t="str">
-        <v/>
+        <v>您的邮政编码是多少？(可选)</v>
       </c>
       <c r="F306" t="str">
-        <v/>
+        <v>¿Cuál es su código postal? (opcional)</v>
       </c>
     </row>
     <row r="307">
@@ -7825,16 +7377,16 @@
         <v>Click here to enter a 5-digit (12345) or 9-digit (12345-1234) ZIP code</v>
       </c>
       <c r="C307" t="str">
-        <v/>
+        <v>5자리(12345) 또는 9자리(12345-1234) 우편번호를 입력하려면 여기를 클릭하십시오</v>
       </c>
       <c r="D307" t="str">
-        <v/>
+        <v>Nhấp vào đây để nhập mã ZIP gồm 5 chữ số (12345) hoặc 9 chữ số (12345-1234)</v>
       </c>
       <c r="E307" t="str">
-        <v/>
+        <v>点击这里输入5位数(12345)或9位数(12345-1234)的邮政编码</v>
       </c>
       <c r="F307" t="str">
-        <v/>
+        <v>Haga clic acá para ingresar un código postal de 5 dígitos (12345) o 9 dígitos (12345-1234)</v>
       </c>
     </row>
     <row r="308">
@@ -7845,16 +7397,16 @@
         <v>Skip</v>
       </c>
       <c r="C308" t="str">
-        <v/>
+        <v>건너뛰기</v>
       </c>
       <c r="D308" t="str">
-        <v/>
+        <v>Bỏ qua</v>
       </c>
       <c r="E308" t="str">
-        <v/>
+        <v>跳过(Skip)</v>
       </c>
       <c r="F308" t="str">
-        <v/>
+        <v>Saltar</v>
       </c>
     </row>
     <row r="309">
@@ -7865,16 +7417,16 @@
         <v>Set ZIP code</v>
       </c>
       <c r="C309" t="str">
-        <v/>
+        <v>우편번호 설정하기</v>
       </c>
       <c r="D309" t="str">
-        <v/>
+        <v>Đặt mã ZIP</v>
       </c>
       <c r="E309" t="str">
-        <v/>
+        <v>设置邮政编码</v>
       </c>
       <c r="F309" t="str">
-        <v/>
+        <v>Fije el código postal</v>
       </c>
     </row>
     <row r="310">
@@ -7885,16 +7437,16 @@
         <v>Please enter only a 5-digit (12345) or 9-digit (12345-1234) ZIP code or press "skip"</v>
       </c>
       <c r="C310" t="str">
-        <v/>
+        <v>5자리(12345) 또는 9자리(12345-1234) 우편번호만 입력하거나 “건너뛰기”를 누르십시오</v>
       </c>
       <c r="D310" t="str">
-        <v/>
+        <v>Vui lòng chỉ nhập mã ZIP gồm 5 chữ số (12345) hoặc 9 chữ số (12345-1234) hoặc nhấn "bỏ qua"</v>
       </c>
       <c r="E310" t="str">
-        <v/>
+        <v>请只输入5位数(12345)或9位数(12345-1234)邮政编码，或按“跳过（Skip）”</v>
       </c>
       <c r="F310" t="str">
-        <v/>
+        <v>Ingrese solo un código postal de 5 dígitos (12345) o 9 dígitos (12345-1234) o presione "saltar"</v>
       </c>
     </row>
     <row r="311">
@@ -7905,16 +7457,16 @@
         <v>["Male","Female","Transgender","I prefer not to say."]</v>
       </c>
       <c r="C311" t="str">
-        <v/>
+        <v>["남성","여성","성전환자","말하고 싶지 않음."]</v>
       </c>
       <c r="D311" t="str">
-        <v/>
+        <v>["Nam", "Nữ", "Chuyển giới", "Tôi không muốn nói."]</v>
       </c>
       <c r="E311" t="str">
-        <v/>
+        <v>["男","女","变性人","我不想说。"]</v>
       </c>
       <c r="F311" t="str">
-        <v/>
+        <v>["Masculino","Femenino","Transgénero","Prefiero no decirlo"]</v>
       </c>
     </row>
     <row r="312">
@@ -7925,16 +7477,16 @@
         <v>How do you currently describe yourself?</v>
       </c>
       <c r="C312" t="str">
-        <v/>
+        <v>현재 귀하는 어떻습니까?</v>
       </c>
       <c r="D312" t="str">
-        <v/>
+        <v>Hiện tại quý vị mô tả về bản thân như thế nào?</v>
       </c>
       <c r="E312" t="str">
-        <v/>
+        <v>您目前如何描述您自己？</v>
       </c>
       <c r="F312" t="str">
-        <v/>
+        <v>¿Cómo se describe usted en la actualidad?</v>
       </c>
     </row>
     <row r="313">
@@ -7945,16 +7497,16 @@
         <v>How do they currently describe themselves?</v>
       </c>
       <c r="C313" t="str">
-        <v/>
+        <v>현재 그 사람은 어떻습니까?</v>
       </c>
       <c r="D313" t="str">
-        <v/>
+        <v xml:space="preserve">Hiện tại họ mô tả bản thân như thế nào? </v>
       </c>
       <c r="E313" t="str">
-        <v/>
+        <v>他们目前如何描述他们自己？</v>
       </c>
       <c r="F313" t="str">
-        <v/>
+        <v>¿Cómo se describe en la actualidad?</v>
       </c>
     </row>
     <row r="314" xml:space="preserve">
@@ -7962,20 +7514,29 @@
         <v>CDC/third_person_questions/latinx_question</v>
       </c>
       <c r="B314" t="str" xml:space="preserve">
-        <v xml:space="preserve">Are they of Hispanic, Latino, or of Spanish origin?
+        <v xml:space="preserve">Are they of Hispanic, Latino, or of Spanish origin?_x000d__x000d_
+_x000d__x000d_
 ###### *This question is optional. We are using this information to evaluate government programs to ensure that they fairly and equitably serve the needs of all racial groups and to monitor compliance with antidiscrimination laws, regulation, and policies.</v>
       </c>
-      <c r="C314" t="str">
-        <v/>
-      </c>
-      <c r="D314" t="str">
-        <v/>
-      </c>
-      <c r="E314" t="str">
-        <v/>
-      </c>
-      <c r="F314" t="str">
-        <v/>
+      <c r="C314" t="str" xml:space="preserve">
+        <v xml:space="preserve">그 사람이 히스패닉, 라틴계 또는 스페인 출신입니까?_x000d__x000d_
+_x000d__x000d_
+###### *이 질문은 선택 사항입니다. 정부가 모든 인종 집단의 요구에 공정하고 공평하게 대응하고, 차별금지법과 법규 및 정책을 준수한다는 것을 확실히 모니터링하기 위한 정부 프로그램 평가를 위해 이 정보를 사용하고 있습니다.</v>
+      </c>
+      <c r="D314" t="str" xml:space="preserve">
+        <v xml:space="preserve">Họ là người gốc Tây Ban Nha, La tinh hay gốc Tây Ban Nha?_x000d__x000d_
+_x000d__x000d_
+###### *Câu hỏi này là không bắt buộc. Chúng tôi đang sử dụng thông tin này để đánh giá các chương trình của chính phủ nhằm đảm bảo rằng các chương trình đó phục vụ nhu cầu của tất cả các nhóm chủng tộc và giám sát việc tuân thủ các luật, quy định và chính sách chống phân biệt đối xử. </v>
+      </c>
+      <c r="E314" t="str" xml:space="preserve">
+        <v xml:space="preserve">他们是西班牙裔、拉丁裔还是西班牙裔？_x000d__x000d_
+_x000d__x000d_
+###### *本题为可选题。我们使用这些信息来评估政府的计划，以确保它们公平和公正地满足所有种族群体的需求，并监测对反歧视法律、法规和政策的遵守情况。</v>
+      </c>
+      <c r="F314" t="str" xml:space="preserve">
+        <v xml:space="preserve">¿Es de origen hispano, latino o español?_x000d__x000d_
+_x000d__x000d_
+###### *Esta pregunta es opcional. Estamos usando esta información para evaluar programas gubernamentales a fin de garantizar que satisfagan de manera justa y equitativa las necesidades de todos los grupos raciales y para vigilar el cumplimiento de las leyes, normas y políticas contra la discriminación.</v>
       </c>
     </row>
     <row r="315" xml:space="preserve">
@@ -7983,20 +7544,29 @@
         <v>CDC/second_person_questions/latinx_question</v>
       </c>
       <c r="B315" t="str" xml:space="preserve">
-        <v xml:space="preserve">Are you of Hispanic, Latino, or Spanish origin?
+        <v xml:space="preserve">Are you of Hispanic, Latino, or Spanish origin?_x000d__x000d_
+_x000d__x000d_
 ###### *This question is optional. We are using this information to evaluate government programs to ensure that they fairly and equitably serve the needs of all racial groups and to monitor compliance with antidiscrimination laws, regulation, and policies.</v>
       </c>
-      <c r="C315" t="str">
-        <v/>
-      </c>
-      <c r="D315" t="str">
-        <v/>
-      </c>
-      <c r="E315" t="str">
-        <v/>
-      </c>
-      <c r="F315" t="str">
-        <v/>
+      <c r="C315" t="str" xml:space="preserve">
+        <v xml:space="preserve">귀하는 히스패닉, 라틴계 또는 스페인 출신입니까?_x000d__x000d_
+_x000d__x000d_
+###### *이 질문은 선택 사항입니다. 정부가 모든 인종 집단의 요구에 공정하고 공평하게 대응하고, 차별금지법과 법규 및 정책을 준수한다는 것을 확실히 모니터링하기 위한 정부 프로그램 평가를 위해 이 정보를 사용하고 있습니다.</v>
+      </c>
+      <c r="D315" t="str" xml:space="preserve">
+        <v xml:space="preserve">Quý vị là người thuộc cộng đồng nói tiếng Tây Ban Nha, La tinh hay gốc Tây Ban Nha?_x000d__x000d_
+_x000d__x000d_
+###### *Câu hỏi này là không bắt buộc. Chúng tôi đang sử dụng thông tin này để đánh giá các chương trình của chính phủ nhằm đảm bảo rằng các chương trình đó phục vụ nhu cầu của tất cả các nhóm chủng tộc và giám sát việc tuân thủ các luật, quy định và chính sách chống phân biệt đối xử. </v>
+      </c>
+      <c r="E315" t="str" xml:space="preserve">
+        <v xml:space="preserve">他们是西班牙裔、拉丁裔还是西班牙裔？_x000d__x000d_
+_x000d__x000d_
+###### *本题为可选题。我们使用这些信息来评估政府的计划，以确保它们公平和公正地满足所有种族群体的需求，并监测对反歧视法律、法规和政策的遵守情况。</v>
+      </c>
+      <c r="F315" t="str" xml:space="preserve">
+        <v xml:space="preserve">¿Es usted de origen hispano, latino o español?_x000d__x000d_
+_x000d__x000d_
+###### *Esta pregunta es opcional. Estamos usando esta información para evaluar programas gubernamentales a fin de garantizar que satisfagan de manera justa y equitativa las necesidades de todos los grupos raciales y para vigilar el cumplimiento de las leyes, normas y políticas contra la discriminación.</v>
       </c>
     </row>
     <row r="316">
@@ -8007,16 +7577,16 @@
         <v>["Yes","No","I prefer not to say."]</v>
       </c>
       <c r="C316" t="str">
-        <v/>
+        <v>["예","아니오","말하고 싶지 않음."]</v>
       </c>
       <c r="D316" t="str">
-        <v/>
+        <v xml:space="preserve">["Có", "Không", "Tôi không muốn nói."] </v>
       </c>
       <c r="E316" t="str">
-        <v/>
+        <v>["是","不是","我不想说。"]</v>
       </c>
       <c r="F316" t="str">
-        <v/>
+        <v>["Sí","No","Prefiero no decirlo."]</v>
       </c>
     </row>
     <row r="317">
@@ -8027,16 +7597,16 @@
         <v>Black or African American</v>
       </c>
       <c r="C317" t="str">
-        <v/>
+        <v>흑인 또는 아프리카계 미국인</v>
       </c>
       <c r="D317" t="str">
-        <v/>
+        <v xml:space="preserve">Người Mỹ da đen hoặc người Mỹ gốc Phi </v>
       </c>
       <c r="E317" t="str">
-        <v/>
+        <v>黑人或非裔美国人</v>
       </c>
       <c r="F317" t="str">
-        <v/>
+        <v>Raza negra o afroamericana</v>
       </c>
     </row>
     <row r="318">
@@ -8047,16 +7617,16 @@
         <v>American Indian or Alaska Native</v>
       </c>
       <c r="C318" t="str">
-        <v/>
+        <v>아메리칸 인디언 또는 알래스카 원주민</v>
       </c>
       <c r="D318" t="str">
-        <v/>
+        <v xml:space="preserve">Người Mỹ da đỏ hoặc thổ dân Alaska </v>
       </c>
       <c r="E318" t="str">
-        <v/>
+        <v>美国印第安人或阿拉斯加原住民</v>
       </c>
       <c r="F318" t="str">
-        <v/>
+        <v>Indoamericana o nativa de Alaska</v>
       </c>
     </row>
     <row r="319">
@@ -8067,16 +7637,16 @@
         <v>Asian</v>
       </c>
       <c r="C319" t="str">
-        <v/>
+        <v>아시아인</v>
       </c>
       <c r="D319" t="str">
-        <v/>
+        <v>Người Châu Á</v>
       </c>
       <c r="E319" t="str">
-        <v/>
+        <v>亚裔</v>
       </c>
       <c r="F319" t="str">
-        <v/>
+        <v>Asiática</v>
       </c>
     </row>
     <row r="320">
@@ -8087,16 +7657,16 @@
         <v>Native Hawaiian or Other Pacific Islander</v>
       </c>
       <c r="C320" t="str">
-        <v/>
+        <v>하와이 원주민 또는 태평양의 섬 주민</v>
       </c>
       <c r="D320" t="str">
-        <v/>
+        <v>Người Hawaii bản địa hoặc Người dân trên đảo Thái Bình Dương khác</v>
       </c>
       <c r="E320" t="str">
-        <v/>
+        <v>夏威夷土著人或其他太平洋岛民</v>
       </c>
       <c r="F320" t="str">
-        <v/>
+        <v>Nativa de Hawái o de otras islas del Pacífico</v>
       </c>
     </row>
     <row r="321">
@@ -8107,16 +7677,16 @@
         <v>I prefer not to say.</v>
       </c>
       <c r="C321" t="str">
-        <v/>
+        <v>말하고 싶지 않음.</v>
       </c>
       <c r="D321" t="str">
-        <v/>
+        <v>Tôi thích không nói ra hơn.</v>
       </c>
       <c r="E321" t="str">
-        <v/>
+        <v>我宁愿不说。</v>
       </c>
       <c r="F321" t="str">
-        <v/>
+        <v>Prefiero no decirlo.</v>
       </c>
     </row>
     <row r="322" xml:space="preserve">
@@ -8124,21 +7694,29 @@
         <v>CDC/second_person_questions/ethnicity_question</v>
       </c>
       <c r="B322" t="str" xml:space="preserve">
-        <v xml:space="preserve">What is your race? (please select all that apply)_x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">What is your race? (please select all that apply)_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
 ###### *This question is optional. We are using this information to evaluate government programs to ensure that they fairly and equitably serve the needs of all racial groups and to monitor compliance with antidiscrimination laws, regulation, and policies.</v>
       </c>
-      <c r="C322" t="str">
-        <v/>
-      </c>
-      <c r="D322" t="str">
-        <v/>
-      </c>
-      <c r="E322" t="str">
-        <v/>
-      </c>
-      <c r="F322" t="str">
-        <v/>
+      <c r="C322" t="str" xml:space="preserve">
+        <v xml:space="preserve">귀하의 인종은 무엇입니까?(해당 사항을 모두 고르십시오)_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
+###### *이 질문은 선택 사항입니다. 정부가 모든 인종 집단의 요구에 공정하고 공평하게 대응하고, 차별금지법과 법규 및 정책을 준수한다는 것을 확실히 모니터링하기 위한 정부 프로그램 평가를 위해 이 정보를 사용하고 있습니다.</v>
+      </c>
+      <c r="D322" t="str" xml:space="preserve">
+        <v xml:space="preserve">Chủng tộc của quý vị là gì? (Vui lòng chọn tất cả các câu trả lời phù hợp)_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
+###### *Câu hỏi này là không bắt buộc. Chúng tôi đang sử dụng thông tin này để đánh giá các chương trình của chính phủ nhằm đảm bảo rằng các chương trình đó phục vụ nhu cầu của tất cả các nhóm chủng tộc và giám sát việc tuân thủ các luật, quy định và chính sách chống phân biệt đối xử. </v>
+      </c>
+      <c r="E322" t="str" xml:space="preserve">
+        <v xml:space="preserve">您的种族是什么？(请选择所有适用的)_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
+###### *本题为可选题。我们使用这些信息来评估政府的计划，以确保它们公平和公正地满足所有种族群体的需求，并监测对反歧视法律、法规和政策的遵守情况。</v>
+      </c>
+      <c r="F322" t="str" xml:space="preserve">
+        <v xml:space="preserve">¿De qué raza es? (Seleccione todo lo que corresponda)_x000d__x000d_
+_x000d__x000d_
+###### *Esta pregunta es opcional. Estamos usando esta información para evaluar programas gubernamentales a fin de garantizar que satisfagan de manera justa y equitativa las necesidades de todos los grupos raciales y para vigilar el cumplimiento de las leyes, normas y políticas contra la discriminación.</v>
       </c>
     </row>
     <row r="323" xml:space="preserve">
@@ -8146,20 +7724,29 @@
         <v>CDC/third_person_questions/ethnicity_question</v>
       </c>
       <c r="B323" t="str" xml:space="preserve">
-        <v xml:space="preserve">What is their race? (please select all that apply)
+        <v xml:space="preserve">What is their race? (please select all that apply)_x000d__x000d_
+_x000d__x000d_
 ###### *This question is optional. We are using this information to evaluate government programs to ensure that they fairly and equitably serve the needs of all racial groups and to monitor compliance with antidiscrimination laws, regulation, and policies.</v>
       </c>
-      <c r="C323" t="str">
-        <v/>
-      </c>
-      <c r="D323" t="str">
-        <v/>
-      </c>
-      <c r="E323" t="str">
-        <v/>
-      </c>
-      <c r="F323" t="str">
-        <v/>
+      <c r="C323" t="str" xml:space="preserve">
+        <v xml:space="preserve">그 사람의 인종은 무엇입니까?(해당 사항을 모두 고르십시오)_x000d__x000d_
+_x000d__x000d_
+###### *이 질문은 선택 사항입니다. 정부가 모든 인종 집단의 요구에 공정하고 공평하게 대응하고, 차별금지법과 법규 및 정책을 준수한다는 것을 확실히 모니터링하기 위한 정부 프로그램 평가를 위해 이 정보를 사용하고 있습니다.</v>
+      </c>
+      <c r="D323" t="str" xml:space="preserve">
+        <v xml:space="preserve">Chủng tộc của họ là gì? (Vui lòng chọn tất cả các câu trả lời phù hợp)_x000d__x000d_
+_x000d__x000d_
+###### *Câu hỏi này là không bắt buộc. Chúng tôi đang sử dụng thông tin này để đánh giá các chương trình của chính phủ nhằm đảm bảo rằng các chương trình đó phục vụ nhu cầu của tất cả các nhóm chủng tộc và giám sát việc tuân thủ các luật, quy định và chính sách chống phân biệt đối xử. </v>
+      </c>
+      <c r="E323" t="str" xml:space="preserve">
+        <v xml:space="preserve">他们的种族是什么？(请选择所有适用的)_x000d__x000d_
+_x000d__x000d_
+###### *本题为可选题。我们使用这些信息来评估政府的计划，以确保它们公平和公正地满足所有种族群体的需求，并监测对反歧视法律、法规和政策的遵守情况。</v>
+      </c>
+      <c r="F323" t="str" xml:space="preserve">
+        <v xml:space="preserve">¿De qué raza es? (Seleccione todo lo que corresponda)_x000d__x000d_
+_x000d__x000d_
+###### *Esta pregunta es opcional. Estamos usando esta información para evaluar programas gubernamentales a fin de garantizar que satisfagan de manera justa y equitativa las necesidades de todos los grupos raciales y para vigilar el cumplimiento de las leyes, normas y políticas contra la discriminación.</v>
       </c>
     </row>
     <row r="324">
@@ -8170,16 +7757,16 @@
         <v>White</v>
       </c>
       <c r="C324" t="str">
-        <v/>
+        <v>백인</v>
       </c>
       <c r="D324" t="str">
-        <v/>
+        <v>Da trắng</v>
       </c>
       <c r="E324" t="str">
-        <v/>
+        <v>白种人</v>
       </c>
       <c r="F324" t="str">
-        <v/>
+        <v>Raza blanca</v>
       </c>
     </row>
     <row r="325">
@@ -8190,16 +7777,16 @@
         <v>Down syndrome or Down’s syndrome</v>
       </c>
       <c r="C325" t="str">
-        <v/>
+        <v>다운증후군</v>
       </c>
       <c r="D325" t="str">
-        <v/>
+        <v>Hội chứng Down</v>
       </c>
       <c r="E325" t="str">
-        <v/>
+        <v>唐氏综合症</v>
       </c>
       <c r="F325" t="str">
-        <v/>
+        <v>Síndrome de Down</v>
       </c>
     </row>
     <row r="326" xml:space="preserve">
@@ -8207,23 +7794,49 @@
         <v>CDC/messages/msg27_addnl</v>
       </c>
       <c r="B326" t="str" xml:space="preserve">
-        <v xml:space="preserve">Please inform your close contacts that they have been potentially exposed to SARS-CoV-2. CDC recommends that all close contacts of people with confirmed or probable COVID-19 should:
-- get tested **and**
-- quarantine for 14 days from the day of their last exposure. You may also receive a call from a contact tracing professional.
- Get rest and stay hydrated. Take over-the-counter medicines, such as acetaminophen, if needed to help you feel better. 
+        <v xml:space="preserve">Please inform your close contacts that they have been potentially exposed to SARS-CoV-2. CDC recommends that all close contacts of people with confirmed or probable COVID-19 should:_x000d__x000d_
+- get tested **and**_x000d__x000d_
+- quarantine for 14 days from the day of their last exposure. You may also receive a call from a contact tracing professional._x000d__x000d_
+_x000d__x000d_
+ Get rest and stay hydrated. Take over-the-counter medicines, such as acetaminophen, if needed to help you feel better. _x000d__x000d_
+_x000d__x000d_
  Separate yourself from other people. As much as possible, stay in a specific room and away from other people and pets in your home.</v>
       </c>
-      <c r="C326" t="str">
-        <v/>
-      </c>
-      <c r="D326" t="str">
-        <v/>
-      </c>
-      <c r="E326" t="str">
-        <v/>
-      </c>
-      <c r="F326" t="str">
-        <v/>
+      <c r="C326" t="str" xml:space="preserve">
+        <v xml:space="preserve">SARS-CoV-2에 노출되었을 수 있는 밀접 접촉자가 있다면 알려주시기 바랍니다. 확진자 또는 COVID-19 가능성이 있는 사람들과 밀접 접촉한 모든 사람이 다음과 같이 할 것을 CDC는 권장합니다._x000d__x000d_
+- 검사를 받으십시오 **그리고**_x000d__x000d_
+- 마지막으로 노출된 날부터 14일 동안 격리하십시오. 또한 추적 전문가의 전화를 받을 수도 있습니다._x000d__x000d_
+_x000d__x000d_
+ 휴식을 취하고 수분을 충분히 보충하십시오. 회복에 도움이 되도록 필요한 경우 아세트아미노펜과 같은 일반의약품을 복용하십시오._x000d__x000d_
+_x000d__x000d_
+ 다른 사람으로부터 분리되어 있으십시오. 가능한 한, 가정 내 특정 공간에 다른 구성원과 반려동물로부터 격리하여 머무르십시오.</v>
+      </c>
+      <c r="D326" t="str" xml:space="preserve">
+        <v xml:space="preserve">Vui lòng thông báo cho những tiếp xúc gần với quý vị rằng họ có khả năng bị nhiễm SARS-CoV-2. CDC khuyến cáo rằng tất cả những người tiếp xúc gần với những người đã được xác nhận mắc hoặc có khả năng mắc COVID-19 nên:_x000d__x000d_
+- xét nghiệm **và**_x000d__x000d_
+- cách ly trong 14 ngày kể từ ngày tiếp xúc cuối cùng của họ. Quý vị cũng có thể nhận được cuộc gọi từ một chuyên gia theo dõi người tiếp xúc._x000d__x000d_
+_x000d__x000d_
+ Nghỉ ngơi và uống đủ nước. Dùng các loại thuốc không cần kê toa, ví dụ như acetaminophen, nếu cần để giúp quý cảm thấy tốt hơn. _x000d__x000d_
+_x000d__x000d_
+ Cách ly quý vị khỏi những người khác. Nên ở một phòng riêng càng nhiều càng tốt và tránh xa những người và vật nuôi khác trong nhà quý vị.</v>
+      </c>
+      <c r="E326" t="str" xml:space="preserve">
+        <v xml:space="preserve">请告知您的密切接触者他们可能接触了 SARS-CoV-2。CDC 建议确诊或疑似 COVID-19（新冠肺炎）的人的密切接触者应该：_x000d__x000d_
+- 接受检测**和**_x000d__x000d_
+- 从最后一次接触之日算起，隔离14天。您也可能会接到专业人员打来的电话。_x000d__x000d_
+_x000d__x000d_
+ 注意休息并保持不要脱水。如果需要帮助您感觉好一些，可使用非处方药，如对乙酰氨基酚。_x000d__x000d_
+_x000d__x000d_
+ 自己远离其他人。尽可能地呆在特定的房间中，并远离家中其他人和宠物。</v>
+      </c>
+      <c r="F326" t="str" xml:space="preserve">
+        <v xml:space="preserve">Infórmeles a sus contactos cercanos que posiblemente han estado espuestos al SARS-CoV-2. Los CDC recomiendan que todos los contactos cercanos de una persona con COVID-19 confirmado o probable:_x000d__x000d_
+- se hagan la prueba **y**_x000d__x000d_
+- se pongan en cuarentena por 14 días desde la fecha de su última exposición. Es posible que también reciba una llamada de un profesional de rastreo de contactos._x000d__x000d_
+_x000d__x000d_
+ Descanse y manténgase hidratado. Tome medicamentos de venta sin receta, como acetaminofeno, si necesita para sentirse mejor. _x000d__x000d_
+_x000d__x000d_
+ Apártese de las otras personas. En la medida de lo posible, permanezca en una habitación específica y lejos de las otras personas y mascotas en su casa.</v>
       </c>
     </row>
     <row r="327" xml:space="preserve">
@@ -8231,32 +7844,89 @@
         <v>CDC/messages/endcap</v>
       </c>
       <c r="B327" t="str" xml:space="preserve">
-        <v xml:space="preserve">## Steps to follow every day: 
-- **Wear** a mask over your nose and mouth.
-- **Stay** at least 6 feet away from people who don’t live with you.
-- **Avoid** crowded areas and poorly ventilated spaces.
-- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol.
-**Click the links below for more information on:**
-- [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)
-- [When to get tested](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)
-- [What your test results mean](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)
-- [Protecting yourself and others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)
-- [When to quarantine or isolate and for how long](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
-- [What to do if you were around someone with COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
-- [Taking care of yourself when you are sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)
+        <v xml:space="preserve">## Steps to follow every day: _x000d__x000d_
+- **Wear** a mask over your nose and mouth._x000d__x000d_
+- **Stay** at least 6 feet away from people who don’t live with you._x000d__x000d_
+- **Avoid** crowded areas and poorly ventilated spaces._x000d__x000d_
+- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d__x000d_
+_x000d__x000d_
+**Click the links below for more information on:**_x000d__x000d_
+- [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d_
+- [When to get tested](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d_
+- [What your test results mean](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d_
+- [Protecting yourself and others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d_
+- [When to quarantine or isolate and for how long](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [What to do if you were around someone with COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [Taking care of yourself when you are sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d_
 - [Taking care of someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
       </c>
-      <c r="C327" t="str">
-        <v/>
-      </c>
-      <c r="D327" t="str">
-        <v/>
-      </c>
-      <c r="E327" t="str">
-        <v/>
-      </c>
-      <c r="F327" t="str">
-        <v/>
+      <c r="C327" t="str" xml:space="preserve">
+        <v xml:space="preserve">## 매일 따라야 할 방법: _x000d__x000d_
+- 코와 입을 가리는 마스크를 **착용하십시오**._x000d__x000d_
+- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**._x000d__x000d_
+- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**._x000d__x000d_
+- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d__x000d_
+_x000d__x000d_
+**자세한 정보를 보려면 아래 링크를 클릭하십시오.**_x000d__x000d_
+- [COVID-19 증상](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d_
+- [검사를 언제 받아야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d_
+- [검사 결과가 의미하는 것](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d_
+- [다른 사람을 질병으로부터 보호하십시오](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d_
+- [언제 그리고 얼마나 오래 격리 또는 분리해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [COVID-19에 걸린 사람 주변에 있었다면 무엇을 해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [아플 때 자신을 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d_
+- [아픈 사람 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
+      </c>
+      <c r="D327" t="str" xml:space="preserve">
+        <v xml:space="preserve">## Các bước cần tuân theo hàng ngày: _x000d_
+- **Đeo** khẩu trang lên mũi và miệng của quý vị._x000d_
+- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet._x000d_
+- **Tránh** những khu vực đông đúc và không gian kém thông thoáng._x000d_
+- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước khử trùng tay có ít nhất 60% cồn._x000d_
+_x000d_
+**Nhấp vào liên kết bên dưới để biết thêm thông tin về:**_x000d_
+-[Các triệu chứng COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)._x000d_
+- [Khi nào cần xét nghiệm](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
+- [Kết quả xét nghiệm của quý vị có ý nghĩa gì](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
+- [Bảo vệ bản thân và những người khác khỏi bị bệnh](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d_
+- [Cách ly hoặc cách ly khi nào và trong bao lâu](https://www.cdc.gov/coroavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [Phải làm gì nếu quý vị ở gần ai đó có COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [Chăm sóc bản thân khi quý vị bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
+- [Chăm sóc người khác bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
+      </c>
+      <c r="E327" t="str" xml:space="preserve">
+        <v xml:space="preserve">## 每天要遵循的步骤：_x000d_
+- **佩戴**口罩遮住您的口鼻。_x000d_
+- 与不和您住在一起的人**保持**至少6英尺的距离。_x000d_
+- **避免**拥挤的地方和通风不良的空间。_x000d_
+- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。_x000d_
+_x000d_
+**点击以下链接了解更多信息：**_x000d_
+-[COVID-19 症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
+- [何时进行检测](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
+- [您的测试结果是什么意思](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
+- [保护自己和他人免于生病](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d_
+- [何时进行检疫隔离或隔离以及隔离多长时间](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [如果您身边的人患有COVID-19，您该怎么办？](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [生病时照顾好自己](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
+- [照顾生病的他人](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
+      </c>
+      <c r="F327" t="str" xml:space="preserve">
+        <v xml:space="preserve">## Medidas para tomar todos los días: _x000d__x000d_
+- **Póngase** una mascarilla que le cubra la nariz y la boca._x000d__x000d_
+- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted._x000d__x000d_
+- **Evite** lugares con mucha gente y áreas con poca ventilación._x000d__x000d_
+- **Lávese** las manos a menudo con agua y jabón o use un desinfectante de manos que contenga al menos un 60 % de alcohol._x000d__x000d_
+_x000d__x000d_
+**Para obtener más información, haga clic en el enlace a continuación:**_x000d__x000d_
+- [Síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d_
+- [Cuándo hacerse la prueba](https://espanol.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html)_x000d__x000d_
+- [Lo que significan los resultados de su prueba](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d_
+- [Cómo protegerse a sí mismo y a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d_
+- [Cuándo ponerse en cuarentena o aislarse y por cuánto tiempo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [Qué hacer si estuvo cerca de alguien con COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [Cómo cuidarse cuando está enfermo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d_
+- [Cómo cuidar a otra persona que está enferma](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
       </c>
     </row>
     <row r="328">
@@ -8267,16 +7937,16 @@
         <v>Additional information</v>
       </c>
       <c r="C328" t="str">
-        <v/>
+        <v>추가 정보</v>
       </c>
       <c r="D328" t="str">
-        <v/>
+        <v>Thông tin thêm</v>
       </c>
       <c r="E328" t="str">
-        <v/>
+        <v>额外信息</v>
       </c>
       <c r="F328" t="str">
-        <v/>
+        <v>Información adicional</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating foreign languages to v68
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -408,16 +408,16 @@
         <v>Nausea or vomiting</v>
       </c>
       <c r="C2" t="str">
-        <v/>
+        <v>메스꺼움 또는 구토</v>
       </c>
       <c r="D2" t="str">
-        <v/>
+        <v>Buồn nôn hoặc nôn</v>
       </c>
       <c r="E2" t="str">
-        <v/>
+        <v>恶心或呕吐</v>
       </c>
       <c r="F2" t="str">
-        <v/>
+        <v>Náuseas o vómitos</v>
       </c>
     </row>
     <row r="3">
@@ -428,16 +428,16 @@
         <v>Diarrhea</v>
       </c>
       <c r="C3" t="str">
-        <v/>
+        <v>설사</v>
       </c>
       <c r="D3" t="str">
-        <v/>
+        <v>Tiêu chảy</v>
       </c>
       <c r="E3" t="str">
-        <v/>
+        <v>腹泻</v>
       </c>
       <c r="F3" t="str">
-        <v/>
+        <v>Diarrea</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
@@ -445,21 +445,29 @@
         <v>CDC/messages/vax-endcap</v>
       </c>
       <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">- [Learn about COVID-19 Vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d__x000d_
-- [How to Protect Yourself and Others When You’ve Been Fully Vaccinated](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d__x000d__x000d_
+        <v xml:space="preserve">- [Learn about COVID-19 Vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [How to Protect Yourself and Others When You’ve Been Fully Vaccinated](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
 - [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)</v>
       </c>
-      <c r="C4" t="str">
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <v/>
-      </c>
-      <c r="E4" t="str">
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <v/>
+      <c r="C4" t="str" xml:space="preserve">
+        <v xml:space="preserve">- [COVID-19 백신 알아보기](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [귀하가 백신 접종을 모두 마친 경우 귀하 자신과 타인을 보호하는 방법](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+- [COVID-19 증상](https://www.cdc.gov/coronavirus/)</v>
+      </c>
+      <c r="D4" t="str" xml:space="preserve">
+        <v xml:space="preserve">- [Tìm hiểu thêm về Vắc-xin ngừa COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [Cách Bảo vệ Bản thân và Những người khác khi Quý vị đã được Tiêm chủng đầy đủ](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+- [Các triệu chứng COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)</v>
+      </c>
+      <c r="E4" t="str" xml:space="preserve">
+        <v xml:space="preserve">- [了解新冠肺炎疫苗](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [当您已完全接种疫苗时，如何保护您自己和他人](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+- [COVID-19 症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)</v>
+      </c>
+      <c r="F4" t="str" xml:space="preserve">
+        <v xml:space="preserve">- [Infórmese sobre las vacunas contra el COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [Cómo protegerse a sí mismo y a los demás cuando usted se ha vacunado completamente](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+- [Síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-A23testing/symptoms.html)</v>
       </c>
     </row>
     <row r="5">
@@ -470,16 +478,16 @@
         <v>**Tell a caregiver in your facility that you are sick and need to see a medical provider as soon as possible.** Stay in your room as much as possible except to get medical care</v>
       </c>
       <c r="C5" t="str">
-        <v/>
+        <v>**귀하가 계시는 시설의 간병인에게 귀하가 아프고 가능한 빨리 의료진을 만나야 한다고 말하십시오.** 의학적 치료를 받는 경우를 제외하고 가급적 방에 머무르십시오</v>
       </c>
       <c r="D5" t="str">
-        <v/>
+        <v>**Báo cho người chăm sóc tại cơ sở của quý vị biết rằng quý vị bị bệnh và cần đến gặp nhà cung cấp dịch vụ y tế sớm nhất có thể.** Ở trong phòng càng nhiều càng tốt ngoại trừ để nhận chăm sóc y tế</v>
       </c>
       <c r="E5" t="str">
-        <v/>
+        <v>**告知您机构的看护者您生病了，需要尽快就医。** 除了就医外，请尽量呆在房间里</v>
       </c>
       <c r="F5" t="str">
-        <v/>
+        <v>**Dígale a un cuidador de su establecimiento que usted está enfermo y que necesita ver a un proveedor de atención médica lo antes posible.** Quédese en su habitación lo más posible, excepto para conseguir atención médica</v>
       </c>
     </row>
     <row r="6">
@@ -490,16 +498,16 @@
         <v>**Call your medical provider, clinician advice line, or telemedicine provider as soon as possible.** You also have medical conditions that may put you at risk of becoming more seriously ill.</v>
       </c>
       <c r="C6" t="str">
-        <v/>
+        <v>**가능한 한 빨리 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오.** 또한 귀하에게는 심각한 질병으로 악화될 수 있는 질환도 있습니다.</v>
       </c>
       <c r="D6" t="str">
-        <v/>
+        <v>**Gọi cho nhà cung cấp dịch vụ y tế, đường dây tư vấn của bác sĩ lâm sàng hoặc nhà cung cấp dịch vụ y tế từ xa càng sớm càng tốt.** Quý vị cũng mắc các bệnh lý có thể khiến quý vị có nguy cơ bị bệnh nặng hơn.</v>
       </c>
       <c r="E6" t="str">
-        <v/>
+        <v>**尽快致电您的医疗服务提供者、临床医生咨询热线或远程医疗服务提供者**。您的身体状况也可能会让您面临更严重的疾病风险。</v>
       </c>
       <c r="F6" t="str">
-        <v/>
+        <v>**Llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina lo más pronto posible.** También tiene afecciones que podrían ponerlo en un mayor riesgo de enfermarse gravemente.</v>
       </c>
     </row>
     <row r="7">
@@ -510,16 +518,16 @@
         <v>**Tell the occupational health provider (or supervisor) in your workplace that you’re feeling sick as soon as possible.**</v>
       </c>
       <c r="C7" t="str">
-        <v/>
+        <v>**가능한 한 빨리 직장의 산업 보건 담당자(또는 직장상사)에게 귀하가 아프다고 말하십시오.**</v>
       </c>
       <c r="D7" t="str">
-        <v/>
+        <v>**Nói với nhà cung cấp dịch vụ sức khỏe nghề nghiệp (hoặc quản lý trực tiếp) ở nơi làm việc của quý vị càng sớm càng tốt rằng quý vị cảm thấy bị bệnh.**</v>
       </c>
       <c r="E7" t="str">
-        <v/>
+        <v>**尽快告知工作场所的职业保健提供者（或主管），您感觉不适。**</v>
       </c>
       <c r="F7" t="str">
-        <v/>
+        <v>**Dígale al proveedor de salud ocupacional (o supervisor) de su lugar de trabajo que se siente mal lo más pronto posible.**</v>
       </c>
     </row>
     <row r="8" xml:space="preserve">
@@ -530,17 +538,23 @@
         <v xml:space="preserve">**Regardless of vaccination status, if you have been in close contact of another person who has tested positive for COVID-19 in the last 14 days, you should quarantine for 14 days from the day of your last exposure.**_x000d__x000d__x000d__x000d_
 Check your local health department’s website for information about options in your area to possibly shorten this quarantine period.  You may also receive a call from a contact tracing professional.</v>
       </c>
-      <c r="C8" t="str">
-        <v/>
-      </c>
-      <c r="D8" t="str">
-        <v/>
-      </c>
-      <c r="E8" t="str">
-        <v/>
-      </c>
-      <c r="F8" t="str">
-        <v/>
+      <c r="C8" t="str" xml:space="preserve">
+        <v xml:space="preserve">**백신 접종 여부와 관계 없이, COVID-19 양성 판정을 받은 사람과 지난 14일 이내에 밀접 접촉자로 판명되면 귀하는 그 후 14일 동안 자가격리해야 합니다.** _x000d_
+거주 지역의 보건부 웹사이트에서 격리 기간 단축 가능여부를 확인하시기 바랍니다. 또한 역학 조사관의 전화를 받을 수도 있습니다.</v>
+      </c>
+      <c r="D8" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Bất kể tình trạng tiêm chủng là gì, nếu quý vị đã tiếp xúc gần với một người có kết quả xét nghiệm dương tính với COVID-19 trong 14 ngày qua, quý vị nên cách ly trong 14 ngày kể từ ngày tiếp xúc cuối cùng.**_x000d_
+Kiểm tra trang web của sở y tế địa phương của quý vị để biết thông tin về các lựa chọn trong khu vực của quý vị để có thể rút ngắn thời gian cách ly này.  Quý vị cũng có thể nhận được cuộc gọi từ một nhân viên phụ trách theo dõi người tiếp xúc.</v>
+      </c>
+      <c r="E8" t="str" xml:space="preserve">
+        <v xml:space="preserve">**无论您疫苗接种的状态如何，如果您在过去 14 天内与其他新冠肺炎检测呈阳性的人员有过密切接触，您应从您最后一次暴露之日起隔离 14 天。**_x000d_
+_x000d_
+查看当地卫生部门的网站，了解您所在地区可能缩短隔离期的选择。您也可能会接到专业人员打来的电话。</v>
+      </c>
+      <c r="F8" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Independientemente de que esté vacunado o no, si ha estado en contacto cercano con otra persona que dio positivo en la prueba del COVID-19 en los últimos 14 días, usted debería ponerse en cuarentena por 14 días desde el día de su última exposición.**_x000d_
+_x000d_
+Consulte el sitio web de su departamento de salud local para obtener información sobre las opciones en su área para posiblemente acortar este periodo de cuarentena.  Es posible que también reciba una llamada de un profesional encargado del rastreo de contactos.</v>
       </c>
     </row>
     <row r="9" xml:space="preserve">
@@ -548,24 +562,54 @@
         <v>CDC/messages/msg304</v>
       </c>
       <c r="B9" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing for 14 days following an exposure.**_x000d__x000d__x000d__x000d_
-If you develop any symptoms, get tested for SARS-CoV-2, and stay home and away from others until:_x000d__x000d__x000d__x000d_
-- it has been 10 days from when your symptoms first appeared and _x000d__x000d__x000d__x000d_
-- you have had no fever for 24 hours without the use of medications and _x000d__x000d__x000d__x000d_
-- your other symptoms of COVID-19 are improving* _x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing for 14 days following an exposure.**_x000d_
+_x000d_
+If you develop any symptoms, get tested for SARS-CoV-2, and stay home and away from others until:_x000d_
+- it has been 10 days from when your symptoms first appeared and _x000d_
+- you have had no fever for 24 hours without the use of medications and _x000d_
+- your other symptoms of COVID-19 are improving* _x000d_
+_x000d_
 (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)</v>
       </c>
-      <c r="C9" t="str">
-        <v/>
-      </c>
-      <c r="D9" t="str">
-        <v/>
-      </c>
-      <c r="E9" t="str">
-        <v/>
-      </c>
-      <c r="F9" t="str">
-        <v/>
+      <c r="C9" t="str" xml:space="preserve">
+        <v xml:space="preserve">**바이러스에 노출된 후 14일 동안 발열, 기침 또는 호흡 곤란과 같은 COVID-19 증상이 있는지 주의하십시오.** _x000d_
+_x000d_
+귀하에게 해당 증상이 발생하는 경우, SARS-CoV-2 검사를 받고, 다음의 조건이 채워질 때까지 자택에 머물며 타인과의 접촉을 피하십시오 _x000d_
+- 첫 증상 발현 후 10일 이후 그리고  _x000d_
+- 해열제 사용 없이 24시간 동안 발열이 없었음, 그리고  _x000d_
+- COVID-19의 기타 증상들이 호전되고 있음*  _x000d_
+_x000d_
+(*회복 후에 미각 및 후각의 상실이 수 주 또는 수 개월 동안 지속될 수 있으나 그로 인해 격리 종료 일자를 늦출 필요 없음)</v>
+      </c>
+      <c r="D9" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Theo dõi các triệu chứng COVID-19 như sốt, ho hoặc khó thở trong 14 ngày sau khi tiếp xúc.**_x000d_
+_x000d_
+Nếu quý vị xuất hiện bất kỳ triệu chứng nào, hãy đi xét nghiệm SARS-CoV-2, ở nhà và tránh xa những người khác cho đến khi:_x000d_
+- đã qua 10 ngày từ khi quý vị xuất hiện các triệu chứng đầu tiên và _x000d_
+- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc và _x000d_
+- các triệu chứng COVID-19 khác của quý vị đang được cải thiện* _x000d_
+_x000d_
+(*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)</v>
+      </c>
+      <c r="E9" t="str" xml:space="preserve">
+        <v xml:space="preserve">**留意新冠肺炎的症状，如发热、咳嗽或呼吸困难，直至暴露后 14 天。**_x000d_
+_x000d_
+如果您出现任何症状，进行 SARS-CoV-2 检测，并呆在家中远离他人，直至：_x000d_
+- 距离您的症状首次出现已经 10 天并且_x000d_
+- 在没有使用药物的情况下，24 小时内没有发烧并且_x000d_
+- 您的其他新冠肺炎症状正在改善*_x000d_
+_x000d_
+(*恢复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）</v>
+      </c>
+      <c r="F9" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Esté atento a síntomas de COVID-19 como fiebre, tos o dificultad para respirar por los 14 días siguientes a una exposición.**_x000d_
+_x000d_
+Si presenta algún síntoma, hágase la prueba del SARS-CoV-2, y quédese en casa y lejos de los demás hasta que:_x000d_
+- hayan pasado 10 días desde el inicio de los síntomas y_x000d_
+- 24 horas sin fiebre sin usar medicamentos para reducirla y_x000d_
+- sus otros síntomas de COVID-19 estén mejorando*_x000d_
+_x000d_
+(*la pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)</v>
       </c>
     </row>
     <row r="10">
@@ -576,16 +620,16 @@
         <v>**Tell a caregiver in your facility that you may have been in close contact with another person who has tested positive for COVID-19 in the last 14 days.**</v>
       </c>
       <c r="C10" t="str">
-        <v/>
+        <v>**입원 중인 시설의 간병인에게 지난 14일 동안 COVID-19에 양성 판정을 받은 사람과 밀접하게 접촉했을 수 있다고 알리십시오.**</v>
       </c>
       <c r="D10" t="str">
-        <v/>
+        <v>**Cho người chăm sóc tại cơ sở của quý vị biết rằng quý vị có thể đã tiếp xúc gần với một người khác có kết quả xét nghiệm dương tính với COVID-19 trong 14 ngày qua.**</v>
       </c>
       <c r="E10" t="str">
-        <v/>
+        <v>**告知您所在机构的看护者，您可能与过去 14 天内 COVID-19 检测呈阳性的其他人有密切接触。**</v>
       </c>
       <c r="F10" t="str">
-        <v/>
+        <v>**Dígale a un cuidador de su establecimiento que usted pudo haber estado en contacto cercano con otra persona que dio positivo en la prueba de COVID-19 en los últimos 14 días.**</v>
       </c>
     </row>
     <row r="11" xml:space="preserve">
@@ -593,23 +637,57 @@
         <v>CDC/messages/t200</v>
       </c>
       <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Although the risk of being infected with the virus that causes COVID-19 is low if you are fully vaccinated, you should get tested and stay home and away from others, except to get medical care, until:**_x000d__x000d__x000d__x000d_
--  it has been 10 days* from when your symptoms first appeared and _x000d__x000d__x000d__x000d_
--  you have had no fever for 24 hours without the use of medications and _x000d__x000d__x000d__x000d_
--  your other symptoms of COVID-19 are improving* (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)_x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Although the risk of being infected with the virus that causes COVID-19 is low if you are fully vaccinated, you should get tested and stay home and away from others, except to get medical care, until:**_x000d_
+_x000d_
+-  it has been 10 days* from when your symptoms first appeared and _x000d_
+_x000d_
+-  you have had no fever for 24 hours without the use of medications and _x000d_
+_x000d_
+-  your other symptoms of COVID-19 are improving* _x000d_
+_x000d_
+(*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)_x000d_
+_x000d_
 *If you have a weakened immune system (immunocompromised) due to a health condition or medication, you might need to stay home and isolate longer than 10 days and possibly 20 days after symptoms begin. In some circumstances, further testing may be needed. Talk to your healthcare provider for more information.</v>
       </c>
-      <c r="C11" t="str">
-        <v/>
-      </c>
-      <c r="D11" t="str">
-        <v/>
-      </c>
-      <c r="E11" t="str">
-        <v/>
-      </c>
-      <c r="F11" t="str">
-        <v/>
+      <c r="C11" t="str" xml:space="preserve">
+        <v xml:space="preserve">**귀하가 백신 접종을 모두 마친 경우 COVID-19를 유발하는 바이러스에 감염되었을 위험성은 낮지만 귀하는 검사를 받아야 하며, 의학적 치료를 받을 때를 제외하고 다음의 조건이 채워질 때까지 자택에 머물며 타인과의 접촉을 피하십시오.** _x000d_
+- 첫 증상 발현 후 10일* 이후 그리고  _x000d_
+- 해열제 사용 없이 24시간 동안 발열이 없었음 그리고  _x000d_
+- COVID-19의 기타 증상이 호전되고 있음*_x000d_
+_x000d_
+(*회복 후에 미각 및 후각의 상실이 수 주 또는 수 개월 동안 지속될 수 있으나 그로인해 격리 종료 일자를 늦출 필요 없음)  _x000d_
+_x000d_
+*건강 상태 또는 약물로 인해 귀하의 면역체계가 약해진 경우(면역저하), 귀하는 증상이 시작된 후 자택에 머물며 10일 이상, 아마도 20일 동안의 격리가 필요할 수 있습니다. 일부 상황에서, 추가 검사가 필요할 수 있습니다. 더 자세한 정보는 담당 의료 서비스 제공자에게 문의하십시오.</v>
+      </c>
+      <c r="D11" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Mặc dù nguy cơ bị nhiễm vi-rút gây ra COVID-19 là thấp nếu quý vị đã được tiêm chủng đầy đủ, quý vị vẫn nên đi xét nghiệm, ở nhà và tránh xa những người khác, trừ khi được chăm sóc y tế, cho đến khi:**_x000d_
+- đã qua 10 ngày* từ khi quý vị xuất hiện các triệu chứng đầu tiên và _x000d_
+- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc và _x000d_
+- các triệu chứng COVID-19 khác của quý vị đang được cải thiện*_x000d_
+_x000d_
+(*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)_x000d_
+_x000d_
+*Nếu quý vị bị suy yếu hệ thống miễn dịch (suy giảm miễn dịch) do tình trạng sức khỏe hoặc do thuốc, quý vị có thể cần phải ở nhà và cách ly lâu hơn 10 ngày và có thể là 20 ngày sau khi các triệu chứng khởi phát. Trong một số trường hợp, có thể cần xét nghiệm thêm. Nói chuyện với nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị để biết thêm thông tin.</v>
+      </c>
+      <c r="E11" t="str" xml:space="preserve">
+        <v xml:space="preserve">**尽管完全接种疫苗后您感染新冠肺炎的风险很低，但您仍应该接受检测并呆在家里远离他人，除非需要去看医生，直至：**_x000d_
+- 距离您的症状首次出现已经 10 天并且_x000d_
+- 在没有使用药物的情况下，24 小时内没有发烧并且_x000d_
+- 您的新冠肺炎的其他症状正在改善*_x000d_
+_x000d_
+(*康复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）_x000d_
+_x000d_
+*如果您由于健康状况或药物导致免疫系统减弱（免疫功能低下），您可能需要留在家中隔离 10 天以上，且可能持续到在症状开始后 20 天。在某些情况下，可能需要进一步测试。更多信息请咨询您的医疗保健提供者。</v>
+      </c>
+      <c r="F11" t="str" xml:space="preserve">
+        <v xml:space="preserve">**A pesar de que el riesgo de estar infectado con el virus que causa el COVID-19 es bajo si usted está vacunado completamente, debería hacerse la prueba y quedarse en casa y lejos de los demás, excepto para conseguir atención médica, hasta que:**_x000d_
+- hayan pasado 10 días* desde el inicio de los síntomas y_x000d_
+- 24 horas sin fiebre, sin usar medicamentos para reducirla y_x000d_
+- sus otros síntomas del COVID-19 estén mejorando*_x000d_
+_x000d_
+(*La pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)_x000d_
+_x000d_
+*Si tiene el sistema inmunitario debilitado (inmunodeprimido) debido a una afección o a medicamentos, podría tener que quedarse en casa y aislado por más de 10 días y, posiblemente, 20 días después del inicio de los síntomas. En algunas circunstancias, puede que sean necesarias más pruebas. Hable con su proveedor de atención médica para obtener más información.</v>
       </c>
     </row>
     <row r="12">
@@ -620,16 +698,16 @@
         <v>**If you continue to have no COVID-19 symptoms, you do not need to quarantine or get tested unless recommended or required by your healthcare provider, employer, or public health official.**</v>
       </c>
       <c r="C12" t="str">
-        <v/>
+        <v>**귀하에게 더이상의 COVID-19 증상이 없는 경우, 귀하의 의료 서비스 제공자, 고용주, 또는 공중 보건 당국이 권고하거나 요구하지 않는 한 자가격리 또는 검사를 받을 필요가 없습니다.**</v>
       </c>
       <c r="D12" t="str">
-        <v/>
+        <v>**Nếu quý vị tiếp tục không có triệu chứng COVID-19, quý vị không cần phải cách ly hoặc đi xét nghiệm trừ khi được khuyến cáo hoặc yêu cầu bởi nhà cung cấp dịch vụ chăm sóc sức khỏe, chủ lao động hoặc quan chức y tế công cộng của quý vị.**</v>
       </c>
       <c r="E12" t="str">
-        <v/>
+        <v>**如果您继续没有新冠肺炎症状，您不需要接受检疫或检测，除非您的医疗保健提供者、雇主或公共卫生官员推荐或要求这样做。**</v>
       </c>
       <c r="F12" t="str">
-        <v/>
+        <v>**Si sigue sin síntomas de COVID-19, no necesita ponerse en cuarentena ni hacerse la prueba a menos que se lo recomiende o exija su proveedor de atención médica, empleador o funcionario de salud pública.**</v>
       </c>
     </row>
     <row r="13">
@@ -640,16 +718,16 @@
         <v>**Based on the answers given, you do not need to quarantine or get tested unless recommended or required by your healthcare provider, employer, or public health official.**</v>
       </c>
       <c r="C13" t="str">
-        <v/>
+        <v>**귀하가 제공한 답변에 따르면, 귀하는 귀하의 의료 서비스 제공자, 고용주, 또는 공중 보건 당국이 권고하거나 요구하지 않는 한 자가격리 또는 검사를 받을 필요가 없습니다.**</v>
       </c>
       <c r="D13" t="str">
-        <v/>
+        <v>**Dựa trên các câu trả lời được đưa ra, quý vị không cần phải cách ly hoặc làm xét nghiệm, trừ khi được khuyến cáo hoặc yêu cầu bởi nhà cung cấp dịch vụ y tế, chủ lao động hoặc quan chức y tế công cộng của quý vị.**</v>
       </c>
       <c r="E13" t="str">
-        <v/>
+        <v>**根据您所提供的答案，您不需要接受隔离或检测，除非您的医疗保健提供者、雇主或公共卫生官员推荐或要求这样做。**</v>
       </c>
       <c r="F13" t="str">
-        <v/>
+        <v>**Según las respuestas que nos ha dado, no necesita ponerse en cuarentena ni hacerse la prueba a menos que se lo recomiende o exija su proveedor de atención médica, empleador o funcionario de salud pública.**</v>
       </c>
     </row>
     <row r="14">
@@ -660,16 +738,16 @@
         <v>Are you fully vaccinated against COVID-19? (You are considered fully vaccinated 2 weeks after your second dose in a two-shot series like Pfizer or Moderna vaccines, or 2 weeks after a single-dose vaccine such as Janssen (Johnson &amp; Johnson) vaccine.)</v>
       </c>
       <c r="C14" t="str">
-        <v/>
+        <v>귀하는 COVID-19에 대하여 백신 접종을 모두 마쳤습니까? (2회 접종이 필요한 화이자 또는 모더나 백신의 2차 접종 2주 후, 또는 1회 접종이 필요한 얀센 (존슨앤존슨) 백신의 1차 접종 2주 후 귀하는 백신 접종을 모두 마친 것으로 간주됩니다.)</v>
       </c>
       <c r="D14" t="str">
-        <v/>
+        <v>Quý vị đã được tiêm phòng COVID-19 đầy đủ chưa? (Quý vị được coi là đã tiêm phòng đầy đủ sau 2 tuần tiêm liều thứ hai đối với loại vắc-xin hai mũi như vắc-xin Pfizer hoặc Moderna, hoặc 2 tuần sau khi tiêm vắc-xin một liều như vắc-xin Janssen (Johnson &amp; Johnson).)</v>
       </c>
       <c r="E14" t="str">
-        <v/>
+        <v>您是否完全接种了新冠肺炎疫苗？ （如果您在接种两针系列疫苗（如 Pfizer 疫苗或 Moderna 疫苗）第二剂后 2 周，或接种单剂疫苗（如 Janssen (Johnson &amp; Johnson) 疫苗）后 2 周，则认为您已完全接种疫苗。）</v>
       </c>
       <c r="F14" t="str">
-        <v/>
+        <v>¿Está completamente vacunado contra el COVID-19? (Usted se considera completamente vacunado dos semanas después de ponerse la segunda dosis de una serie de dos dosis, como es el caso de las vacunas de Pfizer o Moderna; o dos semanas después de ponerse una vacuna de una dosis única, como la Janssen (de Johnson &amp; Johnson).</v>
       </c>
     </row>
     <row r="15" xml:space="preserve">
@@ -677,24 +755,44 @@
         <v>CDC/messages/msg217</v>
       </c>
       <c r="B15" t="str" xml:space="preserve">
-        <v xml:space="preserve">**If you tested negative after being exposed to a person with COVID-19, you are likely not infected, but you still may get sick. Self-quarantine at home for 14 days after your exposure. Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing.** _x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
-If you develop any symptoms, get tested for the virus that causes COVID-19, and stay home and away from others until:_x000d__x000d__x000d__x000d_
-- it has been 10 days from when your symptoms first appeared and _x000d__x000d__x000d__x000d_
-- you have had no fever for 24 hours without the use of medications and _x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**If you tested negative after being exposed to a person with COVID-19, you are likely not infected, but you still may get sick. Self-quarantine at home for 14 days after your exposure. Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing.** _x000d_
+_x000d_
+If you develop any symptoms, get tested for the virus that causes COVID-19, and stay home and away from others until:_x000d_
+- it has been 10 days from when your symptoms first appeared and _x000d_
+- you have had no fever for 24 hours without the use of medications and _x000d_
 - your other symptoms of COVID-19 are improving* (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)</v>
       </c>
-      <c r="C15" t="str">
-        <v/>
-      </c>
-      <c r="D15" t="str">
-        <v/>
-      </c>
-      <c r="E15" t="str">
-        <v/>
-      </c>
-      <c r="F15" t="str">
-        <v/>
+      <c r="C15" t="str" xml:space="preserve">
+        <v xml:space="preserve">**귀하가 COVID-19 환자에 노출된 후 검사 결과가 음성인 경우 귀하가 감염되었을 가능성은 낮으나, 나중에 양성이 될 가능성은 여전히 있습니다. 노출 이후 14일 동안 자택에서 자가 격리 하십시오. 발열, 기침 또는 호흡 곤란과 같은 COVID-19 증상이 나타나는지 잘 살피십시오. ** _x000d_
+_x000d_
+귀하에게 일체의 증상이 발생하는 경우, COVID-19를 유발하는 바이러스에 대하여 검사를 받고, 다음의 조건이 충족될 때까지 자택에 머물며 타인과의 접촉을 피합니다._x000d_
+- 첫 증상 발현 후 10일 이후 그리고 _x000d_
+- 약 사용 없이 24시간 동안 발열이 없음, 그리고 _x000d_
+- COVID-19의 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦출 필요 없음)</v>
+      </c>
+      <c r="D15" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Nếu quý vị có kết quả xét nghiệm âm tính sau khi tiếp xúc với một người mắc COVID-19, quý vị có khả năng không bị nhiễm bệnh, nhưng quý vị vẫn có thể bị ốm. Tự cách ly tại nhà trong 14 ngày sau khi quý vị có tiếp xúc. Theo dõi các triệu chứng COVID-19 như sốt, ho hoặc khó thở.** _x000d_
+_x000d_
+Nếu quý vị xuất hiện bất kỳ triệu chứng nào, hãy đi xét nghiệm vi-rút gây ra COVID-19, ở nhà và tránh xa những người khác cho đến khi:_x000d_
+- đã qua 10 ngày từ khi quý vị xuất hiện các triệu chứng đầu tiên và _x000d_
+- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc và _x000d_
+- các triệu chứng COVID-19 khác của quý vị đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)</v>
+      </c>
+      <c r="E15" t="str" xml:space="preserve">
+        <v xml:space="preserve">**如果您在与新冠肺炎患者接触后检测呈阴性，则您可能没有被感染，但您仍有患病的可能。暴露后在家中自我隔离 14 天。留意新冠肺炎的症状，如发热、咳嗽或呼吸困难。**_x000d_
+_x000d_
+如果您出现任何症状，请接受引起新冠肺炎的病毒检测，并呆在家中远离他人，直至：_x000d_
+- 距离您的症状首次出现已经 10 天并且_x000d_
+- 在没有使用药物的情况下，已24 小时没有发烧并且_x000d_
+- 您的新冠肺炎的其他症状正在改善*（*康复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）</v>
+      </c>
+      <c r="F15" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Si dio positivo en la prueba después de haber estado expuesto a una persona con COVID-19, es probable que no esté infectado, pero aun se podría enfermar. Póngase en cuarentena en casa por 14 días después de su exposición. Esté atento a síntomas del COVID-19 como fiebre, tos o dificultad para respirar.** _x000d_
+_x000d_
+Si presenta algún síntoma, contacte a su proveedor de atención médica para preguntarle acerca de volver a hacerse la prueba, y quédese en casa y lejos de los demás hasta que:_x000d_
+- hayan pasado 10 días desde el inicio de los síntomas **y**_x000d_
+- 24 horas sin fiebre sin usar medicamentos para reducirla **y**_x000d_
+- otros síntomas del COVID-19 estén mejorando* (*la pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)</v>
       </c>
     </row>
     <row r="16">
@@ -705,16 +803,16 @@
         <v>**Please note:** Check your local health department’s website for information about options in your area to possibly shorten this quarantine period.  You may also receive a call from a contact tracing professional.</v>
       </c>
       <c r="C16" t="str">
-        <v/>
+        <v>**주의하십시오.** 이러한 격리 기간 단축 요건에 대한 정보는 해당 지역의 보건부 웹사이트에서 확인하시기 바랍니다. 또한 역학 조사관의 전화를 받을 수도 있습니다.</v>
       </c>
       <c r="D16" t="str">
-        <v/>
+        <v>**Xin lưu ý:** Kiểm tra trang web của sở y tế địa phương của quý vị để biết thông tin về các lựa chọn để có thể rút ngắn thời gian cách ly.  Quý vị cũng có thể nhận được cuộc gọi từ một nhân viên phụ trách theo dõi người tiếp xúc.</v>
       </c>
       <c r="E16" t="str">
-        <v/>
+        <v>**请注意：** 查看当地卫生部门的网站，了解您所在地区可能缩短隔离期的选择。您也可能会接到接触者追踪专业人员打来的电话。</v>
       </c>
       <c r="F16" t="str">
-        <v/>
+        <v>**Por favor, tenga en cuenta:** Consulte el sitio web de su departamento de salud local para obtener información sobre las opciones en su área para posiblemente acortar este periodo de cuarentena.  Es posible que también reciba una llamada de un profesional encargado del rastreo de contactos.</v>
       </c>
     </row>
     <row r="17">
@@ -1546,13 +1644,13 @@
         <v>Pregnant or recently pregnant (for at least 42 days following end of pregnancy)</v>
       </c>
       <c r="C58" t="str">
-        <v>임신 및 최근 임신(임신 종료 이후 최소 42일 간)</v>
+        <v>임신 또는 최근 임신(임신 종료 이후 최소 42일 간)</v>
       </c>
       <c r="D58" t="str">
-        <v>Mang thai và mới mang thai (ít nhất 42 ngày sau khi kết thúc thai kỳ)</v>
+        <v>Đang mang thai hoặc đã mang thai gần đây (cách ít nhất 42 ngày kể từ sau khi kết thúc thai kỳ)</v>
       </c>
       <c r="E58" t="str">
-        <v>怀孕及刚怀孕（妊娠结束后至少 42 天内）</v>
+        <v>怀孕或刚怀孕（妊娠结束后至少 42 天内）</v>
       </c>
       <c r="F58" t="str">
         <v>Está embarazada o estuvo embarazada recientemente (por al menos 42 días después del final del embarazo)</v>
@@ -1846,16 +1944,16 @@
         <v>Mild or moderate difficulty breathing (breathing slightly faster than normal, feeling like you can’t inhale or exhale, or wheezing, especially during exhaling or breathing out)</v>
       </c>
       <c r="C73" t="str">
-        <v>가벼운 또는 중등도의 호흡 곤란</v>
+        <v>경증 또는 중등증의 호흡 곤란(평소보다 조금 빠른 호흡, 숨을 들이쉬거나 내쉴 수 없는 것 같은 느낌, 또는 쌕쌕거림, 특히 숨을 내쉬거나 뱉는 동안)</v>
       </c>
       <c r="D73" t="str">
-        <v>Khó thở nhẹ hoặc trung bình</v>
+        <v>Khó thở ở mức độ nhẹ hoặc trung bình (thở nhanh hơn bình thường một chút, cảm giác như quý vị không thể hít vào hoặc thở ra, hoặc thở khò khè, đặc biệt là khi thở ra)</v>
       </c>
       <c r="E73" t="str">
-        <v>轻度或中度呼吸困难</v>
+        <v>轻度或中度呼吸困难（呼吸略快于正常，感觉无法吸气或呼气，或气喘，尤其是在呼气时）</v>
       </c>
       <c r="F73" t="str">
-        <v>Dificultad leve o moderada para respirar</v>
+        <v>Dificultad leve o moderada para respirar (respirar un poco más rápido de lo normal, sentir como que no puede inhalar o exhalar, o producir sibilancias, especialmente durante la exhalación del aire)</v>
       </c>
     </row>
     <row r="74">
@@ -1866,16 +1964,16 @@
         <v>Mild or moderate difficulty breathing (breathing slightly faster than normal, feeling like you can’t inhale or exhale, or wheezing, especially during exhaling or breathing out)</v>
       </c>
       <c r="C74" t="str">
-        <v>경증 또는 중등도의 호흡곤란(정상보다 약간 빠르게 호흡, 호흡을 돕기 위해 가슴 주위에 다른 근육 사용)</v>
+        <v>경증 또는 중등증의 호흡 곤란(평소보다 조금 빠른 호흡, 숨을 들이쉬거나 내쉴 수 없는 것 같은 느낌, 또는 쌕쌕거림, 특히 숨을 내쉬거나 뱉는 동안)</v>
       </c>
       <c r="D74" t="str">
-        <v>Khó thở nhẹ hoặc vừa (thở hơi gấp hơn bình thường, phải dùng nhiều cơ quanh ngực hơn để trợ thở)</v>
+        <v>Khó thở ở mức độ nhẹ hoặc trung bình (thở nhanh hơn bình thường một chút, cảm giác như quý vị không thể hít vào hoặc thở ra, hoặc thở khò khè, đặc biệt là khi thở ra)</v>
       </c>
       <c r="E74" t="str">
-        <v>轻度或中度呼吸困难（呼吸略快于正常，使用胸部周围额外的肌肉帮助呼吸）</v>
+        <v>轻度或中度呼吸困难（呼吸略快于正常，感觉无法吸气或呼气，或气喘，尤其是在呼气时）</v>
       </c>
       <c r="F74" t="str">
-        <v>Dificultad leve o moderada para respirar (respirar un poco más rápido de lo normal, usando músculos adicionales en el pecho como ayuda)</v>
+        <v>Dificultad leve o moderada para respirar (respirar un poco más rápido de lo normal, sentir como que no puede inhalar o exhalar, o producir sibilancias, especialmente durante la exhalación del aire)</v>
       </c>
     </row>
     <row r="75">
@@ -2063,23 +2161,23 @@
         <v>CDC/covid_testing_response</v>
       </c>
       <c r="B84" t="str" xml:space="preserve">
-        <v xml:space="preserve">["I have been tested in the last 10 days, and my result was positive.", "I have been tested in the last 10 days, and my result was negative.", "I have been tested in the last 10 days, and I am waiting for my results.",_x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">["I have been tested in the last 10 days, and my result was positive.", "I have been tested in the last 10 days, and my result was negative.", "I have been tested in the last 10 days, and I am waiting for my results.",_x000d__x000d__x000d__x000d__x000d_
  "I have not been tested.", "I have been tested, but it has been more than 10 days since my last test."]</v>
       </c>
       <c r="C84" t="str">
         <v>["네, 검사 결과 양성입니다", "아니요, 검사 결과 음성입니다", "결과를 기다리고 있습니다", "검사하지 않았습니다", "검사를 받은 적이 있지만, 마지막으로 검사를 받은 지 10일이 지났습니다."]</v>
       </c>
       <c r="D84" t="str" xml:space="preserve">
-        <v xml:space="preserve">["Tôi đã được xét nghiệm trong 10 ngày qua, và kết quả của tôi là dương tính.", "Tôi đã được xét nghiệm trong 10 ngày qua và kết quả của tôi là âm tính.", "Tôi đã được xét nghiệm trong 10 ngày qua, và tôi đang đợi kết quả của mình.", _x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">["Tôi đã được xét nghiệm trong 10 ngày qua, và kết quả của tôi là dương tính.", "Tôi đã được xét nghiệm trong 10 ngày qua và kết quả của tôi là âm tính.", "Tôi đã được xét nghiệm trong 10 ngày qua, và tôi đang đợi kết quả của mình.", _x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
 "Tôi đã không được xét nghiệm trong 10 ngày qua.", "Tôi đã được xét nghiệm, nhưng đã hơn 10 ngày kể từ lần xét nghiệm cuối cùng của tôi."]</v>
       </c>
       <c r="E84" t="str">
         <v>["我在过去 10 天接受过检测，结果为阳性。","我在过去 10 天接受过检测，结果为阴性。","我在过去 10 天接受过检测，我正在等待检查结果。","我在过去 10 天内没有接受过检测。","我接受过检测，但距离上一次检测已经超过 10 天。"]</v>
       </c>
       <c r="F84" t="str" xml:space="preserve">
-        <v xml:space="preserve">["Me hice Ia prueba en los últimos 10 días y mi resultado fue positivo"., "Me hice Ia prueba en los últimos 10 días y mi resultado fue negativo"., "Me hice Ia prueba en los últimos 10 días y estoy esperando los resultados"., _x000d__x000d__x000d_
-"No me he hecho Ia prueba en los últimos 10 días"., "Me he hecho la prueba, pero han pasado más de 10 días desde mi última prueba".]</v>
+        <v xml:space="preserve">["Me hice Ia prueba en los últimos 10 días y mi resultado fue positivo", "Me hice Ia prueba en los últimos 10 días y mi resultado fue negativo", "Me hice Ia prueba en los últimos 10 días y estoy esperando los resultados", _x000d_
+"No me he hecho Ia prueba en los últimos 10 días", "Me he hecho la prueba, pero han pasado más de 10 días desde mi última prueba"]</v>
       </c>
     </row>
     <row r="85">
@@ -3612,101 +3710,49 @@
         <v>CDC/messages/disclaimer_msg</v>
       </c>
       <c r="B159" t="str" xml:space="preserve">
-        <v xml:space="preserve">The purpose of the Coronavirus Self-Checker is to help you make decisions about seeking appropriate medical care. This system is not intended for the diagnosis or treatment of disease, including COVID-19. _x000d__x000d__x000d_
-_x000d__x000d__x000d_
-This project was made possible through a partnership with the CDC Foundation and is enabled by Microsoft’s Azure platform. CDC’s collaboration with a non-federal organization does not imply an endorsement of any one particular service, product, or enterprise. _x000d__x000d__x000d_
-_x000d__x000d__x000d_
-To continue using this tool, please agree that you have read and understood the contents of this disclaimer._x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">The purpose of the Coronavirus Self-Checker is to help you make decisions about seeking appropriate medical care. This system is not intended for the diagnosis or treatment of disease, including COVID-19. _x000d_
+_x000d_
+This project was made possible through a partnership with the CDC Foundation and is enabled by Microsoft’s Azure platform. CDC’s collaboration with a non-federal organization does not imply an endorsement of any one particular service, product, or enterprise. _x000d_
+_x000d_
+To continue using this tool, please agree that you have read and understood the contents of this disclaimer._x000d_
+_x000d_
 ###### ver68 (06.21.2021)</v>
       </c>
       <c r="C159" t="str" xml:space="preserve">
-        <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 것에 대한 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다._x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-이 프로젝트는 CDC Foundation과의 파트너십을 통해 가능했으며 Microsoft의 Azure 플랫폼에서 가능합니다. CDC가 비연방 조직과 협력한다고 해서 특정 서비스, 제품 또는 기업을 보증한다는 의미는 아닙니다._x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-###### ver67.1(05.22.2021)</v>
+        <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다. _x000d_
+_x000d_
+이 프로젝트는 CDC Foundation과의 파트너십을 통해 가능했으며 Microsoft의 Azure 플랫폼에서 가능합니다. CDC가 비연방 조직과 협력한다고 해서 특정 서비스, 제품 또는 기업을 보증한다는 의미는 아닙니다. _x000d_
+_x000d_
+이 도구를 계속 사용하려면, 이 주의 경고문의 내용을 읽고 이해하였음에 동의해 주십시오._x000d_
+_x000d_
+###### 버전 68 (2021년 6월 21일)</v>
       </c>
       <c r="D159" t="str" xml:space="preserve">
-        <v xml:space="preserve">Mục đích của việc Hệ thống Câu hỏi Tự Kiểm tra Mắc Virus Corona là để giúp quý vị đưa ra quyết định về việc tìm kiếm dịch vụ chăm sóc y tế thích hợp. Hệ thống này không dùng để chẩn đoán hoặc điều trị bệnh, kể cả COVID-19. _x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-Dự án này được thực hiện thông qua sự hợp tác với CDC Foundation và được hỗ trợ bởi nền tảng Azure của Microsoft. Sự hợp tác của CDC với một tổ chức không thuộc liên bang không ngụ ý xác nhận bất kỳ dịch vụ, sản phẩm hoặc doanh nghiệp cụ thể nào. _x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-###### ver67.1(05.22.2021)</v>
+        <v xml:space="preserve">Mục đích của Hệ thống Câu hỏi Tự Kiểm tra Mắc Virus Corona là để giúp quý vị đưa ra quyết định về việc tìm kiếm dịch vụ chăm sóc y tế thích hợp. Hệ thống này không dùng để chẩn đoán hoặc điều trị bệnh, kể cả COVID-19. _x000d_
+_x000d_
+Dự án này được thực hiện thông qua sự hợp tác với CDC Foundation và được hỗ trợ bởi nền tảng Azure của Microsoft. Sự hợp tác của CDC với một tổ chức không thuộc liên bang không ngụ ý xác nhận bất kỳ dịch vụ, sản phẩm hoặc doanh nghiệp cụ thể nào. _x000d_
+_x000d_
+Để tiếp tục sử dụng công cụ này, vui lòng đồng ý rằng quý vị đã đọc và hiểu nội dung của tuyên bố từ chối trách nhiệm này._x000d_
+_x000d_
+###### ver68 (06.21.2021)</v>
       </c>
       <c r="E159" t="str" xml:space="preserve">
-        <v xml:space="preserve">冠状病毒自我检查问卷的目的是帮助您做出寻求适当医疗护理的决策。该系统不适用于疾病的诊断或治疗，包括新冠肺炎。_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-这个项目是通过与 CDC 基金会的合作而实现，并由 Microsoft 的 Azure 平台启用。CDC 与非联邦组织的合作并不意味着对任何特定服务、产品或企业的认可。_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-###### ver67.1(05.22.2021)</v>
+        <v xml:space="preserve">冠状病毒自我检查问卷的目的是帮助您做出寻求适当医疗护理的决策。该系统不适用于疾病的诊断或治疗，包括新冠肺炎。_x000d_
+_x000d_
+这个项目是通过与 CDC 基金会的合作而实现，并由 Microsoft 的 Azure 平台启用。CDC 与非联邦组织的合作并不意味着对任何特定服务、产品或企业的认可。_x000d_
+_x000d_
+若要继续使用此工具，请同意您已阅读并理解此免责声明的内容。_x000d_
+_x000d_
+###### ver68 版（2021 年 6 月 21 日)</v>
       </c>
       <c r="F159" t="str" xml:space="preserve">
-        <v xml:space="preserve">La finalidad del Autoverificador del Coronavirus es ayudarlo a tomar decisiones sobre la obtención de atención médica adecuada. Este sistema no se ha diseñado para fines de diagnóstico o tratamiento de enfermedades, incluido el COVID-19. _x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-Este proyecto ha sido posible mediante la colaboración con la Fundación de los CDC y se ha habilitado a través de la plataforma Azure de Microsoft. La colaboración de los CDC con una organización no federal no implica el respaldo a ningún servicio, producto o empresa específicos. _x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d_
-###### ver67.1 (05.22.2021)</v>
+        <v xml:space="preserve">La finalidad del Autoverificador del Coronavirus es ayudarlo a tomar decisiones sobre la obtención de atención médica adecuada. Este sistema no se ha diseñado para fines de diagnóstico o tratamiento de enfermedades, incluido el COVID-19. _x000d_
+_x000d_
+Este proyecto ha sido posible mediante la colaboración con la Fundación de los CDC y se ha habilitado a través de la plataforma Azure de Microsoft. La colaboración de los CDC con una organización no federal no implica el respaldo a ningún servicio, producto o empresa específicos. _x000d_
+_x000d_
+Para continuar usando esta herramienta, confirme que ha leído y entendido el contenido de este descargo de responsabilidad._x000d_
+_x000d_
+###### ver68 (06.21.2021)</v>
       </c>
     </row>
     <row r="160" xml:space="preserve">
@@ -3714,131 +3760,117 @@
         <v>CDC/messages/endcap</v>
       </c>
       <c r="B160" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Steps to follow every day:**_x000d__x000d_
-_x000d__x000d_
-- **Get a COVID-19 vaccine** as soon as you are eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d__x000d_
-_x000d__x000d_
-- **Wear** a mask over your nose and mouth.*_x000d__x000d_
-_x000d__x000d_
-- **Stay** at least 6 feet away from people who don’t live with you.*_x000d__x000d_
-_x000d__x000d_
-- **Avoid** crowded areas and poorly ventilated spaces.*_x000d__x000d_
-_x000d__x000d_
-- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d__x000d_
-_x000d__x000d_
-_x000d__x000d_
-_x000d__x000d_
-###### *Fully vaccinated people (those at least 2 weeks past their final dose)  can resume activities without wearing a mask or physically distancing, except where required by federal, state, local, tribal, or territorial laws, rules, and regulations, including local business and workplace guidance. _x000d__x000d_
-_x000d__x000d_
-_x000d__x000d_
-_x000d__x000d_
-**Click the links below for more information on:**_x000d__x000d_
-_x000d__x000d_
-- [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d_
-_x000d__x000d_
-- [Post-COVID Conditions](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d__x000d_
-_x000d__x000d_
-- [When to get tested](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d_
-_x000d__x000d_
-- [What your test results mean](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d_
-_x000d__x000d_
-- [Protecting yourself and others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d_
-_x000d__x000d_
-- [When to quarantine or isolate and for how long](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
-_x000d__x000d_
-- [What to do if you were around someone with COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
-_x000d__x000d_
-- [Taking care of yourself when you are sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d_
-_x000d__x000d_
-- [Taking care of someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d__x000d_
-_x000d__x000d_
-- [Learn about COVID-19 Vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d_
-_x000d__x000d_
+        <v xml:space="preserve">**Steps to follow every day:**_x000d_
+- **Get a COVID-19 vaccine** as soon as you are eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d_
+- **Wear** a mask over your nose and mouth.*_x000d_
+- **Stay** at least 6 feet away from people who don’t live with you.*_x000d_
+- **Avoid** crowded areas and poorly ventilated spaces.*_x000d_
+- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d_
+_x000d_
+###### *Fully vaccinated people (those at least 2 weeks past their final dose)  can resume activities without wearing a mask or physically distancing, except where required by federal, state, local, tribal, or territorial laws, rules, and regulations, including local business and workplace guidance. _x000d_
+_x000d_
+**Click the links below for more information on:**_x000d_
+- [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
+- [Post-COVID Conditions](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
+- [When to get tested](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
+- [What your test results mean](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
+- [Protecting yourself and others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d_
+- [When to quarantine or isolate and for how long](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [What to do if you were around someone with COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [Taking care of yourself when you are sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
+- [Taking care of someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
+- [Learn about COVID-19 Vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
 - [Find COVID-19 vaccine locations near you](https://www.vaccines.gov/)</v>
       </c>
       <c r="C160" t="str" xml:space="preserve">
-        <v xml:space="preserve">**매일 따라야 할 단계:**_x000d__x000d__x000d_
-- 자격이 되는대로 **COVID-19 백신을 접종하십시오**. 백신 접종을 모두 마칠 때까지 계속해서 아래의 단계를 매일 따르십시오.*_x000d__x000d__x000d_
-- 코와 입을 가리는 마스크를 **착용하십시오**.*_x000d__x000d__x000d_
-- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**.*_x000d__x000d__x000d_
-- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**.*_x000d__x000d__x000d_
-- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### *백신 접종을 모두 마친 사람(최종 접종 후 적어도 2주가 지난 사람)은 마스크 착용 또는 물리적인 거리두기 없이 일상생활을 다시 이어나갈 수 있습니다. 단, 지역 사업 또는 직장 지침을 포함하여 연방, 주, 지방, 부족 또는 영토 법률, 규칙 및 규정에서 요구하는 경우는 예외입니다._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**자세한 정보를 보려면 아래 링크를 클릭하십시오.**_x000d__x000d__x000d_
-- [COVID-19 증상](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d__x000d_
-- [COVID 이후 상황](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d__x000d__x000d_
-- [검사를 언제 받아야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d__x000d_
-- [검사 결과가 의미하는 것](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d__x000d_
-- [다른 사람을 질병으로부터 보호하십시오](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d__x000d_
-- [언제 그리고 얼마나 오래 격리 또는 분리해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d__x000d_
-- [COVID-19에 걸린 사람 주변에 있었다면 무엇을 해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d__x000d_
-- [아플 때 자신을 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d__x000d_
-- [아픈 사람 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
+        <v xml:space="preserve">**매일 따라야 할 단계:**_x000d_
+- 자격이 되는대로 **COVID-19 백신을 접종하십시오**. 백신 접종을 모두 마칠 때까지 계속해서 아래의 단계를 매일 따르십시오.*_x000d_
+- 코와 입을 가리는 마스크를 **착용하십시오**.*_x000d_
+- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**.*_x000d_
+- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**.*_x000d_
+- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d_
+_x000d_
+###### *백신 접종을 모두 마친 사람(최종 접종 후 적어도 2주가 지난 사람)은 마스크 착용 또는 물리적인 거리두기 없이 일상생활을 다시 이어나갈 수 있습니다. 단, 지역 사업 또는 직장 지침을 포함하여 연방, 주, 지방, 부족 또는 영토 법률, 규칙 및 규정에서 요구하는 경우는 예외입니다. _x000d_
+_x000d_
+**자세한 정보를 보려면 아래 링크를 클릭하십시오.**_x000d_
+- [COVID-19 증상](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
+- [COVID 이후 증상](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
+- [검사를 언제 받아야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
+- [검사 결과가 의미하는 것](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
+- [자신과 다른 사람을 질병으로부터 보호하십시오](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d_
+- [언제 그리고 얼마나 오래 격리 또는 분리해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [COVID-19에 걸린 사람 주변에 있었다면 무엇을 해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [아플 때 자신을 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
+- [아픈 사람 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
+- [COVID-19 백신 알아보기](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [귀하 근처의 COVID-19 백신 접종 장소 찾기](https://www.vaccines.gov/)</v>
       </c>
       <c r="D160" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Các bước cần tuân theo hàng ngày:**_x000d__x000d__x000d_
-- **Tiêm vắc xin COVID-19** ngay khi bạn đủ điều kiện. Tiếp tục làm theo các bước bên dưới mỗi ngày cho đến khi bạn được tiêm vắc xin đầy đủ.*_x000d__x000d__x000d_
-- **Đeo** khẩu trang lên mũi và miệng của quý vị.*_x000d__x000d__x000d_
-- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet.*_x000d__x000d__x000d_
-- **Tránh** những khu vực đông đúc và không gian kém thông thoáng.*_x000d__x000d__x000d_
-- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước khử trùng tay có ít nhất 60% cồn._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### * Những người đã được tiêm vắc xin đầy đủ (ít nhất 2 tuần sau liều cuối cùng) có thể tiếp tục các hoạt động mà không cần đeo khẩu trang hoặc giãn cách, trừ trường hợp được yêu cầu bởi luật, quy tắc và các quy định của liên bang, tiểu bang, địa phương, bộ lạc hoặc lãnh thổ, bao gồm hướng dẫn nơi làm việc và kinh doanh tại địa phương. _x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**Nhấp vào liên kết bên dưới để biết thêm thông tin về:**_x000d__x000d__x000d_
-- [Các triệu chứng COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)._x000d__x000d__x000d_
-- [Điều kiện sau COVID](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d__x000d__x000d_
-- [Khi nào cần xét nghiệm](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d__x000d_
-- [Kết quả xét nghiệm của quý vị có ý nghĩa gì](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d__x000d_
-- [Bảo vệ bản thân và những người khác khỏi bị bệnh](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d__x000d_
-- [Cách ly hoặc cách ly khi nào và trong bao lâu](https://www.cdc.gov/coroavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d__x000d_
-- [Phải làm gì nếu quý vị ở gần ai đó có COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d__x000d_
-- [Chăm sóc bản thân khi quý vị bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d__x000d_
-- [Chăm sóc người khác bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
+        <v xml:space="preserve">**Các bước cần tuân theo hàng ngày:**_x000d_
+- **Tiêm vắc xin COVID-19** ngay khi bạn đủ điều kiện. Tiếp tục làm theo các bước bên dưới mỗi ngày cho đến khi bạn được tiêm vắc xin đầy đủ.*_x000d_
+- **Đeo** khẩu trang che mũi và miệng của quý vị.*_x000d_
+- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet.*_x000d_
+- **Tránh** những khu vực đông đúc và không gian kém thông thoáng.*_x000d_
+- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước sát khuẩn tay có ít nhất 60% cồn._x000d_
+_x000d_
+###### *Những người đã được tiêm vắc xin đầy đủ (ít nhất 2 tuần sau liều cuối cùng) có thể tiếp tục các hoạt động mà không cần đeo khẩu trang hoặc giãn cách, trừ trường hợp được yêu cầu bởi luật, quy tắc và các quy định của liên bang, tiểu bang, địa phương, bộ lạc hoặc lãnh thổ, bao gồm hướng dẫn của nơi làm việc và kinh doanh tại địa phương.  _x000d_
+_x000d_
+**Nhấp vào liên kết bên dưới để biết thêm thông tin về:**_x000d_
+- [Các triệu chứng COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html))_x000d_
+- [Điều kiện sau COVID](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
+- [Khi nào cần xét nghiệm](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
+- [Kết quả xét nghiệm của quý vị có ý nghĩa gì](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pd)_x000d_
+- [Bảo vệ bản thân và những người khác khỏi bị bệnh](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d_
+- [Khi nào cần cách ly và trong bao lâu](https://www.cdc.gov/coroavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [Phải làm gì nếu quý vị ở gần người mắc COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [Chăm sóc bản thân khi quý vị bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
+- [Chăm sóc người khác bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
+- [Tìm hiểu thêm về Vắc-xin Ngừa COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [Tìm địa điểm tiêm vắc-xin ngừa COVID-19 gần quý vị](https://www.vaccines.gov/)</v>
       </c>
       <c r="E160" t="str" xml:space="preserve">
-        <v xml:space="preserve">**每天要遵循的步骤：**_x000d__x000d__x000d_
-- 只有您有资格请尽快**接种 COVID-19 疫苗**。每天继续遵循以下步骤，直到您完全接种疫苗。_x000d__x000d__x000d_
-- **佩戴**口罩遮住您的口鼻。_x000d__x000d__x000d_
-- 与不和您住在一起的人**保持**至少 6 英尺的距离。_x000d__x000d__x000d_
-- **避免**去拥挤的地方和通风不良的空间。_x000d__x000d__x000d_
-- 经常用肥皂和水**洗**手，或者使用酒精含量至少 60% 的洗手液。_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### *已完全接种的人（即接种完最后一剂之后至少 2 周的人）可以恢复活动而无需佩戴口罩或保持社交距离，除非联邦、州、地方、部落或领地的法律、法规和规章（包括当地的商业和工作场所指南）有此类要求。_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**点击以下链接了解更多信息：**_x000d__x000d__x000d_
-- [COVID-19 症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d__x000d_
-- [COVID 后的病症](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d__x000d__x000d_
-- [何时进行检测](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d__x000d_
-- [您的测试结果是什么意思](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d__x000d_
-- [保护自己和他人免于生病](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d__x000d_
-- [何时进行检疫隔离或隔离以及隔离多长时间](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d__x000d_
-- [如果您身边的人患有 COVID-19，您该怎么办？](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d__x000d_
-- [生病时照顾好自己](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d__x000d_
-- [照顾生病的他人](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
+        <v xml:space="preserve">**每天要遵循的步骤：**_x000d_
+- 只有您有资格请尽快**接种 COVID-19 疫苗**。每天继续遵循以下步骤，直到您完全接种疫苗。*_x000d_
+- **佩戴**口罩遮住您的口鼻。*_x000d_
+- 与不和您住在一起的人**保持**至少 6 英尺的距离。*_x000d_
+- **避免**去拥挤的地方和通风不良的空间。*_x000d_
+- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。_x000d_
+_x000d_
+###### *已完全接种的人（即接种完最后一剂之后至少 2 周的人）可以恢复活动而无需佩戴口罩或保持社交距离，除非联邦、州、地方、部落或领地的法律、法规和规章（包括当地的商业和工作场所指南）有此类要求。 _x000d_
+_x000d_
+**点击以下链接了解更多信息：**_x000d_
+- [新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
+- [新冠肺炎后的病症](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
+- [何时进行检测](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
+- [您的测试结果是什么意思](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
+- [保护自己和他人免于生病](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d_
+- [何时进行检疫隔离或隔离以及隔离多长时间](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [如果您身边的人患有新冠肺炎，您该怎么办](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [生病时照顾好自己](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
+- [照顾生病的他人](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
+- [了解新冠肺炎疫苗](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [查找您附近的新冠肺炎疫苗接种位置](https://www.vaccines.gov/)</v>
       </c>
       <c r="F160" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Medidas para tomar todos los días: **_x000d__x000d__x000d_
-- **Vacúnese contra el COVID-19** tan pronto como sea elegible. Continúe tomando las siguientes medidas todos los días hasta que esté completamente vacunado._x000d__x000d__x000d_
-- **Póngase** una mascarilla que le cubra la nariz y la boca._x000d__x000d__x000d_
-- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted._x000d__x000d__x000d_
-- **Evite** lugares con mucha gente y áreas con poca ventilación._x000d__x000d__x000d_
-- **Lávese** las manos a menudo con agua y jabón o use un desinfectante de manos que contenga al menos un 60 % de alcohol._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### *Las personas completamente vacunadas (aquellas que recibieron la última dosis hace al menos 2 semanas) pueden reanudar actividades sin usar mascarilla ni mantener distanciamiento físico, excepto donde lo requieran las leyes, normas y regulaciones federales, estatales, locales, tribales o territoriales, incluidas las directrices de empresas o negocios y lugares de trabajo locales. _x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**Haga clic en los enlaces a continuación para obtener más información sobre lo siguiente:**_x000d__x000d__x000d_
-- [Síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d__x000d_
-- [Afecciones posteriores al COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d__x000d__x000d_
-- [Cuándo hacerse la prueba](https://espanol.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html)_x000d__x000d__x000d_
-- [Lo que significan los resultados de su prueba](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d__x000d_
-- [Cómo protegerse a sí mismo y a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d__x000d_
-- [Cuándo ponerse en cuarentena o aislarse y por cuánto tiempo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d__x000d_
-- [Qué hacer si estuvo cerca de alguien con COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d__x000d_
-- [Cómo cuidarse cuando está enfermo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d__x000d_
-- [Cómo cuidar a otra persona que está enferma](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)</v>
+        <v xml:space="preserve">**Medidas para tomar todos los días:**
+- **Vacúnese contra el COVID-19** tan pronto como sea elegible. Continúe tomando las siguientes medidas todos los días hasta que esté completamente vacunado.*
+- **Póngase** una mascarilla que le cubra la nariz y la boca.*
+- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted.*
+- **Evite** lugares con mucha gente y áreas con poca ventilación.*
+- **Lávese** las manos a menudo con agua y jabón, o use un desinfectante de manos que contenga al menos un 60 % de alcohol.
+###### *Las personas completamente vacunadas (aquellas que recibieron la última dosis hace al menos 2 semanas) pueden reanudar actividades sin usar mascarilla ni mantener distanciamiento físico, excepto donde lo requieran las leyes, normas y regulaciones federales, estatales, locales, tribales o territoriales, incluidas las directrices de empresas o negocios, y lugares de trabajo locales. 
+**Haga clic en los enlaces a continuación para obtener más información sobre lo siguiente:**
+- [Síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)
+- [Afecciones posteriores al COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)
+- [[Cuándo hacerse la prueba](https://espanol.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html)
+- [Lo que significan los resultados de su prueba](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)
+- [Cómo protegerse a sí mismo y a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)
+- [Cuándo ponerse en cuarentena o aislarse, y por cuánto tiempo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
+- [Qué hacer si estuvo cerca de alguien con COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
+- [Cómo cuidarse cuando esté enfermo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)
+- [Cómo cuidar a otra persona que esté enferma](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)
+- [Infórmese sobre las vacunas contra el COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)
+- [Encuentre sitios de vacunación contra el COVID-19 cercanos](https://www.vacunas.gov/)</v>
       </c>
     </row>
     <row r="161" xml:space="preserve">
@@ -4373,98 +4405,58 @@
         <v>CDC/messages/msg23</v>
       </c>
       <c r="B183" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Contact a medical provider if you (they) get sick.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Stay in your room as much as possible except to get medical care._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cover your coughs and sneezes with a tissue._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Clean your hands often._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Avoid close contact with other people. Stay at least 6 feet away from other people._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Wear a mask when around others._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Clean and disinfect commonly touched surfaces in your room._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Contact a medical provider if you (they) get sick.**_x000d_
+Help [protect others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d_
+- Stay in your room as much as possible except to get medical care._x000d_
+- Cover your coughs and sneezes with a tissue._x000d_
+- Clean your hands often._x000d_
+- Avoid close contact with other people. Stay at least 6 feet away from other people._x000d_
+- Wear a mask when around others._x000d_
+- Clean and disinfect commonly touched surfaces in your room._x000d_
 - Monitor your health and notify a medical provider if you think you are getting sicker.</v>
       </c>
       <c r="C183" t="str" xml:space="preserve">
-        <v xml:space="preserve">**귀하(그 사람)가 아플 경우 의료진에게 연락하십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-[다른 사람을 질병으로부터 보호]하도록 도움을 주십시오(https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의학적 치료를 받는 경우를 제외하고 가급적 방에 머무르십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 손을 자주 씻으십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다른 사람과 가까이 하지 마십시오. 다른 사람과 최소 6피트의 간격을 유지하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 다른 사람들과 함께 있을 때는 마스크를 착용하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 방안에서 자주 접촉하는 표면을 청소하고 소독하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**귀하가(그 사람이) 아플 경우 의료진에게 연락하십시오.**_x000d_
+[다른 사람을 질병으로부터 보호](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html) 하도록 도움을 주십시오._x000d_
+- 의학적 치료를 받는 경우를 제외하고 가급적 방에 머무르십시오._x000d_
+- 기침과 재치기를 할 때 티슈로 입을 가리십시오._x000d_
+- 손을 자주 씻으십시오._x000d_
+- 다른 사람과 가까이 하지 마십시오. 다른 사람과 최소 6피트의 간격을 유지하십시오._x000d_
+- 다른 사람들과 함께 있을 때는 마스크를 착용하십시오._x000d_
+- 방안에서 자주 접촉하는 표면을 청소하고 소독하십시오._x000d_
 - 자신의 건강 상태를 모니터링하여, 악화된다고 생각되면 의료진에게 알리십시오.</v>
       </c>
       <c r="D183" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Liên hệ với một nhà cung cấp dịch vụ y tế nếu quý vị (họ) mắc bệnh.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Giúp [bảo vệ người khác không mắc bệnh] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Ở trong phòng của mình càng nhiều càng tốt, ngoại trừ khi cần chăm sóc y tế._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dùng khăn giấy để che khi ho và hắt hơi._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Rửa tay thường xuyên._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Tránh tiếp xúc gần với người khác. - Giữ khoảng cách với người khác ít nhất 6 feet (2 mét)._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đeo khẩu trang khi ở gần người khác._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Làm sạch và khử trùng các bề mặt thường chạm vào trong phòng của quý vị._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Liên hệ với một nhà cung cấp dịch vụ y tế nếu quý vị (họ) mắc bệnh.**_x000d_
+Giúp [bảo vệ người khác không mắc bệnh](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d_
+- Ở trong phòng của mình càng nhiều càng tốt, ngoại trừ khi cần chăm sóc y tế._x000d_
+- Dùng khăn giấy để che khi ho và hắt hơi._x000d_
+- Rửa tay thường xuyên._x000d_
+- Tránh tiếp xúc gần với người khác. - Giữ khoảng cách với người khác ít nhất 6 feet (2 mét)._x000d_
+- Đeo khẩu trang khi ở gần người khác._x000d_
+- Làm sạch và khử trùng các bề mặt thường chạm vào trong phòng của quý vị._x000d_
 - Theo dõi sức khỏe của quý vị và thông báo cho nhà cung cấp dịch vụ y tế nếu quý vị nghĩ rằng mình đang bị bệnh nặng hơn.</v>
       </c>
       <c r="E183" t="str" xml:space="preserve">
-        <v xml:space="preserve">**如果您生病，请联系医务人员。**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-帮助 [保护他人免于生病] (https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 除就医外，尽可能多地待在您的房间里。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 咳嗽以及打喷嚏时，用纸巾捂住口鼻。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 经常洗手。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 避免与他人密切接触。 尝试与他人保持至少 6 英尺的距离。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--在他人周围时戴口罩。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 清洁和消毒您房间中的经常接触的表面。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**如果您生病，请联系医务人员。**_x000d_
+帮助 [保护他人免于生病](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)：_x000d_
+- 除就医外，尽可能多地待在您的房间里。_x000d_
+- 咳嗽以及打喷嚏时，用纸巾捂住口鼻。_x000d_
+- 经常清洁双手。_x000d_
+- 避免与他人密切接触。尝试与他人保持至少 6 英尺的距离。_x000d_
+- 在他人周围佩戴口罩。_x000d_
+- 清洁和消毒您房间中经常被接触的表面。_x000d_
 - 监测您的健康状况，如果您认为您病情加重，请通知医疗服务人员。</v>
       </c>
       <c r="F183" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Comuníquese con un proveedor de atención médica si se enferma.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-Ayude a [proteger a otras personas para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Quédese en su habitación lo más posible, excepto para conseguir atención médica._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cúbrase la nariz y la boca al toser y estornudar con un pañuelo desechable o con la parte interna del codo._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Límpiese las manos con frecuencia._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Evite el contacto cercano con otras personas. Manténgase a por lo menos 6 pies o 2 metros de las otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Póngase una mascarilla cuando esté cerca de otras personas._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Limpie y desinfecte las superficies en su habitación que se tocan con frecuencia._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Comuníquese con un proveedor médico si se enferma.**_x000d_
+Ayude a [proteger a otras personas para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d_
+- Quédese en su habitación lo más posible, excepto para conseguir atención médica._x000d_
+- Cúbrase la nariz y la boca con un pañuelo desechable al toser o estornudar._x000d_
+- Límpiese las manos con frecuencia._x000d_
+- Evite el contacto cercano con otras personas. Manténgase a por lo menos 6 pies o 2 metros de las otras personas._x000d_
+- Póngase una mascarilla cuando esté cerca de otras personas._x000d_
+- Limpie y desinfecte las superficies en su habitación que se tocan con frecuencia._x000d_
 - Monitoree su salud y notifique a un proveedor de atención médica si piensa que está empeorando.</v>
       </c>
     </row>
@@ -4533,36 +4525,44 @@
         <v>CDC/messages/msg27</v>
       </c>
       <c r="B187" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Stay home and away from others until:**_x000d__x000d__x000d__x000d__x000d__x000d_
-- it has been 10 days* from when your symptoms first appeared **and**_x000d__x000d__x000d__x000d__x000d__x000d_
-- you have had no fever for 24 hours without the use medications **and**_x000d__x000d__x000d__x000d__x000d__x000d_
-- your other symptoms of COVID-19 are improving* (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**Stay home and away from others until:**_x000d_
+- it has been 10 days* from when your symptoms first appeared **and**_x000d_
+- you have had no fever for 24 hours without the use medications **and**_x000d_
+- your other symptoms of COVID-19 are improving* (*Loss of taste and smell may persist for weeks or months after recovery and need not delay the end of isolation)_x000d_
+_x000d_
 \* If you have a weakened immune system (immunocompromised) due to a health condition or medication, you might need to stay home and isolate longer than 10 days and possibly 20 days after symptoms begin. In some circumstances, further testing may be needed. Talk to your healthcare provider for more information.</v>
       </c>
       <c r="C187" t="str" xml:space="preserve">
-        <v xml:space="preserve">**다음과 같을 때까지 집에 머물고 다른 사람들과 떨어져 있으십시오.**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 첫 증상 발현 후 10일 이후 **그리고**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 약 사용 없이 24시간 동안 발열이 없었음 **그리고**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- COVID-19의 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦추지 않음)</v>
+        <v xml:space="preserve">**다음의 기간 동안 집에 머물고 다른 사람들과 떨어져 있으십시오.**_x000d_
+- 첫 증상 발현 후 10일* 이후 **그리고**_x000d_
+- 약 사용 없이 24시간 동안 발열이 없음 **그리고**_x000d_
+- COVID-19의 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦출 필요 없음)_x000d_
+_x000d_
+\* 건강 상태 또는 약물로 인해 귀하의 면역계가 쇠약한 경우(면역저하), 귀하는 증상이 시작된 후 자택에 머물며 10일 넘게, 아마도 20일동안 격리해야 할 수 있습니다. 일부 환경에서, 추가 검사가 필요할 수 있습니다. 더 자세한 정보는 담당 의료 서비스 제공자에게 문의하십시오.</v>
       </c>
       <c r="D187" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Ở nhà và tránh xa những người khác cho đến khi:**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- đã qua 10 ngày từ khi quý vị xuất hiện các triệu chứng đầu tiên **và**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc **và**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- các triệu chứng COVID-19 khác của quý vị đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)</v>
+        <v xml:space="preserve">**Ở nhà và tránh xa những người khác cho đến khi:**_x000d_
+- đã qua 10 ngày* từ khi quý vị xuất hiện các triệu chứng đầu tiên **và**_x000d_
+- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc **và**_x000d_
+- các triệu chứng COVID-19 khác của quý vị đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)_x000d_
+_x000d_
+\* Nếu quý vị bị suy yếu hệ thống miễn dịch (suy giảm miễn dịch) do tình trạng sức khỏe hoặc do thuốc, quý vị có thể cần phải ở nhà và cách ly lâu hơn 10 ngày và có thể là 20 ngày sau khi các triệu chứng khởi phát. Trong một số trường hợp, có thể cần xét nghiệm thêm. Nói chuyện với nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị để biết thêm thông tin.</v>
       </c>
       <c r="E187" t="str" xml:space="preserve">
-        <v xml:space="preserve">**待在家里，远离他人，直到：**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 距离您的症状首次出现已经 10 天**并且**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 在没有使用药物的情况下，24小时内没有发烧 **并且**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 您的COVID-19的其他症状正在改善*（*康复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）</v>
+        <v xml:space="preserve">**待在家里，远离他人，直到：**_x000d_
+- 距离您的症状首次出现已经 10 天**并且**_x000d_
+- 在没有使用药物的情况下，已24 小时没有发烧**并且**_x000d_
+- 您的新冠肺炎的其他症状正在改善*（*康复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）_x000d_
+_x000d_
+\* 如果您由于健康状况或药物导致免疫系统减弱（免疫功能低下），您可能需要留在家中隔离 10 天以上，且可能持续到在症状开始后 20 天。在某些情况下，可能需要进一步测试。更多信息请咨询您的医疗保健提供者。</v>
       </c>
       <c r="F187" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quédese en casa y lejos de los demás hasta que:**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- hayan pasado 10 días desde el inicio de los síntomas **y**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 24 horas sin fiebre sin usar medicamentos para reducirla **y**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- otros síntomas del COVID-19 estén mejorando* (*La pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)</v>
+        <v xml:space="preserve">**Quédese en casa y lejos de los demás hasta que:**_x000d_
+- hayan pasado 10 días* desde el inicio de los síntomas **y**_x000d_
+- 24 horas sin fiebre, sin usar medicamentos para reducirla **y**_x000d_
+- sus otros síntomas del COVID-19 estén mejorando* (*La pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)_x000d_
+_x000d_
+\* Si tiene el sistema inmunitario debilitado (inmunodeprimido) debido a una afección o a medicamentos, podría tener que quedarse en casa y aislado por más de 10 días y, posiblemente, 20 días después del inicio de los síntomas. En algunas circunstancias, puede que sean necesarias más pruebas. Hable con su proveedor de atención médica para obtener más información.</v>
       </c>
     </row>
     <row r="188" xml:space="preserve">
@@ -4570,101 +4570,69 @@
         <v>CDC/messages/msg27_addnl</v>
       </c>
       <c r="B188" t="str" xml:space="preserve">
-        <v xml:space="preserve">Please inform your close contacts that they have been potentially exposed to the coronavirus that causes COVID-19. CDC recommends that all close contacts of people with confirmed or probable COVID-19 should:_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- get tested **and**_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- quarantine for 14 days from the day of their last exposure. You may also receive a call from a contact tracing professional._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
- Get rest and stay hydrated. Take over-the-counter medicines, such as acetaminophen, if needed to help you feel better. _x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve"> Please inform your close contacts that they have been potentially exposed to the coronavirus that causes COVID-19. CDC recommends that all close contacts of people with confirmed or probable COVID-19 should:_x000d_
+- get tested **and**_x000d_
+- quarantine for 14 days from the day of their last exposure. You may also receive a call from a contact tracing professional. _x000d_
+_x000d_
+ Get rest and stay hydrated. Take over-the-counter medicines, such as acetaminophen, if needed to help you feel better._x000d_
+_x000d_
  Separate yourself from other people. As much as possible, stay in a specific room and away from other people and pets in your home.</v>
       </c>
       <c r="C188" t="str" xml:space="preserve">
-        <v xml:space="preserve">SARS-CoV-2에 노출되었을 수 있는 밀접 접촉자가 있다면 알려주시기 바랍니다. 확진자 또는 COVID-19 가능성이 있는 사람들과 밀접 접촉한 모든 사람이 다음과 같이 할 것을 CDC는 권장합니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 검사를 받으십시오 **그리고**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 마지막으로 노출된 날부터 14일 동안 격리하십시오. 또한 추적 전문가의 전화를 받을 수도 있습니다._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- 휴식을 취하고 수분을 충분히 보충하십시오. 회복에 도움이 되도록 필요한 경우 아세트아미노펜과 같은 일반의약품을 복용하십시오._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- 다른 사람으로부터 분리되어 있으십시오. 가능한 한, 가정 내 특정 공간에 다른 구성원과 반려동물로부터 격리하여 머무르십시오.</v>
+        <v xml:space="preserve">COVID-19를 유발하는 코로나 바이러스에 노출되었을 수 있는 밀접 접촉자가 있다면 알려주시기 바랍니다. 확진자 또는 COVID-19 가능성이 있는 사람들과 밀접 접촉한 모든 사람은 다음과 같이 할 것을 CDC는 권장합니다._x000d_
+- 검사를 받으십시오 **그리고**_x000d_
+- 마지막 노출일로부터 14일 동안 격리하십시오. 또한 역학 조사관의 전화를 받을 수도 있습니다._x000d_
+_x000d_
+ 휴식을 취하고 수분을 충분히 보충하십시오. 회복에 도움이 되도록 필요한 경우 아세트아미노펜과 같은 일반의약품을 복용하십시오. _x000d_
+_x000d_
+ 다른 사람으로부터 분리되어 있으십시오. 가능한 한, 가정 내 특정 방에 다른 구성원과 반려동물로부터 격리하여 머무르십시오.</v>
       </c>
       <c r="D188" t="str" xml:space="preserve">
-        <v xml:space="preserve">Vui lòng thông báo cho những tiếp xúc gần với quý vị rằng họ có khả năng bị nhiễm SARS-CoV-2. CDC khuyến cáo rằng tất cả những người tiếp xúc gần với những người đã được xác nhận mắc hoặc có khả năng mắc COVID-19 nên:_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- xét nghiệm **và**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- cách ly trong 14 ngày kể từ ngày tiếp xúc cuối cùng của họ. Quý vị cũng có thể nhận được cuộc gọi từ một chuyên gia theo dõi người tiếp xúc._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- Nghỉ ngơi và uống đủ nước. Dùng các loại thuốc không cần kê toa, ví dụ như acetaminophen, nếu cần để giúp quý cảm thấy tốt hơn. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Vui lòng thông báo cho những người tiếp xúc gần với quý vị rằng họ có khả năng bị nhiễm coronavirus gây bệnh COVID-19. CDC khuyến cáo tất cả những người tiếp xúc gần với những người đã được xác nhận mắc hoặc có khả năng mắc COVID-19 nên:_x000d_
+- xét nghiệm **và**_x000d_
+- cách ly trong 14 ngày kể từ ngày tiếp xúc cuối cùng của họ. Quý vị cũng có thể nhận được cuộc gọi từ một nhân viên phụ trách theo dõi người tiếp xúc._x000d_
+_x000d_
+ Nghỉ ngơi và uống đủ nước. Dùng các loại thuốc không cần kê toa, ví dụ như acetaminophen, nếu cần để giúp quý cảm thấy dễ chịu hơn. _x000d_
+_x000d_
  Cách ly quý vị khỏi những người khác. Nên ở một phòng riêng càng nhiều càng tốt và tránh xa những người và vật nuôi khác trong nhà quý vị.</v>
       </c>
       <c r="E188" t="str" xml:space="preserve">
-        <v xml:space="preserve">请告知您的密切接触者他们可能接触了 SARS-CoV-2。CDC 建议确诊或疑似 COVID-19（新冠肺炎）的人的密切接触者应该：_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 接受检测**和**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 从最后一次接触之日算起，隔离14天。您也可能会接到专业人员打来的电话。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- 注意休息并保持不要脱水。如果需要帮助您感觉好一些，可使用非处方药，如对乙酰氨基酚。_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">请告知您的密切接触者，他们可能暴露于引起新冠肺炎的冠状病毒。CDC 建议与确诊或疑似新冠肺炎人有密切接触者应该：_x000d_
+- 接受检测**和**_x000d_
+- 从最后一次接触之日算起，隔离 14 天。您也可能会接到接触者追踪专业人员打来的电话。_x000d_
+_x000d_
+ 注意休息并保持不要脱水。如果需要帮助您感觉好一些，可使用非处方药，如对乙酰氨基酚。_x000d_
+_x000d_
  自己远离其他人。尽可能地呆在特定的房间中，并远离家中其他人和宠物。</v>
       </c>
       <c r="F188" t="str" xml:space="preserve">
-        <v xml:space="preserve">Infórmeles a sus contactos cercanos que posiblemente han estado espuestos al SARS-CoV-2. Los CDC recomiendan que todos los contactos cercanos de una persona con COVID-19 confirmado o probable:_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- se hagan la prueba **y**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- se pongan en cuarentena por 14 días desde la fecha de su última exposición. Es posible que también reciba una llamada de un profesional de rastreo de contactos._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
- Descanse y manténgase hidratado. Tome medicamentos de venta sin receta, como acetaminofeno, si necesita para sentirse mejor. _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Infórmeles a sus contactos cercanos que posiblemente han estado expuestos al coronavirus que causa el COVID-19. Los CDC recomiendan que todos los contactos cercanos de una persona con COVID-19 confirmado o probable:_x000d_
+- se hagan la prueba **y**_x000d_
+- se pongan en cuarentena por 14 días desde la fecha de su última exposición. Es posible que también reciba una llamada de un profesional encargado del rastreo de contactos._x000d_
+_x000d_
+ Descanse y manténgase hidratado. Tome medicamentos de venta sin receta, como acetaminofeno, si necesita para sentirse mejor. _x000d_
+_x000d_
  Apártese de las otras personas. En la medida de lo posible, permanezca en una habitación específica y lejos de las otras personas y mascotas en su casa.</v>
       </c>
     </row>
-    <row r="189" xml:space="preserve">
+    <row r="189">
       <c r="A189" t="str">
         <v>CDC/messages/msg28</v>
       </c>
       <c r="B189" t="str">
         <v>**You may have received a false-negative test result and still might have COVID-19. Contact your healthcare provider about your symptoms, especially if they worsen, about follow-up testing, and how long to isolate.**</v>
       </c>
-      <c r="C189" t="str" xml:space="preserve">
-        <v xml:space="preserve">**다음과 같을 때까지 집에 머물고 다른 사람들과 떨어져 있으십시오.** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 첫 증상 발현 후 10일 이후 **그리고**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 약 사용 없이 24시간 동안 발열이 없었음 **그리고**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 기타 증상이 호전되고 있음*(*회복 후에 미각 및 후각의 상실이 몇 주 또는 몇 개월 동안 지속될 수 있으며 격리 종료 일자를 늦추지 않음)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-**\*참고하십시오**: 검체를 채취할 당시 감염 초기에 있었으며 나중에 검사 결과 양성으로 나타날 수 있습니다. 검사 결과 음성으로 나타난 이후 증상이 악화된 경우 의료 전문가에게 연락하십시오.</v>
-      </c>
-      <c r="D189" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Ở nhà và tránh xa những người khác cho đến khi:** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- đã qua 10 ngày từ khi quý vị xuất hiện các triệu chứng đầu tiên **và**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- quý vị đã không bị sốt trong 24 giờ mà không cần sử dụng thuốc **và**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- các triệu chứng khác của quý vị đang được cải thiện* (*Mất vị giác và khứu giác có thể tồn tại trong vài tuần hoặc vài tháng sau khi hồi phục và không cần trì hoãn việc kết thúc cách ly)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-**\*Xin lưu ý**: Có thể quý vị đã bị nhiễm rất sớm khi mẫu xét nghiệm của quý vị được thu thập và quý vị có thể có kết quả dương tính sau đó. Nếu các triệu chứng của quý vị trở nên xấu đi sau khi xét nghiệm âm tính, vui lòng liên hệ với nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị.</v>
-      </c>
-      <c r="E189" t="str" xml:space="preserve">
-        <v xml:space="preserve">**待在家里，远离他人，直到：** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 距离您的症状首次出现已经 10 天**并且**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 在没有使用药物的情况下，24小时内没有发烧 **并且**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 您的其他症状正在改善*（*康复后味觉和嗅觉丧失可能持续数周或数月，无需推迟隔离结束的时间）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-**、*请注意**：有可能您在采集样本的时候是在感染的早期，您以后可能会检测出阳性。如果您的症状在检测阴性后恶化，请联系您的医疗保健提供者。</v>
-      </c>
-      <c r="F189" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quédese en casa y lejos de los demás hasta que:** _x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- hayan pasado 10 días desde el inicio de los síntomas **y**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 24 horas sin fiebre sin usar medicamentos para reducirla **y**_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- otros síntomas del COVID-19 estén mejorando* (*La pérdida del gusto o del olfato pueden persistir por semanas o meses después de la recuperación y no hacen necesario retrasar el fin del aislamiento)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-**\*Tenga en cuenta**: Es posible que apenas estuviera comenzando la infección cuando le tomaron la muestra y que pudiera dar positivo más adelante. Si los síntomas empeoran después de dar negativo, contacte al proveedor de atención médica.</v>
+      <c r="C189" t="str">
+        <v>**귀하는 위음성 검사 결과를 받았을 수 있으며 여전히 COVID-19에 감염되었을 수 있습니다. 귀하의 증상에 대하여, 특히 증상이 악화되는 경우, 후속 검사 및 격리 기간에 대하여 귀하의 의료 제공자에게 연락하십시오.**</v>
+      </c>
+      <c r="D189" t="str">
+        <v>**Quý vị có thể đã nhận được kết quả xét nghiệm âm tính giả và vẫn có thể mắc COVID-19. Liên hệ với nhà cung cấp dịch vụ chăm sóc sức khỏe của quý vị về các vấn đề liên quan tới các triệu chứng của quý vị, đặc biệt là nếu chúng xấu đi, về xét nghiệm theo dõi và thời gian cách ly.**</v>
+      </c>
+      <c r="E189" t="str">
+        <v>**您可能获得假阴性检测结果，但仍可能已经感染新冠肺炎。关于您的症状，尤其是症状出现恶化时、随访检查以及隔离时间，请联系您的医疗保健提供者。**</v>
+      </c>
+      <c r="F189" t="str">
+        <v>**Es posible que haya recibido un resultado falso negativo de la prueba y aún tener COVID-19. Contacte a su proveedor de atención médica y pregúntele sobre sus síntomas, especialmente si empeoran, y sobre una prueba de seguimiento y por cuánto tiempo aislarse.**</v>
       </c>
     </row>
     <row r="190">
@@ -6487,16 +6455,16 @@
         <v>In the last 10 days, have you experienced any of the symptoms listed below? (check all that apply)</v>
       </c>
       <c r="C270" t="str">
-        <v>다음 중 해당 사항이 있습니까?(해당 사항에 모두 체크)</v>
+        <v>지난 10일 동안 아래에 나열된 증상을 경험한 적이 있습니까?(적용되는 사항 모두 체크)</v>
       </c>
       <c r="D270" t="str">
-        <v>Quý vị có bất cứ triệu chứng nào sau đây? (đánh dấu tất cả câu trả lời phù hợp)</v>
+        <v xml:space="preserve">Trong 10 ngày qua, quý vị có gặp phải bất kỳ triệu chứng nào được liệt kê dưới đây không? (đánh dấu vào tất cả các câu trả lời phù hợp) </v>
       </c>
       <c r="E270" t="str">
-        <v>您是否有以下情况？（勾选任何一项）</v>
+        <v>在过去 10 天内，您是否出现过下列任何症状？（勾选所有适用项）</v>
       </c>
       <c r="F270" t="str">
-        <v>¿Tiene algo de lo siguiente? (marque todas las opciones que correspondan)</v>
+        <v>En los últimos 10 días, ¿ha tenido alguno de los síntomas de la lista a continuación? (marque todo lo que corresponda)</v>
       </c>
     </row>
     <row r="271" xml:space="preserve">
@@ -6794,180 +6762,63 @@
         <v>CDC/second_person_questions/life_threat_question</v>
       </c>
       <c r="B281" t="str" xml:space="preserve">
-        <v xml:space="preserve">Do you have any of these life-threatening symptoms?_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- Severe and constant pain or pressure in the chest_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- Difficulty breathing (such as gasping for air, being unable to walk or talk without catching your breath, severe wheezing, nostrils flaring, grunting, or ribs or stomach moving in and out deeply and rapidly as you breathe)_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- New disorientation (acting confused)_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- Unconscious or very difficult to wake up_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- Slurred speech or difficulty speaking (new or worsening)_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- New or worsening seizures_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-- Signs of low blood pressure (too weak to stand, dizziness, lightheaded, feeling cold, pale, clammy skin)_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">Do you have any of these life-threatening symptoms?_x000d_
+- Pale, gray, or blue-colored skin, lips, or nail beds, depending on skin tone_x000d_
+- Severe and constant pain or pressure in the chest_x000d_
+- Difficulty breathing (such as gasping for air, being unable to walk or talk without catching your breath, severe wheezing, nostrils flaring, grunting, or ribs or stomach moving in and out deeply and rapidly as you breathe)_x000d_
+- New disorientation (acting confused)_x000d_
+- Unconscious or very difficult to wake up_x000d_
+- Slurred speech or difficulty speaking (new or worsening)_x000d_
+- New or worsening seizures_x000d_
+- Signs of low blood pressure (too weak to stand, dizziness, lightheaded, feeling cold, pale, clammy skin)_x000d_
 - Dehydration (dry lips and mouth, not urinating much, sunken eyes)</v>
       </c>
       <c r="C281" t="str" xml:space="preserve">
-        <v xml:space="preserve">이러한 생명을 위협하는 증상이 있습니까?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 창백한 입술 또는 얼굴- 가슴에 심하고 지속적인 통증이나 압박감- 숨쉬기 매우 어려움(예: 숨이 막힘, 숨을 고르지 않고는 말을 할 수 없음, 중증 천명음, 콧구멍이 벌어짐)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 시간, 장소, 또는 관계를 제대로 인식하지 못하게 됨 (혼란스러워함)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 의식이 없거나 깨우기가 매우 어려움- 불분명한 발음 또는 말하기 어려움(새로운 또는 악화된 증상)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 신규 또는 악화된 발작_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 추위를 느낌, 창백함, 차갑고 축축한 피부)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">다음과 같은 생명을 위협하는 증상이 있습니까? _x000d_
+- 피부, 입술 또는 손발톱 밑이 창백해지거나 회색 또는 파란색이 됨(피부 톤에 따라 다름) _x000d_
+- 가슴에 심하고 지속적인 통증이나 압박감 _x000d_
+- 호흡 곤란(예: 숨이 막힘, 숨을 고르지 않고 걷거나 말을 할 수 없음, 심하게 숨을 쌕쌕거림, 콧구멍이 벌어짐, 앓는 소리를 냄, 또는 숨을 쉴 때 가슴뼈와 배가 깊고 빠르게 안팎으로 움직임) _x000d_
+- 전에 없던 방향 감각 상실(혼란스러워 보이는 행동) _x000d_
+- 의식이 없거나 깨우기가 매우 어려움 _x000d_
+- 불분명한 발음 또는 말하기 어려움(새로운 증상 또는 악화되는 증상) _x000d_
+- 새로운 또는 악화되는 발작 _x000d_
+- 저혈압 징후(너무 힘이 없어 서 있을 수 없음, 어지러움, 머리가 핑핑 도는 느낌, 추위를 탐, 창백함, 칙칙한 피부) _x000d_
 - 탈수(입술과 입 건조, 소변량이 많지 않음, 움푹 들어간 눈)</v>
       </c>
       <c r="D281" t="str" xml:space="preserve">
-        <v xml:space="preserve">Bạn có bất cứ triệu chứng đe dọa tính mạng nào trong số này không?_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Môi hoặc mặt thâm_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Đau hoặc có áp lực nặng và liên tục ở ngực_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Vô cùng khó thở (chẳng hạn như thở hổn hển, không thể nói chuyện mà không bị hụt hơn, thở khò khè nặng, mũi phập phồng)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất phương hướng mới xuất hiện (hành động lẫn lộn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất tri giác hoặc rất khó thức dậy_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Nói đớt hoặc khó nói (mới xuất hiện hoặc bị nặng hơn)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Cơn co giật mới xuất hiện hoặc nặng thêm_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Dấu hiệu huyết áp thấp (quá yếu không thể đứng, chóng mặt, choáng vàng, cảm thấy lạnh, da nhợt nhạt, sần sùi)_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- Mất nước (môi và miệng khô, không đi tiểu nhiều, mắt trũng sâu)</v>
+        <v xml:space="preserve">Quý vị có bất kỳ triệu chứng đe dọa đến tính mạng nào dưới đây không?_x000d_
+- Da, môi hoặc móng tay màu nhợt nhạt, xám hoặc xanh, tùy thuộc vào tông màu da_x000d_
+- Đau hoặc tức ngực dữ dội và liên tục_x000d_
+- Khó thở (ví dụ như thở hổn hển, không thể đi lại hoặc nói chuyện liền câu mà không phải lấy hơi, thở khò khè dữ dội, lỗ mũi phập phồng, khụt khịt hoặc xương sườn hoặc thành bụng hõm sâu và nhanh khi quý vị thở)_x000d_
+- Mới mất phương hướng (hành động khó hiểu)_x000d_
+- Bất tỉnh hoặc rất khó thức dậy_x000d_
+- Nói ngọng hoặc khó nói (mới hoặc diễn biến xấu đi)_x000d_
+- Cơn co giật mới hoặc nặng hơn_x000d_
+- Dấu hiệu của huyết áp thấp (không thể đứng vững, chóng mặt, choáng váng, ớn lạnh, xanh xao, da lạnh và mướt mồ hôi)_x000d_
+- Mất nước (môi và miệng khô, không tiểu tiện nhiều, mắt trũng sâu)</v>
       </c>
       <c r="E281" t="str" xml:space="preserve">
-        <v xml:space="preserve">您是否出现这些危及生命的症状？_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 嘴唇或面部青紫_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 重度和持续性胸痛或胸部压迫感_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--极度呼吸困难（如喘不过气或因为喘不上气而无法说话、重度喘息、鼻孔张开）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--新发的定向障碍（行为混乱）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 意识丧失或很难唤醒_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 言语不清或说话困难（新发或恶化）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--新发癫痫发作或癫痫发作恶化_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
--脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）</v>
+        <v xml:space="preserve">您是否出现这些危及生命的症状？_x000d_
+- 根据肤色的不同，皮肤、嘴唇或指甲呈浅色、灰色或蓝色_x000d_
+- 重度和持续性胸痛或胸部压迫感_x000d_
+- 呼吸困难（如喘气、无法行走或说话而未屏住呼吸、重度喘息、鼻孔张开、呼噜声或呼吸时肋骨或胃会快速而深入地进出）_x000d_
+- 新发的定向障碍（行为混乱）_x000d_
+- 意识丧失或很难唤醒_x000d_
+- 言语不清或说话困难（新发或恶化）_x000d_
+- 新发癫痫发作或癫痫发作恶化_x000d_
+- 低血压体征（太虚弱无法站立、眩晕、头晕目眩、感觉寒冷、苍白、皮肤湿冷）_x000d_
+- 脱水（嘴唇和嘴干燥、排尿不多、眼睛凹陷）</v>
       </c>
       <c r="F281" t="str" xml:space="preserve">
-        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-- Color pálido, gris o azulado de la piel, los labios, o el lecho de las uñas, dependiendo del tono de piel_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-- Presión o dolor intensos y constantes en el pecho _x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-- Dificultad extrema para respirar (le falta el aire o no puede hablar sin quedarse sin aliento, sibilancias intensas, se ensanchan los agujeros de la nariz)_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-- Desorientación (actuar confuso) de aparición reciente_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-- Estado inconsciente o mucha dificultad para despertarte_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-- Habla arrastrada o enredada, o dificultad para hablar (de aparición reciente o que empeora) _x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-- Convulsiones de aparición reciente o que empeoran_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-- Signos de presión arterial baja (muy débil para estar de pie, mareos, aturdimiento, sentir frío, palidez, piel húmeda y pegajosa) _x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?_x000d_
+- Color pálido, gris o azulado de la piel, los labios, o el lecho de las uñas, dependiendo del tono de piel_x000d_
+- Presión o dolor intensos y constantes en el pecho_x000d_
+- Dificultad para respirar (como que le falta el aire o no puede caminar o hablar sin quedarse sin aliento, sibilancias intensas, ensanchamiento de los agujeros de la nariz, gruñidos, o las costillas o el estómago se contraen y expanden bastante y rápidamente a medida que respira)_x000d_
+- Desorientación (actuar confuso) de aparición reciente_x000d_
+- Estado inconsciente o mucha dificultad para despertarse_x000d_
+- Habla arrastrada o enredada, o dificultad para hablar (de aparición reciente o que empeora)_x000d_
+- Convulsiones de aparición reciente o que empeoran_x000d_
+- Signos de presión arterial baja (muy débil para estar de pie, mareos, aturdimiento, sensación de frío, palidez, piel húmeda y pegajosa)_x000d_
 - Deshidratación (boca y labios secos, no orinar mucho, ojos hundidos)</v>
       </c>
     </row>
@@ -7079,16 +6930,16 @@
         <v>In the last 10 days, have you been tested for the coronavirus that causes COVID-19?</v>
       </c>
       <c r="C286" t="str">
-        <v>지난 10일 동안 COVID-19(코로나바이러스) 검사를 받은 적이 있습니까?</v>
+        <v>지난 10일 동안 COVID-19를 유발하는 코로나 바이러스에 대하여 검사를 받은 적이 있습니까?</v>
       </c>
       <c r="D286" t="str">
-        <v>Trong 10 ngày qua, quý vị có được xét nghiệm COVID-19 (vi rút corona) không?</v>
+        <v>Trong 10 ngày qua, quý vị có được xét nghiệm coronavirus gây ra COVID-19 không?</v>
       </c>
       <c r="E286" t="str">
-        <v>在过去 10 天内，您是否接受过 COVID-19（冠状病毒）检测？</v>
+        <v>在过去 10 天内，您是否接受过引起新冠肺炎的病毒检测？</v>
       </c>
       <c r="F286" t="str">
-        <v>En los últimos 10 días, ¿se ha hecho la prueba del COVID-19 (coronavirus)?</v>
+        <v>En los últimos 10 días, ¿se ha hecho la prueba del coronavirus que causa COVID-19?</v>
       </c>
     </row>
     <row r="287">
@@ -8596,16 +8447,16 @@
         <v>In the last 14 days, have you been tested for the coronavirus that causes COVID-19?</v>
       </c>
       <c r="C353" t="str">
-        <v>지난 14일 동안 COVID-19(코로나바이러스) 검사를 받은 적이 있습니까?</v>
+        <v>지난 14일 동안 COVID-19를 유발하는 코로나 바이러스에 대하여 검사를 받은 적이 있습니까?</v>
       </c>
       <c r="D353" t="str">
-        <v>Trong 14 ngày qua, quý vị có được xét nghiệm COVID-19 (vi rút corona) không?</v>
+        <v>Trong 14 ngày qua, quý vị có được xét nghiệm coronavirus gây ra COVID-19 không?</v>
       </c>
       <c r="E353" t="str">
-        <v>在过去 14 天内，您是否接受过 COVID-19（冠状病毒）检测？</v>
+        <v>在过去 14 天内，您是否接受过引起新冠肺炎的病毒检测？</v>
       </c>
       <c r="F353" t="str">
-        <v>En los últimos 14 días, ¿se ha hecho la prueba del COVID-19 (coronavirus)?</v>
+        <v>En los últimos 14 días, ¿se ha hecho la prueba del coronavirus que causa COVID-19?</v>
       </c>
     </row>
     <row r="354">
@@ -8836,16 +8687,16 @@
         <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="C365" t="str">
-        <v/>
+        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="D365" t="str">
-        <v/>
+        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="E365" t="str">
-        <v/>
+        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="F365" t="str">
-        <v/>
+        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
     </row>
   </sheetData>
@@ -9088,13 +8939,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8881E2C2-C4E8-4A2B-86B7-4B2602EFC712}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{786EC2D4-0B41-46BB-85E7-DE5A2AD5EAA5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0EDBDF7-17FF-45A1-B70B-E3A56C8E8ACF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F48E2D6F-4126-4170-AC33-9DC795EBD5FB}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5047F90E-B69F-4B60-B8FE-4E770991359F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1006642-85A8-40B0-8168-195985B34C02}"/>
 </file>
</xml_diff>

<commit_message>
updating to version 69
 - Updated intro and endcap messages to match CDC's latest masking guidance
 - Consilidated outcome of pediatric core pathway
 - Added optional user experience questions to the end paths of all flows
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F365"/>
+  <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1345,53 +1345,53 @@
         <v>CDC/messages/intro_msg_addnl</v>
       </c>
       <c r="B42" t="str" xml:space="preserve">
-        <v xml:space="preserve">**CDC recommends these steps to reduce your risk of getting and spreading COVID-19:**_x000d__x000d__x000d__x000d_
-- **Get a COVID-19 vaccine** as soon as you are eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d__x000d__x000d__x000d_
-- **Wear** a mask over your nose and mouth.*_x000d__x000d__x000d__x000d_
-- **Stay** at least 6 feet away from people who don’t live with you.*_x000d__x000d__x000d__x000d_
-- **Avoid** crowded areas and poorly ventilated spaces.*_x000d__x000d__x000d__x000d_
-- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">**CDC recommends these steps to reduce your risk of getting and spreading COVID-19:**_x000d_
+- **Get a COVID-19 vaccine** as soon as you can when eligible. Individuals 12 years old and over are currently eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d_
+- **Wear** a mask over your nose and mouth.*_x000d_
+- **Stay** at least 6 feet away from people who don’t live with you.*_x000d_
+- **Avoid** crowded areas and poorly ventilated spaces.*_x000d_
+- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d_
+_x000d_
+###### *Fully vaccinated people can participate in many of the activities that they did before the pandemic. People are considered fully vaccinated 2 weeks after their second dose in a 2-dose series, such as Pfizer or Moderna vaccines, or 2 weeks after a single-dose vaccine, such as Johnson &amp; Johnson’s vaccine. To maximize protection from the Delta variant and prevent possibly spreading to others, wear a mask indoors in public if you are in an area of substantial or high transmission.</v>
+      </c>
+      <c r="C42" t="str" xml:space="preserve">
+        <v xml:space="preserve">**CDC는 COVID-19의 감염과 확산의 위험을 줄이기 위해 다음과 같은 방법을 권장합니다.**_x000d__x000d__x000d__x000d_
+- 자격이 되는대로 **COVID-19 백신을 접종하십시오**. 백신 접종을 모두 마칠 때까지 계속해서 아래의 단계를 매일 따르십시오._x000d__x000d__x000d__x000d_
+- 코와 입을 가리는 마스크를 **착용하십시오**._x000d__x000d__x000d__x000d_
+- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**._x000d__x000d__x000d__x000d_
+- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**._x000d__x000d__x000d__x000d_
+- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d__x000d__x000d__x000d_
 _x000d__x000d__x000d__x000d_
-###### *Fully vaccinated people (those at least 2 weeks past their final dose)  can resume activities without wearing a mask or physically distancing, except where required by federal, state, local, tribal, or territorial laws, rules, and regulations, including local business and workplace guidance.</v>
-      </c>
-      <c r="C42" t="str" xml:space="preserve">
-        <v xml:space="preserve">**CDC는 COVID-19의 감염과 확산의 위험을 줄이기 위해 다음과 같은 방법을 권장합니다.**_x000d__x000d__x000d_
-- 자격이 되는대로 **COVID-19 백신을 접종하십시오**. 백신 접종을 모두 마칠 때까지 계속해서 아래의 단계를 매일 따르십시오._x000d__x000d__x000d_
-- 코와 입을 가리는 마스크를 **착용하십시오**._x000d__x000d__x000d_
-- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**._x000d__x000d__x000d_
-- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**._x000d__x000d__x000d_
-- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d__x000d__x000d_
-_x000d__x000d__x000d_
 ###### *백신 접종을 모두 마친 사람(최종 접종 후 적어도 2주가 지난 사람)은 마스크 착용 또는 물리적인 거리두기 없이 일상생활을 다시 이어나갈 수 있습니다. 단, 지역 사업 또는 직장 지침을 포함하여 연방, 주, 지방, 부족 또는 영토 법률, 규칙 및 규정에서 요구하는 경우는 예외입니다.</v>
       </c>
       <c r="D42" t="str" xml:space="preserve">
-        <v xml:space="preserve">**CDC đề xuất các bước sau để giảm nguy cơ nhiễm và lây lan COVID-19:**_x000d__x000d__x000d_
-- **Tiêm vắc xin COVID-19** ngay khi bạn đủ điều kiện. Tiếp tục làm theo các bước bên dưới mỗi ngày cho đến khi bạn được tiêm vắc xin đầy đủ._x000d__x000d__x000d_
-- **Đeo** khẩu trang lên mũi và miệng của quý vị._x000d__x000d__x000d_
-- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet._x000d__x000d__x000d_
-- **Tránh** những khu vực đông đúc và không gian kém thông thoáng._x000d__x000d__x000d_
-- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước khử trùng tay có ít nhất 60% cồn._x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">**CDC đề xuất các bước sau để giảm nguy cơ nhiễm và lây lan COVID-19:**_x000d__x000d__x000d__x000d_
+- **Tiêm vắc xin COVID-19** ngay khi bạn đủ điều kiện. Tiếp tục làm theo các bước bên dưới mỗi ngày cho đến khi bạn được tiêm vắc xin đầy đủ._x000d__x000d__x000d__x000d_
+- **Đeo** khẩu trang lên mũi và miệng của quý vị._x000d__x000d__x000d__x000d_
+- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet._x000d__x000d__x000d__x000d_
+- **Tránh** những khu vực đông đúc và không gian kém thông thoáng._x000d__x000d__x000d__x000d_
+- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước khử trùng tay có ít nhất 60% cồn._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
 ###### *Những người đã được tiêm vắc xin đầy đủ (ít nhất 2 tuần sau liều cuối cùng) có thể tiếp tục các hoạt động mà không cần đeo khẩu trang hoặc giãn cách, trừ trường hợp được yêu cầu bởi luật, quy tắc và các quy định của liên bang, tiểu bang, địa phương, bộ lạc hoặc lãnh thổ, bao gồm hướng dẫn nơi làm việc và kinh doanh tại địa phương.</v>
       </c>
       <c r="E42" t="str" xml:space="preserve">
-        <v xml:space="preserve">**疾控中心建议采取这些步骤，以减少感染和传播 COVID-19 的风险：**_x000d__x000d__x000d_
-- 只有您有资格请尽快**接种 COVID-19 疫苗**。每天继续遵循以下步骤，直到您完全接种疫苗。_x000d__x000d__x000d_
-- **佩戴**口罩遮住您的口鼻。_x000d__x000d__x000d_
-- 与不和您住在一起的人**保持**至少 6 英尺的距离。_x000d__x000d__x000d_
-- **避免**去拥挤的地方和通风不良的空间。_x000d__x000d__x000d_
-- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。_x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">**疾控中心建议采取这些步骤，以减少感染和传播 COVID-19 的风险：**_x000d__x000d__x000d__x000d_
+- 只有您有资格请尽快**接种 COVID-19 疫苗**。每天继续遵循以下步骤，直到您完全接种疫苗。_x000d__x000d__x000d__x000d_
+- **佩戴**口罩遮住您的口鼻。_x000d__x000d__x000d__x000d_
+- 与不和您住在一起的人**保持**至少 6 英尺的距离。_x000d__x000d__x000d__x000d_
+- **避免**去拥挤的地方和通风不良的空间。_x000d__x000d__x000d__x000d_
+- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。_x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
 ###### *已完全接种的人（即接种完最后一剂之后至少 2 周的人）可以恢复活动而无需佩戴口罩或保持社交距离，除非联邦、州、地方、部落或领地的法律、法规和规章（包括当地的商业和工作场所指南）有此类要求。</v>
       </c>
       <c r="F42" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Los CDC recomiendan que tome estas medidas para reducir el riesgo de contraer o propagar el COVID-19:**_x000d__x000d__x000d_
-- **Vacúnese contra el COVID-19** tan pronto como sea elegible. Continúe tomando las siguientes medidas todos los días hasta que esté completamente vacunado._x000d__x000d__x000d_
-- **Póngase** una mascarilla que le cubra la nariz y la boca._x000d__x000d__x000d_
-- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted._x000d__x000d__x000d_
-- **Evite** lugares con mucha gente y áreas con poca ventilación._x000d__x000d__x000d_
-- **Lávese** las manos a menudo con agua y jabón o use un desinfectante de manos que contenga al menos un 60 % de alcohol._x000d__x000d__x000d_
-_x000d__x000d__x000d_
+        <v xml:space="preserve">**Los CDC recomiendan que tome estas medidas para reducir el riesgo de contraer o propagar el COVID-19:**_x000d__x000d__x000d__x000d_
+- **Vacúnese contra el COVID-19** tan pronto como sea elegible. Continúe tomando las siguientes medidas todos los días hasta que esté completamente vacunado._x000d__x000d__x000d__x000d_
+- **Póngase** una mascarilla que le cubra la nariz y la boca._x000d__x000d__x000d__x000d_
+- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted._x000d__x000d__x000d__x000d_
+- **Evite** lugares con mucha gente y áreas con poca ventilación._x000d__x000d__x000d__x000d_
+- **Lávese** las manos a menudo con agua y jabón o use un desinfectante de manos que contenga al menos un 60 % de alcohol._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
 ###### *Las personas completamente vacunadas (aquellas que recibieron la última dosis hace al menos 2 semanas) pueden reanudar actividades sin usar mascarilla ni mantener distanciamiento físico, excepto donde lo requieran las leyes, normas y regulaciones federales, estatales, locales, tribales o territoriales, incluidas las directrices de empresas o negocios y lugares de trabajo locales.</v>
       </c>
     </row>
@@ -5125,120 +5125,120 @@
         <v>CDC/messages/intro_msg</v>
       </c>
       <c r="B205" t="str" xml:space="preserve">
-        <v xml:space="preserve">Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the level of medical care you should seek. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-If you are experiencing a life-threatening emergency, please call 911 immediately._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-If you are not experiencing a life-threatening emergency, let’s get started._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**CDC recommends these steps to reduce your risk of getting and spreading COVID-19:**_x000d__x000d__x000d_
-- **Get a COVID-19 vaccine** as soon as you are eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d__x000d__x000d_
-- **Wear** a mask over your nose and mouth.*_x000d__x000d__x000d_
-- **Stay** at least 6 feet away from people who don’t live with you.*_x000d__x000d__x000d_
-- **Avoid** crowded areas and poorly ventilated spaces.*_x000d__x000d__x000d_
-- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### *Fully vaccinated people (those at least 2 weeks past their final dose)  can resume activities without wearing a mask or physically distancing, except where required by federal, state, local, tribal, or territorial laws, rules, and regulations, including local business and workplace guidance.</v>
-      </c>
-      <c r="C205" t="str" xml:space="preserve">
-        <v xml:space="preserve">안녕하세요? 저는 Clara입니다. 몇 가지 질문을 하겠습니다. 귀하의 답변을 통해 귀하에게 어느 정도 수준의 진료가 필요한지 조언할 것입니다. 다른 사람을 위해 응답하고 계시다면 본인이 그 사람인 것처럼 모든 질문에 답하십시오. 처음부터 다시 시작해야 한다면 페이지를 새로 고치고 다시 시작하십시오._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-생명을 위협하는 응급 상황이 발생하면 즉시 911에 전화하십시오._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-생명을 위협하는 응급 상황을 겪고 있지 않다면, 이제 시작하겠습니다._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**CDC는 COVID-19의 감염과 확산의 위험을 줄이기 위해 다음과 같은 방법을 권장합니다.**_x000d__x000d__x000d_
-- 자격이 되는대로 **COVID-19 백신을 접종하십시오**. 백신 접종을 모두 마칠 때까지 계속해서 아래의 단계를 매일 따르십시오._x000d__x000d__x000d_
-- 코와 입을 가리는 마스크를 **착용하십시오**._x000d__x000d__x000d_
-- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**._x000d__x000d__x000d_
-- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**._x000d__x000d__x000d_
-- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### *백신 접종을 모두 마친 사람(최종 접종 후 적어도 2주가 지난 사람)은 마스크 착용 또는 물리적인 거리두기 없이 일상생활을 다시 이어나갈 수 있습니다. 단, 지역 사업 또는 직장 지침을 포함하여 연방, 주, 지방, 부족 또는 영토 법률, 규칙 및 규정에서 요구하는 경우는 예외입니다.</v>
-      </c>
-      <c r="D205" t="str" xml:space="preserve">
-        <v xml:space="preserve">Xin chào, tôi là Clara. Tôi sẽ hỏi quý vị một số câu hỏi. Tôi sẽ sử dụng câu trả lời của quý vị để cung cấp cho quý vị lời khuyên về mức độ chăm sóc y tế mà quý vị nên tìm kiếm.   Nếu trả lời cho người khác, vui lòng trả lời tất cả các câu hỏi như thể quý vị là họ. Nếu quý vị cần bắt đầu lại, hãy làm mới trang và bắt đầu lại._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-Nếu quý vị đang gặp trường hợp khẩn cấp đe dọa tính mạng, vui lòng gọi 911 ngay lập tức.   _x000d__x000d__x000d_
-_x000d__x000d__x000d_
-Nếu quý vị không đang trong tình trạng khẩn cấp đe dọa tính mạng, hãy bắt đầu._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**CDC đề xuất các bước sau để giảm nguy cơ nhiễm và lây lan COVID-19:**_x000d__x000d__x000d_
-- **Tiêm vắc xin COVID-19** ngay khi bạn đủ điều kiện. Tiếp tục làm theo các bước bên dưới mỗi ngày cho đến khi bạn được tiêm vắc xin đầy đủ._x000d__x000d__x000d_
-- **Đeo** khẩu trang lên mũi và miệng của quý vị._x000d__x000d__x000d_
-- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet._x000d__x000d__x000d_
-- **Tránh** những khu vực đông đúc và không gian kém thông thoáng._x000d__x000d__x000d_
-- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước khử trùng tay có ít nhất 60% cồn._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### *Những người đã được tiêm vắc xin đầy đủ (ít nhất 2 tuần sau liều cuối cùng) có thể tiếp tục các hoạt động mà không cần đeo khẩu trang hoặc giãn cách, trừ trường hợp được yêu cầu bởi luật, quy tắc và các quy định của liên bang, tiểu bang, địa phương, bộ lạc hoặc lãnh thổ, bao gồm hướng dẫn nơi làm việc và kinh doanh tại địa phương.</v>
-      </c>
-      <c r="E205" t="str" xml:space="preserve">
-        <v xml:space="preserve">嗨，我是 Clara。我要问您一些问题。我将使用您的回答为您提供关于您应寻求的医疗护理水平的建议。如果替别人回答，请把所有的问题都当作自己的问题来回答。如果您需要重新开始，请刷新页面并重新开始。_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-如果您出现危及生命的紧急情况，请立即拨打 911。_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-如果您没有出现危及生命的紧急情况，我们开始吧。_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**疾控中心建议采取这些步骤，以减少感染和传播 COVID-19 的风险：**_x000d__x000d__x000d_
-- 只有您有资格请尽快**接种 COVID-19 疫苗**。每天继续遵循以下步骤，直到您完全接种疫苗。_x000d__x000d__x000d_
-- **佩戴**口罩遮住您的口鼻。_x000d__x000d__x000d_
-- 与不和您住在一起的人**保持**至少 6 英尺的距离。_x000d__x000d__x000d_
-- **避免**去拥挤的地方和通风不良的空间。_x000d__x000d__x000d_
-- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。_x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### *已完全接种的人（即接种完最后一剂之后至少 2 周的人）可以恢复活动而无需佩戴口罩或保持社交距离，除非联邦、州、地方、部落或领地的法律、法规和规章（包括当地的商业和工作场所指南）有此类要求。</v>
-      </c>
-      <c r="F205" t="str" xml:space="preserve">
-        <v xml:space="preserve">Hola, me llamo Clara. Le voy a hacer algunas preguntas. Usaré sus respuestas para aconsejarle sobre el nivel de atención médica que debe buscar. Si está respondiendo por alguien más, responda todas las preguntas como si fuera esa persona. Si necesita comenzar de nuevo, refresque la página y comience otra vez._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-Si tiene una emergencia potencialmente mortal, llame al 911 inmediatamente. _x000d__x000d__x000d_
-_x000d__x000d__x000d_
-Si no tiene una emergencia potencialmente mortal, comencemos._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-**Los CDC recomiendan que tome estas medidas para reducir el riesgo de contraer o propagar el COVID-19:**_x000d__x000d__x000d_
-- **Vacúnese contra el COVID-19** tan pronto como sea elegible. Continúe tomando las siguientes medidas todos los días hasta que esté completamente vacunado._x000d__x000d__x000d_
-- **Póngase** una mascarilla que le cubra la nariz y la boca._x000d__x000d__x000d_
-- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted._x000d__x000d__x000d_
-- **Evite** lugares con mucha gente y áreas con poca ventilación._x000d__x000d__x000d_
-- **Lávese** las manos a menudo con agua y jabón o use un desinfectante de manos que contenga al menos un 60 % de alcohol._x000d__x000d__x000d_
-_x000d__x000d__x000d_
-###### *Las personas completamente vacunadas (aquellas que recibieron la última dosis hace al menos 2 semanas) pueden reanudar actividades sin usar mascarilla ni mantener distanciamiento físico, excepto donde lo requieran las leyes, normas y regulaciones federales, estatales, locales, tribales o territoriales, incluidas las directrices de empresas o negocios y lugares de trabajo locales.</v>
-      </c>
-    </row>
-    <row r="206" xml:space="preserve">
-      <c r="A206" t="str">
-        <v>CDC/messages/instruct_msg</v>
-      </c>
-      <c r="B206" t="str">
-        <v>During the assessment, you can refresh the page if you need to start again.</v>
-      </c>
-      <c r="C206" t="str">
-        <v>평가 중 다시 시작해야 하는 경우 페이지를 새로 고치면 됩니다.</v>
-      </c>
-      <c r="D206" t="str" xml:space="preserve">
-        <v xml:space="preserve">Trong quá trình đánh giá, quý vị có thể làm mới trang nếu quý vị cần bắt đầu lại_x000d_._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-</v>
-      </c>
-      <c r="E206" t="str">
-        <v>评估期间，如需重新开始，可刷新页面。</v>
-      </c>
-      <c r="F206" t="str">
-        <v>Durante la evaluación, puede actualizar la página si necesita empezar de nuevo.</v>
-      </c>
-    </row>
-    <row r="207" xml:space="preserve">
-      <c r="A207" t="str">
-        <v>CDC/messages/endcap</v>
-      </c>
-      <c r="B207" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Steps to follow every day:**_x000d_
-- **Get a COVID-19 vaccine** as soon as you are eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d_
+        <v xml:space="preserve">Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the level of medical care you should seek. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again._x000d_
+_x000d_
+If you are experiencing a life-threatening emergency, please call 911 immediately._x000d_
+_x000d_
+If you are not experiencing a life-threatening emergency, let’s get started._x000d_
+_x000d_
+**CDC recommends these steps to reduce your risk of getting and spreading COVID-19:**_x000d_
+- **Get a COVID-19 vaccine** as soon as you can when eligible. Individuals 12 years old and over are currently eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d_
 - **Wear** a mask over your nose and mouth.*_x000d_
 - **Stay** at least 6 feet away from people who don’t live with you.*_x000d_
 - **Avoid** crowded areas and poorly ventilated spaces.*_x000d_
 - **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d_
 _x000d_
-###### *Fully vaccinated people (those at least 2 weeks past their final dose)  can resume activities without wearing a mask or physically distancing, except where required by federal, state, local, tribal, or territorial laws, rules, and regulations, including local business and workplace guidance. _x000d_
+###### *Fully vaccinated people can participate in many of the activities that they did before the pandemic. People are considered fully vaccinated 2 weeks after their second dose in a 2-dose series, such as Pfizer or Moderna vaccines, or 2 weeks after a single-dose vaccine, such as Johnson &amp; Johnson’s vaccine. To maximize protection from the Delta variant and prevent possibly spreading to others, wear a mask indoors in public if you are in an area of substantial or high transmission.</v>
+      </c>
+      <c r="C205" t="str" xml:space="preserve">
+        <v xml:space="preserve">안녕하세요? 저는 Clara입니다. 몇 가지 질문을 하겠습니다. 귀하의 답변을 통해 귀하에게 어느 정도 수준의 진료가 필요한지 조언할 것입니다. 다른 사람을 위해 응답하고 계시다면 본인이 그 사람인 것처럼 모든 질문에 답하십시오. 처음부터 다시 시작해야 한다면 페이지를 새로 고치고 다시 시작하십시오._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+생명을 위협하는 응급 상황이 발생하면 즉시 911에 전화하십시오._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+생명을 위협하는 응급 상황을 겪고 있지 않다면, 이제 시작하겠습니다._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+**CDC는 COVID-19의 감염과 확산의 위험을 줄이기 위해 다음과 같은 방법을 권장합니다.**_x000d__x000d__x000d__x000d_
+- 자격이 되는대로 **COVID-19 백신을 접종하십시오**. 백신 접종을 모두 마칠 때까지 계속해서 아래의 단계를 매일 따르십시오._x000d__x000d__x000d__x000d_
+- 코와 입을 가리는 마스크를 **착용하십시오**._x000d__x000d__x000d__x000d_
+- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**._x000d__x000d__x000d__x000d_
+- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**._x000d__x000d__x000d__x000d_
+- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+###### *백신 접종을 모두 마친 사람(최종 접종 후 적어도 2주가 지난 사람)은 마스크 착용 또는 물리적인 거리두기 없이 일상생활을 다시 이어나갈 수 있습니다. 단, 지역 사업 또는 직장 지침을 포함하여 연방, 주, 지방, 부족 또는 영토 법률, 규칙 및 규정에서 요구하는 경우는 예외입니다.</v>
+      </c>
+      <c r="D205" t="str" xml:space="preserve">
+        <v xml:space="preserve">Xin chào, tôi là Clara. Tôi sẽ hỏi quý vị một số câu hỏi. Tôi sẽ sử dụng câu trả lời của quý vị để cung cấp cho quý vị lời khuyên về mức độ chăm sóc y tế mà quý vị nên tìm kiếm.   Nếu trả lời cho người khác, vui lòng trả lời tất cả các câu hỏi như thể quý vị là họ. Nếu quý vị cần bắt đầu lại, hãy làm mới trang và bắt đầu lại._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+Nếu quý vị đang gặp trường hợp khẩn cấp đe dọa tính mạng, vui lòng gọi 911 ngay lập tức.   _x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+Nếu quý vị không đang trong tình trạng khẩn cấp đe dọa tính mạng, hãy bắt đầu._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+**CDC đề xuất các bước sau để giảm nguy cơ nhiễm và lây lan COVID-19:**_x000d__x000d__x000d__x000d_
+- **Tiêm vắc xin COVID-19** ngay khi bạn đủ điều kiện. Tiếp tục làm theo các bước bên dưới mỗi ngày cho đến khi bạn được tiêm vắc xin đầy đủ._x000d__x000d__x000d__x000d_
+- **Đeo** khẩu trang lên mũi và miệng của quý vị._x000d__x000d__x000d__x000d_
+- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet._x000d__x000d__x000d__x000d_
+- **Tránh** những khu vực đông đúc và không gian kém thông thoáng._x000d__x000d__x000d__x000d_
+- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước khử trùng tay có ít nhất 60% cồn._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+###### *Những người đã được tiêm vắc xin đầy đủ (ít nhất 2 tuần sau liều cuối cùng) có thể tiếp tục các hoạt động mà không cần đeo khẩu trang hoặc giãn cách, trừ trường hợp được yêu cầu bởi luật, quy tắc và các quy định của liên bang, tiểu bang, địa phương, bộ lạc hoặc lãnh thổ, bao gồm hướng dẫn nơi làm việc và kinh doanh tại địa phương.</v>
+      </c>
+      <c r="E205" t="str" xml:space="preserve">
+        <v xml:space="preserve">嗨，我是 Clara。我要问您一些问题。我将使用您的回答为您提供关于您应寻求的医疗护理水平的建议。如果替别人回答，请把所有的问题都当作自己的问题来回答。如果您需要重新开始，请刷新页面并重新开始。_x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+如果您出现危及生命的紧急情况，请立即拨打 911。_x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+如果您没有出现危及生命的紧急情况，我们开始吧。_x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+**疾控中心建议采取这些步骤，以减少感染和传播 COVID-19 的风险：**_x000d__x000d__x000d__x000d_
+- 只有您有资格请尽快**接种 COVID-19 疫苗**。每天继续遵循以下步骤，直到您完全接种疫苗。_x000d__x000d__x000d__x000d_
+- **佩戴**口罩遮住您的口鼻。_x000d__x000d__x000d__x000d_
+- 与不和您住在一起的人**保持**至少 6 英尺的距离。_x000d__x000d__x000d__x000d_
+- **避免**去拥挤的地方和通风不良的空间。_x000d__x000d__x000d__x000d_
+- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。_x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+###### *已完全接种的人（即接种完最后一剂之后至少 2 周的人）可以恢复活动而无需佩戴口罩或保持社交距离，除非联邦、州、地方、部落或领地的法律、法规和规章（包括当地的商业和工作场所指南）有此类要求。</v>
+      </c>
+      <c r="F205" t="str" xml:space="preserve">
+        <v xml:space="preserve">Hola, me llamo Clara. Le voy a hacer algunas preguntas. Usaré sus respuestas para aconsejarle sobre el nivel de atención médica que debe buscar. Si está respondiendo por alguien más, responda todas las preguntas como si fuera esa persona. Si necesita comenzar de nuevo, refresque la página y comience otra vez._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+Si tiene una emergencia potencialmente mortal, llame al 911 inmediatamente. _x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+Si no tiene una emergencia potencialmente mortal, comencemos._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+**Los CDC recomiendan que tome estas medidas para reducir el riesgo de contraer o propagar el COVID-19:**_x000d__x000d__x000d__x000d_
+- **Vacúnese contra el COVID-19** tan pronto como sea elegible. Continúe tomando las siguientes medidas todos los días hasta que esté completamente vacunado._x000d__x000d__x000d__x000d_
+- **Póngase** una mascarilla que le cubra la nariz y la boca._x000d__x000d__x000d__x000d_
+- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted._x000d__x000d__x000d__x000d_
+- **Evite** lugares con mucha gente y áreas con poca ventilación._x000d__x000d__x000d__x000d_
+- **Lávese** las manos a menudo con agua y jabón o use un desinfectante de manos que contenga al menos un 60 % de alcohol._x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d_
+###### *Las personas completamente vacunadas (aquellas que recibieron la última dosis hace al menos 2 semanas) pueden reanudar actividades sin usar mascarilla ni mantener distanciamiento físico, excepto donde lo requieran las leyes, normas y regulaciones federales, estatales, locales, tribales o territoriales, incluidas las directrices de empresas o negocios y lugares de trabajo locales.</v>
+      </c>
+    </row>
+    <row r="206" xml:space="preserve">
+      <c r="A206" t="str">
+        <v>CDC/messages/instruct_msg</v>
+      </c>
+      <c r="B206" t="str">
+        <v>During the assessment, you can refresh the page if you need to start again.</v>
+      </c>
+      <c r="C206" t="str">
+        <v>평가 중 다시 시작해야 하는 경우 페이지를 새로 고치면 됩니다.</v>
+      </c>
+      <c r="D206" t="str" xml:space="preserve">
+        <v xml:space="preserve">Trong quá trình đánh giá, quý vị có thể làm mới trang nếu quý vị cần bắt đầu lại_x000d_._x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+</v>
+      </c>
+      <c r="E206" t="str">
+        <v>评估期间，如需重新开始，可刷新页面。</v>
+      </c>
+      <c r="F206" t="str">
+        <v>Durante la evaluación, puede actualizar la página si necesita empezar de nuevo.</v>
+      </c>
+    </row>
+    <row r="207" xml:space="preserve">
+      <c r="A207" t="str">
+        <v>CDC/messages/endcap</v>
+      </c>
+      <c r="B207" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Steps to follow every day:**_x000d_
+- **Get a COVID-19 vaccine** as soon as you can when eligible. Individuals 12 years old and over are currently eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d_
+- **Wear** a mask over your nose and mouth.*_x000d_
+- **Stay** at least 6 feet away from people who don’t live with you.*_x000d_
+- **Avoid** crowded areas and poorly ventilated spaces.*_x000d_
+- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d_
+_x000d_
+###### *Fully vaccinated people can participate in many of the activities that they did before the pandemic. People are considered fully vaccinated 2 weeks after their second dose in a 2-dose series, such as Pfizer or Moderna vaccines, or 2 weeks after a single-dose vaccine, such as Johnson &amp; Johnson’s vaccine. To maximize protection from the Delta variant and prevent possibly spreading to others, wear a mask indoors in public if you are in an area of substantial or high transmission. _x000d_
 _x000d_
 **Click the links below for more information on:**_x000d_
 - [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
@@ -5254,93 +5254,95 @@
 - [Find COVID-19 vaccine locations near you](https://www.vaccines.gov/)</v>
       </c>
       <c r="C207" t="str" xml:space="preserve">
-        <v xml:space="preserve">**매일 따라야 할 단계:**_x000d_
-- 자격이 되는대로 **COVID-19 백신을 접종하십시오**. 백신 접종을 모두 마칠 때까지 계속해서 아래의 단계를 매일 따르십시오.*_x000d_
-- 코와 입을 가리는 마스크를 **착용하십시오**.*_x000d_
-- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**.*_x000d_
-- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**.*_x000d_
-- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d_
+        <v xml:space="preserve">**매일 따라야 할 단계:**_x000d__x000d_
+- 자격이 되는대로 **COVID-19 백신을 접종하십시오**. 백신 접종을 모두 마칠 때까지 계속해서 아래의 단계를 매일 따르십시오.*_x000d__x000d_
+- 코와 입을 가리는 마스크를 **착용하십시오**.*_x000d__x000d_
+- 함께 거주하지 않는 다른 사람과 최소 6피트의 간격을 **유지하십시오**.*_x000d__x000d_
+- 밀집된 장소와 통풍이 안 되는 공간을 **피하십시오**.*_x000d__x000d_
+- 비누와 물로 손을 자주 **씻거나** 알코올이 60% 이상 함유된 손 세정제를 사용하십시오._x000d__x000d_
+_x000d__x000d_
+###### *백신 접종을 모두 마친 사람(최종 접종 후 적어도 2주가 지난 사람)은 마스크 착용 또는 물리적인 거리두기 없이 일상생활을 다시 이어나갈 수 있습니다. 단, 지역 사업 또는 직장 지침을 포함하여 연방, 주, 지방, 부족 또는 영토 법률, 규칙 및 규정에서 요구하는 경우는 예외입니다. _x000d__x000d_
+_x000d__x000d_
+**자세한 정보를 보려면 아래 링크를 클릭하십시오.**_x000d__x000d_
+- [COVID-19 증상](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d_
+- [COVID 이후 증상](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d__x000d_
+- [검사를 언제 받아야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d_
+- [검사 결과가 의미하는 것](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d_
+- [자신과 다른 사람을 질병으로부터 보호하십시오](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d_
+- [언제 그리고 얼마나 오래 격리 또는 분리해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [COVID-19에 걸린 사람 주변에 있었다면 무엇을 해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [아플 때 자신을 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d_
+- [아픈 사람 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d__x000d_
+- [COVID-19 백신 알아보기](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d_
+- [귀하 근처의 COVID-19 백신 접종 장소 찾기](https://www.vaccines.gov/)</v>
+      </c>
+      <c r="D207" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Các bước cần tuân theo hàng ngày:**_x000d__x000d_
+- **Tiêm vắc xin COVID-19** ngay khi bạn đủ điều kiện. Tiếp tục làm theo các bước bên dưới mỗi ngày cho đến khi bạn được tiêm vắc xin đầy đủ.*_x000d__x000d_
+- **Đeo** khẩu trang che mũi và miệng của quý vị.*_x000d__x000d_
+- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet.*_x000d__x000d_
+- **Tránh** những khu vực đông đúc và không gian kém thông thoáng.*_x000d__x000d_
+- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước sát khuẩn tay có ít nhất 60% cồn._x000d__x000d_
+_x000d__x000d_
+###### *Những người đã được tiêm vắc xin đầy đủ (ít nhất 2 tuần sau liều cuối cùng) có thể tiếp tục các hoạt động mà không cần đeo khẩu trang hoặc giãn cách, trừ trường hợp được yêu cầu bởi luật, quy tắc và các quy định của liên bang, tiểu bang, địa phương, bộ lạc hoặc lãnh thổ, bao gồm hướng dẫn của nơi làm việc và kinh doanh tại địa phương.  _x000d__x000d_
+_x000d__x000d_
+**Nhấp vào liên kết bên dưới để biết thêm thông tin về:**_x000d__x000d_
+- [Các triệu chứng COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html))_x000d__x000d_
+- [Điều kiện sau COVID](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d__x000d_
+- [Khi nào cần xét nghiệm](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d_
+- [Kết quả xét nghiệm của quý vị có ý nghĩa gì](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pd)_x000d__x000d_
+- [Bảo vệ bản thân và những người khác khỏi bị bệnh](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d__x000d_
+- [Khi nào cần cách ly và trong bao lâu](https://www.cdc.gov/coroavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [Phải làm gì nếu quý vị ở gần người mắc COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [Chăm sóc bản thân khi quý vị bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d_
+- [Chăm sóc người khác bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d__x000d_
+- [Tìm hiểu thêm về Vắc-xin Ngừa COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d_
+- [Tìm địa điểm tiêm vắc-xin ngừa COVID-19 gần quý vị](https://www.vaccines.gov/)</v>
+      </c>
+      <c r="E207" t="str" xml:space="preserve">
+        <v xml:space="preserve">**每天要遵循的步骤：**_x000d__x000d_
+- 只有您有资格请尽快**接种 COVID-19 疫苗**。每天继续遵循以下步骤，直到您完全接种疫苗。*_x000d__x000d_
+- **佩戴**口罩遮住您的口鼻。*_x000d__x000d_
+- 与不和您住在一起的人**保持**至少 6 英尺的距离。*_x000d__x000d_
+- **避免**去拥挤的地方和通风不良的空间。*_x000d__x000d_
+- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。_x000d__x000d_
+_x000d__x000d_
+###### *已完全接种的人（即接种完最后一剂之后至少 2 周的人）可以恢复活动而无需佩戴口罩或保持社交距离，除非联邦、州、地方、部落或领地的法律、法规和规章（包括当地的商业和工作场所指南）有此类要求。 _x000d__x000d_
+_x000d__x000d_
+**点击以下链接了解更多信息：**_x000d__x000d_
+- [新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d__x000d_
+- [新冠肺炎后的病症](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d__x000d_
+- [何时进行检测](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d__x000d_
+- [您的测试结果是什么意思](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d__x000d_
+- [保护自己和他人免于生病](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d__x000d_
+- [何时进行检疫隔离或隔离以及隔离多长时间](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [如果您身边的人患有新冠肺炎，您该怎么办](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d__x000d_
+- [生病时照顾好自己](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d__x000d_
+- [照顾生病的他人](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d__x000d_
+- [了解新冠肺炎疫苗](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d_
+- [查找您附近的新冠肺炎疫苗接种位置](https://www.vaccines.gov/)</v>
+      </c>
+      <c r="F207" t="str" xml:space="preserve">
+        <v xml:space="preserve">**Medidas para tomar todos los días:**_x000d_
+- **Vacúnese contra el COVID-19** tan pronto como sea elegible. Continúe tomando las siguientes medidas todos los días hasta que esté completamente vacunado.*_x000d_
+- **Póngase** una mascarilla que le cubra la nariz y la boca.*_x000d_
+- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted.*_x000d_
+- **Evite** lugares con mucha gente y áreas con poca ventilación.*_x000d_
+- **Lávese** las manos a menudo con agua y jabón, o use un desinfectante de manos que contenga al menos un 60 % de alcohol._x000d_
 _x000d_
-###### *백신 접종을 모두 마친 사람(최종 접종 후 적어도 2주가 지난 사람)은 마스크 착용 또는 물리적인 거리두기 없이 일상생활을 다시 이어나갈 수 있습니다. 단, 지역 사업 또는 직장 지침을 포함하여 연방, 주, 지방, 부족 또는 영토 법률, 규칙 및 규정에서 요구하는 경우는 예외입니다. _x000d_
+###### *Las personas completamente vacunadas (aquellas que recibieron la última dosis hace al menos 2 semanas) pueden reanudar actividades sin usar mascarilla ni mantener distanciamiento físico, excepto donde lo requieran las leyes, normas y regulaciones federales, estatales, locales, tribales o territoriales, incluidas las directrices de empresas o negocios, y lugares de trabajo locales. _x000d_
 _x000d_
-**자세한 정보를 보려면 아래 링크를 클릭하십시오.**_x000d_
-- [COVID-19 증상](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
-- [COVID 이후 증상](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
-- [검사를 언제 받아야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
-- [검사 결과가 의미하는 것](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
-- [자신과 다른 사람을 질병으로부터 보호하십시오](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d_
-- [언제 그리고 얼마나 오래 격리 또는 분리해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
-- [COVID-19에 걸린 사람 주변에 있었다면 무엇을 해야 하는지](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
-- [아플 때 자신을 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
-- [아픈 사람 돌보기](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
-- [COVID-19 백신 알아보기](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [귀하 근처의 COVID-19 백신 접종 장소 찾기](https://www.vaccines.gov/)</v>
-      </c>
-      <c r="D207" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Các bước cần tuân theo hàng ngày:**_x000d_
-- **Tiêm vắc xin COVID-19** ngay khi bạn đủ điều kiện. Tiếp tục làm theo các bước bên dưới mỗi ngày cho đến khi bạn được tiêm vắc xin đầy đủ.*_x000d_
-- **Đeo** khẩu trang che mũi và miệng của quý vị.*_x000d_
-- **Ở** cách xa những người không sống cùng quý vị ít nhất 6 feet.*_x000d_
-- **Tránh** những khu vực đông đúc và không gian kém thông thoáng.*_x000d_
-- **Rửa** tay thường xuyên bằng xà phòng và nước, hoặc sử dụng nước sát khuẩn tay có ít nhất 60% cồn._x000d_
-_x000d_
-###### *Những người đã được tiêm vắc xin đầy đủ (ít nhất 2 tuần sau liều cuối cùng) có thể tiếp tục các hoạt động mà không cần đeo khẩu trang hoặc giãn cách, trừ trường hợp được yêu cầu bởi luật, quy tắc và các quy định của liên bang, tiểu bang, địa phương, bộ lạc hoặc lãnh thổ, bao gồm hướng dẫn của nơi làm việc và kinh doanh tại địa phương.  _x000d_
-_x000d_
-**Nhấp vào liên kết bên dưới để biết thêm thông tin về:**_x000d_
-- [Các triệu chứng COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html))_x000d_
-- [Điều kiện sau COVID](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
-- [Khi nào cần xét nghiệm](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
-- [Kết quả xét nghiệm của quý vị có ý nghĩa gì](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pd)_x000d_
-- [Bảo vệ bản thân và những người khác khỏi bị bệnh](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d_
-- [Khi nào cần cách ly và trong bao lâu](https://www.cdc.gov/coroavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
-- [Phải làm gì nếu quý vị ở gần người mắc COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
-- [Chăm sóc bản thân khi quý vị bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
-- [Chăm sóc người khác bị ốm](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
-- [Tìm hiểu thêm về Vắc-xin Ngừa COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [Tìm địa điểm tiêm vắc-xin ngừa COVID-19 gần quý vị](https://www.vaccines.gov/)</v>
-      </c>
-      <c r="E207" t="str" xml:space="preserve">
-        <v xml:space="preserve">**每天要遵循的步骤：**_x000d_
-- 只有您有资格请尽快**接种 COVID-19 疫苗**。每天继续遵循以下步骤，直到您完全接种疫苗。*_x000d_
-- **佩戴**口罩遮住您的口鼻。*_x000d_
-- 与不和您住在一起的人**保持**至少 6 英尺的距离。*_x000d_
-- **避免**去拥挤的地方和通风不良的空间。*_x000d_
-- 经常用肥皂和水**洗**手，或者使用酒精含量至少60%的洗手液。_x000d_
-_x000d_
-###### *已完全接种的人（即接种完最后一剂之后至少 2 周的人）可以恢复活动而无需佩戴口罩或保持社交距离，除非联邦、州、地方、部落或领地的法律、法规和规章（包括当地的商业和工作场所指南）有此类要求。 _x000d_
-_x000d_
-**点击以下链接了解更多信息：**_x000d_
-- [新冠肺炎症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
-- [新冠肺炎后的病症](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
-- [何时进行检测](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
-- [您的测试结果是什么意思](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
-- [保护自己和他人免于生病](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html):_x000d_
-- [何时进行检疫隔离或隔离以及隔离多长时间](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
-- [如果您身边的人患有新冠肺炎，您该怎么办](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
-- [生病时照顾好自己](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
-- [照顾生病的他人](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
-- [了解新冠肺炎疫苗](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [查找您附近的新冠肺炎疫苗接种位置](https://www.vaccines.gov/)</v>
-      </c>
-      <c r="F207" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Medidas para tomar todos los días:**
-- **Vacúnese contra el COVID-19** tan pronto como sea elegible. Continúe tomando las siguientes medidas todos los días hasta que esté completamente vacunado.*
-- **Póngase** una mascarilla que le cubra la nariz y la boca.*
-- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted.*
-- **Evite** lugares con mucha gente y áreas con poca ventilación.*
-- **Lávese** las manos a menudo con agua y jabón, o use un desinfectante de manos que contenga al menos un 60 % de alcohol.
-###### *Las personas completamente vacunadas (aquellas que recibieron la última dosis hace al menos 2 semanas) pueden reanudar actividades sin usar mascarilla ni mantener distanciamiento físico, excepto donde lo requieran las leyes, normas y regulaciones federales, estatales, locales, tribales o territoriales, incluidas las directrices de empresas o negocios, y lugares de trabajo locales. 
-**Haga clic en los enlaces a continuación para obtener más información sobre lo siguiente:**
-- [Síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)
-- [Afecciones posteriores al COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)
-- [[Cuándo hacerse la prueba](https://espanol.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html)
-- [Lo que significan los resultados de su prueba](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)
-- [Cómo protegerse a sí mismo y a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)
-- [Cuándo ponerse en cuarentena o aislarse, y por cuánto tiempo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
-- [Qué hacer si estuvo cerca de alguien con COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
-- [Cómo cuidarse cuando esté enfermo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)
-- [Cómo cuidar a otra persona que esté enferma](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)
-- [Infórmese sobre las vacunas contra el COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)
+**Haga clic en los enlaces a continuación para obtener más información sobre lo siguiente:**_x000d_
+- [Síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
+- [Afecciones posteriores al COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
+- [[Cuándo hacerse la prueba](https://espanol.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html)_x000d_
+- [Lo que significan los resultados de su prueba](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
+- [Cómo protegerse a sí mismo y a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d_
+- [Cuándo ponerse en cuarentena o aislarse, y por cuánto tiempo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [Qué hacer si estuvo cerca de alguien con COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
+- [Cómo cuidarse cuando esté enfermo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
+- [Cómo cuidar a otra persona que esté enferma](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
+- [Infórmese sobre las vacunas contra el COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
 - [Encuentre sitios de vacunación contra el COVID-19 cercanos](https://www.vacunas.gov/)</v>
       </c>
     </row>
@@ -5355,7 +5357,7 @@
 _x000d_
 To continue using this tool, please agree that you have read and understood the contents of this disclaimer._x000d_
 _x000d_
-###### ver68 (06.21.2021)</v>
+###### ver69 (08.03.2021)</v>
       </c>
       <c r="C208" t="str" xml:space="preserve">
         <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다. _x000d_
@@ -5364,7 +5366,7 @@
 _x000d_
 이 도구를 계속 사용하려면, 이 주의 경고문의 내용을 읽고 이해하였음에 동의해 주십시오._x000d_
 _x000d_
-###### 버전 68 (2021년 6월 21일)</v>
+###### 버전 6p (2021년 8월 3위)</v>
       </c>
       <c r="D208" t="str" xml:space="preserve">
         <v xml:space="preserve">Mục đích của Hệ thống Câu hỏi Tự Kiểm tra Mắc Virus Corona là để giúp quý vị đưa ra quyết định về việc tìm kiếm dịch vụ chăm sóc y tế thích hợp. Hệ thống này không dùng để chẩn đoán hoặc điều trị bệnh, kể cả COVID-19. _x000d_
@@ -5373,7 +5375,7 @@
 _x000d_
 Để tiếp tục sử dụng công cụ này, vui lòng đồng ý rằng quý vị đã đọc và hiểu nội dung của tuyên bố từ chối trách nhiệm này._x000d_
 _x000d_
-###### ver68 (06.21.2021)</v>
+###### ver69 (08.03.2021)</v>
       </c>
       <c r="E208" t="str" xml:space="preserve">
         <v xml:space="preserve">冠状病毒自我检查问卷的目的是帮助您做出寻求适当医疗护理的决策。该系统不适用于疾病的诊断或治疗，包括新冠肺炎。_x000d_
@@ -5382,7 +5384,7 @@
 _x000d_
 若要继续使用此工具，请同意您已阅读并理解此免责声明的内容。_x000d_
 _x000d_
-###### ver68 版（2021 年 6 月 21 日)</v>
+###### ver68 版（2021年8月3日)</v>
       </c>
       <c r="F208" t="str" xml:space="preserve">
         <v xml:space="preserve">La finalidad del Autoverificador del Coronavirus es ayudarlo a tomar decisiones sobre la obtención de atención médica adecuada. Este sistema no se ha diseñado para fines de diagnóstico o tratamiento de enfermedades, incluido el COVID-19. _x000d_
@@ -5391,7 +5393,7 @@
 _x000d_
 Para continuar usando esta herramienta, confirme que ha leído y entendido el contenido de este descargo de responsabilidad._x000d_
 _x000d_
-###### ver68 (06.21.2021)</v>
+###### ver68 (08.03.2021)</v>
       </c>
     </row>
     <row r="209">
@@ -8634,28 +8636,28 @@
         <v>CDC/messages/vax-endcap</v>
       </c>
       <c r="B363" t="str" xml:space="preserve">
-        <v xml:space="preserve">- [Learn about COVID-19 Vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [How to Protect Yourself and Others When You’ve Been Fully Vaccinated](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+        <v xml:space="preserve">- [Learn about COVID-19 vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+- [How to protect yourself and others when you’ve been fully vaccinated](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
 - [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)</v>
       </c>
       <c r="C363" t="str" xml:space="preserve">
-        <v xml:space="preserve">- [COVID-19 백신 알아보기](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [귀하가 백신 접종을 모두 마친 경우 귀하 자신과 타인을 보호하는 방법](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+        <v xml:space="preserve">- [COVID-19 백신 알아보기](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d_
+- [귀하가 백신 접종을 모두 마친 경우 귀하 자신과 타인을 보호하는 방법](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d__x000d_
 - [COVID-19 증상](https://www.cdc.gov/coronavirus/)</v>
       </c>
       <c r="D363" t="str" xml:space="preserve">
-        <v xml:space="preserve">- [Tìm hiểu thêm về Vắc-xin ngừa COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [Cách Bảo vệ Bản thân và Những người khác khi Quý vị đã được Tiêm chủng đầy đủ](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+        <v xml:space="preserve">- [Tìm hiểu thêm về Vắc-xin ngừa COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d_
+- [Cách Bảo vệ Bản thân và Những người khác khi Quý vị đã được Tiêm chủng đầy đủ](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d__x000d_
 - [Các triệu chứng COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)</v>
       </c>
       <c r="E363" t="str" xml:space="preserve">
-        <v xml:space="preserve">- [了解新冠肺炎疫苗](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [当您已完全接种疫苗时，如何保护您自己和他人](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+        <v xml:space="preserve">- [了解新冠肺炎疫苗](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d_
+- [当您已完全接种疫苗时，如何保护您自己和他人](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d__x000d_
 - [COVID-19 症状](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)</v>
       </c>
       <c r="F363" t="str" xml:space="preserve">
-        <v xml:space="preserve">- [Infórmese sobre las vacunas contra el COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [Cómo protegerse a sí mismo y a los demás cuando usted se ha vacunado completamente](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+        <v xml:space="preserve">- [Infórmese sobre las vacunas contra el COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d__x000d_
+- [Cómo protegerse a sí mismo y a los demás cuando usted se ha vacunado completamente](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d__x000d_
 - [Síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-A23testing/symptoms.html)</v>
       </c>
     </row>
@@ -8699,9 +8701,109 @@
         <v>Náuseas o vómitos</v>
       </c>
     </row>
+    <row r="366">
+      <c r="A366" t="str">
+        <v>CDC/likelyscale</v>
+      </c>
+      <c r="B366" t="str">
+        <v>["Very likely","Somewhat likely","Not very likely","Not likely at all"]</v>
+      </c>
+      <c r="C366" t="str">
+        <v/>
+      </c>
+      <c r="D366" t="str">
+        <v/>
+      </c>
+      <c r="E366" t="str">
+        <v/>
+      </c>
+      <c r="F366" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="str">
+        <v>CDC/yes_no_somewhat_response</v>
+      </c>
+      <c r="B367" t="str">
+        <v>["Yes","Somewhat","No"]</v>
+      </c>
+      <c r="C367" t="str">
+        <v/>
+      </c>
+      <c r="D367" t="str">
+        <v/>
+      </c>
+      <c r="E367" t="str">
+        <v/>
+      </c>
+      <c r="F367" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="str">
+        <v>CDC/second_person_questions/user_experience_followrec</v>
+      </c>
+      <c r="B368" t="str">
+        <v>Based on the information provided here, how likely are you to follow these recommendations?</v>
+      </c>
+      <c r="C368" t="str">
+        <v/>
+      </c>
+      <c r="D368" t="str">
+        <v/>
+      </c>
+      <c r="E368" t="str">
+        <v/>
+      </c>
+      <c r="F368" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="str">
+        <v>CDC/second_person_questions/user_experience_helpful</v>
+      </c>
+      <c r="B369" t="str">
+        <v>Was this screening tool helpful?</v>
+      </c>
+      <c r="C369" t="str">
+        <v/>
+      </c>
+      <c r="D369" t="str">
+        <v/>
+      </c>
+      <c r="E369" t="str">
+        <v/>
+      </c>
+      <c r="F369" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="str">
+        <v>CDC/second_person_questions/user_experience_consent</v>
+      </c>
+      <c r="B370" t="str">
+        <v>Will you answer **two questions** about your experience with this screening tool?</v>
+      </c>
+      <c r="C370" t="str">
+        <v/>
+      </c>
+      <c r="D370" t="str">
+        <v/>
+      </c>
+      <c r="E370" t="str">
+        <v/>
+      </c>
+      <c r="F370" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F365"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F370"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8939,13 +9041,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B01D6A3D-C086-4120-BF57-4241DADF0B82}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{740AF15D-1F79-415A-8AB1-70087B634EE5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD46D4CC-EB40-4701-A9E8-EACE098ACC47}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C27552D-DA7A-4AA6-B213-6E210793AE03}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE9F4226-A119-4781-8A1B-C264EF408EA7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97B3CFD2-8AFB-4D4C-B660-56795C4D7823}"/>
 </file>
</xml_diff>

<commit_message>
Updating to version 69.1
Moved User Experience questions into their own core.
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F370"/>
+  <dimension ref="A1:F371"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8801,9 +8801,29 @@
         <v/>
       </c>
     </row>
+    <row r="371">
+      <c r="A371" t="str">
+        <v>CDC/messages/thankyou</v>
+      </c>
+      <c r="B371" t="str">
+        <v>Thank you for completing the coronavirus self checker.</v>
+      </c>
+      <c r="C371" t="str">
+        <v/>
+      </c>
+      <c r="D371" t="str">
+        <v/>
+      </c>
+      <c r="E371" t="str">
+        <v/>
+      </c>
+      <c r="F371" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F370"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F371"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9041,13 +9061,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{740AF15D-1F79-415A-8AB1-70087B634EE5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6187925B-523A-4B25-8156-11C02DE57B48}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C27552D-DA7A-4AA6-B213-6E210793AE03}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{372322FE-8763-4E72-9F97-9B364BAD5433}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97B3CFD2-8AFB-4D4C-B660-56795C4D7823}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F4534E2-FA2E-4DA3-92C7-709E1F7E27DC}"/>
 </file>
</xml_diff>

<commit_message>
Updating to version 69.2
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F371"/>
+  <dimension ref="A1:F372"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5351,13 +5351,10 @@
         <v>CDC/messages/disclaimer_msg</v>
       </c>
       <c r="B208" t="str" xml:space="preserve">
-        <v xml:space="preserve">The purpose of the Coronavirus Self-Checker is to help you make decisions about seeking appropriate medical care. This system is not intended for the diagnosis or treatment of disease, including COVID-19. _x000d_
-_x000d_
-This project was made possible through a partnership with the CDC Foundation and is enabled by Microsoft’s Azure platform. CDC’s collaboration with a non-federal organization does not imply an endorsement of any one particular service, product, or enterprise. _x000d_
-_x000d_
-To continue using this tool, please agree that you have read and understood the contents of this disclaimer._x000d_
-_x000d_
-###### ver69 (08.03.2021)</v>
+        <v xml:space="preserve">The purpose of the Coronavirus Self-Checker is to help you make decisions about seeking appropriate medical care. This system is not intended for the diagnosis or treatment of disease, including COVID-19. 
+This project was made possible through a partnership with the CDC Foundation and is enabled by Microsoft’s Azure platform. CDC’s collaboration with a non-federal organization does not imply an endorsement of any one particular service, product, or enterprise. 
+To continue using this tool, please agree that you have read and understood the contents of this disclaimer.
+###### ver69.2 (08.16.2021)</v>
       </c>
       <c r="C208" t="str" xml:space="preserve">
         <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다. _x000d_
@@ -8806,7 +8803,7 @@
         <v>CDC/messages/thankyou</v>
       </c>
       <c r="B371" t="str">
-        <v>Thank you for completing the coronavirus self checker.</v>
+        <v>Thank you for completing the Coronavirus Self-Checker.</v>
       </c>
       <c r="C371" t="str">
         <v/>
@@ -8821,9 +8818,29 @@
         <v/>
       </c>
     </row>
+    <row r="372">
+      <c r="A372" t="str">
+        <v>CDC/messages/t203</v>
+      </c>
+      <c r="B372" t="str">
+        <v>**Based on the answers given, you should get tested 3-5 days after exposure and wear a mask in public indoor settings.** To maximize protection from the Delta variant and prevent possibly spreading to others, wear a mask indoors in public if you are in an area of substantial or high transmission.</v>
+      </c>
+      <c r="C372" t="str">
+        <v/>
+      </c>
+      <c r="D372" t="str">
+        <v/>
+      </c>
+      <c r="E372" t="str">
+        <v/>
+      </c>
+      <c r="F372" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F371"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F372"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9061,13 +9078,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6187925B-523A-4B25-8156-11C02DE57B48}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59C5A9C-D3FC-4DC9-948F-E87B3EE9E2DF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{372322FE-8763-4E72-9F97-9B364BAD5433}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E7918C9-941B-4B68-9406-BE3E1FE4CA10}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F4534E2-FA2E-4DA3-92C7-709E1F7E27DC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CA5AC72-F556-42EA-9FB2-C96912335C03}"/>
 </file>
</xml_diff>

<commit_message>
Updating to Version 71
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F391"/>
+  <dimension ref="A1:F393"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -545,7 +545,7 @@
         <v>CDC/vax_age_response</v>
       </c>
       <c r="B9" t="str">
-        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
+        <v>["5-9","10-12","13-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="C9" t="str">
         <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
@@ -4235,7 +4235,7 @@
         <v>CDC/messages/t0</v>
       </c>
       <c r="B174" t="str">
-        <v>**Based on the answers given, you do not need to get tested unless recommended or required by your healthcare provider, employer, or public health official**</v>
+        <v>**Based on the answers given, you do not need to get tested unless recommended or required by your healthcare provider, employer, or public health official.**</v>
       </c>
       <c r="C174" t="str">
         <v>**제공한 답변에 따라 의료 전문가, 고용주, 공중 보건 당국이 권고하거나 요구하지 않는 경우 검사를 받을 필요가 없습니다.**</v>
@@ -4817,7 +4817,7 @@
         <v>CDC/messages/msg19</v>
       </c>
       <c r="B196" t="str">
-        <v>**This tool is intended for people 2 years or older.** Please call the child’s medical provider, clinician advice line, or telemedicine provider if your child is less than 2 years old and sick</v>
+        <v>**This tool is intended for people 2 years or older.** Please call the child’s medical provider, clinician advice line, or telemedicine provider if your child is less than 2 years old and sick.</v>
       </c>
       <c r="C196" t="str">
         <v>**이 도구는 만 2세 이상을 대상으로 합니다.** 귀하의 자녀가 만 2세 미만이며 아픈 경우 아동의 의료 제공자, 임상의 상담 전화 또는 의료진에게 전화하십시오</v>
@@ -4837,7 +4837,7 @@
         <v>CDC/messages/msg18</v>
       </c>
       <c r="B197" t="str">
-        <v>**Stay home for 14 days from the day you last had contact. Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing.** If you develop any of these symptoms, call your medical provider, clinician advice line, or telemedicine provider</v>
+        <v>**Stay home for 14 days from the day you last had contact. Watch for COVID-19 symptoms such as fever, cough, or difficulty breathing.** If you develop any of these symptoms, call your medical provider, clinician advice line, or telemedicine provider.</v>
       </c>
       <c r="C197" t="str">
         <v>**마지막으로 접촉한 날부터 14일 동안 집에 머무르십시오. 발열, 기침, 또는 호흡곤란과 같은 COVID-19 증상이 있는지 관찰하십시오.** 귀하에게 이러한 증상들 중 어느 것이라도 발생하면, 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오</v>
@@ -5137,20 +5137,16 @@
         <v>CDC/messages/intro_msg</v>
       </c>
       <c r="B212" t="str" xml:space="preserve">
-        <v xml:space="preserve">Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the level of medical care you should seek. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again._x000d_
-_x000d_
-If you are experiencing a life-threatening emergency, please call 911 immediately._x000d_
-_x000d_
-If you are not experiencing a life-threatening emergency, let’s get started._x000d_
-_x000d_
-**CDC recommends these steps to reduce your risk of getting and spreading COVID-19:**_x000d_
-- **Get a COVID-19 vaccine** as soon as you can when eligible. People 5 years old and over are currently eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d_
-- **Wear** a mask over your nose and mouth.*_x000d_
-- **Stay** at least 6 feet away from people who don’t live with you.*_x000d_
-- **Avoid** crowded areas and poorly ventilated spaces.*_x000d_
-- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d_
-_x000d_
-###### *Fully vaccinated people can participate in many of the activities that they did before the pandemic. People are considered fully vaccinated 2 weeks after their second dose in a 2-dose series, such as Pfizer-BioNTech or Moderna vaccines, or 2 weeks after a single-dose vaccine, such as Johnson &amp; Johnson’s Janssen vaccine. To maximize protection from the Delta variant and prevent possibly spreading to others, wear a mask indoors in public if you are in an area of substantial or high transmission.</v>
+        <v xml:space="preserve">Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the level of medical care you should seek. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again.
+If you are experiencing a life-threatening emergency, please call 911 immediately.
+If you are not experiencing a life-threatening emergency, let’s get started.
+**CDC recommends these steps to reduce your risk of getting and spreading COVID-19:**
+- **Get a COVID-19 vaccine** as soon as you can when eligible. People 5 years old and over are currently eligible. Continue to follow the steps below every day until you are fully vaccinated.*
+- **Wear** a mask over your nose and mouth.*
+- **Stay** at least 6 feet away from people who don’t live with you.*
+- **Avoid** crowded areas and poorly ventilated spaces.*
+- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol.
+###### *Fully vaccinated people can participate in many of the activities that they did before the pandemic. People are considered fully vaccinated 2 weeks after their second dose in a 2-dose series, such as Pfizer-BioNTech or Moderna vaccines, or 2 weeks after a single-dose vaccine, such as Johnson &amp; Johnson’s Janssen vaccine. To maximize protection from variants such as Delta and Omicron, and prevent possibly spreading to others, wear a mask indoors in public if you are in an area of substantial or high transmission.</v>
       </c>
       <c r="C212" t="str" xml:space="preserve">
         <v xml:space="preserve">안녕하세요? 저는 Clara입니다. 몇 가지 질문을 하겠습니다. 귀하의 답변을 통해 귀하에게 어느 정도 수준의 진료가 필요한지 조언할 것입니다. 다른 사람을 위해 응답하고 계시다면 본인이 그 사람인 것처럼 모든 질문에 답하십시오. 처음부터 다시 시작해야 한다면 페이지를 새로 고치고 다시 시작하십시오._x000d_
@@ -5243,26 +5239,26 @@
         <v>CDC/messages/endcap</v>
       </c>
       <c r="B214" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Steps to follow every day:**_x000d_
-- **Get a COVID-19 vaccine** as soon as you can when eligible. People 5 years old and over are currently eligible. Continue to follow the steps below every day until you are fully vaccinated.*_x000d_
-- **Wear** a mask over your nose and mouth.*_x000d_
-- **Stay** at least 6 feet away from people who don’t live with you.*_x000d_
-- **Avoid** crowded areas and poorly ventilated spaces.*_x000d_
-- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol._x000d_
-_x000d_
-###### *Fully vaccinated people can participate in many of the activities that they did before the pandemic. People are considered fully vaccinated 2 weeks after their second dose in a 2-dose series, such as Pfizer-BioNTech or Moderna vaccines, or 2 weeks after a single-dose vaccine, such as Johnson &amp; Johnson’s Janssen vaccine. To maximize protection from the Delta variant and prevent possibly spreading to others, wear a mask indoors in public if you are in an area of substantial or high transmission. _x000d_
-_x000d_
-**Click the links below for more information on:**_x000d_
-- [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)_x000d_
-- [Post-COVID Conditions](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)_x000d_
-- [When to get tested](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)_x000d_
-- [What your test results mean](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)_x000d_
-- [Protecting yourself and others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)_x000d_
-- [When to quarantine or isolate and for how long](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
-- [What to do if you were around someone with COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)_x000d_
-- [Taking care of yourself when you are sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)_x000d_
-- [Taking care of someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)_x000d_
-- [Learn about COVID-19 Vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
+        <v xml:space="preserve">**This tool is currently in the process of being updated to align with the latest quarantine and isolation guidance. For the most up to date recommendations on isolation and quarantine, please visit CDC’s [Quarantine and Isolation](https://www.cdc.gov/coronavirus/2019-ncov/your-health/quarantine-isolation.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fif-you-are-sick%2Fquarantine.html) page.**
+**Steps to follow every day:**
+- **Get a COVID-19 vaccine** as soon as you can when eligible. People 5 years old and over are currently eligible. Continue to follow the steps below every day until you are fully vaccinated.*
+- **Wear** a mask over your nose and mouth.*
+- **Stay** at least 6 feet away from people who don’t live with you.*
+- **Avoid** crowded areas and poorly ventilated spaces.*
+- **Wash** your hands often with soap and water, or use hand sanitizer with at least 60% alcohol.
+###### *Fully vaccinated people can participate in many of the activities that they did before the pandemic. People are considered fully vaccinated 2 weeks after their second dose in a 2-dose series, such as Pfizer-BioNTech or Moderna vaccines, or 2 weeks after a single-dose vaccine, such as Johnson &amp; Johnson’s Janssen vaccine. To maximize protection from variants such as Delta and Omicron, and prevent possibly spreading to others, wear a mask indoors in public if you are in an area of substantial or high transmission. 
+**Click the links below for more information on:**
+- [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)
+- [Post-COVID Conditions](https://www.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)
+- [When to get tested](https://www.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html#who-should-get-tested)
+- [What your test results mean](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)
+- [Protecting yourself and others from getting sick](https://www.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)
+- [When to quarantine or isolate and for how long](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
+- [What to do if you were around someone with COVID-19](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
+- [Taking care of yourself when you are sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)
+- [Taking care of someone else who is sick](https://www.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)
+- [Treatments your healthcare provider might recommend if you are sick](https://www.cdc.gov/coronavirus/2019-ncov/your-health/treatments-for-severe-illness.html)
+- [Learn about COVID-19 Vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)
 - [Find COVID-19 vaccine locations near you](https://www.vaccines.gov/)</v>
       </c>
       <c r="C214" t="str" xml:space="preserve">
@@ -5363,13 +5359,10 @@
         <v>CDC/messages/disclaimer_msg</v>
       </c>
       <c r="B215" t="str" xml:space="preserve">
-        <v xml:space="preserve">The purpose of the Coronavirus Self-Checker is to help you make decisions about seeking appropriate medical care. This system is not intended for the diagnosis or treatment of disease, including COVID-19. _x000d_
-_x000d_
-This project was made possible through a partnership with the CDC Foundation and is enabled by Microsoft’s Azure platform. CDC’s collaboration with a non-federal organization does not imply an endorsement of any one particular service, product, or enterprise. _x000d_
-_x000d_
-To continue using this tool, please agree that you have read and understood the contents of this disclaimer._x000d_
-_x000d_
-###### ver70 (10.20.2021)</v>
+        <v xml:space="preserve">The purpose of the Coronavirus Self-Checker is to help you make decisions about seeking appropriate medical care. This system is not intended for the diagnosis or treatment of disease, including COVID-19. 
+This project was made possible through a partnership with the CDC Foundation and is enabled by Microsoft’s Azure platform. CDC’s collaboration with a non-federal organization does not imply an endorsement of any one particular service, product, or enterprise. 
+To continue using this tool, please agree that you have read and understood the contents of this disclaimer.
+###### ver71 (01.03.2022)</v>
       </c>
       <c r="C215" t="str" xml:space="preserve">
         <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 것에 대한 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다._x000d_
@@ -8630,9 +8623,9 @@
         <v>CDC/messages/vax-endcap</v>
       </c>
       <c r="B370" t="str" xml:space="preserve">
-        <v xml:space="preserve">_x000d_
-- [Learn about COVID-19 vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)_x000d_
-- [How to protect yourself and others when you’ve been fully vaccinated](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)_x000d_
+        <v xml:space="preserve">**This tool is currently in the process of being updated to align with the latest quarantine and isolation guidance. For the most up to date recommendations on isolation and quarantine, please visit CDC’s [Quarantine and Isolation](https://www.cdc.gov/coronavirus/2019-ncov/your-health/quarantine-isolation.html?CDC_AA_refVal=https%3A%2F%2Fwww.cdc.gov%2Fcoronavirus%2F2019-ncov%2Fif-you-are-sick%2Fquarantine.html) page.**
+- [Learn about COVID-19 vaccines](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/index.html)
+- [How to protect yourself and others when you’ve been fully vaccinated](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/fully-vaccinated.html)
 - [COVID-19 symptoms](https://www.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)</v>
       </c>
       <c r="C370" t="str" xml:space="preserve">
@@ -9077,9 +9070,49 @@
         <v>Enfermedad renal crónica</v>
       </c>
     </row>
+    <row r="392">
+      <c r="A392" t="str">
+        <v>CDC/messages/msg306</v>
+      </c>
+      <c r="B392" t="str">
+        <v>**Tell an administrator or nurse at your school or child care that you have tested positive for COVID-19.**</v>
+      </c>
+      <c r="C392" t="str">
+        <v/>
+      </c>
+      <c r="D392" t="str">
+        <v/>
+      </c>
+      <c r="E392" t="str">
+        <v/>
+      </c>
+      <c r="F392" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="str">
+        <v>CDC/messages/msg307</v>
+      </c>
+      <c r="B393" t="str">
+        <v>**Tell a caregiver in your facility that you have tested positive for COVID-19. Ask about when you can resume being around other people based on the results of your testing.**</v>
+      </c>
+      <c r="C393" t="str">
+        <v/>
+      </c>
+      <c r="D393" t="str">
+        <v/>
+      </c>
+      <c r="E393" t="str">
+        <v/>
+      </c>
+      <c r="F393" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F391"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F393"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9317,13 +9350,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E0A962B-14FA-4CE9-AA1B-EB7D799B395F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF82B987-9FAA-46C7-BA3D-841B14126B93}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{343E1827-7937-4C64-B777-FC535E4B3229}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BFDC7D4-EDD5-455E-B45B-6A340C594D32}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{760CD06A-421D-4BC2-83FA-47E2B3FDB615}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{371FA0D8-9CB2-4963-9D5C-6B195438C859}"/>
 </file>
</xml_diff>

<commit_message>
Fixing bug in FV-255 and CDC/vax_age_response
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -610,16 +610,16 @@
         <v>["5-9","10-12","13-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="C12" t="str">
-        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
+        <v>["5-9","10-12","13-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="D12" t="str">
-        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
+        <v>["5-9","10-12","13-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="E12" t="str">
-        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
+        <v>["5-9","10-12","13-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
       <c r="F12" t="str">
-        <v>["12-15","16-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
+        <v>["5-9","10-12","13-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
       </c>
     </row>
     <row r="13">
@@ -9375,42 +9375,42 @@
     </row>
     <row r="406">
       <c r="A406" t="str">
-        <v>CDC/old_covid_testing_response_asymp</v>
+        <v>CDC/second_person_questions/old_test_asymptomatic</v>
       </c>
       <c r="B406" t="str">
-        <v>["The test showed that I did have COVID-19 (positive test).","The test showed that I did not have COVID-19 (negative test)."]</v>
+        <v>What was the result of your test?</v>
       </c>
       <c r="C406" t="str">
-        <v>["검사 결과 COVID-19에 걸린 것으로 나타났습니다(검사 결과 양성).", "검사 결과 COVID-19에 걸리지 않은 것으로 나타났습니다(검사 결과 음성)."]</v>
+        <v>검사 결과는 어땠습니까?</v>
       </c>
       <c r="D406" t="str">
-        <v>["Xét nghiệm cho thấy tôi đã có COVID-19 (xét nghiệm dương tính).", "Xét nghiệm cho thấy tôi không có COVID-19 (xét nghiệm âm tính)."]</v>
+        <v>Kết quả của xét nghiệm của quý vị là gì?</v>
       </c>
       <c r="E406" t="str">
-        <v>["检测结果显示我确实感染了COVID-19（检测阳性）。", "检测结果显示我没有感染 COVID-19（检测阴性）。"]</v>
+        <v>你的检查结果是什么？</v>
       </c>
       <c r="F406" t="str">
-        <v>["La prueba mostró que sí tuve COVID-19 (resultado positivo).", "La prueba mostró que no tuve COVID-19 (resultado negativo)."]</v>
+        <v>¿Cuál fue el resultado de la prueba?</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="str">
-        <v>CDC/second_person_questions/old_test_asymptomatic</v>
+        <v>CDC/old_covid_testing_response_asymp</v>
       </c>
       <c r="B407" t="str">
-        <v>What was the result of your test?</v>
+        <v>["The test showed that I did have COVID-19 (positive test).","The test showed that I did not have COVID-19 (negative test)."]</v>
       </c>
       <c r="C407" t="str">
-        <v>검사 결과는 어땠습니까?</v>
+        <v>["검사 결과 COVID-19에 걸린 것으로 나타났습니다(검사 결과 양성).", "검사 결과 COVID-19에 걸리지 않은 것으로 나타났습니다(검사 결과 음성)."]</v>
       </c>
       <c r="D407" t="str">
-        <v>Kết quả của xét nghiệm của quý vị là gì?</v>
+        <v>["Xét nghiệm cho thấy tôi đã có COVID-19 (xét nghiệm dương tính).", "Xét nghiệm cho thấy tôi không có COVID-19 (xét nghiệm âm tính)."]</v>
       </c>
       <c r="E407" t="str">
-        <v>你的检查结果是什么？</v>
+        <v>["检测结果显示我确实感染了COVID-19（检测阳性）。", "检测结果显示我没有感染 COVID-19（检测阴性）。"]</v>
       </c>
       <c r="F407" t="str">
-        <v>¿Cuál fue el resultado de la prueba?</v>
+        <v>["La prueba mostró que sí tuve COVID-19 (resultado positivo).", "La prueba mostró que no tuve COVID-19 (resultado negativo)."]</v>
       </c>
     </row>
   </sheetData>
@@ -9653,13 +9653,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94C3A9FF-D086-47C5-92F8-562EF1F43363}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC2FD293-2315-47B8-9D5B-CFFA8DC76619}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9996F702-7E7C-48F3-8812-5E8A956B4F43}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D87A13F4-2EE4-4F7A-99E3-F04820EB6BC1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{660E49E6-4E8A-4175-B564-B7E7EAA03E0B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B82C56-04D5-46D5-8476-E3A048351D00}"/>
 </file>
</xml_diff>

<commit_message>
Updating Non English to Version 73
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -716,40 +716,40 @@
 **Are you up to date with your COVID-19 vaccination?**</v>
       </c>
       <c r="C17" t="str" xml:space="preserve">
-        <v xml:space="preserve">COVID-19 백신 접종 상태가 유효한 상태입니까? _x000d_
-일반적으로, 부스터샷 접종 자격에 해당되는 경우 모든 부스터샷을 포함하여, 권고되는 모든 COVID-19 백신을 접종받으셨다면 귀하의 백신접종 상태가 유효한 것으로 간주됩니다. 2주 전에 2차 접종으로 Pfizer-BioNTech(COMIRNATY) COVID-19 백신 또는 모더나 백신 또는 단회 접종 백신을 접종받았으나 아직 부스터샷 접종 자격에 해당하지 않는다면 귀하의 접종 상태는 유효한 상태입니다. _x000d_
-- 만 18세 이상의 성인은 일반적으로 2차 접종으로 Pfizer-BioNTech 또는 Moderna 백신을 접종한 시점으로부터 5개월 후 또는 Janssen(Johnson &amp; Johnson) COVID-19 백신을 접종한 시점으로부터 2개월 후에 부스터샷 접종을 받을 자격이 됩니다. _x000d_
-- 만 12~17세 아동은 2차 접종으로 Pfizer-BioNTech 백신을 접종받은 시점으로부터 5개월 후에 부스터샷 접종 대상에 해당됩니다. _x000d_
-- 만 11세 이하의 아동은 아직 부스터샷 접종을 받을 자격에 해당되지 않습니다. _x000d_
-- 면역계가 중등증 내지 중증 수준으로 약화된 사람은 Pfizer-BioNTech 또는 Moderna 백신을 3차 접종한 시점으로부터 2주가 지나기 전까지는 유효 접종 상태가 아닐 수 있습니다. 귀하는 3차 접종을 받은 시점으로부터 3개월 후에 부스터샷을 접종 받을 자격에 해당됩니다.</v>
+        <v xml:space="preserve">**COVID-19 백신 접종:**
+ 일반적으로, 부스터샷 접종 자격에 해당하는 경우 모든 부스터샷을 포함하여, [권고되는 모든 COVID-19 백신](https://korean.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html)을 접종하셨다면 접종 상태는 최신 상태인 것으로 간주됩니다. 아직 부스터샷 접종 자격에 해당하지 않는 경우, 기본 시리즈(최초 2회 또는 3회 투여)의 화이자-바이오엔텍(COMIRNATY) COVID-19 백신 또는 모더나 백신을 접종했거나 1회 투여하는 존슨앤드존슨의 얀센 백신을 접종한지 2주 이상 경과했다면 접종 상태는 최신 상태입니다. 
+- 중등도 또는 중증의 면역 저하가 **없는** 만 18세 이상의 성인은 일반적으로 화이자-바이오엔텍 또는 모더나 백신의 2차 접종을 투여한 5개월 후, 또는 얀센(존슨앤드존슨) COVID-19 백신을 투여한 2개월 후에 부스터샷을 접종할 자격이 생깁니다. 
+- 만 5~17세 아동 및 청소년은 화이자-바이오엔텍 또는 모더나 백신의 2차 접종을 투여한 5개월 후에 부스터샷을 접종할 자격이 있습니다.  
+- 생후 6개월~만 4세 영유아는 화이자-바이오엔텍(COMIRNATY) COVID-19 백신 또는 모더나 백신의 기본 시리즈(최초 2회 또는 3회 투여)의 접종 자격이 있으나 아직 부스터샷 접종 자격은 없습니다. 
+- 중등도 또는 중증의 면역 저하가 있는 만 12세 이상은 최신 접종 상태를 유지하기 위해 총 5회의 mRNA COVID-19 백신을 접종해야 합니다. 5회 접종에는 화이자-바이오엔텍 또는 모더나 COVID-19 백신의 기본 시리즈 3회 접종과 화이자-바이오엔텍 또는 모더나 COVID-19 백신의 부스터샷 2회 접종이 포함됩니다. 
+ **당신의 COVID-19 백신 접종 상태는 최신 접종 상태입니까?**</v>
       </c>
       <c r="D17" t="str" xml:space="preserve">
-        <v xml:space="preserve">Quý vị đã tiêm cập nhật vắc-xin phòng COVID-19 chưa?_x000d_
-_x000d_
-Nói chung, quý vị được coi là đã tiêm cập nhật nếu quý vị đã tiêm tất cả các mũi vắc-xin phòng COVID-19 được khuyến nghị, bao gồm bất kỳ (các) liều tăng cường nào khi đủ điều kiện. Quý vị được coi là đã tiêm cập nhật nếu đã tiêm liều thứ hai của vắc-xin phòng COVID-19 của Pfizer-BioNTech (COMIRNATY) hoặc vắc-xin của Moderna hoặc vắc-xin đơn liều cách đây hơn 2 tuần nhưng quý vị chưa đủ điều kiện để tiêm liều tăng cường._x000d_
-- Người lớn từ 18 tuổi trở lên thường đủ điều kiện để tiêm liều tăng cường sau khi tiêm liều thứ hai của vắc-xin Pfizer-BioNTech hoặc Moderna  5 tháng hoặc sau khi tiêm vắc-xin phòng COVID-19 của Janssen (Johnson &amp; Johnson) 2 tháng._x000d_
-- Trẻ em từ 12–17 tuổi đủ điều kiện để tiêm liều tăng cường sau khi tiêm liều thứ hai của vắc-xin của Pfizer-BioNTech 5 tháng._x000d_
-- Trẻ em từ 11 tuổi trở xuống chưa đủ điều kiện để tiêm liều tăng cường._x000d_
-- Những người có hệ thống miễn dịch suy yếu từ trung bình đến nặng có thể không được coi là đã tiêm cập nhật cho đến 2 tuần sau khi tiêm liều thứ ba vắc-xin của Pfizer-BioNTech hoặc của Moderna. Quý vị đủ điều kiện để tiêm liều tăng cường sau khi tiêm liều thứ ba 3 tháng._x000d_
-</v>
+        <v xml:space="preserve">**Chủng ngừa COVID-19:**
+ Nói chung, quý vị được coi là đã chủng ngừa đầy đủ nếu quý vị đã [được tiêm tất cả các mũi vắc-xin COVID-19 được khuyến nghị](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html), bao gồm mọi liều nhắc lại nếu đủ điều kiện. Nếu quý vị chưa đủ điều kiện để tiêm liều nhắc lại, quý vị được coi là đã chủng ngừa đầy đủ nếu đã tiêm các liều cơ bản (2 hoặc 3 mũi ban đầu) của vắc-xin COVID-19 Pfizer-BioNTech (COMIRNATY) hoặc vắc-xin Moderna hoặc một liều đơn của vắc-xin Janssen của Johnson &amp; Johnson hơn 2 tuần trước.
+- Người lớn từ 18 tuổi trở lên **không** bị suy giảm miễn dịch ở mức độ trung bình hoặc nặng thường đủ điều kiện để tiêm liều nhắc lại 5 tháng sau khi tiêm liều thứ hai của vắc-xin COVID-19 Pfizer-BioNTech hoặc Moderna hoặc 2 tháng sau khi tiêm vắc-xin Janssen (Johnson &amp; Johnson).
+- Trẻ em và thanh thiếu niên từ 5–17 đủ điều kiện tiêm liều nhắc lại 5 tháng sau khi tiêm liều thứ hai của vắc-xin Pfizer-BioNTech hoặc Moderna.
+- Trẻ em từ 6 tháng đến 4 tuổi đủ điều kiện tiêm liều cơ bản (2 hoặc 3 mũi ban đầu) của vắc-xin COVID-19 Pfizer-BioNTech (COMIRNATY) hoặc vắc-xin Moderna, nhưng chưa đủ điều kiện tiêm các liều nhắc lại.
+- Những người từ 12 tuổi trở lên bị suy giảm miễn dịch ở mức trung bình hoặc nặng cần tiêm tổng cộng 5 liều vắc-xin COVID-19 mRNA để được coi là chủng ngừa đầy đủ. 5 liều bao gồm các liều cơ bản gồm 3 liều vắc-xin COVID-19 Pfizer-BioNTech hoặc Moderna, cộng với 2 liều nhắc lại vắc-xin COVID-19 Pfizer-BioNTech hoặc Moderna.
+ **Quý vị đã tiêm đủ các mũi vắc-xin COVID-19 của mình chưa?**</v>
       </c>
       <c r="E17" t="str" xml:space="preserve">
-        <v xml:space="preserve">您是否及时接种的最新要求的COVID-19疫苗？ _x000d_
-_x000d_
-一般来说，如果您已经接种了所有推荐的COVID-19疫苗，包括符合条件的任何加强剂，您就被认为是接种了最新要求的疫苗。如果您在两周前接种了辉瑞-BioNTech（COMIRNATY）COVID-19疫苗或莫德纳疫苗的第二剂或单剂疫苗，但您还没有资格接种加强剂，那么您就是接种了最新的疫苗。_x000d_
-- 18岁及以上的成年人在接种辉瑞-BioNTech或莫德纳公司的第二针疫苗5个月后，或接种杨森（强生）COVID-19疫苗2个月后，通常有资格接种加强剂。_x000d_
-- 12-17岁的儿童在接种第二针辉瑞-BioNTech疫苗5个月后有资格接种加强剂量。_x000d_
-- 11岁及以下的儿童还没有资格接种加强剂_x000d_
-- 免疫系统中度至严重受损的患者，在接种第三剂辉瑞-BioNTech或莫德纳疫苗两周后才会是及时接种了最新的疫苗。在接种第三针 3 个月后，您就有资格接种加强针。</v>
+        <v xml:space="preserve">**COVID-19疫苗接种:**
+一般来说，如果您已经[接种了所有推荐的COVID-19疫苗](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html)，包括符合条件的任何加强剂量，您就被认为是及时接种了。如果您还没有资格接种加强剂，但是如果您已在2周以上的时间前接种了辉瑞-BioNTech(COMIRNATY)COVID-19疫苗或莫德纳疫苗的基础免疫（最初2剂或3剂）或Johnson &amp; Johnson’s Janssen疫苗单剂次，那么您就是接种了最新的疫苗。
+- 18岁及以上**非**中度或重度免疫功能低下的成人在接种辉瑞-BioNTech或莫德纳公司的第二针疫苗5个月后，或接种杨森（强生）COVID-19疫苗2个月后，通常有资格接种加强剂。
+- 5-17岁的儿童和青少年在接种第二针辉瑞-BioNTech或莫德纳疫苗5个月后有资格接种一剂加强剂。
+- 6个月至4岁的儿童有资格接种辉瑞-BioNTech(COMIRNATY)COVID-19疫苗或莫德纳疫苗的基础免疫（初始2剂或3剂），但尚未有资格接受加强剂。
+- 12岁及以上中度或重度免疫功能低下的人群应接种共5剂mRNA COVID-19疫苗，以保持接种最新的疫苗。5剂包括3剂辉瑞-BioNTech或莫德纳COVID-19疫苗的基础接种系列，加上2剂辉瑞-BioNTech或莫德纳COVID-19疫苗的加强剂。
+**您是否及时接种的最新要求的COVID-19疫苗？**</v>
       </c>
       <c r="F17" t="str" xml:space="preserve">
-        <v xml:space="preserve">¿Está al día con su vacunación contra el COVID-19?_x000d_
-_x000d_
-Por lo general, se considera que usted está al día si ha recibido todas las vacunas contra el COVID-19 recomendadas, incluidas todas las dosis de refuerzo, cuando sea elegible. Usted está al día si ha recibido la segunda dosis de la vacuna contra el COVID-19 Pfizer-BioNTech (COMIRNATY), de la vacuna Moderna o de una vacuna de una dosis única hace más de 2 semanas, pero todavía no es elegible para una dosis de refuerzo._x000d_
-- Por lo general, los adultos de 18 años o más son elegibles para la dosis de refuerzo 5 meses después de recibir la segunda dosis de las vacunas de Pfizer-BioNTech o de Moderna o 2 meses después de recibir la vacuna contra el COVID-19 Janssen (Johnson &amp; Johnson)._x000d_
-- Los niños de 12-17 años son elegibles para la dosis de refuerzo 5 meses después de recibir la segunda dosis de la vacuna de Pfizer-BioNTech._x000d_
-- Los niños de 11 años o menos todavía no son elegibles para las dosis de refuerzo._x000d_
-- Las personas con el sistema inmunitario moderada a gravemente debilitado podrían no estar al día hasta 2 semanas después de recibir una tercera dosis de las vacunas de Pfizer-BioNTech o de Moderna. Usted es elegible para una dosis de refuerzo 3 meses después de recibir la tercera dosis.</v>
+        <v xml:space="preserve">**Vacunas contra el COVID-19:**
+Por lo general, se considera que usted está al día si ha [recibido todas las vacunas contra el COVID-19 recomendadas](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html), incluida alguna dosis de refuerzo, cuando sea elegible. Si usted todavía no es elegible para recibir la dosis de refuerzo, está al día si ha recibido la serie primaria ( 2 o 3 dosis iniciales) de las vacunas contra el COVID-19 Pfizer-BioNTech (COMIRNATY) o Moderna, o una dosis única de la vacuna Janssen de Johnson &amp; Johnson hace más de 2 semanas.
+- Por lo general, los adultos de 18 años o más que **no** están moderada o gravemente inmunodeprimidos son elegibles para la dosis de refuerzo 5 meses después de recibir la segunda dosis de las vacunas Pfizer-BioNTech o Moderna, o 2 meses después de recibir la vacuna contra el COVID-19 Janssen (Johnson &amp; Johnson). 
+- Los niños y adolescentes de 5-17 años son elegibles para la dosis de refuerzo 5 meses después de recibir la segunda dosis de las vacunas Pfizer-BioNTech o Moderna. 
+- Los niños de 6 meses a 4 años son elegibles para la serie primaria (2 o 3 dosis iniciales) de las vacunas contra el COVID-19 Pfizer-BioNTech (COMIRNATY) o Moderna, pero no son todavía elegibles para recibir las dosis de refuerzo.
+- Las personas de 12 años o más que están moderada o gravemente inmunodeprimidas deben recibir un total de 5 dosis de una vacuna de ARNm contra el COVID-19 para estar al día. Las 5 dosis incluyen una serie primaria de 3 dosis de las vacunas contra el COVID-19 Pfizer-BioNTech o Moderna, más 2 dosis de refuerzo de las vacunas contra el COVID-19 Pfizer-BioNTech o Moderna.
+**¿Está al día con su vacunación contra el COVID-19?**</v>
       </c>
     </row>
     <row r="18">
@@ -6567,25 +6567,25 @@
         <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 것에 대한 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다.
 이 프로젝트는 CDC Foundation과의 파트너십을 통해 가능했으며 Microsoft의 Azure 플랫폼에서 가능합니다. CDC가 비연방 조직과 협력한다고 해서 특정 서비스, 제품 또는 기업을 보증한다는 의미는 아닙니다.
 이 도구를 계속 사용하려면, 이 면책의 내용을 읽고 이해하였음에 동의해 주십시오.
-###### 버전 72 (2022년 03월 23일)</v>
+###### 버전 73 (2022년 06월 22일)</v>
       </c>
       <c r="D268" t="str" xml:space="preserve">
         <v xml:space="preserve">Mục đích của Hệ thống Câu hỏi Tự Kiểm tra Mắc Virus Corona là để giúp quý vị đưa ra quyết định về việc tìm kiếm dịch vụ chăm sóc y tế thích hợp. Hệ thống này không dùng để chẩn đoán hoặc điều trị bệnh, kể cả COVID-19.
 Dự án này được thực hiện thông qua sự hợp tác với CDC Foundation và được hỗ trợ bởi nền tảng Azure của Microsoft. Sự hợp tác của CDC với một tổ chức không thuộc liên bang không ngụ ý xác nhận bất kỳ dịch vụ, sản phẩm hoặc doanh nghiệp cụ thể nào.
 Để tiếp tục sử dụng công cụ này, vui lòng đồng ý rằng quý vị đã đọc và hiểu nội dung của tuyên bố từ chối trách nhiệm này.
-###### ver72 (03.23.2022)</v>
+###### ver73 (06.22.2022)</v>
       </c>
       <c r="E268" t="str" xml:space="preserve">
         <v xml:space="preserve">冠状病毒自我检查问卷的目的是帮助您做出寻求适当医疗护理的决策。该系统不适用于疾病的诊断或治疗，包括 COVID-19。
 这个项目是通过与 CDC 基金会的合作而实现，并由 Microsoft 的 Azure 平台启用。CDC 与非联邦组织的合作并不意味着对任何特定服务、产品或企业的认可。
 若要继续使用此工具，请同意您已阅读并理解此免责声明的内容。
-###### 版本 72 (2022 年 03 月 23 日)</v>
+###### 版本 73 (2022 年 06 月 22 日)</v>
       </c>
       <c r="F268" t="str" xml:space="preserve">
         <v xml:space="preserve">La finalidad del Autoverificador del Coronavirus es ayudarlo a tomar decisiones sobre la obtención de atención médica adecuada. Este sistema no se ha diseñado para fines de diagnóstico o tratamiento de enfermedades, incluido el COVID-19.
 Este proyecto ha sido posible mediante la colaboración con la Fundación de los CDC y se ha habilitado a través de la plataforma Azure de Microsoft. La colaboración de los CDC con una organización no federal no implica el respaldo a ningún servicio, producto o empresa específicos.
 Para continuar usando esta herramienta, confirme que ha leído y entendido el contenido de este descargo de responsabilidad.
-###### ver72 (03.23.2022)</v>
+###### ver73 (06.22.2022)</v>
       </c>
     </row>
     <row r="269">
@@ -9421,16 +9421,16 @@
         <v>Do you have, or have you had any of the following? (check all that apply)</v>
       </c>
       <c r="C408" t="str">
-        <v/>
+        <v>다음에 나열된 증상이 현재 있거나 혹은 과거에 있었던 적이 있습니까? (해당 사항에 모두 체크)</v>
       </c>
       <c r="D408" t="str">
-        <v/>
+        <v>Quý vị đã hoặc đang có bất kỳ tình trạng nào sau đây không? (đánh dấu tất cả đáp án thích hợp)</v>
       </c>
       <c r="E408" t="str">
-        <v/>
+        <v>您是否有或曾经有以下情况？（请勾选所有适用的选项）</v>
       </c>
       <c r="F408" t="str">
-        <v/>
+        <v>¿Tiene o ha tenido alguna de las siguientes cosas? (Marque todo lo que corresponda)</v>
       </c>
     </row>
   </sheetData>
@@ -9664,9 +9664,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{074B2E44-8C46-4E9E-B2EB-36793B4E9E46}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C612A2D-90B6-4229-A264-AF2AD2776EDC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CE92DA1-DE32-4E3B-B200-6DF5E7BC5D17}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{449D8D1B-065E-4A7E-853B-7392E78081B2}"/>
 </file>
</xml_diff>

<commit_message>
Fixed a typo in vaccine question for V74
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -8924,7 +8924,7 @@
         <v>CDC/second_person_questions/vaccine_question</v>
       </c>
       <c r="B397" t="str">
-        <v>**Are you up to date with your COVID-19 vaccination, [meaning you have completed a primary series and received the most recent booster does recommended for you by CDC?](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html)**</v>
+        <v>**Are you up to date with your COVID-19 vaccination, [meaning you have completed a primary series and received the most recent booster dose recommended for you by CDC?](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html)**</v>
       </c>
       <c r="C397" t="str" xml:space="preserve">
         <v xml:space="preserve">**Vacunas contra el COVID-19:**
@@ -9496,9 +9496,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2711066F-26D7-46CF-B678-943A310D41A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15809456-590D-4655-B169-3C26C3F68525}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E10B3E9E-F222-4621-8B47-FAA17930837A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DA9DE58-A3CC-4BE3-90EC-9DF366850955}"/>
 </file>
</xml_diff>

<commit_message>
Updating Foreign Language to V74
</commit_message>
<xml_diff>
--- a/screening_protocols/localization-custom-strings.xlsx
+++ b/screening_protocols/localization-custom-strings.xlsx
@@ -2970,7 +2970,7 @@
         <v>**You have not made a selection. Please start again and select options for each question so that I can help give you recommendations.**</v>
       </c>
       <c r="C129" t="str">
-        <v>**No ha seleccionado ninguna opción. Vuelva a comenzar y seleccione opciones para cada pregunta, para que pueda aconsejarlo.</v>
+        <v>**No ha seleccionado ninguna opción. Vuelva a comenzar y seleccione opciones para cada pregunta, para que yo pueda hacerle recomendaciones.**</v>
       </c>
       <c r="D129" t="str">
         <v>**선택하지 않으셨습니다. 다시 시작하고 제가 조언을 드릴 수 있도록 각 질문에 대한 옵션을 선택하십시오.**</v>
@@ -3190,7 +3190,7 @@
         <v>Thanks! Your location has its own self-assessment tool. Please [select here](</v>
       </c>
       <c r="C140" t="str">
-        <v>¡Gracias! El lugar donde se encuentra tiene su propia herramienta de autoevaluación. Por favor, [haga clic aquí](</v>
+        <v>¡Gracias! El lugar donde se encuentra tiene su propia herramienta de autoevaluación. Por favor [seleccione aquí](</v>
       </c>
       <c r="D140" t="str">
         <v>감사합니다! 귀하의 지역에는 자체 평가 도구가 있습니다. [여기를 클릭하십시오.](</v>
@@ -3270,7 +3270,7 @@
         <v>**Tell an administrator or nurse at your school or child care that you may have been in contact with someone with suspected COVID-19.**</v>
       </c>
       <c r="C144" t="str">
-        <v>** Dígale a un administrador o al personal de enfermería de la escuela o guardería que pudo haber tenido contacto con alguien con COVID-19 presunto.**</v>
+        <v>**Dígale a un administrador o al personal de enfermería de la escuela o guardería que pudo haber tenido contacto con alguien con COVID-19 presunto.**</v>
       </c>
       <c r="D144" t="str">
         <v>**귀하의 학교 또는 보육 관리자나 간호사에게 귀하가 COVID-19가 의심되는 사람과 접촉했을 수 있음을 알리십시오.**</v>
@@ -3650,7 +3650,7 @@
         <v>**Your symptoms may be caused by COVID-19.** While most people will recover and return to normal health, some people have symptoms that can last for weeks or months after having COVID-19. It is important to notify your healthcare provider of your symptoms because it could affect your health care needs in the future.</v>
       </c>
       <c r="C160" t="str">
-        <v>**Sus síntomas podrían ser causados por el COVID-19.** Si bien la mayoría de las personas se recuperan y vuelven a tener su salud normal, algunas tienen síntomas que pueden durar semanas o meses después de tener el COVID-19. Es importante que informe a su proveedor de atención médica sobre sus síntomas porque esto podría afectar sus necesidades médicas en el futuro.</v>
+        <v>**Sus síntomas podrían ser causados por el COVID-19.** Si bien la mayoría de las personas se recuperarán y vuelven a su salud normal, algunas tienen síntomas que pueden durar semanas o meses después de tener el COVID-19. Es importante que informe a su proveedor de atención médica sobre sus síntomas porque esto podría afectar sus necesidades médicas en el futuro.</v>
       </c>
       <c r="D160" t="str">
         <v>**해당 증상은 COVID-19로 인해 발생한 것일 수 있습니다.** 일부 사람들은 COVID-19에 감염된 후 수 주 또는 수 개월 동안 증상이 지속됩니다. 향후 필요한 진료 영역에 영향을 미칠 수 있으므로 나타난 증상을 담당 의료진에게 알리는 것이 중요합니다.</v>
@@ -3860,7 +3860,7 @@
         <v>**Tell a caregiver in your facility that you may have been exposed to COVID-19 in the last 14 days.**</v>
       </c>
       <c r="C168" t="str">
-        <v>**Dígale a un cuidador de su establecimiento que usted pudo haber estado en contacto cercano con otra persona que ha dado positivo en la prueba del COVID-19 en los últimos 14 días.**</v>
+        <v>**Dígale a un cuidador en su establecimiento que usted pudo haber estado expuesto al COVID-19 en los últimos 14 días.**</v>
       </c>
       <c r="D168" t="str">
         <v>**입원 중인 시설의 간병인에게 지난 14일 동안 COVID-19에 양성 판정을 받은 다른 사람과 밀접하게 접촉했을 수 있다고 알리십시오.**</v>
@@ -4101,7 +4101,7 @@
         <v>**Tell the occupational health provider (or supervisor) in your workplace as soon as possible that you’re feeling sick.**</v>
       </c>
       <c r="C176" t="str">
-        <v>**Dígale al proveedor de salud ocupacional (o supervisor) de su lugar de trabajo que se siente mal lo más pronto posible.**</v>
+        <v>**Dígale al proveedor de salud ocupacional (o supervisor) de su lugar de trabajo que se está sintiendo enfermo, lo antes posible.**</v>
       </c>
       <c r="D176" t="str">
         <v>**가능한 한 빨리 직장의 산업 보건 담당자(또는 직장상사)에게 귀하가 아프다고 말하십시오.**</v>
@@ -4252,10 +4252,10 @@
 - **Avoid people who are immunocompromised or at high risk for severe disease, and avoid nursing homes and other high-risk settings, until after at least 10 days following exposure.**</v>
       </c>
       <c r="C182" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Quédese en casa y aislado de los demás por al menos 5 días (para calcular su periodo de aislamiento de 5 días, el día 0 es el primer día de síntomas o el día de la prueba que dio positivo si es asintomático; el día 1 es el primer día completo después de que presentó síntomas o de la prueba que dio positivo). Use una mascarilla bien ajustada si tiene que estar cerca de otras personas en su casa y vigile sus síntomas.**
-- **Puede terminar el aislamiento después de 5 días completos si lleva 24 horas sin fiebre sin el uso de medicamentos para reducirla y sus otros síntomas han mejorado. Si está inmunodeprimido o tiene síntomas de COVID-19 de moderados a graves, deberá aislarse por al menos 10 días y consultar a un proveedor de atención médica sobre cuándo estaría bien terminar su aislamiento.**
-- **Debe seguir usando una mascarilla bien ajustada cuando esté cerca de otras personas en casa y en sitios públicos por otros 5 días (día 6 a día 10) después de ponerle fin al periodo de aislamiento de 5 días. Si no puede usar una mascarilla cuando esté cerca de los demás, debe continuar el aislamiento por 10 días completos.**
-- **Evite estar cerca de personas que estén inmunodeprimidas o en alto riesgo de enfermarse gravemente, y de hogares de ancianos y otros entornos de alto riesgo, hasta que hayan pasado al menos 10 días desde que tuvo contacto cercano con alguien con COVID-19.**</v>
+        <v xml:space="preserve">**Aíslese de las demás personas por al menos 5 días.** Para calcular su periodo de aislamiento de 5 días, el día 0 es el primer día de síntomas o el día de la prueba (no el día que recibió el resultado positivo de la prueba) si no tiene síntomas. El día 1 es el primer día entero después de que comenzaron sus síntomas o el primer día entero después del día en que se hizo la prueba. Use una mascarilla de alta calidad si tiene que estar alrededor de otras personas en su casa y vigile sus síntomas.
+- **Puede terminar el aislamiento después de 5 días completos si lleva 24 horas sin fiebre sin el uso de medicamentos para reducirla y sus otros síntomas han mejorado.** Si está inmunodeprimido o tiene síntomas de COVID-19 de moderados a graves, deberá aislarse hasta el día 10. Si está inmunodeprimido o se enfermó gravemente, también deberá consultar a un proveedor de atención médica sobre cuándo sería adecuado terminar su aislamiento.
+- **Debería seguir usando una mascarilla de alta calidad cuando esté cerca de otras personas en casa y en sitios públicos por otros 5 días (del día 6 al día 10) después de que termine su periodo de aislamiento de 5 días.** Si tiene acceso a pruebas de antígenos, debería considerar usarlas después de salir del aislamiento el día 6. Si tiene dos pruebas negativas secuenciales con una separación de 48 horas (se puede hacer la primera tan pronto como el día 6), puede quitarse la mascarilla antes del día 10. Si los resultados de la prueba de antígenos son positivos, usted todavía podría ser infeccioso y no debería quitarse la mascarilla cuando esté alrededor de otras personas. Siga haciéndose pruebas de antígenos con una separación de al menos 48 horas, hasta que tenga dos resultados negativos secuenciales. Esto podría significar que debe seguir usando una mascarilla y haciéndose pruebas más allá del día 10. No se acerque a las personas que estén inmunodeprimidas o en alto riesgo de enfermarse gravemente, y no vaya a hogares de ancianos y otros entornos de alto riesgo, hasta después de al menos 10 días después de la exposición.
+- **No se acerque a las personas que estén inmunodeprimidas o en alto riesgo de enfermarse gravemente, y no vaya a hogares de ancianos y otros entornos de alto riesgo, hasta después de al menos 10 días después de la exposición.**</v>
       </c>
       <c r="D182" t="str" xml:space="preserve">
         <v xml:space="preserve">**최소 5일 동안 자택에서 머무르면서 다른 사람들로부터 확진 격리 조치를 실시하십시오(5일간의 확진 격리 기간을 계산할 때, 증상이 나타난 첫 날 또는 증상이 없는 경우에는 검사 결과 양성 확진을 받은 날을 제0일로 계산합니다. 증상이 나타나거나 검사 결과 양성 확진을 받은 후 완전한 하루가 된 첫 날이 제1일입니다.). 집 안에서 다른 사람들과 함께 있어야 한다면 밀착력이 좋은 마스크를 착용하고 자신의 증상을 모니터링하십시오.**
@@ -4330,8 +4330,8 @@
 Wear a high-quality mask if you must be around others in your facility and monitor your symptoms. If you are unable to wear a mask when around others, you should continue to isolate for a full 10 days. Your facility may have more specific guidance. Please follow the guidance of your facility while exercising caution.</v>
       </c>
       <c r="C185" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Los CDC recomiendan que usted se aísle y permanezca lejos de las demás personas en su establecimiento por al menos 5 días (para calcular su periodo de aislamiento de 5 días, el día 0 es el primer día de síntomas o el día de la prueba que dio positivo si es asintomático. El día 1 es el primer día completo después de que presentó síntomas o de la prueba que dio positivo). Si está inmunodeprimido o tiene síntomas de COVID-19 de moderados a graves, deberá aislarse por al menos 10 días y consultar a un proveedor de atención médica sobre cuándo estaría bien terminar su aislamiento.**
-**Use una mascarilla bien ajustada si tiene que estar alrededor de otras personas en su casa y vigile sus síntomas. Si no puede usar una mascarilla cuando esté alrededor de los demás, debe continuar el aislamiento por 10 días completos. Puede que su establecimiento tenga directrices más específicas. Siga las directrices de su establecimiento cuanto tome precauciones.**</v>
+        <v xml:space="preserve">**Los CDC recomiendan que usted se aísle y se mantenga alejado de las demás personas en su establecimiento por al menos 5 días.** Para calcular su periodo de aislamiento de 5 días, el día 0 es el primer día de síntomas o el día de la prueba que dio positivo si no tiene síntomas. El día 1 es el primer día completo después de que presentó síntomas o de la prueba que dio positivo. Si está inmunodeprimido o tiene síntomas de COVID-19 de moderados a graves, deberá aislarse por al menos 10 días y consultar a un proveedor de atención médica sobre cuándo sería adecuado terminar su aislamiento.
+Use una mascarilla de alta calidad si tiene que estar alrededor de otras personas en su establecimiento y vigile sus síntomas. Si no puede usar una mascarilla cuando esté alrededor de los demás, debe continuar el aislamiento por 10 días completos. Puede que su establecimiento tenga directrices más específicas. Siga las directrices de su establecimiento cuanto tome precauciones.</v>
       </c>
       <c r="D185" t="str" xml:space="preserve">
         <v xml:space="preserve">**CDC에서 권고하는 바에 따르면 귀하는 최소 5일 동안 확진 격리 조치를 실시하고 해당 시설 내에서 다른 사람들과의 거리를 두어야 합니다(5일간의 확진 격리 기간을 계산할 때, 증상이 나타난 첫 날 또는 증상이 없는 경우에는 검사 결과 양성 확진을 받은 날을 제0일로 계산합니다. 증상이 나타나거나 검사 결과 양성 확진을 받은 후 만 하루가 제1일입니다.). 면역력이 약화된 상태이거나 COVID-19의 중등증 내지 중증 증상이 있는 경우, 최소 10일 동안 확진 격리 조치를 실시하고, 본인이 확진 격리를 중단하기에 적절한 시기에 대해서는 의료인과 상의해야 합니다.**
@@ -4374,7 +4374,7 @@
         <v>**If you have developed new symptoms, you should isolate and get tested for COVID-19. Continue to stay home until you know the results.**</v>
       </c>
       <c r="C187" t="str">
-        <v>**Si presenta síntomas nuevos, deberá aislarse y hacerse la prueba de COVID-19. Siga quedándose en casa hasta que sepa los resultados.**</v>
+        <v>**Si presenta síntomas nuevos, deberá aislarse y hacerse la prueba de COVID-19. Siga quedándose en casa hasta que tenga los resultados.**</v>
       </c>
       <c r="D187" t="str">
         <v>**새로운 증상이 나타났다면, 확진 격리 조치를 실시하고 COVID-19 검사를 받으셔야 합니다. 결과를 알게 될 때까지 자택에서 계속 대기하시기 바랍니다.**</v>
@@ -4394,7 +4394,7 @@
         <v>**Until you are able to receive results of a COVID-19 test, isolate and stay away from others for at least 5 full days from when you began to experience symptoms.** If you still do not have the results of a COVID-19 tests, wear a high-quality mask when around others at home and in public for an additional 5 days. Do not go to places where you are not able to wear a mask, avoid travel, and avoid being around people who are more likely to get very sick from COVID-19. To calculate your 5-day isolation period, day 0 is your first day of symptoms. Day 1 is the first full day after your symptoms developed.</v>
       </c>
       <c r="C188" t="str">
-        <v>**Hasta que pueda recibir los resultados de  la prueba de COVID-19, aíslese y permanezca lejos de otras personas por al menos 5 días completos desde que comenzó a tener síntomas. Si todavía no tiene los resultados de la prueba de COVID-19, use una mascarilla cuando esté alrededor de otras personas en casa y en sitios públicos por otros 5 días. No vaya a sitios donde no pueda usar una mascarilla, evite viajar y estar alrededor de personas que estén en alto riesgo. Para calcular su periodo de aislamiento de 5 días, el día 0 es el primer día de síntomas. El día 1 es el primer día completo después de que presentó síntomas.**</v>
+        <v>**Hasta que pueda recibir los resultados de la prueba de COVID-19, aíslese y manténgase alejado de otras personas por al menos 5 días completos desde que comenzó a tener síntomas.** Si todavía no tiene los resultados de la prueba de COVID-19, use una mascarilla de alta calidad cuando esté alrededor de otras personas en casa y en sitios públicos por otros 5 días. No vaya a sitios donde no pueda usar una mascarilla, evite viajar y estar alrededor de personas que tengan más probabilidad de enfermarse gravemente de COVID-19. Para calcular su periodo de aislamiento de 5 días, el día 0 es el primer día de síntomas. El día 1 es el primer día completo después de que presentó síntomas.</v>
       </c>
       <c r="D188" t="str">
         <v>**COVID-19 검사 결과를 받을 수 있을 때까지, 증상이 나타나기 시작한 날로부터 최소 만 5일 동안 확진 격리 조치를 실시하고 다른 사람과의 거리를 두십시오. 아직 COVID-19 검사 결과가 나오지 않았다면, 추가로 5일 동안 집에서 그리고 공공 장소에서 다른 사람들이 주변에 있을 때 마스크를 착용하십시오. 마스크를 착용 할 수 없는 장소에 가지 말고, 여행을 삼가며, 고위험군에 해당하는 사람 주변에 있지 마십시오. 5일간의 확진 격리 기간을 계산할 때, 증상이 나타난 첫 날을 제0일로 계산합니다. 증상이 나타난 후 만 하루가 제1일입니다.**</v>
@@ -4434,7 +4434,7 @@
         <v>**Call your medical provider, clinician advice line, or telemedicine provider as soon as possible.** You also have medical conditions that may put you at risk of becoming more seriously ill.</v>
       </c>
       <c r="C190" t="str">
-        <v>** Llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina lo más pronto posible.** También tiene afecciones que podrían ponerlo en un mayor riesgo de enfermarse gravemente.</v>
+        <v>**Llame a su proveedor médico, a una línea de asesoría clínica o a un proveedor de telemedicina lo más pronto posible.** También tiene afecciones que podrían ponerlo en un mayor riesgo de enfermarse gravemente.</v>
       </c>
       <c r="D190" t="str">
         <v>**가능한 한 빨리 귀하의 의료진, 임상의 상담 전화 또는 원격 의료 제공자에게 전화하십시오.** 또한 귀하에게는 중대한 질병으로 악화될 수 있는 질환도 있습니다.</v>
@@ -4580,7 +4580,7 @@
         <v xml:space="preserve">La finalidad del Autoverificador del Coronavirus es ayudarlo a tomar decisiones sobre la obtención de atención médica adecuada. Este sistema no se ha diseñado para fines de diagnóstico o tratamiento de enfermedades, incluido el COVID-19.
 Este proyecto ha sido posible mediante la colaboración con la Fundación de los CDC y se ha habilitado a través de la plataforma Azure de Microsoft. La colaboración de los CDC con una organización no federal no implica el respaldo a ningún servicio, producto o empresa específicos.
 Para continuar usando esta herramienta, confirme que ha leído y entendido el contenido de este descargo de responsabilidad.
-###### ver73 (06.22.2022)</v>
+###### ver74 (9.12.2022)</v>
       </c>
       <c r="D197" t="str" xml:space="preserve">
         <v xml:space="preserve">Coronavirus Self-Checker의 목적은 적절한 의료 서비스를 찾는 것에 대한 결정을 내리는 데 도움을 주기 위한 것입니다. 이 시스템은 COVID-19를 포함한 질병의 진단 또는 치료를 위한 것이 아닙니다.
@@ -4607,8 +4607,7 @@
       </c>
       <c r="B198" t="str" xml:space="preserve">
         <v xml:space="preserve">**Steps to follow every day:**
-- Stay up to date on vaccination, including recommended booster doses. You are up to date if you have 
-completed a primary series and received the most recent booster dose recommended for you by CDC.
+- Stay up to date on vaccination, including recommended booster doses. You are up to date if you have completed a primary series and received the most recent booster dose recommended for you by CDC.
 - Maintain ventilation improvements.
 - Avoid contact with people who have suspected or confirmed COVID-19.
 - Follow recommendations for isolation if you have suspected or confirmed COVID-19.
@@ -4629,19 +4628,19 @@
       </c>
       <c r="C198" t="str" xml:space="preserve">
         <v xml:space="preserve">**Medidas para tomar todos los días:**
-- **Vacúnese contra el COVID-19** apenas pueda y póngase las dosis de refuerzo recomendadas cuando sea elegible. Por lo general, se considera que usted está al día con la vacunación contra el COVID-19 si ha recibido [todas las vacunas contra el COVID-19 recomendadas](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html), incluidas todas las dosis de refuerzo, cuando sea elegible.
-- **Use** una mascarilla bien ajustada que le cubra la nariz y la boca cuando esté en sitios cerrados con otras personas si está en un área donde el nivel de COVID-19 en la comunidad sea alto.
-- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted.
-- **Evite** lugares con mucha gente y áreas con poca ventilación.
-- **Lávese** las manos frecuentemente con agua y jabón por al menos 20 segundos o use un desinfectante de manos que contenga al menos un 60 % de alcohol.
-**Haga clic en los enlaces a continuación para obtener más información sobre lo siguiente:**
+- Mantenerse al día con las vacunas, incluso las dosis de refuerzo recomendadas. Usted está al día si ha completado una serie primaria y recibido la dosis de refuerzo más reciente que los CDC hayan recomendado para usted.
+- Mantener las mejoras en la ventilación.
+- Evitar el contacto con las personas con COVID-19 presunto o confirmado.
+- Seguir las recomendaciones de aislamiento si usted tiene COVID-19 presunto o confirmado.
+- Seguir las recomendaciones acerca de qué hacer si se expone a alguien con COVID-19.
+- Si está en alto riesgo de enfermarse gravemente, hable con un proveedor de atención médica acerca de medidas de prevención adicionales.
+**Seleccione los enlaces a continuación para obtener más información sobre lo siguiente:**
 - [Síntomas del COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/symptoms-testing/symptoms.html)
-- [Afecciones posteriores al COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)
+- [Afecciones pos-COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/long-term-effects.html)
 - [Cuándo hacerse la prueba](https://espanol.cdc.gov/coronavirus/2019-ncov/testing/diagnostic-testing.html)
-- [Lo que significan los resultados de su prueba](https://www.cdc.gov/coronavirus/2019-ncov/downloads/What-Your-Test-Results-Mean.pdf)
 - [Cómo protegerse a sí mismo y a los demás para que no se enfermen](https://espanol.cdc.gov/coronavirus/2019-ncov/prevent-getting-sick/prevention.html)
-- [Cuándo ponerse en cuarentena o aislarse, y por cuánto tiempo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
-- [Qué hacer si estuvo cerca de alguien con COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
+- [Cuándo aislarse y por cuánto tiempo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
+- [Qué hacer si se expuso al COVID-19](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/quarantine.html)
 - [Cómo cuidarse cuando esté enfermo](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/steps-when-sick.html)
 - [Cómo cuidar a otra persona que esté enferma](https://espanol.cdc.gov/coronavirus/2019-ncov/if-you-are-sick/care-for-someone.html)
 - [Tratamientos que su proveedor de atención médica podría recomendarle si está enfermo](https://espanol.cdc.gov/coronavirus/2019-ncov/your-health/treatments-for-severe-illness.html)
@@ -4737,11 +4736,13 @@
       <c r="A200" t="str">
         <v>CDC/messages/intro_msg_title</v>
       </c>
-      <c r="B200" t="str">
-        <v>Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the steps you should take to protect yourself and others from COVID-19. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again.</v>
+      <c r="B200" t="str" xml:space="preserve">
+        <v xml:space="preserve">Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the steps you should take to protect yourself and others from COVID-19. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again.
+If you are experiencing a life-threatening emergency, please call 911 immediately.
+If you are not experiencing a life-threatening emergency, let’s get started.</v>
       </c>
       <c r="C200" t="str" xml:space="preserve">
-        <v xml:space="preserve">Hola, me llamo Clara. Le voy a hacer algunas preguntas. Usaré sus respuestas para aconsejarle sobre el nivel de atención médica que debe buscar. Si está respondiendo por alguien más, responda todas las preguntas como si fuera esa persona. Si necesita comenzar de nuevo, refresque la página y comience otra vez.
+        <v xml:space="preserve">Hola, me llamo Clara. Le voy a hacer algunas preguntas. Usaré sus respuestas para aconsejarle sobre las medidas que debería tomar para protegerse y proteger a los demás del COVID-19. Si está respondiendo por alguien más, responda todas las preguntas como si fuera esa persona. Si necesita comenzar de nuevo, refresque la página y comience otra vez.
 Si tiene una emergencia potencialmente mortal, llame al 911 inmediatamente.
 Si no tiene una emergencia potencialmente mortal, comencemos.</v>
       </c>
@@ -4767,8 +4768,7 @@
       </c>
       <c r="B201" t="str" xml:space="preserve">
         <v xml:space="preserve">**CDC recommends these steps to protect you and others from COVID-19:**
-- **Stay up to date on vaccination, including recommended booster doses. You are up to date if you have completed a 
-primary series and received the most recent booster dose recommended for you by CDC.**
+- **Stay up to date on vaccination, including recommended booster doses. You are up to date if you have completed a primary series and received the most recent booster dose recommended for you by CDC.**
 - **Maintain ventilation improvements.**
 - **Avoid contact with people who have suspected or confirmed COVID-19.**
 - **Follow recommendations for isolation if you have suspected or confirmed COVID-19.**
@@ -4777,12 +4777,13 @@
 </v>
       </c>
       <c r="C201" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Los CDC recomiendan que tome estas medidas para reducir el riesgo de contraer o propagar el COVID-19:**
-- **Vacúnese contra el COVID-19** apenas pueda y póngase las dosis de refuerzo recomendadas cuando sea elegible. Por lo general, se considera que usted está al día con la vacunación contra el COVID-19 si ha recibido [todas las vacunas contra el COVID-19 recomendadas](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html), incluidas todas las dosis de refuerzo, cuando sea elegible.
-- **Use** una mascarilla bien ajustada que le cubra la nariz y la boca cuando esté en sitios cerrados con otras personas si está en un área donde el nivel de COVID-19 en la comunidad sea alto.
-- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted.
-- **Evite** lugares con mucha gente y áreas con poca ventilación.
-- **Lávese** las manos a menudo con agua y jabón, o use un desinfectante de manos que contenga al menos un 60 % de alcohol.</v>
+        <v xml:space="preserve">**Los CDC recomiendan estas medidas para protegerse y proteger a los demás del COVID-19:**
+- **Mantenerse al día con las vacunas, incluso las dosis de refuerzo recomendadas. Usted está al día si ha completado una serie primaria y recibido la dosis de refuerzo más reciente que los CDC hayan recomendado para usted.**
+- **Mantener las mejoras en la ventilación.**
+- **Evitar el contacto con las personas con COVID-19 presunto o confirmado.**
+- **Seguir las recomendaciones de aislamiento si usted tiene COVID-19 presunto o confirmado.**
+- **Seguir las recomendaciones acerca de qué hacer si se expone a alguien con COVID-19.**
+- **Si está en alto riesgo de enfermarse gravemente, hable con un proveedor de atención médica acerca de medidas de prevención adicionales.**</v>
       </c>
       <c r="D201" t="str" xml:space="preserve">
         <v xml:space="preserve">**COVID-19 감염 및 확산 위험을 줄이기 위해 CDC에서 권고하는 조치:**
@@ -4813,19 +4814,29 @@
       <c r="A202" t="str">
         <v>CDC/messages/intro_msg</v>
       </c>
-      <c r="B202" t="str">
-        <v>Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the steps you should take to protect yourself and others from COVID-19. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again.</v>
+      <c r="B202" t="str" xml:space="preserve">
+        <v xml:space="preserve">Hi, I’m Clara. I’m going to ask you some questions. I will use your answers to give you advice about the steps you should take to protect yourself and others from COVID-19. If answering for someone else, please respond to all questions as if you are them. If you need to start over, refresh the page and start again.
+If you are experiencing a life-threatening emergency, please call 911 immediately.
+If you are not experiencing a life-threatening emergency, let’s get started.
+**CDC recommends these steps to protect you and others from COVID-19:**
+- **Stay up to date on vaccination, including recommended booster doses. You are up to date if you have completed a primary series and received the most recent booster dose recommended for you by CDC.**
+- **Maintain ventilation improvements.**
+- **Avoid contact with people who have suspected or confirmed COVID-19.**
+- **Follow recommendations for isolation if you have suspected or confirmed COVID-19.**
+- **Follow the recommendations for what to do if you are exposed to someone with COVID-19.**
+- **If you are at high risk of getting very sick, talk with a healthcare provider about additional prevention actions.**</v>
       </c>
       <c r="C202" t="str" xml:space="preserve">
-        <v xml:space="preserve">Hola, me llamo Clara. Le voy a hacer algunas preguntas. Usaré sus respuestas para aconsejarlo sobre el nivel de atención médica que debe buscar. Si está respondiendo por alguien más, responda todas las preguntas como si fuera esa persona. Si necesita comenzar de nuevo, refresque la página y comience otra vez.
+        <v xml:space="preserve">Hola, me llamo Clara. Le voy a hacer algunas preguntas. Usaré sus respuestas para aconsejarle sobre las medidas que debería tomar para protegerse y proteger a los demás del COVID-19. Si está respondiendo por alguien más, responda todas las preguntas como si fuera esa persona. Si necesita comenzar de nuevo, refresque la página y comience otra vez.
 Si tiene una emergencia potencialmente mortal, llame al 911 inmediatamente.
 Si no tiene una emergencia potencialmente mortal, comencemos.
-**Los CDC recomiendan que tome estas medidas para reducir el riesgo de contraer o propagar el COVID-19:**
-- **Vacúnese contra el COVID-19** apenas pueda y póngase las dosis de refuerzo recomendadas cuando sea elegible. Por lo general, se considera que usted está al día con la vacunación contra el COVID-19 si ha recibido [todas las vacunas contra el COVID-19 recomendadas](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html), incluidas todas las dosis de refuerzo, cuando sea elegible.
-- **Use** una mascarilla bien ajustada que le cubra la nariz y la boca cuando esté en sitios cerrados con otras personas si está en un área donde el nivel de COVID-19 en la comunidad sea alto.
-- **Manténgase** al menos a 6 pies o 2 metros de las personas que no vivan con usted.
-- **Evite** lugares con mucha gente y áreas con poca ventilación.
-- **Lávese** las manos a menudo con agua y jabón, o use un desinfectante de manos que contenga al menos un 60 % de alcohol.</v>
+**Los CDC recomiendan estas medidas para protegerse y proteger a los demás del COVID-19:**
+- **Mantenerse al día con las vacunas, incluso las dosis de refuerzo recomendadas. Usted está al día si ha completado una serie primaria y recibido la dosis de refuerzo más reciente que los CDC hayan recomendado para usted.**
+- **Mantener las mejoras en la ventilación.**
+- **Evitar el contacto con las personas con COVID-19 presunto o confirmado.**
+- **Seguir las recomendaciones de aislamiento si usted tiene COVID-19 presunto o confirmado.**
+- **Seguir las recomendaciones acerca de qué hacer si se expone a alguien con COVID-19.**
+- **Si está en alto riesgo de enfermarse gravemente, hable con un proveedor de atención médica acerca de medidas de prevención adicionales.**</v>
       </c>
       <c r="D202" t="str" xml:space="preserve">
         <v xml:space="preserve">안녕하세요? 저는 Clara입니다. 몇 가지 질문을 하겠습니다. 귀하의 답변을 통해 귀하에게 어느 정도 수준의 진료가 필요한지 조언할 것입니다. 다른 사람을 위해 응답하고 계시다면 본인이 그 사람인 것처럼 모든 질문에 답하십시오. 처음부터 다시 시작해야 한다면 페이지를 새로 고치고 다시 시작하십시오. 
@@ -4970,7 +4981,7 @@
         <v>**Because some symptoms of flu and COVID-19 are similar, you may want to consider asking your provider about testing or treatment for influenza.** See this [CDC webpage](https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm) for more information about COVID-19 and influenza.</v>
       </c>
       <c r="C208" t="str">
-        <v>**Debido a que algunos de los síntomas de la influenza y del COVID-19 son similares, quizás considere preguntarle al proveedor sobre la prueba y el tratamiento de la influenza.** Consulte esta [página web de los CDC](https://espanol.cdc.gov/flu/symptoms/flu-vs-covid19.htm) para obtener más información sobre el COVID-19 y la influenza.</v>
+        <v>**Debido a que algunos de los síntomas de la influenza y del COVID-19 son similares, es recomendable que le pregunte a su proveedor si le aconseja la prueba o tratamiento para la influenza.** Consulte esta [página web de los CDC](https://espanol.cdc.gov/flu/symptoms/flu-vs-covid19.htm) para obtener más información sobre el COVID-19 y la influenza.</v>
       </c>
       <c r="D208" t="str">
         <v>**독감과 COVID-19의 일부 증상이 비슷하기 때문에 귀하는 제공자에게 인플루엔자 검사와 치료에 대해 문의할 것을 고려할 수 있습니다.** COVID-19와 인플루엔자에 대한 더 자세한 정보는 이 [CDC 웹페이지](https://www.cdc.gov/flu/symptoms/flu-vs-covid19.htm)를 확인하십시오.</v>
@@ -5125,7 +5136,7 @@
         <v>**Regardless of vaccination status or prior infection, you may need to be tested again if there is no other cause identified for your symptoms.** Consider getting tested again for SARS-CoV-2 infection to consider the possibility of reinfection.</v>
       </c>
       <c r="C215" t="str">
-        <v>**Independientemente de si se ha vacunado o si tuvo una infección anterior, usted podría necesitar hacerse la prueba de nuevo si no hay otra causa identificada para sus síntomas.** Pregúntele a su proveedor de atención médica acerca de volver a hacerse la prueba de la infección por SARS-CoV-2 para considerar la posibilidad de reinfección.</v>
+        <v>**Independientemente de si se ha vacunado o si tuvo una infección anterior, usted podría necesitar hacerse la prueba de nuevo si no hay otra causa identificada para sus síntomas.** Considere volver a hacerse la prueba de la infección por SARS-CoV-2 debido a la posibilidad de reinfección.</v>
       </c>
       <c r="D215" t="str">
         <v>**백신 접종 상태 또는 이전 감염 여부와 상관없이, 나타난 증상의 다른 원인이 확인되지 않으면 검사를 다시 받아야 할 수 있습니다.** 재감염 가능성을 알아보려면 담당 의료서비스 제공자에게 SARS-CoV-2 감염 관련 재검사에 대해서 문의하시기 바랍니다.</v>
@@ -5165,7 +5176,7 @@
         <v>**If you have questions, talk with your healthcare provider about your test result and the type of test you took to understand what your results mean.**</v>
       </c>
       <c r="C217" t="str">
-        <v>**Hable con su proveedor de atención médica acerca de los resultados de su prueba y el tipo de prueba que se hizo para entender el significado de sus resultados.**</v>
+        <v>**Si tiene preguntas, hable con su proveedor de atención médica acerca de los resultados de su prueba y el tipo de prueba que se hizo para entender lo que significan esos resultados.**</v>
       </c>
       <c r="D217" t="str">
         <v>**담당 의료 서비스 제공자와 진행한 검사 종류 및 결과와 관련한 상담을 통해 검사 결과가 의미하는 바에 대해 알아보시기 바랍니다.**</v>
@@ -5185,7 +5196,7 @@
         <v>**If there is no other cause identified for your symptoms, consider getting tested again.** If you have questions, talk with your healthcare provider about your test result and the type of test you took to understand what your results mean.</v>
       </c>
       <c r="C218" t="str">
-        <v>**Si no se ha identificado otra causa para sus síntomas. Pregúntele a su proveedor de atención médica acerca de volver a hacerse la prueba.** Hable con su proveedor de atención médica acerca de los resultados de su prueba y el tipo de prueba que se hizo para entender el significado de sus resultados.</v>
+        <v>**Si no se ha identificado otra causa para sus síntomas, considere volver a hacerse la prueba.** Si tiene preguntas, hable con su proveedor de atención médica acerca de los resultados de su prueba y el tipo de prueba que se hizo para entender lo que significan esos resultados.</v>
       </c>
       <c r="D218" t="str">
         <v>**나타난 증상의 다른 원인이 확인되지 않은 경우. 담당 의료 전문가에게 재검사에 대해 문의하십시오.**담당 의료 서비스 제공자와 진행한 검사 종류 및 결과와 관련한 상담을 통해 검사 결과가 의미하는 바에 대해 알아보시기 바랍니다.</v>
@@ -5344,7 +5355,7 @@
         <v>If you continue to have no COVID-19 symptoms, you do not need to quarantine or get tested unless recommended or required by your healthcare provider, employer, or public health official.</v>
       </c>
       <c r="C224" t="str">
-        <v>**Si sigue sin síntomas de COVID-19, no necesita ponerse en cuarentena ni hacerse la prueba a menos que se lo recomiende o exija su proveedor de atención médica, empleador o funcionario de salud pública.**</v>
+        <v>Si sigue sin síntomas de COVID-19, no necesita ponerse en cuarentena ni hacerse la prueba a menos que se lo recomiende o exija su proveedor de atención médica, empleador o funcionario de salud pública.</v>
       </c>
       <c r="D224" t="str">
         <v>**귀하에게 더이상의 COVID-19 증상이 없는 경우, 귀하의 의료 서비스 제공자, 고용주, 또는 공중 보건 당국이 권고하거나 요구하지 않는 한 자가격리 또는 검사를 받을 필요가 없습니다.**</v>
@@ -5364,7 +5375,7 @@
         <v>Based on the answers given, you do not need to quarantine or get tested unless recommended or required by your healthcare provider, employer, or public health official.</v>
       </c>
       <c r="C225" t="str">
-        <v>**Según las respuestas que nos ha dado, no necesita ponerse en cuarentena ni hacerse la prueba a menos que se lo recomiende o exija su proveedor de atención médica, empleador o funcionario de salud pública.**</v>
+        <v>Según las respuestas que nos ha dado, no necesita ponerse en cuarentena ni hacerse la prueba a menos que se lo recomiende o exija su proveedor de atención médica, empleador o funcionario de salud pública.</v>
       </c>
       <c r="D225" t="str">
         <v>**귀하가 제공한 답변에 따르면, 귀하는 귀하의 의료 서비스 제공자, 고용주, 또는 공중 보건 당국이 권고하거나 요구하지 않는 한 자가격리 또는 검사를 받을 필요가 없습니다.**</v>
@@ -5494,6 +5505,9 @@
       <c r="B231" t="str">
         <v>**Because you are experiencing symptoms of COVID-19, you should isolate from others immediately.** You should continue to isolate, wearing a high-quality mask if you must be around others, until you are able to receive results of a COVID-19 test.</v>
       </c>
+      <c r="C231" t="str">
+        <v>**Debido a que usted tiene síntomas de COVID-19, deberá aislarse de los demás inmediatamente.** Deberá seguir aislándose y usar una mascarilla de alta calidad si tiene que estar alrededor de otras personas, hasta que pueda recibir los resultados de la prueba de COVID-19.</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
@@ -5501,6 +5515,9 @@
       </c>
       <c r="B232" t="str">
         <v>**Because you were or may have been exposed to someone with COVID-19, CDC recommends you wear a high-quality mask when around others for 10 full days after your exposure.  You should get tested 5 full days after you were exposed to someone with COVID-19, even if you don’t develop symptoms. If you do develop symptoms, isolate immediately and get tested.** For 10 full days following exposure, you should also take extra precautions with travel or if you will be around people who are more likely to get very sick from COVID-19.</v>
+      </c>
+      <c r="C232" t="str">
+        <v>**Debido a que usted estuvo o puede haber estado expuesto a alguien con COVID-19, los CDC recomiendan que use una mascarilla de alta calidad cuando esté alrededor de otras personas por 10 días completos después de su exposición.  Debería hacerse la prueba después de 5 días completos de haber estado expuesto a alguien con COVID-19, aunque no presente síntomas. Si presenta síntomas, aíslese inmediatamente y hágase la prueba.** Por 10 días completos después de la exposición, también deberá tomar precauciones adicionales con los viajes o si va a estar alrededor de personas que tengan más probabilidad de enfermarse gravemente de COVID-19.</v>
       </c>
     </row>
     <row r="233">
@@ -5857,7 +5874,7 @@
         <v>["Younger than 2 years","2-4 years","5-9 years","10-12 years","13-17 years","18-29 years","30-39 years","40-49 years","50-59 years","60-64 years","65-69 years","70-79 years","80+ years"]</v>
       </c>
       <c r="C249" t="str">
-        <v>["Menor de 2 años","2-4","5-9","10-12","13-17","18-29","30-39","40-49","50-59","60-64","65-69","70-79","80+"]</v>
+        <v>["Menores de 2 años","2-4 años","5-9 años","10-12 años","13-17 años","18-29 años","30-39 años","40-49 años","50-59 años","60-64 años","65-69 años","70-79 años","80 años o más"]</v>
       </c>
       <c r="D249" t="str">
         <v>["2세 미만", "2-4", "5-9", "10-12", "13-17", "18-29", "30-39", "40-49" , "50-59", "60-64", "65-69", "70-79", "80 이상"]</v>
@@ -6019,6 +6036,9 @@
       <c r="B257" t="str">
         <v>Asthma</v>
       </c>
+      <c r="C257" t="str">
+        <v>Asma</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
@@ -6047,6 +6067,9 @@
       <c r="B259" t="str">
         <v>Cystic fibrosis</v>
       </c>
+      <c r="C259" t="str">
+        <v>Fibrosis quística</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
@@ -6536,7 +6559,7 @@
         <v>Immunocompromised state (weakened immune system) or use of immunosuppressant medication</v>
       </c>
       <c r="C284" t="str">
-        <v>Estado inmunodeprimido (sistema inmunitario debilitado)</v>
+        <v>Estado de inmunodepresión (sistema inmunitario debilitado) o uso de medicamentos inmunodepresores</v>
       </c>
       <c r="D284" t="str">
         <v>면역저하 상태(쇠약한 면역계)</v>
@@ -7987,10 +8010,10 @@
         <v xml:space="preserve">¿Tiene alguno de estos síntomas potencialmente mortales?
 - Dificultad para respirar
 - Dolor o presión persistentes en el pecho
-- Estado de confusión de aparición reciente
-- No puede despertarse o permanecer despierto
-- Color pálido, gris o azulado de la piel, los labios, o el lecho de las uñas, dependiendo del tono de piel
-*Esta lista no incluye todos los síntomas posibles. Llame a su proveedor de atención médica en el caso de que tenga cualquier otro síntoma que sea grave o que le preocupe.</v>
+- Confusión de aparición reciente
+- No poder despertarse o permanecer despierto
+- Color pálido, gris o azulado de la piel, los labios o el lecho de las uñas, dependiendo del tono de piel
+*Esta lista no tiene todos los síntomas posibles. Llame a un proveedor de atención médica si tiene algún síntoma grave o que le preocupe.</v>
       </c>
       <c r="D356" t="str" xml:space="preserve">
         <v xml:space="preserve">이러한 생명을 위협하는 증상이 있습니까?
@@ -8421,9 +8444,8 @@
       <c r="B375" t="str">
         <v>In the last two weeks, have you been [exposed to](https://www.cdc.gov/coronavirus/2019-ncov/your-health/risks-exposure.html) COVID-19?</v>
       </c>
-      <c r="C375" t="str" xml:space="preserve">
-        <v xml:space="preserve">En las últimas dos semanas, ¿ha estado en contacto cercano con alguien que tuviera COVID-19?
-Usted tuvo contacto cercano si estuvo a menos de 6 pies o 2 metros de una persona infectada (con confirmación en laboratorio o diagnóstico clínico) por un total acumulado de 15 minutos o más durante un periodo de 24 horas. El contacto cercano no incluye la exposición dentro de un entorno de salones de clase K-12 cerrados, si tanto el estudiante infectado como los expuestos   usaron correctamente y de manera constante mascarillas que se ajustaban bien todo el tiempo.</v>
+      <c r="C375" t="str">
+        <v>En las últimas dos semanas, ¿ha estado [expuesto al](https://espanol.cdc.gov/coronavirus/2019-ncov/your-health/risks-exposure.html) COVID-19?</v>
       </c>
       <c r="D375" t="str" xml:space="preserve">
         <v xml:space="preserve">지난 2주 동안, COVID-19에 걸린 사람과 밀접하게 접촉한 적이 있습니까?
@@ -8556,7 +8578,7 @@
         <v>In the last two weeks, have you worked or volunteered in a healthcare facility? Healthcare facilities include a hospital, medical or dental clinic, long-term care facility, or nursing home.</v>
       </c>
       <c r="C381" t="str">
-        <v>En las últimas dos semanas, ¿ha trabajado o ha realizado tareas de voluntariado en un establecimiento de atención médica o como personal de respuesta? Los establecimientos de atención médica incluyen hospitales, otros entornos médicos (incluidos los entornos de atención dental) o establecimientos de cuidados a largo plazo.</v>
+        <v>En las últimas dos semanas, ¿ha trabajado o ha servido como voluntario en un establecimiento de atención médica? Los establecimientos de atención médica incluyen hospitales, centros médicos o dentales, establecimientos de cuidados a largo plazo u hogares de ancianos.</v>
       </c>
       <c r="D381" t="str">
         <v>지난 2주 동안 의료 시설에서 또는 초동 대응자로서 일하거나 자원봉사한 적이 있습니까? 의료 시설에는 병원, 기타 의료 시설(치과 치료 시설 포함) 또는 장기 요양 시설이 포함됩니다.</v>
@@ -8636,7 +8658,7 @@
         <v>Do you live in a long-term care facility, nursing home, correctional facility, or homeless shelter?</v>
       </c>
       <c r="C385" t="str">
-        <v>¿Vive en un establecimiento de cuidados a largo plazo, hogar de ancianos o refugio para personas “sin hogar"?</v>
+        <v>¿Vive en un establecimiento de cuidados a largo plazo, hogar de ancianos, centro correccional o refugio para personas sin hogar?</v>
       </c>
       <c r="D385" t="str">
         <v>장기 요양 시설, 요양원 또는 노숙자 보호소에 살고 있습니까?</v>
@@ -8926,14 +8948,8 @@
       <c r="B397" t="str">
         <v>**Are you up to date with your COVID-19 vaccination, [meaning you have completed a primary series and received the most recent booster dose recommended for you by CDC?](https://www.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html)**</v>
       </c>
-      <c r="C397" t="str" xml:space="preserve">
-        <v xml:space="preserve">**Vacunas contra el COVID-19:**
-Por lo general, se considera que usted está al día si ha [recibido todas las vacunas contra el COVID-19 recomendadas](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html), incluida alguna dosis de refuerzo, cuando sea elegible. Si usted todavía no es elegible para recibir la dosis de refuerzo, está al día si ha recibido la serie primaria ( 2 o 3 dosis iniciales) de las vacunas contra el COVID-19 Pfizer-BioNTech (COMIRNATY) o Moderna, o una dosis única de la vacuna Janssen de Johnson &amp; Johnson hace más de 2 semanas.
-- Por lo general, los adultos de 18 años o más que **no** están moderada o gravemente inmunodeprimidos son elegibles para la dosis de refuerzo 5 meses después de recibir la segunda dosis de las vacunas Pfizer-BioNTech o Moderna, o 2 meses después de recibir la vacuna contra el COVID-19 Janssen (Johnson &amp; Johnson). 
-- Los niños y adolescentes de 5-17 años son elegibles para la dosis de refuerzo 5 meses después de recibir la segunda dosis de las vacunas Pfizer-BioNTech o Moderna. 
-- Los niños de 6 meses a 4 años son elegibles para la serie primaria (2 o 3 dosis iniciales) de las vacunas contra el COVID-19 Pfizer-BioNTech (COMIRNATY) o Moderna, pero no son todavía elegibles para recibir las dosis de refuerzo.
-- Las personas de 12 años o más que están moderada o gravemente inmunodeprimidas deben recibir un total de 5 dosis de una vacuna de ARNm contra el COVID-19 para estar al día. Las 5 dosis incluyen una serie primaria de 3 dosis de las vacunas contra el COVID-19 Pfizer-BioNTech o Moderna, más 2 dosis de refuerzo de las vacunas contra el COVID-19 Pfizer-BioNTech o Moderna.
-**¿Está al día con su vacunación contra el COVID-19?**</v>
+      <c r="C397" t="str">
+        <v>**¿Está al día con sus vacunas contra el COVID-19 [es decir que ha completado una serie primaria y recibido la dosis de refuerzo más reciente que los CDC recomendaron para usted?](https://espanol.cdc.gov/coronavirus/2019-ncov/vaccines/stay-up-to-date.html)**</v>
       </c>
       <c r="D397" t="str" xml:space="preserve">
         <v xml:space="preserve">**COVID-19 백신 접종:**
@@ -9496,9 +9512,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15809456-590D-4655-B169-3C26C3F68525}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498C317F-11CE-473C-A237-D81A7B01AB16}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DA9DE58-A3CC-4BE3-90EC-9DF366850955}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63D0098-0F40-41B8-B376-FE23BB88FBA7}"/>
 </file>
</xml_diff>